<commit_message>
se agrego el calculo del punto de equilibrio
</commit_message>
<xml_diff>
--- a/Analisis_financiero_Inclusoft_test.xlsx
+++ b/Analisis_financiero_Inclusoft_test.xlsx
@@ -5,15 +5,15 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Andres Santana\Documents\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Andres Santana\Dropbox\PROYECTO INCLUSOFT\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="21570" windowHeight="8145" tabRatio="920" firstSheet="3" activeTab="10"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="21570" windowHeight="8145" tabRatio="920" firstSheet="3" activeTab="9"/>
   </bookViews>
   <sheets>
-    <sheet name="Tabla Crecimiento" sheetId="11" r:id="rId1"/>
-    <sheet name="Presupuesto Inicial" sheetId="1" r:id="rId2"/>
+    <sheet name="Presupuesto Inicial" sheetId="1" r:id="rId1"/>
+    <sheet name="Tabla Crecimiento" sheetId="11" r:id="rId2"/>
     <sheet name="Salarios, gastos y costos" sheetId="3" r:id="rId3"/>
     <sheet name="Estado de situacion financiera " sheetId="2" r:id="rId4"/>
     <sheet name="Prestamo" sheetId="14" r:id="rId5"/>
@@ -23,9 +23,10 @@
     <sheet name="Flujo de caja - 5 años" sheetId="6" r:id="rId9"/>
     <sheet name="Flujo de Caja (Profesor) - 5 añ" sheetId="7" r:id="rId10"/>
     <sheet name="VAN y TIR" sheetId="9" r:id="rId11"/>
-    <sheet name="Balance General" sheetId="10" r:id="rId12"/>
-    <sheet name="Calculo % Rentabilidad" sheetId="12" r:id="rId13"/>
-    <sheet name="Análisis metros cuadrados" sheetId="13" r:id="rId14"/>
+    <sheet name="Punto de Equilibrio" sheetId="15" r:id="rId12"/>
+    <sheet name="Balance General" sheetId="10" r:id="rId13"/>
+    <sheet name="Calculo % Rentabilidad" sheetId="12" r:id="rId14"/>
+    <sheet name="Análisis metros cuadrados" sheetId="13" r:id="rId15"/>
   </sheets>
   <calcPr calcId="152511"/>
 </workbook>
@@ -55,7 +56,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="424" uniqueCount="286">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="451" uniqueCount="296">
   <si>
     <t xml:space="preserve">Concepto
 </t>
@@ -720,12 +721,6 @@
     <t>Equipos</t>
   </si>
   <si>
-    <t>Admon</t>
-  </si>
-  <si>
-    <t>Gastos ventas</t>
-  </si>
-  <si>
     <t>TOTAL COSTO AÑO DE PRODUCCION</t>
   </si>
   <si>
@@ -925,6 +920,42 @@
   </si>
   <si>
     <t>CONCEPTO</t>
+  </si>
+  <si>
+    <t>Pago de alojamiento servidor</t>
+  </si>
+  <si>
+    <t>Punto de Equilibrio</t>
+  </si>
+  <si>
+    <t>Ingresos Totales</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Costos Variables </t>
+  </si>
+  <si>
+    <t>PE capacidad instalada</t>
+  </si>
+  <si>
+    <t>Sueldos</t>
+  </si>
+  <si>
+    <t>Depreciacion</t>
+  </si>
+  <si>
+    <t>Capacidad Instalada</t>
+  </si>
+  <si>
+    <t>Capacidad a Producir</t>
+  </si>
+  <si>
+    <t>Precio Unitario Promedio</t>
+  </si>
+  <si>
+    <t>Costo Variable Unitario</t>
+  </si>
+  <si>
+    <t>Costos Totales</t>
   </si>
 </sst>
 </file>
@@ -944,9 +975,9 @@
     <numFmt numFmtId="171" formatCode="_-[$$-240A]\ * #,##0.000_-;\-[$$-240A]\ * #,##0.000_-;_-[$$-240A]\ * &quot;-&quot;??_-;_-@_-"/>
     <numFmt numFmtId="172" formatCode="_-[$$-240A]\ * #,##0.000_-;\-[$$-240A]\ * #,##0.000_-;_-[$$-240A]\ * &quot;-&quot;???_-;_-@_-"/>
     <numFmt numFmtId="173" formatCode="_-[$$-240A]\ * #,##0_-;\-[$$-240A]\ * #,##0_-;_-[$$-240A]\ * &quot;-&quot;??_-;_-@_-"/>
-    <numFmt numFmtId="176" formatCode="0.0"/>
+    <numFmt numFmtId="174" formatCode="0.0"/>
   </numFmts>
-  <fonts count="26">
+  <fonts count="27">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -1087,6 +1118,13 @@
       <color theme="1"/>
       <name val="Arial"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="6">
     <fill>
@@ -1118,7 +1156,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="18">
+  <borders count="30">
     <border>
       <left/>
       <right/>
@@ -1341,16 +1379,161 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="double">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="double">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="double">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="double">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="double">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="double">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="double">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="6">
+  <cellStyleXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="44" fontId="17" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="18" fillId="3" borderId="11" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="19" fillId="4" borderId="12" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="9" fontId="17" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="43" fontId="17" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="222">
+  <cellXfs count="250">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1647,7 +1830,6 @@
     <xf numFmtId="0" fontId="10" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="164" fontId="10" fillId="0" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="164" fontId="10" fillId="0" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="4" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="169" fontId="0" fillId="0" borderId="0" xfId="4" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
@@ -1668,6 +1850,11 @@
     </xf>
     <xf numFmtId="170" fontId="19" fillId="4" borderId="12" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="173" fontId="19" fillId="4" borderId="12" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="174" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="170" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="2" fontId="4" fillId="0" borderId="0" xfId="4" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1764,17 +1951,72 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="18" fillId="3" borderId="17" xfId="2" applyBorder="1"/>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="164" fontId="8" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="4" borderId="19" xfId="3" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="4" borderId="20" xfId="3" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="4" borderId="21" xfId="3" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="3" borderId="22" xfId="2" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="3" borderId="23" xfId="2" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="170" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="170" fontId="0" fillId="0" borderId="25" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="25" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="170" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="170" fontId="0" fillId="0" borderId="25" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="27" xfId="6" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="28" xfId="6" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="170" fontId="26" fillId="0" borderId="28" xfId="6" applyNumberFormat="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="170" fontId="26" fillId="0" borderId="29" xfId="6" applyNumberFormat="1" applyBorder="1" applyAlignment="1"/>
   </cellXfs>
-  <cellStyles count="6">
+  <cellStyles count="7">
     <cellStyle name="Celda de comprobación" xfId="3" builtinId="23"/>
     <cellStyle name="Millares" xfId="5" builtinId="3"/>
     <cellStyle name="Moneda" xfId="1" builtinId="4"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Porcentaje" xfId="4" builtinId="5"/>
     <cellStyle name="Salida" xfId="2" builtinId="21"/>
+    <cellStyle name="Texto de advertencia" xfId="6" builtinId="11"/>
   </cellStyles>
   <dxfs count="42">
     <dxf>
@@ -2715,8 +2957,8 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="315068744"/>
-        <c:axId val="315070312"/>
+        <c:axId val="292692920"/>
+        <c:axId val="292688608"/>
         <c:extLst>
           <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
             <c15:filteredBarSeries>
@@ -2804,7 +3046,7 @@
         </c:extLst>
       </c:barChart>
       <c:catAx>
-        <c:axId val="315068744"/>
+        <c:axId val="292692920"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2903,7 +3145,7 @@
             <a:endParaRPr lang="es-ES"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="315070312"/>
+        <c:crossAx val="292688608"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -2911,7 +3153,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="315070312"/>
+        <c:axId val="292688608"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3025,7 +3267,7 @@
             <a:endParaRPr lang="es-ES"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="315068744"/>
+        <c:crossAx val="292692920"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -3474,11 +3716,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="315069528"/>
-        <c:axId val="315071488"/>
+        <c:axId val="292693312"/>
+        <c:axId val="292690960"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="315069528"/>
+        <c:axId val="292693312"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3593,7 +3835,7 @@
             <a:endParaRPr lang="es-ES"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="315071488"/>
+        <c:crossAx val="292690960"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -3601,7 +3843,7 @@
         <c:noMultiLvlLbl val="1"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="315071488"/>
+        <c:axId val="292690960"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3702,7 +3944,7 @@
             <a:endParaRPr lang="es-ES"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="315069528"/>
+        <c:crossAx val="292693312"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -5533,492 +5775,343 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:O35"/>
+  <dimension ref="A1:J25"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3:C13"/>
+    <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="B14" sqref="B14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1"/>
   <cols>
-    <col min="2" max="2" width="18.140625" customWidth="1"/>
-    <col min="8" max="8" width="17.7109375" customWidth="1"/>
-    <col min="14" max="14" width="23.85546875" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="19.140625" customWidth="1"/>
+    <col min="1" max="1" width="49.5703125" customWidth="1"/>
+    <col min="2" max="2" width="16.85546875" customWidth="1"/>
+    <col min="3" max="3" width="37.42578125" customWidth="1"/>
+    <col min="4" max="4" width="18.7109375" customWidth="1"/>
+    <col min="5" max="5" width="15.85546875" customWidth="1"/>
+    <col min="7" max="7" width="36.85546875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="42" customWidth="1"/>
+    <col min="10" max="10" width="19.28515625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="21.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" ht="15.75" customHeight="1">
-      <c r="A1" s="79" t="s">
-        <v>125</v>
-      </c>
-      <c r="B1" s="79" t="s">
-        <v>126</v>
-      </c>
-      <c r="C1" s="83" t="s">
-        <v>243</v>
-      </c>
-      <c r="E1" t="s">
-        <v>133</v>
-      </c>
-      <c r="F1" t="s">
-        <v>134</v>
-      </c>
-      <c r="H1" t="s">
-        <v>135</v>
-      </c>
-    </row>
-    <row r="2" spans="1:15" ht="15.75" customHeight="1">
-      <c r="A2" s="85" t="s">
-        <v>136</v>
-      </c>
-      <c r="B2" s="86">
-        <v>0</v>
-      </c>
-      <c r="C2" s="117"/>
-      <c r="E2">
+    <row r="1" spans="1:10" ht="12" customHeight="1" thickTop="1" thickBot="1">
+      <c r="A1" s="116" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="116" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" ht="13.5" thickTop="1">
+      <c r="A2" s="5" t="s">
+        <v>246</v>
+      </c>
+      <c r="B2" s="122">
+        <f>SUM(B3:B9
+)</f>
+        <v>116700</v>
+      </c>
+      <c r="C2" s="3"/>
+    </row>
+    <row r="3" spans="1:10" ht="12.75">
+      <c r="A3" s="7" t="s">
+        <v>44</v>
+      </c>
+      <c r="B3" s="123">
+        <f>B25</f>
+        <v>51000</v>
+      </c>
+      <c r="C3" s="4"/>
+    </row>
+    <row r="4" spans="1:10" ht="12.75">
+      <c r="A4" s="7" t="s">
+        <v>47</v>
+      </c>
+      <c r="B4" s="124">
+        <v>0</v>
+      </c>
+      <c r="C4" s="4" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" ht="12.75">
+      <c r="A5" s="7" t="s">
+        <v>49</v>
+      </c>
+      <c r="B5" s="124">
+        <v>0</v>
+      </c>
+      <c r="C5" s="3"/>
+    </row>
+    <row r="6" spans="1:10" ht="12.75">
+      <c r="A6" s="7" t="s">
+        <v>50</v>
+      </c>
+      <c r="B6" s="124">
+        <f>5400</f>
+        <v>5400</v>
+      </c>
+      <c r="C6" s="4" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" ht="12.75">
+      <c r="A7" s="7" t="s">
+        <v>52</v>
+      </c>
+      <c r="B7" s="124">
+        <v>0</v>
+      </c>
+      <c r="C7" s="3"/>
+    </row>
+    <row r="8" spans="1:10" ht="12.75">
+      <c r="A8" s="7" t="s">
+        <v>53</v>
+      </c>
+      <c r="B8" s="124">
+        <v>10300</v>
+      </c>
+      <c r="C8" s="3"/>
+    </row>
+    <row r="9" spans="1:10" ht="12.75">
+      <c r="A9" s="7" t="s">
+        <v>54</v>
+      </c>
+      <c r="B9" s="124">
+        <v>50000</v>
+      </c>
+      <c r="C9" s="3"/>
+    </row>
+    <row r="10" spans="1:10" ht="12.75">
+      <c r="A10" s="5" t="s">
+        <v>248</v>
+      </c>
+      <c r="B10" s="122">
+        <f>SUM(B11:B14
+)</f>
+        <v>5552860</v>
+      </c>
+      <c r="C10" s="3"/>
+    </row>
+    <row r="11" spans="1:10" ht="12.75">
+      <c r="A11" s="7" t="s">
+        <v>58</v>
+      </c>
+      <c r="B11" s="124">
+        <v>60800</v>
+      </c>
+      <c r="C11" s="4"/>
+    </row>
+    <row r="12" spans="1:10" ht="22.5">
+      <c r="A12" s="95" t="s">
+        <v>171</v>
+      </c>
+      <c r="B12" s="124">
+        <v>3000000</v>
+      </c>
+    </row>
+    <row r="13" spans="1:10" ht="12.75">
+      <c r="A13" s="120" t="s">
+        <v>60</v>
+      </c>
+      <c r="B13" s="125">
+        <v>500000</v>
+      </c>
+      <c r="C13" s="4"/>
+    </row>
+    <row r="14" spans="1:10" ht="13.5" thickBot="1">
+      <c r="A14" s="121" t="s">
+        <v>247</v>
+      </c>
+      <c r="B14" s="126">
+        <f>'Salarios, gastos y costos'!K11*6</f>
+        <v>1992060</v>
+      </c>
+      <c r="C14" s="3"/>
+    </row>
+    <row r="15" spans="1:10" ht="16.5" thickTop="1" thickBot="1">
+      <c r="A15" s="127" t="s">
+        <v>61</v>
+      </c>
+      <c r="B15" s="128">
+        <f>B10+B2</f>
+        <v>5669560</v>
+      </c>
+    </row>
+    <row r="16" spans="1:10" ht="13.5" thickTop="1">
+      <c r="D16" s="3"/>
+      <c r="E16" s="3"/>
+      <c r="F16" s="3"/>
+      <c r="G16" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="H16" s="96" t="s">
+        <v>4</v>
+      </c>
+      <c r="I16" s="96" t="s">
+        <v>5</v>
+      </c>
+      <c r="J16" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="F2">
-        <f>$I$2/(1+EXP((-1)*$I$4*(E2-$I$3)))</f>
-        <v>2577.2486775983025</v>
-      </c>
-      <c r="H2" t="s">
-        <v>138</v>
-      </c>
-      <c r="I2">
-        <f>O2*L4</f>
-        <v>96900</v>
-      </c>
-      <c r="K2" t="s">
-        <v>175</v>
-      </c>
-      <c r="N2" t="s">
-        <v>176</v>
-      </c>
-      <c r="O2">
-        <v>190000</v>
-      </c>
-    </row>
-    <row r="3" spans="1:15" ht="15.75" customHeight="1">
-      <c r="A3" s="85" t="s">
-        <v>67</v>
-      </c>
-      <c r="B3" s="86">
-        <f t="shared" ref="B3:B8" si="0">F3</f>
-        <v>3252.8577359756564</v>
-      </c>
-      <c r="C3" s="117">
-        <f>B3*($O$3+($O$3*0.19))</f>
-        <v>17241349.195529614</v>
-      </c>
-      <c r="E3">
-        <v>7</v>
-      </c>
-      <c r="F3">
-        <f>$I$2/(1+EXP((-1)*$I$4*(E3-$I$3)))</f>
-        <v>3252.8577359756564</v>
-      </c>
-      <c r="H3" t="s">
-        <v>140</v>
-      </c>
-      <c r="I3">
-        <f>AVERAGE(E2:E12)</f>
-        <v>21</v>
-      </c>
-      <c r="K3" t="s">
-        <v>177</v>
-      </c>
-      <c r="L3" s="98">
-        <v>0.32</v>
-      </c>
-      <c r="N3" t="s">
-        <v>281</v>
-      </c>
-      <c r="O3" s="220">
-        <f>('Salarios, gastos y costos'!G66/F29)+(('Salarios, gastos y costos'!G66/F29*O4))</f>
-        <v>4454.0923433263852</v>
-      </c>
-    </row>
-    <row r="4" spans="1:15" ht="15.75" customHeight="1">
-      <c r="A4" s="85" t="s">
-        <v>68</v>
-      </c>
-      <c r="B4" s="86">
-        <f t="shared" si="0"/>
-        <v>4097.8788914930747</v>
-      </c>
-      <c r="C4" s="117">
-        <f t="shared" ref="C4:C13" si="1">B4*($O$3+($O$3*0.19))</f>
-        <v>21720273.883428961</v>
-      </c>
-      <c r="E4">
-        <v>8</v>
-      </c>
-      <c r="F4">
-        <f t="shared" ref="F4:F12" si="2">$I$2/(1+EXP((-1)*$I$4*(E4-$I$3)))</f>
-        <v>4097.8788914930747</v>
-      </c>
-      <c r="H4" t="s">
-        <v>143</v>
-      </c>
-      <c r="I4">
-        <v>0.24</v>
-      </c>
-      <c r="K4" t="s">
-        <v>178</v>
-      </c>
-      <c r="L4" s="98">
-        <v>0.51</v>
-      </c>
-      <c r="N4" s="97" t="s">
-        <v>282</v>
-      </c>
-      <c r="O4" s="148">
-        <v>0.62350000000000005</v>
-      </c>
-    </row>
-    <row r="5" spans="1:15" ht="15.75" customHeight="1">
-      <c r="A5" s="85" t="s">
-        <v>69</v>
-      </c>
-      <c r="B5" s="86">
-        <f t="shared" si="0"/>
-        <v>5150.3451169723749</v>
-      </c>
-      <c r="C5" s="117">
-        <f>B5*($O$3+($O$3*0.19))</f>
-        <v>27298734.173684157</v>
-      </c>
-      <c r="E5">
-        <v>9</v>
-      </c>
-      <c r="F5">
-        <f t="shared" si="2"/>
-        <v>5150.3451169723749</v>
-      </c>
-      <c r="K5" t="s">
-        <v>179</v>
-      </c>
-      <c r="L5" s="98">
-        <v>0.16</v>
-      </c>
-      <c r="O5" s="219">
-        <f>('Salarios, gastos y costos'!G66/F29)</f>
-        <v>2743.5123765484354</v>
-      </c>
-    </row>
-    <row r="6" spans="1:15" ht="15.75" customHeight="1">
-      <c r="A6" s="85" t="s">
-        <v>70</v>
-      </c>
-      <c r="B6" s="86">
-        <f t="shared" si="0"/>
-        <v>6454.3186472262878</v>
-      </c>
-      <c r="C6" s="117">
-        <f t="shared" si="1"/>
-        <v>34210276.20891919</v>
-      </c>
-      <c r="E6">
-        <v>10</v>
-      </c>
-      <c r="F6">
-        <f t="shared" si="2"/>
-        <v>6454.3186472262878</v>
-      </c>
-    </row>
-    <row r="7" spans="1:15" ht="15.75" customHeight="1">
-      <c r="A7" s="85" t="s">
-        <v>71</v>
-      </c>
-      <c r="B7" s="86">
-        <f t="shared" si="0"/>
-        <v>8059.4342902610779</v>
-      </c>
-      <c r="C7" s="117">
-        <f t="shared" si="1"/>
-        <v>42717982.83091484</v>
-      </c>
-      <c r="E7">
-        <v>11</v>
-      </c>
-      <c r="F7">
-        <f t="shared" si="2"/>
-        <v>8059.4342902610779</v>
-      </c>
-    </row>
-    <row r="8" spans="1:15" ht="15.75" customHeight="1">
-      <c r="A8" s="85" t="s">
-        <v>72</v>
-      </c>
-      <c r="B8" s="86">
-        <f t="shared" si="0"/>
-        <v>10019.503746304383</v>
-      </c>
-      <c r="C8" s="117">
-        <f t="shared" si="1"/>
-        <v>53107075.955209814</v>
-      </c>
-      <c r="D8" t="s">
-        <v>180</v>
-      </c>
-      <c r="E8">
+    </row>
+    <row r="17" spans="1:10" ht="12.75">
+      <c r="A17" s="11"/>
+      <c r="D17" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="E17" s="18">
+        <v>1500000</v>
+      </c>
+      <c r="F17" s="3"/>
+      <c r="G17" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="H17" s="4">
+        <v>5</v>
+      </c>
+      <c r="I17" s="3">
+        <f>H17*12</f>
+        <v>60</v>
+      </c>
+      <c r="J17" s="21">
+        <f>SUM(B12,B13)/I17</f>
+        <v>58333.333333333336</v>
+      </c>
+    </row>
+    <row r="18" spans="1:10" ht="12.75">
+      <c r="A18" s="107" t="s">
+        <v>165</v>
+      </c>
+      <c r="B18" s="115" t="s">
+        <v>1</v>
+      </c>
+      <c r="D18" s="4" t="s">
+        <v>43</v>
+      </c>
+      <c r="E18" s="21">
+        <v>975000</v>
+      </c>
+      <c r="F18" s="3"/>
+    </row>
+    <row r="19" spans="1:10" ht="15.75" customHeight="1">
+      <c r="A19" s="100" t="s">
+        <v>166</v>
+      </c>
+      <c r="B19" s="113">
+        <f>39000</f>
+        <v>39000</v>
+      </c>
+      <c r="D19" s="3"/>
+      <c r="E19" s="3"/>
+      <c r="F19" s="3"/>
+      <c r="G19" s="3"/>
+      <c r="H19" s="3"/>
+      <c r="I19" s="3"/>
+      <c r="J19" s="3"/>
+    </row>
+    <row r="20" spans="1:10" ht="15.75" customHeight="1">
+      <c r="A20" s="100" t="s">
+        <v>167</v>
+      </c>
+      <c r="B20" s="113">
+        <v>4760</v>
+      </c>
+      <c r="D20" s="11" t="s">
+        <v>56</v>
+      </c>
+      <c r="E20" s="3"/>
+      <c r="F20" s="3"/>
+      <c r="G20" s="3"/>
+      <c r="H20" s="3"/>
+      <c r="I20" s="4" t="s">
+        <v>46</v>
+      </c>
+      <c r="J20" s="21">
+        <f>SUM(J17:J19
+)</f>
+        <v>58333.333333333336</v>
+      </c>
+    </row>
+    <row r="21" spans="1:10" ht="15.75" customHeight="1">
+      <c r="A21" s="100" t="s">
+        <v>167</v>
+      </c>
+      <c r="B21" s="113">
+        <v>2040</v>
+      </c>
+      <c r="D21" s="25">
+        <f>SUM(B12:B13
+)</f>
+        <v>3500000</v>
+      </c>
+    </row>
+    <row r="22" spans="1:10" ht="15.75" customHeight="1">
+      <c r="A22" s="100" t="s">
+        <v>168</v>
+      </c>
+      <c r="B22" s="113">
+        <v>39000</v>
+      </c>
+    </row>
+    <row r="23" spans="1:10" ht="15.75" customHeight="1">
+      <c r="A23" s="100" t="s">
+        <v>169</v>
+      </c>
+      <c r="B23" s="113">
+        <v>-39000</v>
+      </c>
+      <c r="D23" s="18">
+        <f>SUM(B11:B13
+)</f>
+        <v>3560800</v>
+      </c>
+    </row>
+    <row r="24" spans="1:10" ht="15.75" customHeight="1">
+      <c r="A24" s="100" t="s">
+        <v>170</v>
+      </c>
+      <c r="B24" s="113">
+        <v>5200</v>
+      </c>
+      <c r="G24" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="H24" s="4">
+        <v>1</v>
+      </c>
+      <c r="I24" s="3">
+        <f>H24*12</f>
         <v>12</v>
       </c>
-      <c r="F8">
-        <f t="shared" si="2"/>
-        <v>10019.503746304383</v>
-      </c>
-    </row>
-    <row r="9" spans="1:15" ht="15.75" customHeight="1">
-      <c r="A9" s="85" t="s">
-        <v>74</v>
-      </c>
-      <c r="B9" s="86">
-        <f>F8</f>
-        <v>10019.503746304383</v>
-      </c>
-      <c r="C9" s="117">
-        <f t="shared" si="1"/>
-        <v>53107075.955209814</v>
-      </c>
-      <c r="D9" t="s">
-        <v>181</v>
-      </c>
-      <c r="E9">
-        <v>24</v>
-      </c>
-      <c r="F9">
-        <f t="shared" si="2"/>
-        <v>65175.619953865986</v>
-      </c>
-    </row>
-    <row r="10" spans="1:15" ht="15.75" customHeight="1">
-      <c r="A10" s="85" t="s">
-        <v>75</v>
-      </c>
-      <c r="B10" s="86">
-        <f>F9</f>
-        <v>65175.619953865986</v>
-      </c>
-      <c r="C10" s="117">
-        <f t="shared" si="1"/>
-        <v>345454893.47159714</v>
-      </c>
-      <c r="D10" t="s">
-        <v>182</v>
-      </c>
-      <c r="E10">
-        <v>36</v>
-      </c>
-      <c r="F10">
-        <f>$I$2/(1+EXP((-1)*$I$4*(E10-$I$3)))</f>
-        <v>94322.751322401688</v>
-      </c>
-    </row>
-    <row r="11" spans="1:15" ht="15.75" customHeight="1">
-      <c r="A11" s="85" t="s">
-        <v>76</v>
-      </c>
-      <c r="B11" s="86">
-        <f>F10</f>
-        <v>94322.751322401688</v>
-      </c>
-      <c r="C11" s="117">
-        <f t="shared" si="1"/>
-        <v>499945470.91523975</v>
-      </c>
-      <c r="D11" t="s">
-        <v>183</v>
-      </c>
-      <c r="E11">
-        <v>48</v>
-      </c>
-      <c r="F11">
-        <f t="shared" si="2"/>
-        <v>96751.601360591376</v>
-      </c>
-    </row>
-    <row r="12" spans="1:15" ht="15.75" customHeight="1">
-      <c r="A12" s="85" t="s">
-        <v>78</v>
-      </c>
-      <c r="B12" s="86">
-        <f>F11</f>
-        <v>96751.601360591376</v>
-      </c>
-      <c r="C12" s="117">
-        <f t="shared" si="1"/>
-        <v>512819274.52148426</v>
-      </c>
-      <c r="D12" t="s">
-        <v>184</v>
-      </c>
-      <c r="E12">
-        <v>60</v>
-      </c>
-      <c r="F12">
-        <f t="shared" si="2"/>
-        <v>96891.657618714249</v>
-      </c>
-    </row>
-    <row r="13" spans="1:15" ht="15.75" customHeight="1">
-      <c r="A13" s="85" t="s">
-        <v>79</v>
-      </c>
-      <c r="B13" s="86">
-        <f>F12</f>
-        <v>96891.657618714249</v>
-      </c>
-      <c r="C13" s="117">
-        <f t="shared" si="1"/>
-        <v>513561624.49474293</v>
-      </c>
-    </row>
-    <row r="14" spans="1:15" ht="15.75" customHeight="1">
-      <c r="A14" s="11"/>
-    </row>
-    <row r="15" spans="1:15" ht="15.75" customHeight="1">
-      <c r="A15" s="11"/>
-    </row>
-    <row r="22" spans="5:6" ht="15.75" customHeight="1">
-      <c r="E22">
-        <v>12</v>
-      </c>
-      <c r="F22" s="221">
-        <f>$I$2/(1+EXP((-1)*$I$4*(E22-$I$3)))</f>
-        <v>10019.503746304383</v>
-      </c>
-    </row>
-    <row r="23" spans="5:6" ht="15.75" customHeight="1">
-      <c r="E23">
-        <v>13</v>
-      </c>
-      <c r="F23" s="221">
-        <f t="shared" ref="F23:F35" si="3">$I$2/(1+EXP((-1)*$I$4*(E23-$I$3)))</f>
-        <v>12389.78577631898</v>
-      </c>
-    </row>
-    <row r="24" spans="5:6" ht="15.75" customHeight="1">
-      <c r="E24">
-        <v>14</v>
-      </c>
-      <c r="F24" s="221">
-        <f t="shared" si="3"/>
-        <v>15222.55093500037</v>
-      </c>
-    </row>
-    <row r="25" spans="5:6" ht="15.75" customHeight="1">
-      <c r="E25">
-        <v>15</v>
-      </c>
-      <c r="F25" s="221">
-        <f t="shared" si="3"/>
-        <v>18560.744275606201</v>
-      </c>
-    </row>
-    <row r="26" spans="5:6" ht="15.75" customHeight="1">
-      <c r="E26">
-        <v>16</v>
-      </c>
-      <c r="F26" s="221">
-        <f t="shared" si="3"/>
-        <v>22429.948478945193</v>
-      </c>
-    </row>
-    <row r="27" spans="5:6" ht="15.75" customHeight="1">
-      <c r="E27">
-        <v>17</v>
-      </c>
-      <c r="F27" s="221">
-        <f t="shared" si="3"/>
-        <v>26829.497083446626</v>
-      </c>
-    </row>
-    <row r="28" spans="5:6" ht="15.75" customHeight="1">
-      <c r="E28">
-        <v>18</v>
-      </c>
-      <c r="F28" s="221">
-        <f t="shared" si="3"/>
-        <v>31724.380046134014</v>
-      </c>
-    </row>
-    <row r="29" spans="5:6" ht="15.75" customHeight="1">
-      <c r="E29">
-        <v>19</v>
-      </c>
-      <c r="F29" s="221">
-        <f t="shared" si="3"/>
-        <v>37040.23093485977</v>
-      </c>
-    </row>
-    <row r="30" spans="5:6" ht="15.75" customHeight="1">
-      <c r="E30">
-        <v>20</v>
-      </c>
-      <c r="F30" s="221">
-        <f t="shared" si="3"/>
-        <v>42663.747386009003</v>
-      </c>
-    </row>
-    <row r="31" spans="5:6" ht="15.75" customHeight="1">
-      <c r="E31">
-        <v>21</v>
-      </c>
-      <c r="F31" s="221">
-        <f t="shared" si="3"/>
-        <v>48450</v>
-      </c>
-    </row>
-    <row r="32" spans="5:6" ht="15.75" customHeight="1">
-      <c r="E32">
-        <v>22</v>
-      </c>
-      <c r="F32" s="221">
-        <f t="shared" si="3"/>
-        <v>54236.252613990997</v>
-      </c>
-    </row>
-    <row r="33" spans="5:6" ht="15.75" customHeight="1">
-      <c r="E33">
-        <v>23</v>
-      </c>
-      <c r="F33" s="221">
-        <f t="shared" si="3"/>
-        <v>59859.769065140223</v>
-      </c>
-    </row>
-    <row r="34" spans="5:6" ht="15.75" customHeight="1">
-      <c r="E34">
-        <v>24</v>
-      </c>
-      <c r="F34" s="221">
-        <f t="shared" si="3"/>
-        <v>65175.619953865986</v>
-      </c>
-    </row>
-    <row r="35" spans="5:6" ht="15.75" customHeight="1">
-      <c r="E35">
-        <v>25</v>
-      </c>
-      <c r="F35" s="221">
-        <f t="shared" si="3"/>
-        <v>70070.502916553378</v>
+      <c r="J24" s="21">
+        <f>SUM($B$12,$B$13)/I24</f>
+        <v>291666.66666666669</v>
+      </c>
+    </row>
+    <row r="25" spans="1:10" ht="15.75" customHeight="1">
+      <c r="A25" s="107" t="s">
+        <v>46</v>
+      </c>
+      <c r="B25" s="114">
+        <f>SUM(B19:B24)</f>
+        <v>51000</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:S30"/>
+  <dimension ref="A1:S31"/>
   <sheetViews>
-    <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="D19" sqref="D19"/>
+    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="F20" sqref="F20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1"/>
@@ -6036,26 +6129,26 @@
     <row r="1" spans="1:19" ht="12.75">
       <c r="A1" s="26"/>
       <c r="B1" s="26"/>
-      <c r="C1" s="209" t="s">
+      <c r="C1" s="213" t="s">
         <v>74</v>
       </c>
-      <c r="D1" s="182"/>
-      <c r="E1" s="209" t="s">
+      <c r="D1" s="186"/>
+      <c r="E1" s="213" t="s">
         <v>75</v>
       </c>
-      <c r="F1" s="182"/>
-      <c r="G1" s="209" t="s">
+      <c r="F1" s="186"/>
+      <c r="G1" s="213" t="s">
         <v>76</v>
       </c>
-      <c r="H1" s="182"/>
-      <c r="I1" s="209" t="s">
+      <c r="H1" s="186"/>
+      <c r="I1" s="213" t="s">
         <v>78</v>
       </c>
-      <c r="J1" s="182"/>
-      <c r="K1" s="211" t="s">
+      <c r="J1" s="186"/>
+      <c r="K1" s="215" t="s">
         <v>79</v>
       </c>
-      <c r="L1" s="216"/>
+      <c r="L1" s="220"/>
       <c r="M1" s="28"/>
       <c r="N1" s="28"/>
       <c r="O1" s="28"/>
@@ -6206,9 +6299,10 @@
         <v>101129582.464</v>
       </c>
       <c r="M4" s="45"/>
-      <c r="N4" s="45"/>
-      <c r="O4" s="45"/>
-      <c r="P4" s="45"/>
+      <c r="N4" s="45">
+        <f>D4+F4+H4+J4+L4</f>
+        <v>496935272.97257292</v>
+      </c>
       <c r="Q4" s="45"/>
       <c r="R4" s="45"/>
       <c r="S4" s="45"/>
@@ -6259,9 +6353,14 @@
         <v>782131.19999999995</v>
       </c>
       <c r="M5" s="53"/>
-      <c r="N5" s="53"/>
-      <c r="O5" s="53"/>
-      <c r="P5" s="53"/>
+      <c r="N5" s="45">
+        <f>D5+F5+H5+J5+L5</f>
+        <v>3842803.212898233</v>
+      </c>
+      <c r="O5" s="224" t="s">
+        <v>284</v>
+      </c>
+      <c r="P5" s="224"/>
       <c r="Q5" s="53"/>
       <c r="R5" s="53"/>
       <c r="S5" s="53"/>
@@ -6313,8 +6412,10 @@
       </c>
       <c r="M6" s="53"/>
       <c r="N6" s="53"/>
-      <c r="O6" s="53"/>
-      <c r="P6" s="53"/>
+      <c r="O6" s="224" t="s">
+        <v>289</v>
+      </c>
+      <c r="P6" s="224"/>
       <c r="Q6" s="53"/>
       <c r="R6" s="53"/>
       <c r="S6" s="53"/>
@@ -6366,8 +6467,10 @@
       </c>
       <c r="M7" s="53"/>
       <c r="N7" s="53"/>
-      <c r="O7" s="53"/>
-      <c r="P7" s="53"/>
+      <c r="O7" s="224" t="s">
+        <v>290</v>
+      </c>
+      <c r="P7" s="224"/>
       <c r="Q7" s="53"/>
       <c r="R7" s="53"/>
       <c r="S7" s="53"/>
@@ -6419,8 +6522,8 @@
       </c>
       <c r="M8" s="56"/>
       <c r="N8" s="45"/>
-      <c r="O8" s="45"/>
-      <c r="P8" s="45"/>
+      <c r="O8" s="223"/>
+      <c r="P8" s="223"/>
       <c r="Q8" s="45"/>
       <c r="R8" s="45"/>
       <c r="S8" s="45"/>
@@ -6472,8 +6575,10 @@
       </c>
       <c r="M9" s="53"/>
       <c r="N9" s="53"/>
-      <c r="O9" s="53"/>
-      <c r="P9" s="53"/>
+      <c r="O9" s="224" t="s">
+        <v>11</v>
+      </c>
+      <c r="P9" s="224"/>
       <c r="Q9" s="53"/>
       <c r="R9" s="53"/>
       <c r="S9" s="53"/>
@@ -6525,8 +6630,10 @@
       </c>
       <c r="M10" s="53"/>
       <c r="N10" s="53"/>
-      <c r="O10" s="53"/>
-      <c r="P10" s="53"/>
+      <c r="O10" s="224" t="s">
+        <v>252</v>
+      </c>
+      <c r="P10" s="224"/>
       <c r="Q10" s="53"/>
       <c r="R10" s="53"/>
       <c r="S10" s="53"/>
@@ -6980,10 +7087,20 @@
         <v>267054579.8232539</v>
       </c>
     </row>
+    <row r="20" spans="1:19" ht="15.75" customHeight="1">
+      <c r="D20" s="103">
+        <f>B19+D19</f>
+        <v>-16713038.93100372</v>
+      </c>
+      <c r="F20" s="103">
+        <f>D20+F19</f>
+        <v>140198569.59992108</v>
+      </c>
+    </row>
     <row r="22" spans="1:19" ht="12.75">
       <c r="C22" s="11"/>
       <c r="D22" s="99" t="s">
-        <v>253</v>
+        <v>251</v>
       </c>
       <c r="F22" s="62">
         <f>'Tabla Crecimiento'!B10</f>
@@ -7050,7 +7167,7 @@
     </row>
     <row r="25" spans="1:19" ht="12.75">
       <c r="D25" s="97" t="s">
-        <v>252</v>
+        <v>250</v>
       </c>
       <c r="F25" s="147">
         <v>0.06</v>
@@ -7077,8 +7194,20 @@
         <v>150818737.17869031</v>
       </c>
     </row>
+    <row r="31" spans="1:19" ht="15.75" customHeight="1">
+      <c r="D31">
+        <f>D30/10022</f>
+        <v>15048.766431719248</v>
+      </c>
+    </row>
   </sheetData>
-  <mergeCells count="5">
+  <mergeCells count="11">
+    <mergeCell ref="O5:P5"/>
+    <mergeCell ref="O6:P6"/>
+    <mergeCell ref="O9:P9"/>
+    <mergeCell ref="O10:P10"/>
+    <mergeCell ref="O7:P7"/>
+    <mergeCell ref="O8:P8"/>
     <mergeCell ref="E1:F1"/>
     <mergeCell ref="C1:D1"/>
     <mergeCell ref="G1:H1"/>
@@ -7096,6 +7225,7 @@
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -7103,8 +7233,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M66"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="F4" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="Q24" sqref="Q24"/>
+    <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="J11" sqref="J11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1"/>
@@ -7139,7 +7269,7 @@
     </row>
     <row r="2" spans="1:13" ht="15.75" customHeight="1">
       <c r="A2" s="99" t="s">
-        <v>279</v>
+        <v>277</v>
       </c>
       <c r="B2" s="11">
         <v>0.15</v>
@@ -7251,7 +7381,7 @@
         <v>0</v>
       </c>
       <c r="M6" s="44">
-        <f t="shared" ref="M6:M45" si="0">NPV(L6,$J$2:$J$6)+$J$1</f>
+        <f t="shared" ref="M6:M27" si="0">NPV(L6,$J$2:$J$6)+$J$1</f>
         <v>932491300.11207008</v>
       </c>
     </row>
@@ -7286,16 +7416,16 @@
     </row>
     <row r="9" spans="1:13" ht="15.75" customHeight="1">
       <c r="G9" s="11" t="s">
-        <v>285</v>
+        <v>283</v>
       </c>
       <c r="H9" s="44" t="s">
-        <v>266</v>
+        <v>264</v>
       </c>
       <c r="I9" t="s">
-        <v>283</v>
+        <v>281</v>
       </c>
       <c r="J9" s="44" t="s">
-        <v>284</v>
+        <v>282</v>
       </c>
       <c r="L9" s="11">
         <v>0.15</v>
@@ -7333,7 +7463,7 @@
         <f>IRR(H1:H6)</f>
         <v>2.7290981934208092</v>
       </c>
-      <c r="J11" s="77">
+      <c r="J11" s="184">
         <f>IRR(J1:J6)</f>
         <v>1.6242343162061208</v>
       </c>
@@ -7461,25 +7591,25 @@
     </row>
     <row r="21" spans="1:13" ht="15.75" customHeight="1">
       <c r="A21" s="119" t="s">
+        <v>263</v>
+      </c>
+      <c r="B21" s="119" t="s">
+        <v>264</v>
+      </c>
+      <c r="C21" s="97" t="s">
         <v>265</v>
       </c>
-      <c r="B21" s="119" t="s">
+      <c r="D21" s="97" t="s">
         <v>266</v>
       </c>
-      <c r="C21" s="97" t="s">
+      <c r="E21" s="97" t="s">
         <v>267</v>
       </c>
-      <c r="D21" s="97" t="s">
+      <c r="F21" s="97" t="s">
         <v>268</v>
       </c>
-      <c r="E21" s="97" t="s">
+      <c r="G21" s="97" t="s">
         <v>269</v>
-      </c>
-      <c r="F21" s="97" t="s">
-        <v>270</v>
-      </c>
-      <c r="G21" s="97" t="s">
-        <v>271</v>
       </c>
       <c r="L21" s="11">
         <v>0.75</v>
@@ -7519,29 +7649,29 @@
     </row>
     <row r="23" spans="1:13" ht="15.75" customHeight="1">
       <c r="A23" s="118" t="s">
-        <v>261</v>
-      </c>
-      <c r="B23" s="178">
+        <v>259</v>
+      </c>
+      <c r="B23" s="177">
         <f>B1*-1</f>
         <v>-62189202</v>
       </c>
-      <c r="C23" s="170">
+      <c r="C23" s="183">
         <f>'Flujo de Caja (Profesor) - 5 añ'!D19</f>
         <v>45476961.06899628</v>
       </c>
-      <c r="D23" s="170">
+      <c r="D23" s="183">
         <f>'Flujo de Caja (Profesor) - 5 añ'!F19</f>
         <v>156911608.5309248</v>
       </c>
-      <c r="E23" s="170">
+      <c r="E23" s="183">
         <f>'Flujo de Caja (Profesor) - 5 añ'!H19</f>
         <v>258538943.31750089</v>
       </c>
-      <c r="F23" s="170">
+      <c r="F23" s="183">
         <f>'Flujo de Caja (Profesor) - 5 añ'!J19</f>
         <v>266699207.37139431</v>
       </c>
-      <c r="G23" s="170">
+      <c r="G23" s="183">
         <f>'Flujo de Caja (Profesor) - 5 añ'!L19</f>
         <v>267054579.8232539</v>
       </c>
@@ -7565,13 +7695,13 @@
     </row>
     <row r="25" spans="1:13" ht="12.75">
       <c r="A25" s="118" t="s">
+        <v>263</v>
+      </c>
+      <c r="B25" s="119" t="s">
+        <v>264</v>
+      </c>
+      <c r="C25" s="170" t="s">
         <v>265</v>
-      </c>
-      <c r="B25" s="119" t="s">
-        <v>266</v>
-      </c>
-      <c r="C25" s="171" t="s">
-        <v>267</v>
       </c>
       <c r="L25" s="11">
         <v>0.95</v>
@@ -7583,10 +7713,10 @@
     </row>
     <row r="26" spans="1:13" ht="12.75">
       <c r="A26" s="118" t="s">
-        <v>262</v>
+        <v>260</v>
       </c>
       <c r="B26" s="119"/>
-      <c r="C26" s="171">
+      <c r="C26" s="170">
         <f>J1+(C23/C47)+(D23/C47*C48)+(E23/C47*C48*C49)+(F23/C47*C48*C49*C50)+(G23/C47*C48*C49*C50*C51)</f>
         <v>1045731715.0794715</v>
       </c>
@@ -7600,10 +7730,10 @@
     </row>
     <row r="27" spans="1:13" ht="12.75">
       <c r="A27" s="150" t="s">
-        <v>278</v>
+        <v>276</v>
       </c>
       <c r="B27" s="150"/>
-      <c r="C27" s="171">
+      <c r="C27" s="170">
         <f>-B1+(C23/(1+B2))+(D23/(1+B2)^2)+(E23/(1+B2)^3)+(F23/(1+B2)^4)+(G23/(1+B2)^5)</f>
         <v>551256714.1560055</v>
       </c>
@@ -7656,10 +7786,10 @@
     </row>
     <row r="31" spans="1:13" ht="12.75">
       <c r="A31" s="118" t="s">
-        <v>265</v>
-      </c>
-      <c r="B31" s="175" t="s">
-        <v>266</v>
+        <v>263</v>
+      </c>
+      <c r="B31" s="174" t="s">
+        <v>264</v>
       </c>
       <c r="L31" s="11">
         <v>1.25</v>
@@ -7671,16 +7801,16 @@
     </row>
     <row r="32" spans="1:13" ht="12.75">
       <c r="A32" s="118" t="s">
-        <v>272</v>
-      </c>
-      <c r="B32" s="175">
+        <v>270</v>
+      </c>
+      <c r="B32" s="174">
         <f>(((C23+D23+E23+F23+G23)/B1)-1)/5</f>
         <v>2.9988874856830292</v>
       </c>
       <c r="D32" t="s">
-        <v>280</v>
-      </c>
-      <c r="E32" s="177">
+        <v>278</v>
+      </c>
+      <c r="E32" s="176">
         <f>-$B$1+($C$23/(1+B32))+($D$23/((1+B32)^2))+($E$23/((1+B32)^3))+($F$23/((1+B32)^4))+($G$23/((1+B32)^5))</f>
         <v>-35657210.16321066</v>
       </c>
@@ -7694,13 +7824,13 @@
     </row>
     <row r="33" spans="1:13" ht="12.75">
       <c r="A33" s="150"/>
-      <c r="B33" s="175">
+      <c r="B33" s="174">
         <v>3.2</v>
       </c>
       <c r="D33" t="s">
-        <v>280</v>
-      </c>
-      <c r="E33" s="177">
+        <v>278</v>
+      </c>
+      <c r="E33" s="176">
         <f t="shared" ref="E33:E34" si="2">-$B$1+($C$23/(1+B33))+($D$23/((1+B33)^2))+($E$23/((1+B33)^3))+($F$23/((1+B33)^4))+($G$23/((1+B33)^5))</f>
         <v>-37915092.127963498</v>
       </c>
@@ -7714,16 +7844,16 @@
     </row>
     <row r="34" spans="1:13" ht="12.75">
       <c r="A34" s="118" t="s">
-        <v>273</v>
-      </c>
-      <c r="B34" s="176">
+        <v>271</v>
+      </c>
+      <c r="B34" s="175">
         <f>B32+0.1</f>
         <v>3.0988874856830293</v>
       </c>
       <c r="D34" t="s">
-        <v>280</v>
-      </c>
-      <c r="E34" s="177">
+        <v>278</v>
+      </c>
+      <c r="E34" s="176">
         <f t="shared" si="2"/>
         <v>-36824813.032067746</v>
       </c>
@@ -7748,10 +7878,10 @@
     </row>
     <row r="36" spans="1:13" ht="12.75">
       <c r="A36" s="118" t="s">
-        <v>265</v>
-      </c>
-      <c r="B36" s="174" t="s">
-        <v>266</v>
+        <v>263</v>
+      </c>
+      <c r="B36" s="173" t="s">
+        <v>264</v>
       </c>
       <c r="L36" s="11">
         <v>1.5</v>
@@ -7763,9 +7893,9 @@
     </row>
     <row r="37" spans="1:13" ht="12.75">
       <c r="A37" s="118" t="s">
-        <v>274</v>
-      </c>
-      <c r="B37" s="174"/>
+        <v>272</v>
+      </c>
+      <c r="B37" s="173"/>
       <c r="L37" s="11">
         <v>1.55</v>
       </c>
@@ -7776,9 +7906,9 @@
     </row>
     <row r="38" spans="1:13" ht="12.75">
       <c r="A38" s="118" t="s">
-        <v>275</v>
-      </c>
-      <c r="B38" s="174">
+        <v>273</v>
+      </c>
+      <c r="B38" s="173">
         <f>-B1+(C23/(1+B34))+(D23/((1+B34)^2))+(E23/((1+B34)^3))+(F23/((1+B34)^4))+(G23/((1+B34)^5))</f>
         <v>-36824813.032067746</v>
       </c>
@@ -7792,9 +7922,9 @@
     </row>
     <row r="39" spans="1:13" ht="12.75">
       <c r="A39" s="118" t="s">
-        <v>277</v>
-      </c>
-      <c r="B39" s="174">
+        <v>275</v>
+      </c>
+      <c r="B39" s="173">
         <f>E32*-1</f>
         <v>35657210.16321066</v>
       </c>
@@ -7808,9 +7938,9 @@
     </row>
     <row r="40" spans="1:13" ht="12.75">
       <c r="A40" s="118" t="s">
-        <v>276</v>
-      </c>
-      <c r="B40" s="174">
+        <v>274</v>
+      </c>
+      <c r="B40" s="173">
         <f>B38*-1</f>
         <v>36824813.032067746</v>
       </c>
@@ -7826,7 +7956,7 @@
       <c r="A41" s="118" t="s">
         <v>118</v>
       </c>
-      <c r="B41" s="174">
+      <c r="B41" s="173">
         <f>B32+(B39/(B39+B40))</f>
         <v>3.4908330549608668</v>
       </c>
@@ -7870,13 +8000,13 @@
     </row>
     <row r="45" spans="1:13" ht="12.75">
       <c r="A45" s="118" t="s">
+        <v>263</v>
+      </c>
+      <c r="B45" s="119" t="s">
+        <v>264</v>
+      </c>
+      <c r="C45" s="97" t="s">
         <v>265</v>
-      </c>
-      <c r="B45" s="119" t="s">
-        <v>266</v>
-      </c>
-      <c r="C45" s="97" t="s">
-        <v>267</v>
       </c>
       <c r="L45" s="11">
         <v>1.95</v>
@@ -7888,11 +8018,11 @@
     </row>
     <row r="46" spans="1:13" ht="12.75">
       <c r="A46" s="118" t="s">
-        <v>263</v>
+        <v>261</v>
       </c>
       <c r="B46" s="119"/>
       <c r="C46" s="97" t="s">
-        <v>264</v>
+        <v>262</v>
       </c>
       <c r="L46" s="11">
         <v>2</v>
@@ -7906,10 +8036,10 @@
       <c r="A47" s="97" t="s">
         <v>74</v>
       </c>
-      <c r="B47" s="172">
+      <c r="B47" s="171">
         <v>5.7500000000000002E-2</v>
       </c>
-      <c r="C47" s="173">
+      <c r="C47" s="172">
         <f xml:space="preserve"> 1 +B47</f>
         <v>1.0575000000000001</v>
       </c>
@@ -7925,10 +8055,10 @@
       <c r="A48" s="97" t="s">
         <v>75</v>
       </c>
-      <c r="B48" s="172">
+      <c r="B48" s="171">
         <v>0.06</v>
       </c>
-      <c r="C48" s="173">
+      <c r="C48" s="172">
         <f t="shared" ref="C48:C51" si="3" xml:space="preserve"> 1 +B48</f>
         <v>1.06</v>
       </c>
@@ -7944,10 +8074,10 @@
       <c r="A49" s="97" t="s">
         <v>76</v>
       </c>
-      <c r="B49" s="172">
+      <c r="B49" s="171">
         <v>6.5000000000000002E-2</v>
       </c>
-      <c r="C49" s="173">
+      <c r="C49" s="172">
         <f t="shared" si="3"/>
         <v>1.0649999999999999</v>
       </c>
@@ -7963,10 +8093,10 @@
       <c r="A50" s="97" t="s">
         <v>78</v>
       </c>
-      <c r="B50" s="172">
+      <c r="B50" s="171">
         <v>7.0000000000000007E-2</v>
       </c>
-      <c r="C50" s="173">
+      <c r="C50" s="172">
         <f t="shared" si="3"/>
         <v>1.07</v>
       </c>
@@ -7982,10 +8112,10 @@
       <c r="A51" s="97" t="s">
         <v>79</v>
       </c>
-      <c r="B51" s="172">
+      <c r="B51" s="171">
         <v>7.1999999999999995E-2</v>
       </c>
-      <c r="C51" s="173">
+      <c r="C51" s="172">
         <f t="shared" si="3"/>
         <v>1.0720000000000001</v>
       </c>
@@ -8148,6 +8278,395 @@
 </file>
 
 <file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="B1:N32"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B2" sqref="B2:H15"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="12.75"/>
+  <cols>
+    <col min="4" max="8" width="16.5703125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="12.28515625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="2:8" ht="13.5" thickBot="1"/>
+    <row r="2" spans="2:8" ht="15.75" thickBot="1">
+      <c r="B2" s="226" t="s">
+        <v>285</v>
+      </c>
+      <c r="C2" s="227"/>
+      <c r="D2" s="227"/>
+      <c r="E2" s="227"/>
+      <c r="F2" s="227"/>
+      <c r="G2" s="227"/>
+      <c r="H2" s="228"/>
+    </row>
+    <row r="3" spans="2:8" ht="15.75" thickTop="1">
+      <c r="B3" s="229" t="s">
+        <v>291</v>
+      </c>
+      <c r="C3" s="221"/>
+      <c r="D3" s="221"/>
+      <c r="E3" s="221"/>
+      <c r="F3" s="221"/>
+      <c r="G3" s="221"/>
+      <c r="H3" s="230"/>
+    </row>
+    <row r="4" spans="2:8">
+      <c r="B4" s="231"/>
+      <c r="C4" s="232"/>
+      <c r="D4" s="233" t="s">
+        <v>74</v>
+      </c>
+      <c r="E4" s="233" t="s">
+        <v>75</v>
+      </c>
+      <c r="F4" s="233" t="s">
+        <v>76</v>
+      </c>
+      <c r="G4" s="233" t="s">
+        <v>78</v>
+      </c>
+      <c r="H4" s="234" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="5" spans="2:8">
+      <c r="B5" s="235" t="s">
+        <v>122</v>
+      </c>
+      <c r="C5" s="232"/>
+      <c r="D5" s="237">
+        <f>'Flujo de Caja (Profesor) - 5 añ'!D6+'Flujo de Caja (Profesor) - 5 añ'!D7</f>
+        <v>93654713.655674696</v>
+      </c>
+      <c r="E5" s="237">
+        <f>'Flujo de Caja (Profesor) - 5 añ'!F6+'Flujo de Caja (Profesor) - 5 añ'!F7</f>
+        <v>99231994.719999999</v>
+      </c>
+      <c r="F5" s="237">
+        <f>'Flujo de Caja (Profesor) - 5 añ'!H6+'Flujo de Caja (Profesor) - 5 añ'!H7</f>
+        <v>99696768.280000001</v>
+      </c>
+      <c r="G5" s="237">
+        <f>'Flujo de Caja (Profesor) - 5 añ'!J6+'Flujo de Caja (Profesor) - 5 añ'!J7</f>
+        <v>100161541.84</v>
+      </c>
+      <c r="H5" s="238">
+        <f>'Flujo de Caja (Profesor) - 5 añ'!L6+'Flujo de Caja (Profesor) - 5 añ'!L7</f>
+        <v>100347451.264</v>
+      </c>
+    </row>
+    <row r="6" spans="2:8">
+      <c r="B6" s="235" t="s">
+        <v>286</v>
+      </c>
+      <c r="C6" s="232"/>
+      <c r="D6" s="237">
+        <f>'Flujo de Caja (Profesor) - 5 añ'!D3</f>
+        <v>196295698.24768659</v>
+      </c>
+      <c r="E6" s="237">
+        <f>'Flujo de Caja (Profesor) - 5 añ'!F3</f>
+        <v>345454893.47159714</v>
+      </c>
+      <c r="F6" s="237">
+        <f>'Flujo de Caja (Profesor) - 5 añ'!H3</f>
+        <v>499945470.91523975</v>
+      </c>
+      <c r="G6" s="237">
+        <f>'Flujo de Caja (Profesor) - 5 añ'!J3</f>
+        <v>512819274.52148426</v>
+      </c>
+      <c r="H6" s="238">
+        <f>'Flujo de Caja (Profesor) - 5 añ'!L3</f>
+        <v>513561624.49474293</v>
+      </c>
+    </row>
+    <row r="7" spans="2:8">
+      <c r="B7" s="235" t="s">
+        <v>287</v>
+      </c>
+      <c r="C7" s="232"/>
+      <c r="D7" s="237">
+        <f>'Flujo de Caja (Profesor) - 5 añ'!D10</f>
+        <v>4285000.1198602207</v>
+      </c>
+      <c r="E7" s="237">
+        <f>'Flujo de Caja (Profesor) - 5 añ'!F10</f>
+        <v>4542100.127051834</v>
+      </c>
+      <c r="F7" s="237">
+        <f>'Flujo de Caja (Profesor) - 5 añ'!H10</f>
+        <v>4563525.1276511354</v>
+      </c>
+      <c r="G7" s="237">
+        <f>'Flujo de Caja (Profesor) - 5 añ'!J10</f>
+        <v>4584950.1282504359</v>
+      </c>
+      <c r="H7" s="238">
+        <f>'Flujo de Caja (Profesor) - 5 añ'!L10</f>
+        <v>4593520.1284901565</v>
+      </c>
+    </row>
+    <row r="8" spans="2:8">
+      <c r="B8" s="235" t="s">
+        <v>295</v>
+      </c>
+      <c r="C8" s="239"/>
+      <c r="D8" s="237">
+        <f>D5+D7</f>
+        <v>97939713.775534913</v>
+      </c>
+      <c r="E8" s="237">
+        <f t="shared" ref="E8:G8" si="0">E5+E7</f>
+        <v>103774094.84705183</v>
+      </c>
+      <c r="F8" s="237">
+        <f t="shared" si="0"/>
+        <v>104260293.40765114</v>
+      </c>
+      <c r="G8" s="237">
+        <f t="shared" si="0"/>
+        <v>104746491.96825044</v>
+      </c>
+      <c r="H8" s="238">
+        <f>H5+H7</f>
+        <v>104940971.39249015</v>
+      </c>
+    </row>
+    <row r="9" spans="2:8">
+      <c r="B9" s="235" t="s">
+        <v>288</v>
+      </c>
+      <c r="C9" s="232"/>
+      <c r="D9" s="240">
+        <f>D5/(D6-D7)</f>
+        <v>0.48775778937758141</v>
+      </c>
+      <c r="E9" s="240">
+        <f>E5/(E6-E7)</f>
+        <v>0.2910773566062998</v>
+      </c>
+      <c r="F9" s="240">
+        <f>F5/(F6-F7)</f>
+        <v>0.2012523248530908</v>
+      </c>
+      <c r="G9" s="240">
+        <f>G5/(G6-G7)</f>
+        <v>0.19707748381532467</v>
+      </c>
+      <c r="H9" s="241">
+        <f>H5/(H6-H7)</f>
+        <v>0.1971586242893329</v>
+      </c>
+    </row>
+    <row r="10" spans="2:8" ht="15">
+      <c r="B10" s="229" t="s">
+        <v>292</v>
+      </c>
+      <c r="C10" s="221"/>
+      <c r="D10" s="221"/>
+      <c r="E10" s="221"/>
+      <c r="F10" s="221"/>
+      <c r="G10" s="221"/>
+      <c r="H10" s="230"/>
+    </row>
+    <row r="11" spans="2:8">
+      <c r="B11" s="242"/>
+      <c r="C11" s="225"/>
+      <c r="D11" s="236" t="s">
+        <v>74</v>
+      </c>
+      <c r="E11" s="236" t="s">
+        <v>75</v>
+      </c>
+      <c r="F11" s="236" t="s">
+        <v>76</v>
+      </c>
+      <c r="G11" s="236" t="s">
+        <v>78</v>
+      </c>
+      <c r="H11" s="243" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="12" spans="2:8">
+      <c r="B12" s="235" t="s">
+        <v>122</v>
+      </c>
+      <c r="C12" s="232"/>
+      <c r="D12" s="237">
+        <f>'Flujo de Caja (Profesor) - 5 añ'!D11+'Flujo de Caja (Profesor) - 5 añ'!D12</f>
+        <v>93642264.388820186</v>
+      </c>
+      <c r="E12" s="237">
+        <f>'Flujo de Caja (Profesor) - 5 añ'!F11+'Flujo de Caja (Profesor) - 5 añ'!F12</f>
+        <v>236684255.34988606</v>
+      </c>
+      <c r="F12" s="237">
+        <f>'Flujo de Caja (Profesor) - 5 añ'!H11+'Flujo de Caja (Profesor) - 5 añ'!H12</f>
+        <v>390665065.63257712</v>
+      </c>
+      <c r="G12" s="237">
+        <f>'Flujo de Caja (Profesor) - 5 añ'!J11+'Flujo de Caja (Profesor) - 5 añ'!J12</f>
+        <v>403029102.07787019</v>
+      </c>
+      <c r="H12" s="238">
+        <f>'Flujo de Caja (Profesor) - 5 añ'!L11+'Flujo de Caja (Profesor) - 5 añ'!L12</f>
+        <v>403567545.18674833</v>
+      </c>
+    </row>
+    <row r="13" spans="2:8">
+      <c r="B13" s="235" t="s">
+        <v>293</v>
+      </c>
+      <c r="C13" s="232"/>
+      <c r="D13" s="244">
+        <v>5000</v>
+      </c>
+      <c r="E13" s="244">
+        <v>5000</v>
+      </c>
+      <c r="F13" s="244">
+        <v>5000</v>
+      </c>
+      <c r="G13" s="244">
+        <v>5000</v>
+      </c>
+      <c r="H13" s="245">
+        <v>5000</v>
+      </c>
+    </row>
+    <row r="14" spans="2:8">
+      <c r="B14" s="235" t="s">
+        <v>294</v>
+      </c>
+      <c r="C14" s="232"/>
+      <c r="D14" s="244">
+        <f>('Flujo de Caja (Profesor) - 5 añ'!D6+'Flujo de Caja (Profesor) - 5 añ'!D7)/'Tabla Crecimiento'!B9</f>
+        <v>9347.2407443550801</v>
+      </c>
+      <c r="E14" s="244">
+        <f>('Flujo de Caja (Profesor) - 5 añ'!F6+'Flujo de Caja (Profesor) - 5 añ'!F7)/'Tabla Crecimiento'!B10</f>
+        <v>1522.5324253185552</v>
+      </c>
+      <c r="F14" s="244">
+        <f>('Flujo de Caja (Profesor) - 5 añ'!H6+'Flujo de Caja (Profesor) - 5 añ'!H7)/'Tabla Crecimiento'!B11</f>
+        <v>1056.9747688893165</v>
+      </c>
+      <c r="G14" s="244">
+        <f>('Flujo de Caja (Profesor) - 5 añ'!J6+'Flujo de Caja (Profesor) - 5 añ'!J7)/'Tabla Crecimiento'!B12</f>
+        <v>1035.2442794894923</v>
+      </c>
+      <c r="H14" s="245">
+        <f>('Flujo de Caja (Profesor) - 5 añ'!L6+'Flujo de Caja (Profesor) - 5 añ'!L7)/'Tabla Crecimiento'!B13</f>
+        <v>1035.6665757426188</v>
+      </c>
+    </row>
+    <row r="15" spans="2:8" ht="15.75" thickBot="1">
+      <c r="B15" s="246" t="s">
+        <v>292</v>
+      </c>
+      <c r="C15" s="247"/>
+      <c r="D15" s="248">
+        <f>D12/D13-D14</f>
+        <v>9381.212133408957</v>
+      </c>
+      <c r="E15" s="248">
+        <f t="shared" ref="E15:H15" si="1">E12/E13-E14</f>
+        <v>45814.318644658655</v>
+      </c>
+      <c r="F15" s="248">
+        <f t="shared" si="1"/>
+        <v>77076.038357626108</v>
+      </c>
+      <c r="G15" s="248">
+        <f t="shared" si="1"/>
+        <v>79570.57613608455</v>
+      </c>
+      <c r="H15" s="249">
+        <f t="shared" si="1"/>
+        <v>79677.842461607041</v>
+      </c>
+    </row>
+    <row r="23" spans="2:14">
+      <c r="D23" s="97"/>
+      <c r="E23" s="97"/>
+      <c r="F23" s="97"/>
+      <c r="G23" s="97"/>
+      <c r="H23" s="97"/>
+      <c r="I23" s="97"/>
+      <c r="J23" s="97"/>
+      <c r="K23" s="97"/>
+      <c r="L23" s="97"/>
+      <c r="M23" s="97"/>
+      <c r="N23" s="97"/>
+    </row>
+    <row r="24" spans="2:14">
+      <c r="B24" s="196"/>
+      <c r="C24" s="197"/>
+    </row>
+    <row r="25" spans="2:14">
+      <c r="B25" s="196"/>
+      <c r="C25" s="197"/>
+    </row>
+    <row r="26" spans="2:14">
+      <c r="B26" s="196"/>
+      <c r="C26" s="197"/>
+    </row>
+    <row r="27" spans="2:14">
+      <c r="B27" s="196"/>
+      <c r="C27" s="196"/>
+    </row>
+    <row r="28" spans="2:14">
+      <c r="B28" s="196"/>
+      <c r="C28" s="197"/>
+    </row>
+    <row r="30" spans="2:14">
+      <c r="B30" s="196"/>
+      <c r="C30" s="197"/>
+    </row>
+    <row r="31" spans="2:14">
+      <c r="B31" s="196"/>
+      <c r="C31" s="197"/>
+    </row>
+    <row r="32" spans="2:14">
+      <c r="B32" s="196"/>
+      <c r="C32" s="197"/>
+    </row>
+  </sheetData>
+  <mergeCells count="22">
+    <mergeCell ref="B26:C26"/>
+    <mergeCell ref="B27:C27"/>
+    <mergeCell ref="B28:C28"/>
+    <mergeCell ref="B30:C30"/>
+    <mergeCell ref="B31:C31"/>
+    <mergeCell ref="B32:C32"/>
+    <mergeCell ref="B13:C13"/>
+    <mergeCell ref="B14:C14"/>
+    <mergeCell ref="B15:C15"/>
+    <mergeCell ref="B8:C8"/>
+    <mergeCell ref="B24:C24"/>
+    <mergeCell ref="B25:C25"/>
+    <mergeCell ref="B10:H10"/>
+    <mergeCell ref="B11:C11"/>
+    <mergeCell ref="B9:C9"/>
+    <mergeCell ref="B12:C12"/>
+    <mergeCell ref="B3:H3"/>
+    <mergeCell ref="B2:H2"/>
+    <mergeCell ref="B5:C5"/>
+    <mergeCell ref="B4:C4"/>
+    <mergeCell ref="B6:C6"/>
+    <mergeCell ref="B7:C7"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K16"/>
   <sheetViews>
@@ -8171,26 +8690,26 @@
   <sheetData>
     <row r="1" spans="1:11" ht="15.75" customHeight="1">
       <c r="A1" s="158"/>
-      <c r="B1" s="213" t="s">
+      <c r="B1" s="217" t="s">
         <v>74</v>
       </c>
-      <c r="C1" s="214"/>
-      <c r="D1" s="213" t="s">
+      <c r="C1" s="218"/>
+      <c r="D1" s="217" t="s">
         <v>75</v>
       </c>
-      <c r="E1" s="214"/>
-      <c r="F1" s="213" t="s">
+      <c r="E1" s="218"/>
+      <c r="F1" s="217" t="s">
         <v>76</v>
       </c>
-      <c r="G1" s="214"/>
-      <c r="H1" s="213" t="s">
+      <c r="G1" s="218"/>
+      <c r="H1" s="217" t="s">
         <v>78</v>
       </c>
-      <c r="I1" s="214"/>
-      <c r="J1" s="217" t="s">
+      <c r="I1" s="218"/>
+      <c r="J1" s="221" t="s">
         <v>79</v>
       </c>
-      <c r="K1" s="218"/>
+      <c r="K1" s="222"/>
     </row>
     <row r="2" spans="1:11" ht="15.75" customHeight="1">
       <c r="A2" s="31" t="s">
@@ -8512,7 +9031,7 @@
     </row>
     <row r="11" spans="1:11" ht="15.75" customHeight="1">
       <c r="A11" s="40" t="s">
-        <v>257</v>
+        <v>255</v>
       </c>
       <c r="B11" s="90">
         <f>C11/$C$9</f>
@@ -8557,7 +9076,7 @@
     </row>
     <row r="12" spans="1:11" ht="15.75" customHeight="1">
       <c r="A12" s="40" t="s">
-        <v>258</v>
+        <v>256</v>
       </c>
       <c r="B12" s="90">
         <f>C12/$C$9</f>
@@ -8602,7 +9121,7 @@
     </row>
     <row r="13" spans="1:11" ht="15.75" customHeight="1">
       <c r="A13" s="40" t="s">
-        <v>259</v>
+        <v>257</v>
       </c>
       <c r="B13" s="90">
         <f>C13/$C$9</f>
@@ -8647,7 +9166,7 @@
     </row>
     <row r="14" spans="1:11" ht="15.75" customHeight="1">
       <c r="A14" s="40" t="s">
-        <v>260</v>
+        <v>258</v>
       </c>
       <c r="B14" s="90">
         <f>C14/$C$9</f>
@@ -8797,7 +9316,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F7"/>
   <sheetViews>
@@ -8943,7 +9462,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D10"/>
   <sheetViews>
@@ -9089,334 +9608,483 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J25"/>
+  <dimension ref="A1:O35"/>
   <sheetViews>
-    <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="B14" sqref="B14"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="H18" sqref="H18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1"/>
   <cols>
-    <col min="1" max="1" width="49.5703125" customWidth="1"/>
-    <col min="2" max="2" width="16.85546875" customWidth="1"/>
-    <col min="3" max="3" width="37.42578125" customWidth="1"/>
-    <col min="4" max="4" width="18.7109375" customWidth="1"/>
-    <col min="5" max="5" width="15.85546875" customWidth="1"/>
-    <col min="7" max="7" width="36.85546875" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="42" customWidth="1"/>
-    <col min="10" max="10" width="19.28515625" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="21.85546875" customWidth="1"/>
+    <col min="2" max="2" width="18.140625" customWidth="1"/>
+    <col min="8" max="8" width="17.7109375" customWidth="1"/>
+    <col min="14" max="14" width="23.85546875" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="19.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" ht="12" customHeight="1" thickTop="1" thickBot="1">
-      <c r="A1" s="116" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="116" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="2" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="2" spans="1:10" ht="13.5" thickTop="1">
-      <c r="A2" s="5" t="s">
-        <v>248</v>
-      </c>
-      <c r="B2" s="122">
-        <f>SUM(B3:B9
-)</f>
-        <v>116700</v>
-      </c>
-      <c r="C2" s="3"/>
-    </row>
-    <row r="3" spans="1:10" ht="12.75">
-      <c r="A3" s="7" t="s">
-        <v>44</v>
-      </c>
-      <c r="B3" s="123">
-        <f>B25</f>
-        <v>51000</v>
-      </c>
-      <c r="C3" s="4"/>
-    </row>
-    <row r="4" spans="1:10" ht="12.75">
-      <c r="A4" s="7" t="s">
-        <v>47</v>
-      </c>
-      <c r="B4" s="124">
-        <v>0</v>
-      </c>
-      <c r="C4" s="4" t="s">
+    <row r="1" spans="1:15" ht="15.75" customHeight="1">
+      <c r="A1" s="79" t="s">
+        <v>125</v>
+      </c>
+      <c r="B1" s="79" t="s">
+        <v>126</v>
+      </c>
+      <c r="C1" s="83" t="s">
+        <v>241</v>
+      </c>
+      <c r="E1" t="s">
+        <v>133</v>
+      </c>
+      <c r="F1" t="s">
+        <v>134</v>
+      </c>
+      <c r="H1" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="2" spans="1:15" ht="15.75" customHeight="1">
+      <c r="A2" s="85" t="s">
+        <v>136</v>
+      </c>
+      <c r="B2" s="86">
+        <v>0</v>
+      </c>
+      <c r="C2" s="117"/>
+      <c r="E2">
+        <v>6</v>
+      </c>
+      <c r="F2">
+        <f>$I$2/(1+EXP((-1)*$I$4*(E2-$I$3)))</f>
+        <v>2577.2486775983025</v>
+      </c>
+      <c r="H2" t="s">
+        <v>138</v>
+      </c>
+      <c r="I2">
+        <f>O2*L4</f>
+        <v>96900</v>
+      </c>
+      <c r="K2" t="s">
+        <v>175</v>
+      </c>
+      <c r="N2" t="s">
+        <v>176</v>
+      </c>
+      <c r="O2">
+        <v>190000</v>
+      </c>
+    </row>
+    <row r="3" spans="1:15" ht="15.75" customHeight="1">
+      <c r="A3" s="85" t="s">
+        <v>67</v>
+      </c>
+      <c r="B3" s="86">
+        <f t="shared" ref="B3:B8" si="0">F3</f>
+        <v>3252.8577359756564</v>
+      </c>
+      <c r="C3" s="117">
+        <f>B3*($O$3+($O$3*0.19))</f>
+        <v>17241349.195529614</v>
+      </c>
+      <c r="E3">
+        <v>7</v>
+      </c>
+      <c r="F3">
+        <f>$I$2/(1+EXP((-1)*$I$4*(E3-$I$3)))</f>
+        <v>3252.8577359756564</v>
+      </c>
+      <c r="H3" t="s">
+        <v>140</v>
+      </c>
+      <c r="I3">
+        <f>AVERAGE(E2:E12)</f>
+        <v>21</v>
+      </c>
+      <c r="K3" t="s">
+        <v>177</v>
+      </c>
+      <c r="L3" s="98">
+        <v>0.32</v>
+      </c>
+      <c r="N3" t="s">
+        <v>279</v>
+      </c>
+      <c r="O3" s="181">
+        <f>('Salarios, gastos y costos'!G66/F29)+(('Salarios, gastos y costos'!G66/F29*O4))</f>
+        <v>4454.0923433263852</v>
+      </c>
+    </row>
+    <row r="4" spans="1:15" ht="15.75" customHeight="1">
+      <c r="A4" s="85" t="s">
+        <v>68</v>
+      </c>
+      <c r="B4" s="86">
+        <f t="shared" si="0"/>
+        <v>4097.8788914930747</v>
+      </c>
+      <c r="C4" s="117">
+        <f t="shared" ref="C4:C13" si="1">B4*($O$3+($O$3*0.19))</f>
+        <v>21720273.883428961</v>
+      </c>
+      <c r="E4">
+        <v>8</v>
+      </c>
+      <c r="F4">
+        <f t="shared" ref="F4:F12" si="2">$I$2/(1+EXP((-1)*$I$4*(E4-$I$3)))</f>
+        <v>4097.8788914930747</v>
+      </c>
+      <c r="H4" t="s">
+        <v>143</v>
+      </c>
+      <c r="I4">
+        <v>0.24</v>
+      </c>
+      <c r="K4" t="s">
+        <v>178</v>
+      </c>
+      <c r="L4" s="98">
+        <v>0.51</v>
+      </c>
+      <c r="N4" s="97" t="s">
+        <v>280</v>
+      </c>
+      <c r="O4" s="148">
+        <v>0.62350000000000005</v>
+      </c>
+    </row>
+    <row r="5" spans="1:15" ht="15.75" customHeight="1">
+      <c r="A5" s="85" t="s">
+        <v>69</v>
+      </c>
+      <c r="B5" s="86">
+        <f t="shared" si="0"/>
+        <v>5150.3451169723749</v>
+      </c>
+      <c r="C5" s="117">
+        <f>B5*($O$3+($O$3*0.19))</f>
+        <v>27298734.173684157</v>
+      </c>
+      <c r="E5">
+        <v>9</v>
+      </c>
+      <c r="F5">
+        <f t="shared" si="2"/>
+        <v>5150.3451169723749</v>
+      </c>
+      <c r="K5" t="s">
+        <v>179</v>
+      </c>
+      <c r="L5" s="98">
+        <v>0.16</v>
+      </c>
+      <c r="O5" s="180">
+        <f>('Salarios, gastos y costos'!G66/F29)</f>
+        <v>2743.5123765484354</v>
+      </c>
+    </row>
+    <row r="6" spans="1:15" ht="15.75" customHeight="1">
+      <c r="A6" s="85" t="s">
+        <v>70</v>
+      </c>
+      <c r="B6" s="86">
+        <f t="shared" si="0"/>
+        <v>6454.3186472262878</v>
+      </c>
+      <c r="C6" s="117">
+        <f t="shared" si="1"/>
+        <v>34210276.20891919</v>
+      </c>
+      <c r="E6">
+        <v>10</v>
+      </c>
+      <c r="F6">
+        <f t="shared" si="2"/>
+        <v>6454.3186472262878</v>
+      </c>
+    </row>
+    <row r="7" spans="1:15" ht="15.75" customHeight="1">
+      <c r="A7" s="85" t="s">
+        <v>71</v>
+      </c>
+      <c r="B7" s="86">
+        <f t="shared" si="0"/>
+        <v>8059.4342902610779</v>
+      </c>
+      <c r="C7" s="117">
+        <f t="shared" si="1"/>
+        <v>42717982.83091484</v>
+      </c>
+      <c r="E7">
+        <v>11</v>
+      </c>
+      <c r="F7">
+        <f t="shared" si="2"/>
+        <v>8059.4342902610779</v>
+      </c>
+    </row>
+    <row r="8" spans="1:15" ht="15.75" customHeight="1">
+      <c r="A8" s="85" t="s">
+        <v>72</v>
+      </c>
+      <c r="B8" s="86">
+        <f t="shared" si="0"/>
+        <v>10019.503746304383</v>
+      </c>
+      <c r="C8" s="117">
+        <f t="shared" si="1"/>
+        <v>53107075.955209814</v>
+      </c>
+      <c r="D8" t="s">
+        <v>180</v>
+      </c>
+      <c r="E8">
+        <v>12</v>
+      </c>
+      <c r="F8">
+        <f t="shared" si="2"/>
+        <v>10019.503746304383</v>
+      </c>
+    </row>
+    <row r="9" spans="1:15" ht="15.75" customHeight="1">
+      <c r="A9" s="85" t="s">
+        <v>74</v>
+      </c>
+      <c r="B9" s="86">
+        <f>F8</f>
+        <v>10019.503746304383</v>
+      </c>
+      <c r="C9" s="117">
+        <f t="shared" si="1"/>
+        <v>53107075.955209814</v>
+      </c>
+      <c r="D9" t="s">
+        <v>181</v>
+      </c>
+      <c r="E9">
+        <v>24</v>
+      </c>
+      <c r="F9">
+        <f t="shared" si="2"/>
+        <v>65175.619953865986</v>
+      </c>
+    </row>
+    <row r="10" spans="1:15" ht="15.75" customHeight="1">
+      <c r="A10" s="85" t="s">
+        <v>75</v>
+      </c>
+      <c r="B10" s="86">
+        <f>F9</f>
+        <v>65175.619953865986</v>
+      </c>
+      <c r="C10" s="117">
+        <f t="shared" si="1"/>
+        <v>345454893.47159714</v>
+      </c>
+      <c r="D10" t="s">
+        <v>182</v>
+      </c>
+      <c r="E10">
+        <v>36</v>
+      </c>
+      <c r="F10">
+        <f>$I$2/(1+EXP((-1)*$I$4*(E10-$I$3)))</f>
+        <v>94322.751322401688</v>
+      </c>
+    </row>
+    <row r="11" spans="1:15" ht="15.75" customHeight="1">
+      <c r="A11" s="85" t="s">
+        <v>76</v>
+      </c>
+      <c r="B11" s="86">
+        <f>F10</f>
+        <v>94322.751322401688</v>
+      </c>
+      <c r="C11" s="117">
+        <f t="shared" si="1"/>
+        <v>499945470.91523975</v>
+      </c>
+      <c r="D11" t="s">
+        <v>183</v>
+      </c>
+      <c r="E11">
         <v>48</v>
       </c>
-    </row>
-    <row r="5" spans="1:10" ht="12.75">
-      <c r="A5" s="7" t="s">
-        <v>49</v>
-      </c>
-      <c r="B5" s="124">
-        <v>0</v>
-      </c>
-      <c r="C5" s="3"/>
-    </row>
-    <row r="6" spans="1:10" ht="12.75">
-      <c r="A6" s="7" t="s">
-        <v>50</v>
-      </c>
-      <c r="B6" s="124">
-        <f>5400</f>
-        <v>5400</v>
-      </c>
-      <c r="C6" s="4" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="7" spans="1:10" ht="12.75">
-      <c r="A7" s="7" t="s">
-        <v>52</v>
-      </c>
-      <c r="B7" s="124">
-        <v>0</v>
-      </c>
-      <c r="C7" s="3"/>
-    </row>
-    <row r="8" spans="1:10" ht="12.75">
-      <c r="A8" s="7" t="s">
-        <v>53</v>
-      </c>
-      <c r="B8" s="124">
-        <v>10300</v>
-      </c>
-      <c r="C8" s="3"/>
-    </row>
-    <row r="9" spans="1:10" ht="12.75">
-      <c r="A9" s="7" t="s">
-        <v>54</v>
-      </c>
-      <c r="B9" s="124">
-        <v>50000</v>
-      </c>
-      <c r="C9" s="3"/>
-    </row>
-    <row r="10" spans="1:10" ht="12.75">
-      <c r="A10" s="5" t="s">
-        <v>250</v>
-      </c>
-      <c r="B10" s="122">
-        <f>SUM(B11:B14
-)</f>
-        <v>5552860</v>
-      </c>
-      <c r="C10" s="3"/>
-    </row>
-    <row r="11" spans="1:10" ht="12.75">
-      <c r="A11" s="7" t="s">
-        <v>58</v>
-      </c>
-      <c r="B11" s="124">
-        <v>60800</v>
-      </c>
-      <c r="C11" s="4"/>
-    </row>
-    <row r="12" spans="1:10" ht="22.5">
-      <c r="A12" s="95" t="s">
-        <v>171</v>
-      </c>
-      <c r="B12" s="124">
-        <v>3000000</v>
-      </c>
-    </row>
-    <row r="13" spans="1:10" ht="12.75">
-      <c r="A13" s="120" t="s">
+      <c r="F11">
+        <f t="shared" si="2"/>
+        <v>96751.601360591376</v>
+      </c>
+    </row>
+    <row r="12" spans="1:15" ht="15.75" customHeight="1">
+      <c r="A12" s="85" t="s">
+        <v>78</v>
+      </c>
+      <c r="B12" s="86">
+        <f>F11</f>
+        <v>96751.601360591376</v>
+      </c>
+      <c r="C12" s="117">
+        <f t="shared" si="1"/>
+        <v>512819274.52148426</v>
+      </c>
+      <c r="D12" t="s">
+        <v>184</v>
+      </c>
+      <c r="E12">
         <v>60</v>
       </c>
-      <c r="B13" s="125">
-        <v>500000</v>
-      </c>
-      <c r="C13" s="4"/>
-    </row>
-    <row r="14" spans="1:10" ht="13.5" thickBot="1">
-      <c r="A14" s="121" t="s">
-        <v>249</v>
-      </c>
-      <c r="B14" s="126">
-        <f>'Salarios, gastos y costos'!K11*6</f>
-        <v>1992060</v>
-      </c>
-      <c r="C14" s="3"/>
-    </row>
-    <row r="15" spans="1:10" ht="16.5" thickTop="1" thickBot="1">
-      <c r="A15" s="127" t="s">
-        <v>61</v>
-      </c>
-      <c r="B15" s="128">
-        <f>B10+B2</f>
-        <v>5669560</v>
-      </c>
-    </row>
-    <row r="16" spans="1:10" ht="13.5" thickTop="1">
-      <c r="D16" s="3"/>
-      <c r="E16" s="3"/>
-      <c r="F16" s="3"/>
-      <c r="G16" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="H16" s="96" t="s">
-        <v>4</v>
-      </c>
-      <c r="I16" s="96" t="s">
-        <v>5</v>
-      </c>
-      <c r="J16" s="4" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="17" spans="1:10" ht="12.75">
-      <c r="A17" s="11"/>
-      <c r="D17" s="4" t="s">
-        <v>27</v>
-      </c>
-      <c r="E17" s="18">
-        <v>1500000</v>
-      </c>
-      <c r="F17" s="3"/>
-      <c r="G17" s="4" t="s">
-        <v>36</v>
-      </c>
-      <c r="H17" s="4">
-        <v>5</v>
-      </c>
-      <c r="I17" s="3">
-        <f>H17*12</f>
-        <v>60</v>
-      </c>
-      <c r="J17" s="21">
-        <f>SUM(B12,B13)/I17</f>
-        <v>58333.333333333336</v>
-      </c>
-    </row>
-    <row r="18" spans="1:10" ht="12.75">
-      <c r="A18" s="107" t="s">
-        <v>165</v>
-      </c>
-      <c r="B18" s="115" t="s">
-        <v>1</v>
-      </c>
-      <c r="D18" s="4" t="s">
-        <v>43</v>
-      </c>
-      <c r="E18" s="21">
-        <v>975000</v>
-      </c>
-      <c r="F18" s="3"/>
-    </row>
-    <row r="19" spans="1:10" ht="15.75" customHeight="1">
-      <c r="A19" s="100" t="s">
-        <v>166</v>
-      </c>
-      <c r="B19" s="113">
-        <f>39000</f>
-        <v>39000</v>
-      </c>
-      <c r="D19" s="3"/>
-      <c r="E19" s="3"/>
-      <c r="F19" s="3"/>
-      <c r="G19" s="3"/>
-      <c r="H19" s="3"/>
-      <c r="I19" s="3"/>
-      <c r="J19" s="3"/>
-    </row>
-    <row r="20" spans="1:10" ht="15.75" customHeight="1">
-      <c r="A20" s="100" t="s">
-        <v>167</v>
-      </c>
-      <c r="B20" s="113">
-        <v>4760</v>
-      </c>
-      <c r="D20" s="11" t="s">
-        <v>56</v>
-      </c>
-      <c r="E20" s="3"/>
-      <c r="F20" s="3"/>
-      <c r="G20" s="3"/>
-      <c r="H20" s="3"/>
-      <c r="I20" s="4" t="s">
-        <v>46</v>
-      </c>
-      <c r="J20" s="21">
-        <f>SUM(J17:J19
-)</f>
-        <v>58333.333333333336</v>
-      </c>
-    </row>
-    <row r="21" spans="1:10" ht="15.75" customHeight="1">
-      <c r="A21" s="100" t="s">
-        <v>167</v>
-      </c>
-      <c r="B21" s="113">
-        <v>2040</v>
-      </c>
-      <c r="D21" s="25">
-        <f>SUM(B12:B13
-)</f>
-        <v>3500000</v>
-      </c>
-    </row>
-    <row r="22" spans="1:10" ht="15.75" customHeight="1">
-      <c r="A22" s="100" t="s">
-        <v>168</v>
-      </c>
-      <c r="B22" s="113">
-        <v>39000</v>
-      </c>
-    </row>
-    <row r="23" spans="1:10" ht="15.75" customHeight="1">
-      <c r="A23" s="100" t="s">
-        <v>169</v>
-      </c>
-      <c r="B23" s="113">
-        <v>-39000</v>
-      </c>
-      <c r="D23" s="18">
-        <f>SUM(B11:B13
-)</f>
-        <v>3560800</v>
-      </c>
-    </row>
-    <row r="24" spans="1:10" ht="15.75" customHeight="1">
-      <c r="A24" s="100" t="s">
-        <v>170</v>
-      </c>
-      <c r="B24" s="113">
-        <v>5200</v>
-      </c>
-      <c r="G24" s="4" t="s">
-        <v>36</v>
-      </c>
-      <c r="H24" s="4">
-        <v>1</v>
-      </c>
-      <c r="I24" s="3">
-        <f>H24*12</f>
+      <c r="F12">
+        <f t="shared" si="2"/>
+        <v>96891.657618714249</v>
+      </c>
+    </row>
+    <row r="13" spans="1:15" ht="15.75" customHeight="1">
+      <c r="A13" s="85" t="s">
+        <v>79</v>
+      </c>
+      <c r="B13" s="86">
+        <f>F12</f>
+        <v>96891.657618714249</v>
+      </c>
+      <c r="C13" s="117">
+        <f t="shared" si="1"/>
+        <v>513561624.49474293</v>
+      </c>
+    </row>
+    <row r="14" spans="1:15" ht="15.75" customHeight="1">
+      <c r="A14" s="11"/>
+    </row>
+    <row r="15" spans="1:15" ht="15.75" customHeight="1">
+      <c r="A15" s="11"/>
+    </row>
+    <row r="22" spans="5:6" ht="15.75" customHeight="1">
+      <c r="E22">
         <v>12</v>
       </c>
-      <c r="J24" s="21">
-        <f>SUM($B$12,$B$13)/I24</f>
-        <v>291666.66666666669</v>
-      </c>
-    </row>
-    <row r="25" spans="1:10" ht="15.75" customHeight="1">
-      <c r="A25" s="107" t="s">
-        <v>46</v>
-      </c>
-      <c r="B25" s="114">
-        <f>SUM(B19:B24)</f>
-        <v>51000</v>
+      <c r="F22" s="182">
+        <f>$I$2/(1+EXP((-1)*$I$4*(E22-$I$3)))</f>
+        <v>10019.503746304383</v>
+      </c>
+    </row>
+    <row r="23" spans="5:6" ht="15.75" customHeight="1">
+      <c r="E23">
+        <v>13</v>
+      </c>
+      <c r="F23" s="182">
+        <f t="shared" ref="F23:F35" si="3">$I$2/(1+EXP((-1)*$I$4*(E23-$I$3)))</f>
+        <v>12389.78577631898</v>
+      </c>
+    </row>
+    <row r="24" spans="5:6" ht="15.75" customHeight="1">
+      <c r="E24">
+        <v>14</v>
+      </c>
+      <c r="F24" s="182">
+        <f t="shared" si="3"/>
+        <v>15222.55093500037</v>
+      </c>
+    </row>
+    <row r="25" spans="5:6" ht="15.75" customHeight="1">
+      <c r="E25">
+        <v>15</v>
+      </c>
+      <c r="F25" s="182">
+        <f t="shared" si="3"/>
+        <v>18560.744275606201</v>
+      </c>
+    </row>
+    <row r="26" spans="5:6" ht="15.75" customHeight="1">
+      <c r="E26">
+        <v>16</v>
+      </c>
+      <c r="F26" s="182">
+        <f t="shared" si="3"/>
+        <v>22429.948478945193</v>
+      </c>
+    </row>
+    <row r="27" spans="5:6" ht="15.75" customHeight="1">
+      <c r="E27">
+        <v>17</v>
+      </c>
+      <c r="F27" s="182">
+        <f t="shared" si="3"/>
+        <v>26829.497083446626</v>
+      </c>
+    </row>
+    <row r="28" spans="5:6" ht="15.75" customHeight="1">
+      <c r="E28">
+        <v>18</v>
+      </c>
+      <c r="F28" s="182">
+        <f t="shared" si="3"/>
+        <v>31724.380046134014</v>
+      </c>
+    </row>
+    <row r="29" spans="5:6" ht="15.75" customHeight="1">
+      <c r="E29">
+        <v>19</v>
+      </c>
+      <c r="F29" s="182">
+        <f t="shared" si="3"/>
+        <v>37040.23093485977</v>
+      </c>
+    </row>
+    <row r="30" spans="5:6" ht="15.75" customHeight="1">
+      <c r="E30">
+        <v>20</v>
+      </c>
+      <c r="F30" s="182">
+        <f t="shared" si="3"/>
+        <v>42663.747386009003</v>
+      </c>
+    </row>
+    <row r="31" spans="5:6" ht="15.75" customHeight="1">
+      <c r="E31">
+        <v>21</v>
+      </c>
+      <c r="F31" s="182">
+        <f t="shared" si="3"/>
+        <v>48450</v>
+      </c>
+    </row>
+    <row r="32" spans="5:6" ht="15.75" customHeight="1">
+      <c r="E32">
+        <v>22</v>
+      </c>
+      <c r="F32" s="182">
+        <f t="shared" si="3"/>
+        <v>54236.252613990997</v>
+      </c>
+    </row>
+    <row r="33" spans="5:6" ht="15.75" customHeight="1">
+      <c r="E33">
+        <v>23</v>
+      </c>
+      <c r="F33" s="182">
+        <f t="shared" si="3"/>
+        <v>59859.769065140223</v>
+      </c>
+    </row>
+    <row r="34" spans="5:6" ht="15.75" customHeight="1">
+      <c r="E34">
+        <v>24</v>
+      </c>
+      <c r="F34" s="182">
+        <f t="shared" si="3"/>
+        <v>65175.619953865986</v>
+      </c>
+    </row>
+    <row r="35" spans="5:6" ht="15.75" customHeight="1">
+      <c r="E35">
+        <v>25</v>
+      </c>
+      <c r="F35" s="182">
+        <f t="shared" si="3"/>
+        <v>70070.502916553378</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -9424,7 +10092,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N67"/>
   <sheetViews>
-    <sheetView topLeftCell="A49" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+    <sheetView topLeftCell="A46" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
       <selection activeCell="G66" sqref="G66"/>
     </sheetView>
   </sheetViews>
@@ -9440,22 +10108,22 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:14" ht="15.75" customHeight="1">
-      <c r="A1" s="181" t="s">
+      <c r="A1" s="185" t="s">
         <v>8</v>
       </c>
-      <c r="B1" s="182"/>
-      <c r="D1" s="181" t="s">
+      <c r="B1" s="186"/>
+      <c r="D1" s="185" t="s">
         <v>9</v>
       </c>
-      <c r="E1" s="182"/>
-      <c r="G1" s="181" t="s">
+      <c r="E1" s="186"/>
+      <c r="G1" s="185" t="s">
         <v>10</v>
       </c>
-      <c r="H1" s="182"/>
-      <c r="J1" s="181" t="s">
+      <c r="H1" s="186"/>
+      <c r="J1" s="185" t="s">
         <v>11</v>
       </c>
-      <c r="K1" s="182"/>
+      <c r="K1" s="186"/>
       <c r="M1" s="6" t="s">
         <v>12</v>
       </c>
@@ -9613,7 +10281,7 @@
     </row>
     <row r="11" spans="1:14" ht="15.75" customHeight="1">
       <c r="A11" s="5" t="s">
-        <v>221</v>
+        <v>219</v>
       </c>
       <c r="B11" s="16">
         <f>SUM(B2:B10)</f>
@@ -9650,7 +10318,7 @@
     </row>
     <row r="12" spans="1:14" ht="15.75" customHeight="1">
       <c r="A12" s="109" t="s">
-        <v>222</v>
+        <v>220</v>
       </c>
       <c r="B12" s="16">
         <f>B11*12</f>
@@ -9666,10 +10334,10 @@
       </c>
     </row>
     <row r="17" spans="1:6" ht="15.75" customHeight="1">
-      <c r="A17" s="181" t="s">
+      <c r="A17" s="185" t="s">
         <v>35</v>
       </c>
-      <c r="B17" s="182"/>
+      <c r="B17" s="186"/>
       <c r="E17" s="11" t="s">
         <v>37</v>
       </c>
@@ -9830,26 +10498,26 @@
     </row>
     <row r="33" spans="1:8" ht="15.75" customHeight="1" thickBot="1"/>
     <row r="34" spans="1:8" ht="15.75" customHeight="1" thickTop="1" thickBot="1">
-      <c r="A34" s="184" t="s">
-        <v>220</v>
-      </c>
-      <c r="B34" s="184"/>
-      <c r="C34" s="184"/>
-      <c r="D34" s="184"/>
-      <c r="E34" s="184"/>
-      <c r="F34" s="184"/>
-      <c r="G34" s="184"/>
-      <c r="H34" s="184"/>
+      <c r="A34" s="188" t="s">
+        <v>218</v>
+      </c>
+      <c r="B34" s="188"/>
+      <c r="C34" s="188"/>
+      <c r="D34" s="188"/>
+      <c r="E34" s="188"/>
+      <c r="F34" s="188"/>
+      <c r="G34" s="188"/>
+      <c r="H34" s="188"/>
     </row>
     <row r="35" spans="1:8" ht="15.75" customHeight="1" thickTop="1" thickBot="1">
-      <c r="A35" s="185"/>
-      <c r="B35" s="185"/>
-      <c r="C35" s="185"/>
-      <c r="D35" s="185"/>
-      <c r="E35" s="185"/>
-      <c r="F35" s="185"/>
-      <c r="G35" s="185"/>
-      <c r="H35" s="185"/>
+      <c r="A35" s="189"/>
+      <c r="B35" s="189"/>
+      <c r="C35" s="189"/>
+      <c r="D35" s="189"/>
+      <c r="E35" s="189"/>
+      <c r="F35" s="189"/>
+      <c r="G35" s="189"/>
+      <c r="H35" s="189"/>
     </row>
     <row r="36" spans="1:8" ht="46.5" customHeight="1" thickTop="1" thickBot="1">
       <c r="A36" s="112" t="s">
@@ -10055,244 +10723,244 @@
     </row>
     <row r="45" spans="1:8" ht="15.75" customHeight="1" thickBot="1"/>
     <row r="46" spans="1:8" ht="15.75" customHeight="1" thickTop="1" thickBot="1">
-      <c r="A46" s="184" t="s">
-        <v>238</v>
-      </c>
-      <c r="B46" s="184"/>
-      <c r="C46" s="184"/>
-      <c r="D46" s="184"/>
-      <c r="E46" s="184"/>
-      <c r="F46" s="184"/>
+      <c r="A46" s="188" t="s">
+        <v>236</v>
+      </c>
+      <c r="B46" s="188"/>
+      <c r="C46" s="188"/>
+      <c r="D46" s="188"/>
+      <c r="E46" s="188"/>
+      <c r="F46" s="188"/>
     </row>
     <row r="47" spans="1:8" ht="15.75" customHeight="1" thickTop="1">
-      <c r="A47" s="186" t="s">
+      <c r="A47" s="190" t="s">
+        <v>221</v>
+      </c>
+      <c r="B47" s="190"/>
+      <c r="C47" s="190"/>
+      <c r="D47" s="190"/>
+      <c r="E47" s="190" t="s">
+        <v>74</v>
+      </c>
+      <c r="F47" s="190"/>
+    </row>
+    <row r="48" spans="1:8" ht="15.75" customHeight="1">
+      <c r="A48" s="192" t="s">
+        <v>229</v>
+      </c>
+      <c r="B48" s="193"/>
+      <c r="C48" s="196" t="s">
+        <v>222</v>
+      </c>
+      <c r="D48" s="197"/>
+      <c r="E48" s="187">
+        <v>0</v>
+      </c>
+      <c r="F48" s="187"/>
+    </row>
+    <row r="49" spans="1:6" ht="15.75" customHeight="1">
+      <c r="A49" s="193"/>
+      <c r="B49" s="193"/>
+      <c r="C49" s="196" t="s">
         <v>223</v>
       </c>
-      <c r="B47" s="186"/>
-      <c r="C47" s="186"/>
-      <c r="D47" s="186"/>
-      <c r="E47" s="186" t="s">
-        <v>74</v>
-      </c>
-      <c r="F47" s="186"/>
-    </row>
-    <row r="48" spans="1:8" ht="15.75" customHeight="1">
-      <c r="A48" s="188" t="s">
-        <v>231</v>
-      </c>
-      <c r="B48" s="189"/>
-      <c r="C48" s="192" t="s">
-        <v>224</v>
-      </c>
-      <c r="D48" s="193"/>
-      <c r="E48" s="183">
-        <v>0</v>
-      </c>
-      <c r="F48" s="183"/>
-    </row>
-    <row r="49" spans="1:6" ht="15.75" customHeight="1">
-      <c r="A49" s="189"/>
-      <c r="B49" s="189"/>
-      <c r="C49" s="192" t="s">
-        <v>225</v>
-      </c>
-      <c r="D49" s="193"/>
-      <c r="E49" s="183">
+      <c r="D49" s="197"/>
+      <c r="E49" s="187">
         <f>B2*12</f>
         <v>19200000</v>
       </c>
-      <c r="F49" s="183"/>
+      <c r="F49" s="187"/>
     </row>
     <row r="50" spans="1:6" ht="15.75" customHeight="1">
-      <c r="A50" s="189"/>
-      <c r="B50" s="189"/>
-      <c r="C50" s="192" t="s">
-        <v>226</v>
-      </c>
-      <c r="D50" s="193"/>
-      <c r="E50" s="183">
+      <c r="A50" s="193"/>
+      <c r="B50" s="193"/>
+      <c r="C50" s="196" t="s">
+        <v>224</v>
+      </c>
+      <c r="D50" s="197"/>
+      <c r="E50" s="187">
         <f>(B19*12+B22*12)</f>
         <v>39415992</v>
       </c>
-      <c r="F50" s="183"/>
+      <c r="F50" s="187"/>
     </row>
     <row r="51" spans="1:6" ht="15.75" customHeight="1">
-      <c r="A51" s="189"/>
-      <c r="B51" s="189"/>
-      <c r="C51" s="192" t="s">
-        <v>227</v>
-      </c>
-      <c r="D51" s="192"/>
-      <c r="E51" s="183">
+      <c r="A51" s="193"/>
+      <c r="B51" s="193"/>
+      <c r="C51" s="196" t="s">
+        <v>225</v>
+      </c>
+      <c r="D51" s="196"/>
+      <c r="E51" s="187">
         <f>B4*12</f>
         <v>2400000</v>
       </c>
-      <c r="F51" s="183"/>
+      <c r="F51" s="187"/>
     </row>
     <row r="52" spans="1:6" ht="15.75" customHeight="1">
-      <c r="A52" s="189"/>
-      <c r="B52" s="189"/>
-      <c r="C52" s="192" t="s">
-        <v>228</v>
-      </c>
-      <c r="D52" s="193"/>
-      <c r="E52" s="183">
+      <c r="A52" s="193"/>
+      <c r="B52" s="193"/>
+      <c r="C52" s="196" t="s">
+        <v>226</v>
+      </c>
+      <c r="D52" s="197"/>
+      <c r="E52" s="187">
         <f>(B21+B23)*12</f>
         <v>31938720</v>
       </c>
-      <c r="F52" s="183"/>
+      <c r="F52" s="187"/>
     </row>
     <row r="53" spans="1:6" ht="15.75" customHeight="1" thickBot="1">
-      <c r="A53" s="189"/>
-      <c r="B53" s="189"/>
-      <c r="C53" s="192" t="s">
-        <v>229</v>
-      </c>
-      <c r="D53" s="193"/>
-      <c r="E53" s="183">
-        <v>0</v>
-      </c>
-      <c r="F53" s="183"/>
+      <c r="A53" s="193"/>
+      <c r="B53" s="193"/>
+      <c r="C53" s="196" t="s">
+        <v>227</v>
+      </c>
+      <c r="D53" s="197"/>
+      <c r="E53" s="187">
+        <v>0</v>
+      </c>
+      <c r="F53" s="187"/>
     </row>
     <row r="54" spans="1:6" ht="15.75" customHeight="1" thickTop="1" thickBot="1">
-      <c r="A54" s="189"/>
-      <c r="B54" s="189"/>
-      <c r="C54" s="184" t="s">
-        <v>230</v>
-      </c>
-      <c r="D54" s="184"/>
-      <c r="E54" s="187">
+      <c r="A54" s="193"/>
+      <c r="B54" s="193"/>
+      <c r="C54" s="188" t="s">
+        <v>228</v>
+      </c>
+      <c r="D54" s="188"/>
+      <c r="E54" s="191">
         <f>SUM(E48:F53)</f>
         <v>92954712</v>
       </c>
-      <c r="F54" s="187"/>
+      <c r="F54" s="191"/>
     </row>
     <row r="55" spans="1:6" ht="15.75" customHeight="1" thickTop="1">
-      <c r="A55" s="188" t="s">
-        <v>237</v>
-      </c>
-      <c r="B55" s="189"/>
-      <c r="C55" s="190" t="s">
-        <v>232</v>
-      </c>
-      <c r="D55" s="191"/>
-      <c r="E55" s="194">
-        <v>0</v>
-      </c>
-      <c r="F55" s="194"/>
+      <c r="A55" s="192" t="s">
+        <v>235</v>
+      </c>
+      <c r="B55" s="193"/>
+      <c r="C55" s="194" t="s">
+        <v>230</v>
+      </c>
+      <c r="D55" s="195"/>
+      <c r="E55" s="198">
+        <v>0</v>
+      </c>
+      <c r="F55" s="198"/>
     </row>
     <row r="56" spans="1:6" ht="15.75" customHeight="1">
-      <c r="A56" s="189"/>
-      <c r="B56" s="189"/>
-      <c r="C56" s="192" t="s">
-        <v>233</v>
-      </c>
-      <c r="D56" s="193"/>
-      <c r="E56" s="195">
+      <c r="A56" s="193"/>
+      <c r="B56" s="193"/>
+      <c r="C56" s="196" t="s">
+        <v>231</v>
+      </c>
+      <c r="D56" s="197"/>
+      <c r="E56" s="199">
         <f>'Presupuesto Inicial'!J20*12</f>
         <v>700000</v>
       </c>
-      <c r="F56" s="195"/>
+      <c r="F56" s="199"/>
     </row>
     <row r="57" spans="1:6" ht="15.75" customHeight="1">
-      <c r="A57" s="189"/>
-      <c r="B57" s="189"/>
-      <c r="C57" s="192" t="s">
+      <c r="A57" s="193"/>
+      <c r="B57" s="193"/>
+      <c r="C57" s="196" t="s">
+        <v>232</v>
+      </c>
+      <c r="D57" s="197"/>
+      <c r="E57" s="199">
+        <v>0</v>
+      </c>
+      <c r="F57" s="199"/>
+    </row>
+    <row r="58" spans="1:6" ht="15.75" customHeight="1" thickBot="1">
+      <c r="A58" s="193"/>
+      <c r="B58" s="193"/>
+      <c r="C58" s="196" t="s">
+        <v>233</v>
+      </c>
+      <c r="D58" s="197"/>
+      <c r="E58" s="199">
+        <v>0</v>
+      </c>
+      <c r="F58" s="199"/>
+    </row>
+    <row r="59" spans="1:6" ht="15.75" customHeight="1" thickTop="1" thickBot="1">
+      <c r="A59" s="193"/>
+      <c r="B59" s="193"/>
+      <c r="C59" s="188" t="s">
         <v>234</v>
       </c>
-      <c r="D57" s="193"/>
-      <c r="E57" s="195">
-        <v>0</v>
-      </c>
-      <c r="F57" s="195"/>
-    </row>
-    <row r="58" spans="1:6" ht="15.75" customHeight="1" thickBot="1">
-      <c r="A58" s="189"/>
-      <c r="B58" s="189"/>
-      <c r="C58" s="192" t="s">
-        <v>235</v>
-      </c>
-      <c r="D58" s="193"/>
-      <c r="E58" s="195">
-        <v>0</v>
-      </c>
-      <c r="F58" s="195"/>
-    </row>
-    <row r="59" spans="1:6" ht="15.75" customHeight="1" thickTop="1" thickBot="1">
-      <c r="A59" s="189"/>
-      <c r="B59" s="189"/>
-      <c r="C59" s="184" t="s">
-        <v>236</v>
-      </c>
-      <c r="D59" s="184"/>
-      <c r="E59" s="187">
+      <c r="D59" s="188"/>
+      <c r="E59" s="191">
         <f>SUM(E55:F58)</f>
         <v>700000</v>
       </c>
-      <c r="F59" s="184"/>
+      <c r="F59" s="188"/>
     </row>
     <row r="60" spans="1:6" ht="15.75" customHeight="1" thickTop="1">
-      <c r="A60" s="188" t="s">
-        <v>241</v>
-      </c>
-      <c r="B60" s="188"/>
-      <c r="C60" s="190" t="s">
-        <v>251</v>
-      </c>
-      <c r="D60" s="190"/>
-      <c r="E60" s="194">
+      <c r="A60" s="192" t="s">
+        <v>239</v>
+      </c>
+      <c r="B60" s="192"/>
+      <c r="C60" s="194" t="s">
+        <v>249</v>
+      </c>
+      <c r="D60" s="194"/>
+      <c r="E60" s="198">
         <f>('Presupuesto Inicial'!B12+'Presupuesto Inicial'!B13)+('Presupuesto Inicial'!B11*6)+('Salarios, gastos y costos'!K11*12)</f>
         <v>7848920</v>
       </c>
-      <c r="F60" s="194"/>
+      <c r="F60" s="198"/>
     </row>
     <row r="61" spans="1:6" ht="15.75" customHeight="1" thickBot="1">
-      <c r="A61" s="188"/>
-      <c r="B61" s="188"/>
-      <c r="C61" s="192" t="s">
-        <v>239</v>
-      </c>
-      <c r="D61" s="192"/>
-      <c r="E61" s="195">
+      <c r="A61" s="192"/>
+      <c r="B61" s="192"/>
+      <c r="C61" s="196" t="s">
+        <v>237</v>
+      </c>
+      <c r="D61" s="196"/>
+      <c r="E61" s="199">
         <f>'Presupuesto Inicial'!B2</f>
         <v>116700</v>
       </c>
-      <c r="F61" s="195"/>
+      <c r="F61" s="199"/>
     </row>
     <row r="62" spans="1:6" ht="15.75" customHeight="1" thickTop="1" thickBot="1">
-      <c r="A62" s="188"/>
-      <c r="B62" s="188"/>
-      <c r="C62" s="184" t="s">
-        <v>240</v>
-      </c>
-      <c r="D62" s="184"/>
-      <c r="E62" s="187">
+      <c r="A62" s="192"/>
+      <c r="B62" s="192"/>
+      <c r="C62" s="188" t="s">
+        <v>238</v>
+      </c>
+      <c r="D62" s="188"/>
+      <c r="E62" s="191">
         <f>E60+E61</f>
         <v>7965620</v>
       </c>
-      <c r="F62" s="187"/>
+      <c r="F62" s="191"/>
     </row>
     <row r="63" spans="1:6" ht="15.75" customHeight="1" thickTop="1" thickBot="1">
-      <c r="A63" s="184" t="s">
-        <v>245</v>
-      </c>
-      <c r="B63" s="184"/>
-      <c r="C63" s="184"/>
-      <c r="D63" s="184"/>
-      <c r="E63" s="196">
+      <c r="A63" s="188" t="s">
+        <v>243</v>
+      </c>
+      <c r="B63" s="188"/>
+      <c r="C63" s="188"/>
+      <c r="D63" s="188"/>
+      <c r="E63" s="200">
         <f>E54+E59+E62</f>
         <v>101620332</v>
       </c>
-      <c r="F63" s="196"/>
+      <c r="F63" s="200"/>
     </row>
     <row r="64" spans="1:6" ht="15.75" customHeight="1" thickTop="1"/>
     <row r="65" spans="7:8" ht="15.75" customHeight="1" thickBot="1"/>
     <row r="66" spans="7:8" ht="15.75" customHeight="1" thickTop="1" thickBot="1">
-      <c r="G66" s="180">
+      <c r="G66" s="179">
         <f>E54+E59+E62</f>
         <v>101620332</v>
       </c>
-      <c r="H66" s="179"/>
+      <c r="H66" s="178"/>
     </row>
     <row r="67" spans="7:8" ht="15.75" customHeight="1" thickTop="1"/>
   </sheetData>
@@ -10372,28 +11040,28 @@
   <sheetData>
     <row r="1" spans="1:4" ht="15.75" customHeight="1" thickBot="1"/>
     <row r="2" spans="1:4" ht="15.75" customHeight="1" thickTop="1" thickBot="1">
-      <c r="A2" s="184" t="s">
+      <c r="A2" s="188" t="s">
         <v>7</v>
       </c>
-      <c r="B2" s="197"/>
-      <c r="C2" s="197"/>
-      <c r="D2" s="197"/>
+      <c r="B2" s="201"/>
+      <c r="C2" s="201"/>
+      <c r="D2" s="201"/>
     </row>
     <row r="3" spans="1:4" ht="15.75" customHeight="1" thickTop="1">
-      <c r="A3" s="199" t="s">
+      <c r="A3" s="203" t="s">
         <v>14</v>
       </c>
-      <c r="B3" s="182"/>
-      <c r="C3" s="199" t="s">
+      <c r="B3" s="186"/>
+      <c r="C3" s="203" t="s">
         <v>15</v>
       </c>
-      <c r="D3" s="182"/>
+      <c r="D3" s="186"/>
     </row>
     <row r="4" spans="1:4" ht="15.75" customHeight="1">
-      <c r="A4" s="200" t="s">
+      <c r="A4" s="204" t="s">
         <v>16</v>
       </c>
-      <c r="B4" s="203">
+      <c r="B4" s="207">
         <v>1500000</v>
       </c>
       <c r="C4" s="19" t="s">
@@ -10404,16 +11072,16 @@
       </c>
     </row>
     <row r="5" spans="1:4" ht="15.75" customHeight="1">
-      <c r="A5" s="201"/>
-      <c r="B5" s="201"/>
-      <c r="C5" s="199" t="s">
+      <c r="A5" s="205"/>
+      <c r="B5" s="205"/>
+      <c r="C5" s="203" t="s">
         <v>39</v>
       </c>
-      <c r="D5" s="182"/>
+      <c r="D5" s="186"/>
     </row>
     <row r="6" spans="1:4" ht="15.75" customHeight="1">
-      <c r="A6" s="201"/>
-      <c r="B6" s="201"/>
+      <c r="A6" s="205"/>
+      <c r="B6" s="205"/>
       <c r="C6" s="19" t="s">
         <v>40</v>
       </c>
@@ -10422,8 +11090,8 @@
       </c>
     </row>
     <row r="7" spans="1:4" ht="15.75" customHeight="1">
-      <c r="A7" s="201"/>
-      <c r="B7" s="201"/>
+      <c r="A7" s="205"/>
+      <c r="B7" s="205"/>
       <c r="C7" s="19" t="s">
         <v>43</v>
       </c>
@@ -10432,10 +11100,10 @@
       </c>
     </row>
     <row r="8" spans="1:4" ht="15.75" customHeight="1">
-      <c r="A8" s="202"/>
-      <c r="B8" s="202"/>
+      <c r="A8" s="206"/>
+      <c r="B8" s="206"/>
       <c r="C8" s="19" t="s">
-        <v>242</v>
+        <v>240</v>
       </c>
       <c r="D8" s="22">
         <v>525000</v>
@@ -10458,15 +11126,15 @@
       </c>
     </row>
     <row r="10" spans="1:4" ht="15.75" customHeight="1" thickTop="1" thickBot="1">
-      <c r="A10" s="184" t="s">
+      <c r="A10" s="188" t="s">
         <v>57</v>
       </c>
-      <c r="B10" s="197"/>
-      <c r="C10" s="198">
+      <c r="B10" s="201"/>
+      <c r="C10" s="202">
         <f>D4+D9</f>
         <v>1500000</v>
       </c>
-      <c r="D10" s="197"/>
+      <c r="D10" s="201"/>
     </row>
     <row r="11" spans="1:4" ht="15.75" customHeight="1" thickTop="1"/>
     <row r="12" spans="1:4" ht="15.75" customHeight="1">
@@ -10502,49 +11170,49 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:6" ht="15">
-      <c r="B2" s="204" t="s">
+      <c r="B2" s="208" t="s">
+        <v>242</v>
+      </c>
+      <c r="C2" s="208"/>
+      <c r="D2" s="208"/>
+      <c r="E2" s="208"/>
+      <c r="F2" s="208"/>
+    </row>
+    <row r="3" spans="2:6">
+      <c r="B3" s="189" t="s">
         <v>244</v>
       </c>
-      <c r="C2" s="204"/>
-      <c r="D2" s="204"/>
-      <c r="E2" s="204"/>
-      <c r="F2" s="204"/>
-    </row>
-    <row r="3" spans="2:6">
-      <c r="B3" s="185" t="s">
-        <v>246</v>
-      </c>
-      <c r="C3" s="185"/>
-      <c r="D3" s="185"/>
-      <c r="E3" s="206">
+      <c r="C3" s="189"/>
+      <c r="D3" s="189"/>
+      <c r="E3" s="210">
         <f>'Salarios, gastos y costos'!E62:F62</f>
         <v>7965620</v>
       </c>
-      <c r="F3" s="206"/>
+      <c r="F3" s="210"/>
     </row>
     <row r="4" spans="2:6">
-      <c r="B4" s="207" t="s">
-        <v>247</v>
-      </c>
-      <c r="C4" s="185"/>
-      <c r="D4" s="185"/>
-      <c r="E4" s="208">
+      <c r="B4" s="211" t="s">
+        <v>245</v>
+      </c>
+      <c r="C4" s="189"/>
+      <c r="D4" s="189"/>
+      <c r="E4" s="212">
         <f>'Salarios, gastos y costos'!B11*7</f>
         <v>54223582</v>
       </c>
-      <c r="F4" s="208"/>
+      <c r="F4" s="212"/>
     </row>
     <row r="5" spans="2:6" ht="15">
-      <c r="B5" s="204" t="s">
+      <c r="B5" s="208" t="s">
         <v>214</v>
       </c>
-      <c r="C5" s="204"/>
-      <c r="D5" s="204"/>
-      <c r="E5" s="205">
+      <c r="C5" s="208"/>
+      <c r="D5" s="208"/>
+      <c r="E5" s="209">
         <f>SUM(E3:F4)</f>
         <v>62189202</v>
       </c>
-      <c r="F5" s="205"/>
+      <c r="F5" s="209"/>
     </row>
   </sheetData>
   <mergeCells count="7">
@@ -10568,9 +11236,9 @@
   </sheetPr>
   <dimension ref="A1:Y24"/>
   <sheetViews>
-    <sheetView topLeftCell="A13" zoomScale="175" zoomScaleNormal="175" workbookViewId="0">
-      <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="H16" sqref="H16"/>
+    <sheetView zoomScale="175" zoomScaleNormal="175" workbookViewId="0">
+      <pane xSplit="1" topLeftCell="C1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="S24" sqref="S24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1"/>
@@ -10615,30 +11283,30 @@
       <c r="G1" s="129" t="s">
         <v>66</v>
       </c>
-      <c r="H1" s="210" t="s">
+      <c r="H1" s="214" t="s">
         <v>67</v>
       </c>
-      <c r="I1" s="182"/>
-      <c r="J1" s="209" t="s">
+      <c r="I1" s="186"/>
+      <c r="J1" s="213" t="s">
         <v>68</v>
       </c>
-      <c r="K1" s="182"/>
-      <c r="L1" s="209" t="s">
+      <c r="K1" s="186"/>
+      <c r="L1" s="213" t="s">
         <v>69</v>
       </c>
-      <c r="M1" s="182"/>
-      <c r="N1" s="209" t="s">
+      <c r="M1" s="186"/>
+      <c r="N1" s="213" t="s">
         <v>70</v>
       </c>
-      <c r="O1" s="182"/>
-      <c r="P1" s="209" t="s">
+      <c r="O1" s="186"/>
+      <c r="P1" s="213" t="s">
         <v>71</v>
       </c>
-      <c r="Q1" s="182"/>
-      <c r="R1" s="209" t="s">
+      <c r="Q1" s="186"/>
+      <c r="R1" s="213" t="s">
         <v>72</v>
       </c>
-      <c r="S1" s="182"/>
+      <c r="S1" s="186"/>
       <c r="U1" s="146" t="s">
         <v>74</v>
       </c>
@@ -10714,7 +11382,7 @@
         <v>53107075.955209814</v>
       </c>
       <c r="U2" s="44">
-        <f t="shared" ref="U2:U16" si="1">SUM(B2:S2)</f>
+        <f t="shared" ref="U2:U15" si="1">SUM(B2:S2)</f>
         <v>196295698.24768659</v>
       </c>
     </row>
@@ -11033,7 +11701,7 @@
         <v>215</v>
       </c>
       <c r="X6" s="97" t="s">
-        <v>219</v>
+        <v>217</v>
       </c>
       <c r="Y6" s="103">
         <f>U6+U7+U9+U10</f>
@@ -11286,7 +11954,7 @@
         <v>3984120.070433259</v>
       </c>
       <c r="V9" s="97" t="s">
-        <v>217</v>
+        <v>11</v>
       </c>
     </row>
     <row r="10" spans="1:25" ht="12.75">
@@ -11369,7 +12037,7 @@
         <v>4285000.1198602207</v>
       </c>
       <c r="V10" s="97" t="s">
-        <v>218</v>
+        <v>252</v>
       </c>
     </row>
     <row r="11" spans="1:25" s="130" customFormat="1" ht="12.75">
@@ -11983,7 +12651,7 @@
   <dimension ref="A1:R25"/>
   <sheetViews>
     <sheetView zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <selection sqref="A1:K16"/>
+      <selection activeCell="C25" sqref="C25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1"/>
@@ -12000,26 +12668,26 @@
   <sheetData>
     <row r="1" spans="1:18" ht="12.75">
       <c r="A1" s="26"/>
-      <c r="B1" s="209" t="s">
+      <c r="B1" s="213" t="s">
         <v>74</v>
       </c>
-      <c r="C1" s="182"/>
-      <c r="D1" s="209" t="s">
+      <c r="C1" s="186"/>
+      <c r="D1" s="213" t="s">
         <v>75</v>
       </c>
-      <c r="E1" s="182"/>
-      <c r="F1" s="209" t="s">
+      <c r="E1" s="186"/>
+      <c r="F1" s="213" t="s">
         <v>76</v>
       </c>
-      <c r="G1" s="182"/>
-      <c r="H1" s="209" t="s">
+      <c r="G1" s="186"/>
+      <c r="H1" s="213" t="s">
         <v>78</v>
       </c>
-      <c r="I1" s="182"/>
-      <c r="J1" s="211" t="s">
+      <c r="I1" s="186"/>
+      <c r="J1" s="215" t="s">
         <v>79</v>
       </c>
-      <c r="K1" s="212"/>
+      <c r="K1" s="216"/>
       <c r="L1" s="28"/>
       <c r="M1" s="28"/>
       <c r="N1" s="28"/>
@@ -12795,7 +13463,7 @@
     <row r="18" spans="2:18" ht="12.75">
       <c r="B18" s="11"/>
       <c r="C18" s="99" t="s">
-        <v>253</v>
+        <v>251</v>
       </c>
       <c r="E18" s="62">
         <f>'Tabla Crecimiento'!B10</f>
@@ -12862,7 +13530,7 @@
     </row>
     <row r="21" spans="2:18" ht="12.75">
       <c r="C21" s="97" t="s">
-        <v>252</v>
+        <v>250</v>
       </c>
       <c r="D21">
         <v>5.75</v>
@@ -12952,58 +13620,58 @@
   <sheetData>
     <row r="1" spans="1:29" s="155" customFormat="1" ht="15.75" customHeight="1">
       <c r="A1" s="158"/>
-      <c r="B1" s="213" t="s">
+      <c r="B1" s="217" t="s">
         <v>108</v>
       </c>
-      <c r="C1" s="214"/>
-      <c r="D1" s="213" t="s">
+      <c r="C1" s="218"/>
+      <c r="D1" s="217" t="s">
         <v>59</v>
       </c>
-      <c r="E1" s="214"/>
-      <c r="F1" s="213" t="s">
+      <c r="E1" s="218"/>
+      <c r="F1" s="217" t="s">
         <v>62</v>
       </c>
-      <c r="G1" s="214"/>
-      <c r="H1" s="213" t="s">
+      <c r="G1" s="218"/>
+      <c r="H1" s="217" t="s">
         <v>63</v>
       </c>
-      <c r="I1" s="214"/>
-      <c r="J1" s="213" t="s">
+      <c r="I1" s="218"/>
+      <c r="J1" s="217" t="s">
         <v>64</v>
       </c>
-      <c r="K1" s="214"/>
-      <c r="L1" s="213" t="s">
+      <c r="K1" s="218"/>
+      <c r="L1" s="217" t="s">
         <v>65</v>
       </c>
-      <c r="M1" s="214"/>
-      <c r="N1" s="213" t="s">
+      <c r="M1" s="218"/>
+      <c r="N1" s="217" t="s">
         <v>66</v>
       </c>
-      <c r="O1" s="214"/>
-      <c r="P1" s="213" t="s">
+      <c r="O1" s="218"/>
+      <c r="P1" s="217" t="s">
         <v>67</v>
       </c>
-      <c r="Q1" s="214"/>
-      <c r="R1" s="213" t="s">
+      <c r="Q1" s="218"/>
+      <c r="R1" s="217" t="s">
         <v>68</v>
       </c>
-      <c r="S1" s="214"/>
-      <c r="T1" s="213" t="s">
+      <c r="S1" s="218"/>
+      <c r="T1" s="217" t="s">
         <v>69</v>
       </c>
-      <c r="U1" s="214"/>
-      <c r="V1" s="213" t="s">
+      <c r="U1" s="218"/>
+      <c r="V1" s="217" t="s">
         <v>70</v>
       </c>
-      <c r="W1" s="214"/>
-      <c r="X1" s="213" t="s">
+      <c r="W1" s="218"/>
+      <c r="X1" s="217" t="s">
         <v>71</v>
       </c>
-      <c r="Y1" s="214"/>
-      <c r="Z1" s="213" t="s">
+      <c r="Y1" s="218"/>
+      <c r="Z1" s="217" t="s">
         <v>72</v>
       </c>
-      <c r="AA1" s="214"/>
+      <c r="AA1" s="218"/>
     </row>
     <row r="2" spans="1:29" ht="15.75" customHeight="1">
       <c r="A2" s="31" t="s">
@@ -13457,7 +14125,7 @@
     </row>
     <row r="6" spans="1:29" ht="15.75" customHeight="1">
       <c r="A6" s="40" t="s">
-        <v>255</v>
+        <v>253</v>
       </c>
       <c r="B6" s="64">
         <f t="shared" si="0"/>
@@ -13570,7 +14238,7 @@
     </row>
     <row r="7" spans="1:29" ht="15.75" customHeight="1">
       <c r="A7" s="40" t="s">
-        <v>254</v>
+        <v>252</v>
       </c>
       <c r="B7" s="64">
         <f>C7/$C$2</f>
@@ -14257,7 +14925,7 @@
     </row>
     <row r="16" spans="1:29" ht="15.75" customHeight="1">
       <c r="C16" s="97" t="s">
-        <v>256</v>
+        <v>254</v>
       </c>
     </row>
   </sheetData>
@@ -14303,30 +14971,30 @@
   <sheetData>
     <row r="1" spans="1:20" ht="15.75" customHeight="1">
       <c r="A1" s="27"/>
-      <c r="B1" s="215" t="s">
+      <c r="B1" s="219" t="s">
         <v>77</v>
       </c>
-      <c r="C1" s="182"/>
-      <c r="D1" s="215" t="s">
+      <c r="C1" s="186"/>
+      <c r="D1" s="219" t="s">
         <v>74</v>
       </c>
-      <c r="E1" s="182"/>
-      <c r="F1" s="215" t="s">
+      <c r="E1" s="186"/>
+      <c r="F1" s="219" t="s">
         <v>75</v>
       </c>
-      <c r="G1" s="182"/>
-      <c r="H1" s="215" t="s">
+      <c r="G1" s="186"/>
+      <c r="H1" s="219" t="s">
         <v>76</v>
       </c>
-      <c r="I1" s="182"/>
-      <c r="J1" s="215" t="s">
+      <c r="I1" s="186"/>
+      <c r="J1" s="219" t="s">
         <v>78</v>
       </c>
-      <c r="K1" s="182"/>
-      <c r="L1" s="215" t="s">
+      <c r="K1" s="186"/>
+      <c r="L1" s="219" t="s">
         <v>79</v>
       </c>
-      <c r="M1" s="182"/>
+      <c r="M1" s="186"/>
       <c r="N1" s="29"/>
       <c r="O1" s="29"/>
       <c r="P1" s="29"/>
@@ -14635,7 +15303,7 @@
     </row>
     <row r="7" spans="1:20" ht="15.75" customHeight="1">
       <c r="A7" s="40" t="s">
-        <v>254</v>
+        <v>252</v>
       </c>
       <c r="B7" s="64">
         <f>C7/$C$2</f>

</xml_diff>

<commit_message>
se mejora la estructura del documento y en el exce se modifican tablas
</commit_message>
<xml_diff>
--- a/Analisis_financiero_Inclusoft_test.xlsx
+++ b/Analisis_financiero_Inclusoft_test.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="21570" windowHeight="8145" tabRatio="920" firstSheet="4" activeTab="12"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="21570" windowHeight="8145" tabRatio="920" firstSheet="4" activeTab="9"/>
   </bookViews>
   <sheets>
     <sheet name="Presupuesto Inicial" sheetId="1" r:id="rId1"/>
@@ -2054,6 +2054,60 @@
     <xf numFmtId="170" fontId="1" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
+    <xf numFmtId="2" fontId="7" fillId="0" borderId="1" xfId="5" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="2" fontId="1" fillId="0" borderId="1" xfId="5" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="43" fontId="1" fillId="0" borderId="5" xfId="5" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="43" fontId="12" fillId="0" borderId="13" xfId="5" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="10" fontId="0" fillId="0" borderId="28" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="19" fillId="4" borderId="12" xfId="3" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="170" fontId="19" fillId="4" borderId="12" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="14" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="167" fontId="19" fillId="4" borderId="12" xfId="3" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="3" borderId="11" xfId="2" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -2062,48 +2116,6 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="4" borderId="12" xfId="3" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="3" borderId="11" xfId="2" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="167" fontId="19" fillId="4" borderId="12" xfId="3" applyNumberFormat="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="167" fontId="0" fillId="0" borderId="14" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="170" fontId="19" fillId="4" borderId="12" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="19" fillId="4" borderId="12" xfId="3"/>
     <xf numFmtId="164" fontId="19" fillId="4" borderId="12" xfId="3" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -2149,17 +2161,26 @@
     <xf numFmtId="0" fontId="11" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="164" fontId="8" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="20" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="27" xfId="6" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="28" xfId="6" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="18" fillId="3" borderId="22" xfId="2" applyBorder="1" applyAlignment="1">
@@ -2169,6 +2190,12 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="18" fillId="3" borderId="23" xfId="2" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="19" fillId="4" borderId="19" xfId="3" applyBorder="1" applyAlignment="1">
@@ -2183,45 +2210,18 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="26" fillId="0" borderId="27" xfId="6" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="26" fillId="0" borderId="28" xfId="6" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
+    <xf numFmtId="0" fontId="18" fillId="3" borderId="17" xfId="2" applyBorder="1"/>
     <xf numFmtId="0" fontId="27" fillId="3" borderId="13" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="27" fillId="3" borderId="13" xfId="2" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="27" fillId="3" borderId="30" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="27" fillId="3" borderId="30" xfId="2" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="18" fillId="3" borderId="13" xfId="2" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="27" fillId="3" borderId="13" xfId="2" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="18" fillId="3" borderId="17" xfId="2" applyBorder="1"/>
-    <xf numFmtId="2" fontId="7" fillId="0" borderId="1" xfId="5" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="2" fontId="1" fillId="0" borderId="1" xfId="5" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="43" fontId="1" fillId="0" borderId="5" xfId="5" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="43" fontId="12" fillId="0" borderId="13" xfId="5" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="10" fontId="0" fillId="0" borderId="28" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="27" fillId="3" borderId="30" xfId="2" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="7">
     <cellStyle name="Celda de comprobación" xfId="3" builtinId="23"/>
@@ -2232,7 +2232,7 @@
     <cellStyle name="Salida" xfId="2" builtinId="21"/>
     <cellStyle name="Texto de advertencia" xfId="6" builtinId="11"/>
   </cellStyles>
-  <dxfs count="49">
+  <dxfs count="48">
     <dxf>
       <font>
         <color rgb="FFC53929"/>
@@ -2316,164 +2316,6 @@
         <top/>
         <bottom/>
       </border>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FFC53929"/>
-      </font>
-      <fill>
-        <patternFill patternType="none"/>
-      </fill>
-      <border>
-        <left/>
-        <right/>
-        <top/>
-        <bottom/>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FFC53929"/>
-      </font>
-      <fill>
-        <patternFill patternType="none"/>
-      </fill>
-      <border>
-        <left/>
-        <right/>
-        <top/>
-        <bottom/>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FFC53929"/>
-      </font>
-      <fill>
-        <patternFill patternType="none"/>
-      </fill>
-      <border>
-        <left/>
-        <right/>
-        <top/>
-        <bottom/>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FFC53929"/>
-      </font>
-      <fill>
-        <patternFill patternType="none"/>
-      </fill>
-      <border>
-        <left/>
-        <right/>
-        <top/>
-        <bottom/>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <fgColor theme="1"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FFC53929"/>
-      </font>
-      <fill>
-        <patternFill patternType="none"/>
-      </fill>
-      <border>
-        <left/>
-        <right/>
-        <top/>
-        <bottom/>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="10"/>
-        <color rgb="FF000000"/>
-        <name val="Arial"/>
-        <scheme val="none"/>
-      </font>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="10"/>
-        <color rgb="FF000000"/>
-        <name val="Arial"/>
-        <scheme val="none"/>
-      </font>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <font>
@@ -2656,6 +2498,150 @@
         <scheme val="none"/>
       </font>
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <name val="Arial"/>
+        <scheme val="none"/>
+      </font>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <name val="Arial"/>
+        <scheme val="none"/>
+      </font>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FFC53929"/>
+      </font>
+      <fill>
+        <patternFill patternType="none"/>
+      </fill>
+      <border>
+        <left/>
+        <right/>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FFC53929"/>
+      </font>
+      <fill>
+        <patternFill patternType="none"/>
+      </fill>
+      <border>
+        <left/>
+        <right/>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FFC53929"/>
+      </font>
+      <fill>
+        <patternFill patternType="none"/>
+      </fill>
+      <border>
+        <left/>
+        <right/>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <fgColor theme="1"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FFC53929"/>
+      </font>
+      <fill>
+        <patternFill patternType="none"/>
+      </fill>
+      <border>
+        <left/>
+        <right/>
+        <top/>
+        <bottom/>
+      </border>
     </dxf>
     <dxf>
       <font>
@@ -3111,7 +3097,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -3263,11 +3248,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="318094920"/>
-        <c:axId val="318091392"/>
+        <c:axId val="303801208"/>
+        <c:axId val="303800424"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="318094920"/>
+        <c:axId val="303801208"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3299,7 +3284,6 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -3366,7 +3350,7 @@
             <a:endParaRPr lang="es-ES"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="318091392"/>
+        <c:crossAx val="303800424"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -3374,7 +3358,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="318091392"/>
+        <c:axId val="303800424"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3420,7 +3404,6 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -3481,7 +3464,7 @@
             <a:endParaRPr lang="es-ES"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="318094920"/>
+        <c:crossAx val="303801208"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -3495,7 +3478,6 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -3607,7 +3589,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -3759,11 +3740,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="318094136"/>
-        <c:axId val="318094528"/>
+        <c:axId val="303801600"/>
+        <c:axId val="303801992"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="318094136"/>
+        <c:axId val="303801600"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3795,7 +3776,6 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -3862,7 +3842,7 @@
             <a:endParaRPr lang="es-ES"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="318094528"/>
+        <c:crossAx val="303801992"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -3870,7 +3850,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="318094528"/>
+        <c:axId val="303801992"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3916,7 +3896,6 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -3977,7 +3956,7 @@
             <a:endParaRPr lang="es-ES"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="318094136"/>
+        <c:crossAx val="303801600"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -3991,7 +3970,6 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -4256,8 +4234,8 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="318092960"/>
-        <c:axId val="318093352"/>
+        <c:axId val="303803560"/>
+        <c:axId val="303800032"/>
         <c:extLst>
           <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
             <c15:filteredBarSeries>
@@ -4345,7 +4323,7 @@
         </c:extLst>
       </c:barChart>
       <c:catAx>
-        <c:axId val="318092960"/>
+        <c:axId val="303803560"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4444,7 +4422,7 @@
             <a:endParaRPr lang="es-ES"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="318093352"/>
+        <c:crossAx val="303800032"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -4452,7 +4430,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="318093352"/>
+        <c:axId val="303800032"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4566,7 +4544,7 @@
             <a:endParaRPr lang="es-ES"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="318092960"/>
+        <c:crossAx val="303803560"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -5015,11 +4993,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="319183056"/>
-        <c:axId val="319185408"/>
+        <c:axId val="306162792"/>
+        <c:axId val="306166712"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="319183056"/>
+        <c:axId val="306162792"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -5134,7 +5112,7 @@
             <a:endParaRPr lang="es-ES"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="319185408"/>
+        <c:crossAx val="306166712"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -5142,7 +5120,7 @@
         <c:noMultiLvlLbl val="1"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="319185408"/>
+        <c:axId val="306166712"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -5243,7 +5221,7 @@
             <a:endParaRPr lang="es-ES"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="319183056"/>
+        <c:crossAx val="306162792"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -7856,29 +7834,29 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="PUBLICIDAD" displayName="PUBLICIDAD" ref="A36:H43" totalsRowCount="1" headerRowDxfId="48" totalsRowDxfId="47" headerRowCellStyle="Celda de comprobación">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="PUBLICIDAD" displayName="PUBLICIDAD" ref="A36:H43" totalsRowCount="1" headerRowDxfId="47" totalsRowDxfId="46" headerRowCellStyle="Celda de comprobación">
   <tableColumns count="8">
-    <tableColumn id="1" name="Promoción" dataDxfId="46"/>
-    <tableColumn id="2" name="Tiempo aproximado de duración" dataDxfId="45" totalsRowDxfId="44"/>
-    <tableColumn id="3" name="Objetivo " dataDxfId="43" totalsRowDxfId="42"/>
-    <tableColumn id="4" name="Cantidad" dataDxfId="41" totalsRowDxfId="40"/>
-    <tableColumn id="5" name="Se requieren" dataDxfId="39" totalsRowDxfId="38"/>
-    <tableColumn id="6" name="Costo Unitario" totalsRowLabel="Total anual" dataDxfId="37" totalsRowDxfId="36" dataCellStyle="Moneda"/>
-    <tableColumn id="7" name="Costo total" totalsRowFunction="sum" dataDxfId="35" totalsRowDxfId="34" dataCellStyle="Moneda">
+    <tableColumn id="1" name="Promoción" dataDxfId="45"/>
+    <tableColumn id="2" name="Tiempo aproximado de duración" dataDxfId="44" totalsRowDxfId="43"/>
+    <tableColumn id="3" name="Objetivo " dataDxfId="42" totalsRowDxfId="41"/>
+    <tableColumn id="4" name="Cantidad" dataDxfId="40" totalsRowDxfId="39"/>
+    <tableColumn id="5" name="Se requieren" dataDxfId="38" totalsRowDxfId="37"/>
+    <tableColumn id="6" name="Costo Unitario" totalsRowLabel="Total anual" dataDxfId="36" totalsRowDxfId="35" dataCellStyle="Moneda"/>
+    <tableColumn id="7" name="Costo total" totalsRowFunction="sum" dataDxfId="34" totalsRowDxfId="33" dataCellStyle="Moneda">
       <calculatedColumnFormula>F37*E37</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="8" name="Proveedor" dataDxfId="33" totalsRowDxfId="32"/>
+    <tableColumn id="8" name="Proveedor" dataDxfId="32" totalsRowDxfId="31"/>
   </tableColumns>
   <tableStyleInfo showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="Tabla3" displayName="Tabla3" ref="A21:G23" totalsRowShown="0" headerRowDxfId="20">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="Tabla3" displayName="Tabla3" ref="A21:G23" totalsRowShown="0" headerRowDxfId="18">
   <autoFilter ref="A21:G23"/>
   <tableColumns count="7">
     <tableColumn id="1" name="Columna1"/>
-    <tableColumn id="2" name="Columna2" dataDxfId="19"/>
+    <tableColumn id="2" name="Columna2" dataDxfId="17"/>
     <tableColumn id="3" name="Columna3">
       <calculatedColumnFormula>'Flujo de Caja (Profesor) - 5 añ'!D18</calculatedColumnFormula>
     </tableColumn>
@@ -7903,7 +7881,7 @@
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="5" name="Tabla5" displayName="Tabla5" ref="A31:B34" totalsRowShown="0">
   <autoFilter ref="A31:B34"/>
   <tableColumns count="2">
-    <tableColumn id="1" name="Columna1" dataDxfId="31"/>
+    <tableColumn id="1" name="Columna1" dataDxfId="16"/>
     <tableColumn id="2" name="Columna2">
       <calculatedColumnFormula>B31*2</calculatedColumnFormula>
     </tableColumn>
@@ -7916,8 +7894,8 @@
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="6" name="Tabla6" displayName="Tabla6" ref="A36:B41" totalsRowShown="0">
   <autoFilter ref="A36:B41"/>
   <tableColumns count="2">
-    <tableColumn id="1" name="Columna1" dataDxfId="30"/>
-    <tableColumn id="2" name="Columna2" dataDxfId="29"/>
+    <tableColumn id="1" name="Columna1" dataDxfId="15"/>
+    <tableColumn id="2" name="Columna2" dataDxfId="14"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium16" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -7927,9 +7905,9 @@
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="4" name="Tabla4" displayName="Tabla4" ref="A25:C28" totalsRowShown="0">
   <autoFilter ref="A25:C28"/>
   <tableColumns count="3">
-    <tableColumn id="1" name="Columna1" dataDxfId="28"/>
-    <tableColumn id="2" name="Columna2" dataDxfId="27"/>
-    <tableColumn id="3" name="Columna3" dataDxfId="26"/>
+    <tableColumn id="1" name="Columna1" dataDxfId="13"/>
+    <tableColumn id="2" name="Columna2" dataDxfId="12"/>
+    <tableColumn id="3" name="Columna3" dataDxfId="11"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium16" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -7939,9 +7917,9 @@
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Tabla2" displayName="Tabla2" ref="A45:C51" totalsRowShown="0">
   <autoFilter ref="A45:C51"/>
   <tableColumns count="3">
-    <tableColumn id="1" name="Columna1" dataDxfId="25"/>
-    <tableColumn id="2" name="Columna2" dataDxfId="24" dataCellStyle="Porcentaje"/>
-    <tableColumn id="3" name="Columna3" dataDxfId="23" dataCellStyle="Porcentaje">
+    <tableColumn id="1" name="Columna1" dataDxfId="10"/>
+    <tableColumn id="2" name="Columna2" dataDxfId="9" dataCellStyle="Porcentaje"/>
+    <tableColumn id="3" name="Columna3" dataDxfId="8" dataCellStyle="Porcentaje">
       <calculatedColumnFormula xml:space="preserve"> 1 +B46</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -7953,7 +7931,7 @@
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="7" name="Tabla7" displayName="Tabla7" ref="G9:J11" totalsRowShown="0">
   <autoFilter ref="G9:J11"/>
   <tableColumns count="4">
-    <tableColumn id="1" name="CONCEPTO" dataDxfId="22"/>
+    <tableColumn id="1" name="CONCEPTO" dataDxfId="7"/>
     <tableColumn id="2" name="Columna2"/>
     <tableColumn id="3" name="-"/>
     <tableColumn id="4" name="VALOR"/>
@@ -8601,18 +8579,18 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:S31"/>
   <sheetViews>
-    <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection sqref="A1:L19"/>
+    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="B21" sqref="B21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1"/>
   <cols>
     <col min="1" max="1" width="25.7109375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="12.28515625" hidden="1" customWidth="1"/>
-    <col min="3" max="3" width="9.5703125" hidden="1" customWidth="1"/>
-    <col min="4" max="4" width="14.7109375" hidden="1" customWidth="1"/>
-    <col min="5" max="5" width="7.42578125" hidden="1" customWidth="1"/>
-    <col min="6" max="6" width="14.42578125" hidden="1" customWidth="1"/>
+    <col min="2" max="2" width="12.28515625" customWidth="1"/>
+    <col min="3" max="3" width="9.5703125" customWidth="1"/>
+    <col min="4" max="4" width="14.7109375" customWidth="1"/>
+    <col min="5" max="5" width="7.42578125" customWidth="1"/>
+    <col min="6" max="6" width="14.42578125" customWidth="1"/>
     <col min="7" max="7" width="7" customWidth="1"/>
     <col min="8" max="8" width="15.28515625" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="7.28515625" customWidth="1"/>
@@ -8626,26 +8604,26 @@
       <c r="B1" s="200" t="s">
         <v>73</v>
       </c>
-      <c r="C1" s="281" t="s">
+      <c r="C1" s="287" t="s">
         <v>70</v>
       </c>
-      <c r="D1" s="251"/>
-      <c r="E1" s="280" t="s">
+      <c r="D1" s="271"/>
+      <c r="E1" s="286" t="s">
         <v>71</v>
       </c>
-      <c r="F1" s="251"/>
-      <c r="G1" s="280" t="s">
+      <c r="F1" s="271"/>
+      <c r="G1" s="286" t="s">
         <v>72</v>
       </c>
-      <c r="H1" s="251"/>
-      <c r="I1" s="280" t="s">
+      <c r="H1" s="271"/>
+      <c r="I1" s="286" t="s">
         <v>74</v>
       </c>
-      <c r="J1" s="251"/>
-      <c r="K1" s="282" t="s">
+      <c r="J1" s="271"/>
+      <c r="K1" s="288" t="s">
         <v>75</v>
       </c>
-      <c r="L1" s="287"/>
+      <c r="L1" s="295"/>
       <c r="M1" s="27"/>
       <c r="N1" s="27"/>
       <c r="O1" s="27"/>
@@ -8854,10 +8832,10 @@
         <f>D5+F5+H5+J5+L5</f>
         <v>3842803.2126632677</v>
       </c>
-      <c r="O5" s="288" t="s">
+      <c r="O5" s="293" t="s">
         <v>280</v>
       </c>
-      <c r="P5" s="288"/>
+      <c r="P5" s="293"/>
       <c r="Q5" s="52"/>
       <c r="R5" s="52"/>
       <c r="S5" s="52"/>
@@ -8909,10 +8887,10 @@
       </c>
       <c r="M6" s="52"/>
       <c r="N6" s="52"/>
-      <c r="O6" s="288" t="s">
+      <c r="O6" s="293" t="s">
         <v>285</v>
       </c>
-      <c r="P6" s="288"/>
+      <c r="P6" s="293"/>
       <c r="Q6" s="52"/>
       <c r="R6" s="52"/>
       <c r="S6" s="52"/>
@@ -8964,10 +8942,10 @@
       </c>
       <c r="M7" s="52"/>
       <c r="N7" s="52"/>
-      <c r="O7" s="288" t="s">
+      <c r="O7" s="293" t="s">
         <v>286</v>
       </c>
-      <c r="P7" s="288"/>
+      <c r="P7" s="293"/>
       <c r="Q7" s="52"/>
       <c r="R7" s="52"/>
       <c r="S7" s="52"/>
@@ -9019,8 +8997,8 @@
       </c>
       <c r="M8" s="55"/>
       <c r="N8" s="44"/>
-      <c r="O8" s="289"/>
-      <c r="P8" s="289"/>
+      <c r="O8" s="294"/>
+      <c r="P8" s="294"/>
       <c r="Q8" s="44"/>
       <c r="R8" s="44"/>
       <c r="S8" s="44"/>
@@ -9072,10 +9050,10 @@
       </c>
       <c r="M9" s="52"/>
       <c r="N9" s="52"/>
-      <c r="O9" s="288" t="s">
+      <c r="O9" s="293" t="s">
         <v>11</v>
       </c>
-      <c r="P9" s="288"/>
+      <c r="P9" s="293"/>
       <c r="Q9" s="52"/>
       <c r="R9" s="52"/>
       <c r="S9" s="52"/>
@@ -9127,10 +9105,10 @@
       </c>
       <c r="M10" s="52"/>
       <c r="N10" s="52"/>
-      <c r="O10" s="288" t="s">
+      <c r="O10" s="293" t="s">
         <v>248</v>
       </c>
-      <c r="P10" s="288"/>
+      <c r="P10" s="293"/>
       <c r="Q10" s="52"/>
       <c r="R10" s="52"/>
       <c r="S10" s="52"/>
@@ -9700,25 +9678,25 @@
     </row>
   </sheetData>
   <mergeCells count="11">
+    <mergeCell ref="E1:F1"/>
+    <mergeCell ref="C1:D1"/>
+    <mergeCell ref="G1:H1"/>
+    <mergeCell ref="I1:J1"/>
+    <mergeCell ref="K1:L1"/>
     <mergeCell ref="O5:P5"/>
     <mergeCell ref="O6:P6"/>
     <mergeCell ref="O9:P9"/>
     <mergeCell ref="O10:P10"/>
     <mergeCell ref="O7:P7"/>
     <mergeCell ref="O8:P8"/>
-    <mergeCell ref="E1:F1"/>
-    <mergeCell ref="C1:D1"/>
-    <mergeCell ref="G1:H1"/>
-    <mergeCell ref="I1:J1"/>
-    <mergeCell ref="K1:L1"/>
   </mergeCells>
   <conditionalFormatting sqref="A1:B16 C1:C19 D1:D16 E1:E19 F1:F16 G1:G19 H1:H16 I6:I19 J6:J16 K6:K19 L6:L16 I1:L5">
-    <cfRule type="cellIs" dxfId="8" priority="1" operator="lessThan">
+    <cfRule type="cellIs" dxfId="20" priority="1" operator="lessThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B17:L19">
-    <cfRule type="cellIs" dxfId="7" priority="2" operator="lessThan">
+    <cfRule type="cellIs" dxfId="19" priority="2" operator="lessThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
@@ -9731,7 +9709,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M66"/>
   <sheetViews>
-    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+    <sheetView topLeftCell="A16" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <selection activeCell="J10" sqref="J10"/>
     </sheetView>
   </sheetViews>
@@ -10791,30 +10769,30 @@
   <sheetData>
     <row r="1" spans="2:8" ht="13.5" thickBot="1"/>
     <row r="2" spans="2:8" ht="15.75" thickBot="1">
-      <c r="B2" s="295" t="s">
+      <c r="B2" s="306" t="s">
         <v>281</v>
       </c>
-      <c r="C2" s="296"/>
-      <c r="D2" s="296"/>
-      <c r="E2" s="296"/>
-      <c r="F2" s="296"/>
-      <c r="G2" s="296"/>
-      <c r="H2" s="297"/>
+      <c r="C2" s="307"/>
+      <c r="D2" s="307"/>
+      <c r="E2" s="307"/>
+      <c r="F2" s="307"/>
+      <c r="G2" s="307"/>
+      <c r="H2" s="308"/>
     </row>
     <row r="3" spans="2:8" ht="15.75" thickTop="1">
-      <c r="B3" s="292" t="s">
+      <c r="B3" s="301" t="s">
         <v>287</v>
       </c>
-      <c r="C3" s="293"/>
-      <c r="D3" s="293"/>
-      <c r="E3" s="293"/>
-      <c r="F3" s="293"/>
-      <c r="G3" s="293"/>
-      <c r="H3" s="294"/>
+      <c r="C3" s="302"/>
+      <c r="D3" s="302"/>
+      <c r="E3" s="302"/>
+      <c r="F3" s="302"/>
+      <c r="G3" s="302"/>
+      <c r="H3" s="303"/>
     </row>
     <row r="4" spans="2:8">
-      <c r="B4" s="298"/>
-      <c r="C4" s="291"/>
+      <c r="B4" s="309"/>
+      <c r="C4" s="297"/>
       <c r="D4" s="179" t="s">
         <v>70</v>
       </c>
@@ -10832,10 +10810,10 @@
       </c>
     </row>
     <row r="5" spans="2:8">
-      <c r="B5" s="290" t="s">
+      <c r="B5" s="296" t="s">
         <v>118</v>
       </c>
-      <c r="C5" s="291"/>
+      <c r="C5" s="297"/>
       <c r="D5" s="182">
         <f>'Flujo de Caja (Profesor) - 5 añ'!D6+'Flujo de Caja (Profesor) - 5 añ'!D7</f>
         <v>111254717.93098715</v>
@@ -10858,10 +10836,10 @@
       </c>
     </row>
     <row r="6" spans="2:8">
-      <c r="B6" s="290" t="s">
+      <c r="B6" s="296" t="s">
         <v>282</v>
       </c>
-      <c r="C6" s="291"/>
+      <c r="C6" s="297"/>
       <c r="D6" s="182">
         <f>'Flujo de Caja (Profesor) - 5 añ'!D3</f>
         <v>199937934.20591292</v>
@@ -10884,10 +10862,10 @@
       </c>
     </row>
     <row r="7" spans="2:8">
-      <c r="B7" s="290" t="s">
+      <c r="B7" s="296" t="s">
         <v>283</v>
       </c>
-      <c r="C7" s="291"/>
+      <c r="C7" s="297"/>
       <c r="D7" s="182">
         <f>'Flujo de Caja (Profesor) - 5 añ'!D10</f>
         <v>4285000.1176767461</v>
@@ -10910,10 +10888,10 @@
       </c>
     </row>
     <row r="8" spans="2:8">
-      <c r="B8" s="290" t="s">
+      <c r="B8" s="296" t="s">
         <v>291</v>
       </c>
-      <c r="C8" s="301"/>
+      <c r="C8" s="300"/>
       <c r="D8" s="182">
         <f>D5+D7</f>
         <v>115539718.0486639</v>
@@ -10936,10 +10914,10 @@
       </c>
     </row>
     <row r="9" spans="2:8">
-      <c r="B9" s="290" t="s">
+      <c r="B9" s="296" t="s">
         <v>284</v>
       </c>
-      <c r="C9" s="291"/>
+      <c r="C9" s="297"/>
       <c r="D9" s="184">
         <f>D5/(D6-D7)</f>
         <v>0.56863301564807167</v>
@@ -10962,19 +10940,19 @@
       </c>
     </row>
     <row r="10" spans="2:8" ht="15">
-      <c r="B10" s="292" t="s">
+      <c r="B10" s="301" t="s">
         <v>288</v>
       </c>
-      <c r="C10" s="293"/>
-      <c r="D10" s="293"/>
-      <c r="E10" s="293"/>
-      <c r="F10" s="293"/>
-      <c r="G10" s="293"/>
-      <c r="H10" s="294"/>
+      <c r="C10" s="302"/>
+      <c r="D10" s="302"/>
+      <c r="E10" s="302"/>
+      <c r="F10" s="302"/>
+      <c r="G10" s="302"/>
+      <c r="H10" s="303"/>
     </row>
     <row r="11" spans="2:8">
-      <c r="B11" s="302"/>
-      <c r="C11" s="303"/>
+      <c r="B11" s="304"/>
+      <c r="C11" s="305"/>
       <c r="D11" s="181" t="s">
         <v>70</v>
       </c>
@@ -10992,10 +10970,10 @@
       </c>
     </row>
     <row r="12" spans="2:8">
-      <c r="B12" s="290" t="s">
+      <c r="B12" s="296" t="s">
         <v>118</v>
       </c>
-      <c r="C12" s="291"/>
+      <c r="C12" s="297"/>
       <c r="D12" s="182">
         <f>'Flujo de Caja (Profesor) - 5 añ'!D11+'Flujo de Caja (Profesor) - 5 añ'!D12</f>
         <v>79684496.075435549</v>
@@ -11018,10 +10996,10 @@
       </c>
     </row>
     <row r="13" spans="2:8">
-      <c r="B13" s="290" t="s">
+      <c r="B13" s="296" t="s">
         <v>289</v>
       </c>
-      <c r="C13" s="291"/>
+      <c r="C13" s="297"/>
       <c r="D13" s="187">
         <v>5000</v>
       </c>
@@ -11039,10 +11017,10 @@
       </c>
     </row>
     <row r="14" spans="2:8">
-      <c r="B14" s="290" t="s">
+      <c r="B14" s="296" t="s">
         <v>290</v>
       </c>
-      <c r="C14" s="291"/>
+      <c r="C14" s="297"/>
       <c r="D14" s="187">
         <f>('Flujo de Caja (Profesor) - 5 añ'!D6+'Flujo de Caja (Profesor) - 5 añ'!D7)/'Tabla Crecimiento'!B9</f>
         <v>11103.815193643957</v>
@@ -11065,10 +11043,10 @@
       </c>
     </row>
     <row r="15" spans="2:8" ht="15.75" thickBot="1">
-      <c r="B15" s="299" t="s">
+      <c r="B15" s="298" t="s">
         <v>288</v>
       </c>
-      <c r="C15" s="300"/>
+      <c r="C15" s="299"/>
       <c r="D15" s="189">
         <f>D12/D13-D14</f>
         <v>4833.0840214431519</v>
@@ -11104,39 +11082,45 @@
       <c r="N23" s="93"/>
     </row>
     <row r="24" spans="2:14">
-      <c r="B24" s="263"/>
+      <c r="B24" s="259"/>
       <c r="C24" s="264"/>
     </row>
     <row r="25" spans="2:14">
-      <c r="B25" s="263"/>
+      <c r="B25" s="259"/>
       <c r="C25" s="264"/>
     </row>
     <row r="26" spans="2:14">
-      <c r="B26" s="263"/>
+      <c r="B26" s="259"/>
       <c r="C26" s="264"/>
     </row>
     <row r="27" spans="2:14">
-      <c r="B27" s="263"/>
-      <c r="C27" s="263"/>
+      <c r="B27" s="259"/>
+      <c r="C27" s="259"/>
     </row>
     <row r="28" spans="2:14">
-      <c r="B28" s="263"/>
+      <c r="B28" s="259"/>
       <c r="C28" s="264"/>
     </row>
     <row r="30" spans="2:14">
-      <c r="B30" s="263"/>
+      <c r="B30" s="259"/>
       <c r="C30" s="264"/>
     </row>
     <row r="31" spans="2:14">
-      <c r="B31" s="263"/>
+      <c r="B31" s="259"/>
       <c r="C31" s="264"/>
     </row>
     <row r="32" spans="2:14">
-      <c r="B32" s="263"/>
+      <c r="B32" s="259"/>
       <c r="C32" s="264"/>
     </row>
   </sheetData>
   <mergeCells count="22">
+    <mergeCell ref="B7:C7"/>
+    <mergeCell ref="B3:H3"/>
+    <mergeCell ref="B2:H2"/>
+    <mergeCell ref="B5:C5"/>
+    <mergeCell ref="B4:C4"/>
+    <mergeCell ref="B6:C6"/>
     <mergeCell ref="B32:C32"/>
     <mergeCell ref="B13:C13"/>
     <mergeCell ref="B14:C14"/>
@@ -11153,12 +11137,6 @@
     <mergeCell ref="B28:C28"/>
     <mergeCell ref="B30:C30"/>
     <mergeCell ref="B31:C31"/>
-    <mergeCell ref="B7:C7"/>
-    <mergeCell ref="B3:H3"/>
-    <mergeCell ref="B2:H2"/>
-    <mergeCell ref="B5:C5"/>
-    <mergeCell ref="B4:C4"/>
-    <mergeCell ref="B6:C6"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -11168,7 +11146,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AA19"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="H1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView topLeftCell="H1" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="X23" sqref="X23"/>
     </sheetView>
   </sheetViews>
@@ -11203,44 +11181,44 @@
   <sheetData>
     <row r="1" spans="1:27" ht="15.75" customHeight="1">
       <c r="A1" s="152"/>
-      <c r="B1" s="284" t="s">
+      <c r="B1" s="290" t="s">
         <v>70</v>
       </c>
-      <c r="C1" s="285"/>
-      <c r="D1" s="284" t="s">
+      <c r="C1" s="291"/>
+      <c r="D1" s="290" t="s">
         <v>71</v>
       </c>
-      <c r="E1" s="285"/>
-      <c r="F1" s="284" t="s">
+      <c r="E1" s="291"/>
+      <c r="F1" s="290" t="s">
         <v>72</v>
       </c>
-      <c r="G1" s="285"/>
-      <c r="H1" s="284" t="s">
+      <c r="G1" s="291"/>
+      <c r="H1" s="290" t="s">
         <v>74</v>
       </c>
-      <c r="I1" s="285"/>
-      <c r="J1" s="293" t="s">
+      <c r="I1" s="291"/>
+      <c r="J1" s="302" t="s">
         <v>75</v>
       </c>
-      <c r="K1" s="309"/>
+      <c r="K1" s="310"/>
       <c r="M1" s="193"/>
-      <c r="N1" s="304" t="s">
+      <c r="N1" s="311" t="s">
         <v>70</v>
       </c>
-      <c r="O1" s="308"/>
-      <c r="P1" s="304" t="s">
+      <c r="O1" s="312"/>
+      <c r="P1" s="311" t="s">
         <v>71</v>
       </c>
-      <c r="Q1" s="308"/>
+      <c r="Q1" s="312"/>
       <c r="U1" s="194"/>
-      <c r="V1" s="304" t="s">
+      <c r="V1" s="311" t="s">
         <v>70</v>
       </c>
-      <c r="W1" s="304"/>
-      <c r="X1" s="304" t="s">
+      <c r="W1" s="311"/>
+      <c r="X1" s="311" t="s">
         <v>71</v>
       </c>
-      <c r="Y1" s="304"/>
+      <c r="Y1" s="311"/>
     </row>
     <row r="2" spans="1:27" ht="15.75" customHeight="1">
       <c r="A2" s="30" t="s">
@@ -11289,17 +11267,17 @@
       <c r="M2" s="203" t="s">
         <v>137</v>
       </c>
-      <c r="N2" s="304"/>
-      <c r="O2" s="304"/>
-      <c r="P2" s="304"/>
-      <c r="Q2" s="304"/>
+      <c r="N2" s="311"/>
+      <c r="O2" s="311"/>
+      <c r="P2" s="311"/>
+      <c r="Q2" s="311"/>
       <c r="U2" s="195" t="s">
         <v>292</v>
       </c>
-      <c r="V2" s="307"/>
-      <c r="W2" s="307"/>
-      <c r="X2" s="307"/>
-      <c r="Y2" s="307"/>
+      <c r="V2" s="314"/>
+      <c r="W2" s="314"/>
+      <c r="X2" s="314"/>
+      <c r="Y2" s="314"/>
     </row>
     <row r="3" spans="1:27" ht="15.75" customHeight="1">
       <c r="A3" s="30" t="s">
@@ -11340,7 +11318,7 @@
       <c r="U3" s="205" t="s">
         <v>251</v>
       </c>
-      <c r="V3" s="314">
+      <c r="V3" s="254">
         <f>W3*1/O7</f>
         <v>3.5987345084564889E-3</v>
       </c>
@@ -11348,7 +11326,7 @@
         <f>C11</f>
         <v>729600</v>
       </c>
-      <c r="X3" s="314">
+      <c r="X3" s="254">
         <f>Y3/Q7</f>
         <v>2.1529627859572012E-3</v>
       </c>
@@ -11405,19 +11383,19 @@
         <v>154</v>
       </c>
       <c r="N4" s="219">
-        <f>B6</f>
+        <f t="shared" ref="N4:Q6" si="0">B6</f>
         <v>1.7263666090457389E-2</v>
       </c>
       <c r="O4" s="220">
-        <f>C6</f>
+        <f t="shared" si="0"/>
         <v>3500000</v>
       </c>
       <c r="P4" s="219">
-        <f>D6</f>
+        <f t="shared" si="0"/>
         <v>2.4358687594553636E-2</v>
       </c>
       <c r="Q4" s="220">
-        <f>E6</f>
+        <f t="shared" si="0"/>
         <v>8750000</v>
       </c>
       <c r="U4" s="205" t="s">
@@ -11428,15 +11406,15 @@
         <v>0.2323771472279017</v>
       </c>
       <c r="W4" s="207">
-        <f t="shared" ref="W4:W6" si="0">C12</f>
+        <f t="shared" ref="W4:W6" si="1">C12</f>
         <v>47111662.785648078</v>
       </c>
-      <c r="X4" s="314">
+      <c r="X4" s="254">
         <f>Y4/Q7</f>
         <v>0.22909125677385642</v>
       </c>
       <c r="Y4" s="207">
-        <f t="shared" ref="Y4:Y6" si="1">E12</f>
+        <f t="shared" ref="Y4:Y6" si="2">E12</f>
         <v>82292959.708528847</v>
       </c>
     </row>
@@ -11458,19 +11436,19 @@
         <v>155</v>
       </c>
       <c r="N5" s="219">
-        <f>B7</f>
+        <f t="shared" si="0"/>
         <v>3.452733218091478E-3</v>
       </c>
       <c r="O5" s="220">
-        <f>C7</f>
+        <f t="shared" si="0"/>
         <v>700000</v>
       </c>
       <c r="P5" s="219">
-        <f>D7</f>
+        <f t="shared" si="0"/>
         <v>3.8973900151285817E-3</v>
       </c>
       <c r="Q5" s="220">
-        <f>E7</f>
+        <f t="shared" si="0"/>
         <v>1400000</v>
       </c>
       <c r="U5" s="205" t="s">
@@ -11481,15 +11459,15 @@
         <v>0.54530849567871975</v>
       </c>
       <c r="W5" s="207">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>110554717.91883764</v>
       </c>
-      <c r="X5" s="314">
+      <c r="X5" s="254">
         <f>Y5/Q7</f>
         <v>0.27723804084555675</v>
       </c>
       <c r="Y5" s="207">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>99587994.959999993</v>
       </c>
     </row>
@@ -11541,19 +11519,19 @@
         <v>156</v>
       </c>
       <c r="N6" s="225">
-        <f>B8</f>
+        <f t="shared" si="0"/>
         <v>1.3810932872365912E-2</v>
       </c>
       <c r="O6" s="226">
-        <f>C8</f>
+        <f t="shared" si="0"/>
         <v>2800000</v>
       </c>
       <c r="P6" s="225">
-        <f>D8</f>
+        <f t="shared" si="0"/>
         <v>2.0461297579425053E-2</v>
       </c>
       <c r="Q6" s="226">
-        <f>E8</f>
+        <f t="shared" si="0"/>
         <v>7350000</v>
       </c>
       <c r="U6" s="213" t="s">
@@ -11564,15 +11542,15 @@
         <v>1.9651576725171104E-2</v>
       </c>
       <c r="W6" s="215">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>3984120.0691501889</v>
       </c>
-      <c r="X6" s="315">
+      <c r="X6" s="255">
         <f>Y6/Q7</f>
         <v>1.1756664259410072E-2</v>
       </c>
       <c r="Y6" s="215">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>4223167.2732992005</v>
       </c>
     </row>
@@ -11677,7 +11655,7 @@
         <v>2.0461297579425053E-2</v>
       </c>
       <c r="E8" s="87">
-        <f t="shared" ref="E8:K8" si="2">E6-E7</f>
+        <f t="shared" ref="E8:K8" si="3">E6-E7</f>
         <v>7350000</v>
       </c>
       <c r="F8" s="78">
@@ -11685,7 +11663,7 @@
         <v>3.7382072946240727E-2</v>
       </c>
       <c r="G8" s="87">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>19775000</v>
       </c>
       <c r="H8" s="78">
@@ -11693,7 +11671,7 @@
         <v>9.0361384486733018E-2</v>
       </c>
       <c r="I8" s="87">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>51887500</v>
       </c>
       <c r="J8" s="32">
@@ -11701,7 +11679,7 @@
         <v>0.20298161787654592</v>
       </c>
       <c r="K8" s="162">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>133218750</v>
       </c>
       <c r="U8" s="216" t="s">
@@ -11846,38 +11824,38 @@
         <v>773376</v>
       </c>
       <c r="M11" s="193"/>
-      <c r="N11" s="304" t="s">
+      <c r="N11" s="311" t="s">
         <v>72</v>
       </c>
-      <c r="O11" s="308"/>
-      <c r="P11" s="304" t="s">
+      <c r="O11" s="312"/>
+      <c r="P11" s="311" t="s">
         <v>74</v>
       </c>
-      <c r="Q11" s="308"/>
-      <c r="R11" s="304" t="s">
+      <c r="Q11" s="312"/>
+      <c r="R11" s="311" t="s">
         <v>75</v>
       </c>
-      <c r="S11" s="308"/>
+      <c r="S11" s="312"/>
       <c r="U11" s="208"/>
-      <c r="V11" s="305" t="s">
+      <c r="V11" s="313" t="s">
         <v>72</v>
       </c>
-      <c r="W11" s="305"/>
-      <c r="X11" s="305" t="s">
+      <c r="W11" s="313"/>
+      <c r="X11" s="313" t="s">
         <v>74</v>
       </c>
-      <c r="Y11" s="305"/>
-      <c r="Z11" s="305" t="s">
+      <c r="Y11" s="313"/>
+      <c r="Z11" s="313" t="s">
         <v>75</v>
       </c>
-      <c r="AA11" s="306"/>
+      <c r="AA11" s="315"/>
     </row>
     <row r="12" spans="1:27" ht="15.75" customHeight="1">
       <c r="A12" s="39" t="s">
         <v>252</v>
       </c>
       <c r="B12" s="86">
-        <f t="shared" ref="B12:B14" si="3">C12/$C$2</f>
+        <f t="shared" ref="B12:B14" si="4">C12/$C$2</f>
         <v>0.2323771472279017</v>
       </c>
       <c r="C12" s="42">
@@ -11919,28 +11897,28 @@
       <c r="M12" s="203" t="s">
         <v>137</v>
       </c>
-      <c r="N12" s="304"/>
-      <c r="O12" s="304"/>
-      <c r="P12" s="304"/>
-      <c r="Q12" s="304"/>
-      <c r="R12" s="304"/>
-      <c r="S12" s="304"/>
+      <c r="N12" s="311"/>
+      <c r="O12" s="311"/>
+      <c r="P12" s="311"/>
+      <c r="Q12" s="311"/>
+      <c r="R12" s="311"/>
+      <c r="S12" s="311"/>
       <c r="U12" s="195" t="s">
         <v>292</v>
       </c>
-      <c r="V12" s="307"/>
-      <c r="W12" s="307"/>
-      <c r="X12" s="307"/>
-      <c r="Y12" s="307"/>
-      <c r="Z12" s="307"/>
-      <c r="AA12" s="307"/>
+      <c r="V12" s="314"/>
+      <c r="W12" s="314"/>
+      <c r="X12" s="314"/>
+      <c r="Y12" s="314"/>
+      <c r="Z12" s="314"/>
+      <c r="AA12" s="314"/>
     </row>
     <row r="13" spans="1:27" ht="15.75" customHeight="1">
       <c r="A13" s="39" t="s">
         <v>253</v>
       </c>
       <c r="B13" s="86">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>0.54530849567871975</v>
       </c>
       <c r="C13" s="42">
@@ -11983,54 +11961,54 @@
         <v>142</v>
       </c>
       <c r="N13" s="222">
-        <f t="shared" ref="N13:S13" si="4">F4</f>
+        <f t="shared" ref="N13:S13" si="5">F4</f>
         <v>0.96261792705375926</v>
       </c>
       <c r="O13" s="223">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>509221881.16382653</v>
       </c>
       <c r="P13" s="222">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>0.90963861551326697</v>
       </c>
       <c r="Q13" s="223">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>522334556.18837321</v>
       </c>
       <c r="R13" s="210">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>0.79701838212345411</v>
       </c>
       <c r="S13" s="211">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>523090680.34961951</v>
       </c>
       <c r="U13" s="205" t="s">
         <v>251</v>
       </c>
-      <c r="V13" s="314">
+      <c r="V13" s="254">
         <f>W13/O17</f>
         <v>1.4619670314473764E-3</v>
       </c>
       <c r="W13" s="207">
-        <f t="shared" ref="V13:AA16" si="5">G11</f>
+        <f t="shared" ref="W13:AA16" si="6">G11</f>
         <v>773376</v>
       </c>
-      <c r="X13" s="314">
+      <c r="X13" s="254">
         <f>Y13/$Q$17</f>
         <v>1.3468239188400219E-3</v>
       </c>
       <c r="Y13" s="207">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>773376</v>
       </c>
-      <c r="Z13" s="314">
+      <c r="Z13" s="254">
         <f>AA13/$S$17</f>
         <v>1.1783710003801385E-3</v>
       </c>
       <c r="AA13" s="207">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>773376</v>
       </c>
     </row>
@@ -12039,7 +12017,7 @@
         <v>254</v>
       </c>
       <c r="B14" s="86">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>1.9651576725171104E-2</v>
       </c>
       <c r="C14" s="42">
@@ -12082,54 +12060,54 @@
         <v>154</v>
       </c>
       <c r="N14" s="219">
-        <f>F6</f>
+        <f t="shared" ref="N14:S16" si="7">F6</f>
         <v>4.1351850604248591E-2</v>
       </c>
       <c r="O14" s="220">
-        <f>G6</f>
+        <f t="shared" si="7"/>
         <v>21875000</v>
       </c>
       <c r="P14" s="219">
-        <f>H6</f>
+        <f t="shared" si="7"/>
         <v>9.5237546887366159E-2</v>
       </c>
       <c r="Q14" s="220">
-        <f>I6</f>
+        <f t="shared" si="7"/>
         <v>54687500</v>
       </c>
       <c r="R14" s="206">
-        <f>J6</f>
+        <f t="shared" si="7"/>
         <v>0.20831446826410707</v>
       </c>
       <c r="S14" s="207">
-        <f>K6</f>
+        <f t="shared" si="7"/>
         <v>136718750</v>
       </c>
       <c r="U14" s="205" t="s">
         <v>252</v>
       </c>
-      <c r="V14" s="314">
+      <c r="V14" s="254">
         <f>W14/O17</f>
         <v>0.25631746904469815</v>
       </c>
       <c r="W14" s="207">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>135591141.71245098</v>
       </c>
-      <c r="X14" s="314">
-        <f t="shared" ref="X14:X16" si="6">Y14/$Q$17</f>
+      <c r="X14" s="254">
+        <f t="shared" ref="X14:X16" si="8">Y14/$Q$17</f>
         <v>0.24354029747231237</v>
       </c>
       <c r="Y14" s="207">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>139846210.37927929</v>
       </c>
-      <c r="Z14" s="314">
-        <f t="shared" ref="Z14:Z16" si="7">AA14/$S$17</f>
+      <c r="Z14" s="254">
+        <f t="shared" ref="Z14:Z16" si="9">AA14/$S$17</f>
         <v>0.21334753057396344</v>
       </c>
       <c r="AA14" s="207">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>140021996.25749597</v>
       </c>
     </row>
@@ -12181,54 +12159,54 @@
         <v>155</v>
       </c>
       <c r="N15" s="219">
-        <f>F7</f>
+        <f t="shared" si="7"/>
         <v>3.9697776580078651E-3</v>
       </c>
       <c r="O15" s="220">
-        <f>G7</f>
+        <f t="shared" si="7"/>
         <v>2100000</v>
       </c>
       <c r="P15" s="219">
-        <f>H7</f>
+        <f t="shared" si="7"/>
         <v>4.8761624006331472E-3</v>
       </c>
       <c r="Q15" s="220">
-        <f>I7</f>
+        <f t="shared" si="7"/>
         <v>2800000</v>
       </c>
       <c r="R15" s="206">
-        <f>J7</f>
+        <f t="shared" si="7"/>
         <v>5.3328503875611413E-3</v>
       </c>
       <c r="S15" s="207">
-        <f>K7</f>
+        <f t="shared" si="7"/>
         <v>3500000</v>
       </c>
       <c r="U15" s="205" t="s">
         <v>253</v>
       </c>
-      <c r="V15" s="314">
+      <c r="V15" s="254">
         <f>W15/O17</f>
         <v>0.18930313600277565</v>
       </c>
       <c r="W15" s="207">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>100140768.54000001</v>
       </c>
-      <c r="X15" s="314">
+      <c r="X15" s="254">
+        <f t="shared" si="8"/>
+        <v>0.17535645145432649</v>
+      </c>
+      <c r="Y15" s="207">
         <f t="shared" si="6"/>
-        <v>0.17535645145432649</v>
-      </c>
-      <c r="Y15" s="207">
-        <f t="shared" si="5"/>
         <v>100693542.12</v>
       </c>
-      <c r="Z15" s="314">
-        <f t="shared" si="7"/>
+      <c r="Z15" s="254">
+        <f t="shared" si="9"/>
         <v>0.15376078246848021</v>
       </c>
       <c r="AA15" s="207">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>100914651.552</v>
       </c>
     </row>
@@ -12280,54 +12258,54 @@
         <v>156</v>
       </c>
       <c r="N16" s="225">
-        <f>F8</f>
+        <f t="shared" si="7"/>
         <v>3.7382072946240727E-2</v>
       </c>
       <c r="O16" s="226">
-        <f>G8</f>
+        <f t="shared" si="7"/>
         <v>19775000</v>
       </c>
       <c r="P16" s="225">
-        <f>H8</f>
+        <f t="shared" si="7"/>
         <v>9.0361384486733018E-2</v>
       </c>
       <c r="Q16" s="226">
-        <f>I8</f>
+        <f t="shared" si="7"/>
         <v>51887500</v>
       </c>
       <c r="R16" s="227">
-        <f>J8</f>
+        <f t="shared" si="7"/>
         <v>0.20298161787654592</v>
       </c>
       <c r="S16" s="228">
-        <f>K8</f>
+        <f t="shared" si="7"/>
         <v>133218750</v>
       </c>
       <c r="U16" s="213" t="s">
         <v>254</v>
       </c>
-      <c r="V16" s="315">
+      <c r="V16" s="255">
         <f>W16/O17</f>
         <v>8.0210073532189629E-3</v>
       </c>
       <c r="W16" s="215">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>4243087.8736449508</v>
       </c>
-      <c r="X16" s="315">
+      <c r="X16" s="255">
+        <f t="shared" si="8"/>
+        <v>7.4239720123049826E-3</v>
+      </c>
+      <c r="Y16" s="215">
         <f t="shared" si="6"/>
-        <v>7.4239720123049826E-3</v>
-      </c>
-      <c r="Y16" s="215">
-        <f t="shared" si="5"/>
         <v>4263008.4739907021</v>
       </c>
-      <c r="Z16" s="315">
-        <f t="shared" si="7"/>
+      <c r="Z16" s="255">
+        <f t="shared" si="9"/>
         <v>6.5075656643449886E-3</v>
       </c>
       <c r="AA16" s="215">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>4270976.7141290028</v>
       </c>
     </row>
@@ -12420,37 +12398,37 @@
     <row r="19" spans="2:27" ht="15.75" customHeight="1">
       <c r="U19" s="181"/>
       <c r="V19" s="184">
-        <f>V17+V18</f>
+        <f t="shared" ref="V19:AA19" si="10">V17+V18</f>
         <v>1</v>
       </c>
       <c r="W19" s="212">
-        <f>W17+W18</f>
+        <f t="shared" si="10"/>
         <v>528996881.16382653</v>
       </c>
       <c r="X19" s="184">
-        <f>X17+X18</f>
+        <f t="shared" si="10"/>
         <v>1</v>
       </c>
       <c r="Y19" s="212">
-        <f>Y17+Y18</f>
+        <f t="shared" si="10"/>
         <v>574222056.18837321</v>
       </c>
       <c r="Z19" s="184">
-        <f>Z17+Z18</f>
+        <f t="shared" si="10"/>
         <v>1</v>
       </c>
       <c r="AA19" s="212">
-        <f>AA17+AA18</f>
+        <f t="shared" si="10"/>
         <v>656309430.34961951</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="19">
-    <mergeCell ref="B1:C1"/>
-    <mergeCell ref="D1:E1"/>
-    <mergeCell ref="F1:G1"/>
-    <mergeCell ref="H1:I1"/>
-    <mergeCell ref="J1:K1"/>
+    <mergeCell ref="V12:AA12"/>
+    <mergeCell ref="N12:S12"/>
+    <mergeCell ref="Z11:AA11"/>
+    <mergeCell ref="V2:Y2"/>
+    <mergeCell ref="R11:S11"/>
     <mergeCell ref="V1:W1"/>
     <mergeCell ref="X1:Y1"/>
     <mergeCell ref="N2:Q2"/>
@@ -12460,11 +12438,11 @@
     <mergeCell ref="X11:Y11"/>
     <mergeCell ref="N1:O1"/>
     <mergeCell ref="P1:Q1"/>
-    <mergeCell ref="V12:AA12"/>
-    <mergeCell ref="N12:S12"/>
-    <mergeCell ref="Z11:AA11"/>
-    <mergeCell ref="V2:Y2"/>
-    <mergeCell ref="R11:S11"/>
+    <mergeCell ref="B1:C1"/>
+    <mergeCell ref="D1:E1"/>
+    <mergeCell ref="F1:G1"/>
+    <mergeCell ref="H1:I1"/>
+    <mergeCell ref="J1:K1"/>
   </mergeCells>
   <conditionalFormatting sqref="M1:Q1 A1:K16 M2:M7">
     <cfRule type="cellIs" dxfId="6" priority="13" operator="lessThan">
@@ -13303,18 +13281,18 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:14" ht="15.75" customHeight="1">
-      <c r="A1" s="250" t="s">
+      <c r="A1" s="270" t="s">
         <v>8</v>
       </c>
-      <c r="B1" s="251"/>
-      <c r="D1" s="250" t="s">
+      <c r="B1" s="271"/>
+      <c r="D1" s="270" t="s">
         <v>9</v>
       </c>
-      <c r="E1" s="251"/>
-      <c r="J1" s="250" t="s">
+      <c r="E1" s="271"/>
+      <c r="J1" s="270" t="s">
         <v>11</v>
       </c>
-      <c r="K1" s="251"/>
+      <c r="K1" s="271"/>
       <c r="M1" s="6" t="s">
         <v>12</v>
       </c>
@@ -13329,7 +13307,7 @@
       <c r="D2" s="233" t="s">
         <v>296</v>
       </c>
-      <c r="E2" s="310">
+      <c r="E2" s="250">
         <v>0</v>
       </c>
       <c r="J2" s="9" t="s">
@@ -13356,7 +13334,7 @@
       <c r="D3" s="233" t="s">
         <v>297</v>
       </c>
-      <c r="E3" s="310">
+      <c r="E3" s="250">
         <v>0</v>
       </c>
       <c r="J3" s="9" t="s">
@@ -13382,7 +13360,7 @@
       <c r="D4" s="233" t="s">
         <v>298</v>
       </c>
-      <c r="E4" s="310">
+      <c r="E4" s="250">
         <v>0</v>
       </c>
       <c r="J4" s="12"/>
@@ -13398,7 +13376,7 @@
       <c r="D5" s="233" t="s">
         <v>299</v>
       </c>
-      <c r="E5" s="310">
+      <c r="E5" s="250">
         <v>0</v>
       </c>
       <c r="J5" s="12"/>
@@ -13414,7 +13392,7 @@
       <c r="D6" s="233" t="s">
         <v>300</v>
       </c>
-      <c r="E6" s="310">
+      <c r="E6" s="250">
         <v>0</v>
       </c>
       <c r="J6" s="12"/>
@@ -13430,7 +13408,7 @@
       <c r="D7" s="235" t="s">
         <v>25</v>
       </c>
-      <c r="E7" s="311">
+      <c r="E7" s="251">
         <f>E2+E3+E4+E5+E6</f>
         <v>0</v>
       </c>
@@ -13443,7 +13421,7 @@
       <c r="D8" s="235" t="s">
         <v>293</v>
       </c>
-      <c r="E8" s="311">
+      <c r="E8" s="251">
         <v>0</v>
       </c>
       <c r="J8" s="12"/>
@@ -13476,7 +13454,7 @@
       <c r="J11" s="230" t="s">
         <v>28</v>
       </c>
-      <c r="K11" s="312">
+      <c r="K11" s="252">
         <f>K2+K3</f>
         <v>332010</v>
       </c>
@@ -13499,7 +13477,7 @@
       <c r="J12" s="231" t="s">
         <v>294</v>
       </c>
-      <c r="K12" s="313">
+      <c r="K12" s="253">
         <f>K11*12</f>
         <v>3984120</v>
       </c>
@@ -13513,14 +13491,14 @@
       </c>
     </row>
     <row r="17" spans="1:14" ht="15.75" customHeight="1">
-      <c r="A17" s="250" t="s">
+      <c r="A17" s="270" t="s">
         <v>31</v>
       </c>
-      <c r="B17" s="251"/>
-      <c r="D17" s="252" t="s">
+      <c r="B17" s="271"/>
+      <c r="D17" s="272" t="s">
         <v>10</v>
       </c>
-      <c r="E17" s="253"/>
+      <c r="E17" s="273"/>
       <c r="M17" s="11" t="s">
         <v>33</v>
       </c>
@@ -13717,26 +13695,26 @@
     </row>
     <row r="33" spans="1:8" ht="15.75" customHeight="1" thickBot="1"/>
     <row r="34" spans="1:8" ht="15.75" customHeight="1" thickTop="1" thickBot="1">
-      <c r="A34" s="255" t="s">
+      <c r="A34" s="256" t="s">
         <v>214</v>
       </c>
-      <c r="B34" s="255"/>
-      <c r="C34" s="255"/>
-      <c r="D34" s="255"/>
-      <c r="E34" s="255"/>
-      <c r="F34" s="255"/>
-      <c r="G34" s="255"/>
-      <c r="H34" s="255"/>
+      <c r="B34" s="256"/>
+      <c r="C34" s="256"/>
+      <c r="D34" s="256"/>
+      <c r="E34" s="256"/>
+      <c r="F34" s="256"/>
+      <c r="G34" s="256"/>
+      <c r="H34" s="256"/>
     </row>
     <row r="35" spans="1:8" ht="15.75" customHeight="1" thickTop="1" thickBot="1">
-      <c r="A35" s="256"/>
-      <c r="B35" s="256"/>
-      <c r="C35" s="256"/>
-      <c r="D35" s="256"/>
-      <c r="E35" s="256"/>
-      <c r="F35" s="256"/>
-      <c r="G35" s="256"/>
-      <c r="H35" s="256"/>
+      <c r="A35" s="268"/>
+      <c r="B35" s="268"/>
+      <c r="C35" s="268"/>
+      <c r="D35" s="268"/>
+      <c r="E35" s="268"/>
+      <c r="F35" s="268"/>
+      <c r="G35" s="268"/>
+      <c r="H35" s="268"/>
     </row>
     <row r="36" spans="1:8" ht="46.5" customHeight="1" thickTop="1" thickBot="1">
       <c r="A36" s="106" t="s">
@@ -13942,235 +13920,235 @@
     </row>
     <row r="45" spans="1:8" ht="15.75" customHeight="1" thickBot="1"/>
     <row r="46" spans="1:8" ht="15.75" customHeight="1" thickTop="1" thickBot="1">
-      <c r="A46" s="255" t="s">
+      <c r="A46" s="256" t="s">
         <v>232</v>
       </c>
-      <c r="B46" s="255"/>
-      <c r="C46" s="255"/>
-      <c r="D46" s="255"/>
-      <c r="E46" s="255"/>
-      <c r="F46" s="255"/>
+      <c r="B46" s="256"/>
+      <c r="C46" s="256"/>
+      <c r="D46" s="256"/>
+      <c r="E46" s="256"/>
+      <c r="F46" s="256"/>
     </row>
     <row r="47" spans="1:8" ht="15.75" customHeight="1" thickTop="1">
-      <c r="A47" s="257" t="s">
+      <c r="A47" s="269" t="s">
         <v>217</v>
       </c>
-      <c r="B47" s="257"/>
-      <c r="C47" s="257"/>
-      <c r="D47" s="257"/>
-      <c r="E47" s="257" t="s">
+      <c r="B47" s="269"/>
+      <c r="C47" s="269"/>
+      <c r="D47" s="269"/>
+      <c r="E47" s="269" t="s">
         <v>70</v>
       </c>
-      <c r="F47" s="257"/>
+      <c r="F47" s="269"/>
     </row>
     <row r="48" spans="1:8" ht="15.75" customHeight="1">
-      <c r="A48" s="259" t="s">
+      <c r="A48" s="262" t="s">
         <v>225</v>
       </c>
-      <c r="B48" s="260"/>
-      <c r="C48" s="263" t="s">
+      <c r="B48" s="265"/>
+      <c r="C48" s="259" t="s">
         <v>218</v>
       </c>
       <c r="D48" s="264"/>
-      <c r="E48" s="254">
-        <v>0</v>
-      </c>
-      <c r="F48" s="254"/>
+      <c r="E48" s="267">
+        <v>0</v>
+      </c>
+      <c r="F48" s="267"/>
     </row>
     <row r="49" spans="1:6" ht="15.75" customHeight="1">
-      <c r="A49" s="260"/>
-      <c r="B49" s="260"/>
-      <c r="C49" s="263" t="s">
+      <c r="A49" s="265"/>
+      <c r="B49" s="265"/>
+      <c r="C49" s="259" t="s">
         <v>219</v>
       </c>
       <c r="D49" s="264"/>
-      <c r="E49" s="254">
+      <c r="E49" s="267">
         <f>B2*12</f>
         <v>36800004</v>
       </c>
-      <c r="F49" s="254"/>
+      <c r="F49" s="267"/>
     </row>
     <row r="50" spans="1:6" ht="15.75" customHeight="1">
-      <c r="A50" s="260"/>
-      <c r="B50" s="260"/>
-      <c r="C50" s="263" t="s">
+      <c r="A50" s="265"/>
+      <c r="B50" s="265"/>
+      <c r="C50" s="259" t="s">
         <v>220</v>
       </c>
       <c r="D50" s="264"/>
-      <c r="E50" s="254">
+      <c r="E50" s="267">
         <f>(B19*12+B22*12)</f>
         <v>39415992</v>
       </c>
-      <c r="F50" s="254"/>
+      <c r="F50" s="267"/>
     </row>
     <row r="51" spans="1:6" ht="15.75" customHeight="1">
-      <c r="A51" s="260"/>
-      <c r="B51" s="260"/>
-      <c r="C51" s="263" t="s">
+      <c r="A51" s="265"/>
+      <c r="B51" s="265"/>
+      <c r="C51" s="259" t="s">
         <v>221</v>
       </c>
-      <c r="D51" s="263"/>
-      <c r="E51" s="254">
+      <c r="D51" s="259"/>
+      <c r="E51" s="267">
         <f>B4*12</f>
         <v>2400000</v>
       </c>
-      <c r="F51" s="254"/>
+      <c r="F51" s="267"/>
     </row>
     <row r="52" spans="1:6" ht="15.75" customHeight="1">
-      <c r="A52" s="260"/>
-      <c r="B52" s="260"/>
-      <c r="C52" s="263" t="s">
+      <c r="A52" s="265"/>
+      <c r="B52" s="265"/>
+      <c r="C52" s="259" t="s">
         <v>222</v>
       </c>
       <c r="D52" s="264"/>
-      <c r="E52" s="254">
+      <c r="E52" s="267">
         <f>(B21+B23)*12</f>
         <v>31938720</v>
       </c>
-      <c r="F52" s="254"/>
+      <c r="F52" s="267"/>
     </row>
     <row r="53" spans="1:6" ht="15.75" customHeight="1" thickBot="1">
-      <c r="A53" s="260"/>
-      <c r="B53" s="260"/>
-      <c r="C53" s="263" t="s">
+      <c r="A53" s="265"/>
+      <c r="B53" s="265"/>
+      <c r="C53" s="259" t="s">
         <v>223</v>
       </c>
       <c r="D53" s="264"/>
-      <c r="E53" s="254">
-        <v>0</v>
-      </c>
-      <c r="F53" s="254"/>
+      <c r="E53" s="267">
+        <v>0</v>
+      </c>
+      <c r="F53" s="267"/>
     </row>
     <row r="54" spans="1:6" ht="15.75" customHeight="1" thickTop="1" thickBot="1">
-      <c r="A54" s="260"/>
-      <c r="B54" s="260"/>
-      <c r="C54" s="255" t="s">
+      <c r="A54" s="265"/>
+      <c r="B54" s="265"/>
+      <c r="C54" s="256" t="s">
         <v>224</v>
       </c>
-      <c r="D54" s="255"/>
-      <c r="E54" s="258">
+      <c r="D54" s="256"/>
+      <c r="E54" s="263">
         <f>SUM(E48:F53)</f>
         <v>110554716</v>
       </c>
-      <c r="F54" s="258"/>
+      <c r="F54" s="263"/>
     </row>
     <row r="55" spans="1:6" ht="15.75" customHeight="1" thickTop="1">
-      <c r="A55" s="259" t="s">
+      <c r="A55" s="262" t="s">
         <v>231</v>
       </c>
-      <c r="B55" s="260"/>
-      <c r="C55" s="261" t="s">
+      <c r="B55" s="265"/>
+      <c r="C55" s="258" t="s">
         <v>226</v>
       </c>
-      <c r="D55" s="262"/>
-      <c r="E55" s="265">
-        <v>0</v>
-      </c>
-      <c r="F55" s="265"/>
+      <c r="D55" s="266"/>
+      <c r="E55" s="260">
+        <v>0</v>
+      </c>
+      <c r="F55" s="260"/>
     </row>
     <row r="56" spans="1:6" ht="15.75" customHeight="1">
-      <c r="A56" s="260"/>
-      <c r="B56" s="260"/>
-      <c r="C56" s="263" t="s">
+      <c r="A56" s="265"/>
+      <c r="B56" s="265"/>
+      <c r="C56" s="259" t="s">
         <v>227</v>
       </c>
       <c r="D56" s="264"/>
-      <c r="E56" s="266">
+      <c r="E56" s="261">
         <f>'Presupuesto Inicial'!J20*12</f>
         <v>700000</v>
       </c>
-      <c r="F56" s="266"/>
+      <c r="F56" s="261"/>
     </row>
     <row r="57" spans="1:6" ht="15.75" customHeight="1">
-      <c r="A57" s="260"/>
-      <c r="B57" s="260"/>
-      <c r="C57" s="263" t="s">
+      <c r="A57" s="265"/>
+      <c r="B57" s="265"/>
+      <c r="C57" s="259" t="s">
         <v>228</v>
       </c>
       <c r="D57" s="264"/>
-      <c r="E57" s="266">
-        <v>0</v>
-      </c>
-      <c r="F57" s="266"/>
+      <c r="E57" s="261">
+        <v>0</v>
+      </c>
+      <c r="F57" s="261"/>
     </row>
     <row r="58" spans="1:6" ht="15.75" customHeight="1" thickBot="1">
-      <c r="A58" s="260"/>
-      <c r="B58" s="260"/>
-      <c r="C58" s="263" t="s">
+      <c r="A58" s="265"/>
+      <c r="B58" s="265"/>
+      <c r="C58" s="259" t="s">
         <v>229</v>
       </c>
       <c r="D58" s="264"/>
-      <c r="E58" s="266">
-        <v>0</v>
-      </c>
-      <c r="F58" s="266"/>
+      <c r="E58" s="261">
+        <v>0</v>
+      </c>
+      <c r="F58" s="261"/>
     </row>
     <row r="59" spans="1:6" ht="15.75" customHeight="1" thickTop="1" thickBot="1">
-      <c r="A59" s="260"/>
-      <c r="B59" s="260"/>
-      <c r="C59" s="255" t="s">
+      <c r="A59" s="265"/>
+      <c r="B59" s="265"/>
+      <c r="C59" s="256" t="s">
         <v>230</v>
       </c>
-      <c r="D59" s="255"/>
-      <c r="E59" s="258">
+      <c r="D59" s="256"/>
+      <c r="E59" s="263">
         <f>SUM(E55:F58)</f>
         <v>700000</v>
       </c>
-      <c r="F59" s="255"/>
+      <c r="F59" s="256"/>
     </row>
     <row r="60" spans="1:6" ht="15.75" customHeight="1" thickTop="1">
-      <c r="A60" s="259" t="s">
+      <c r="A60" s="262" t="s">
         <v>235</v>
       </c>
-      <c r="B60" s="259"/>
-      <c r="C60" s="261" t="s">
+      <c r="B60" s="262"/>
+      <c r="C60" s="258" t="s">
         <v>245</v>
       </c>
-      <c r="D60" s="261"/>
-      <c r="E60" s="265">
+      <c r="D60" s="258"/>
+      <c r="E60" s="260">
         <f>('Presupuesto Inicial'!B12+'Presupuesto Inicial'!B13)+('Presupuesto Inicial'!B11*6)+('Salarios, gastos y costos'!K11*12)</f>
         <v>7848920</v>
       </c>
-      <c r="F60" s="265"/>
+      <c r="F60" s="260"/>
     </row>
     <row r="61" spans="1:6" ht="15.75" customHeight="1" thickBot="1">
-      <c r="A61" s="259"/>
-      <c r="B61" s="259"/>
-      <c r="C61" s="263" t="s">
+      <c r="A61" s="262"/>
+      <c r="B61" s="262"/>
+      <c r="C61" s="259" t="s">
         <v>233</v>
       </c>
-      <c r="D61" s="263"/>
-      <c r="E61" s="266">
+      <c r="D61" s="259"/>
+      <c r="E61" s="261">
         <f>'Presupuesto Inicial'!B2</f>
         <v>116700</v>
       </c>
-      <c r="F61" s="266"/>
+      <c r="F61" s="261"/>
     </row>
     <row r="62" spans="1:6" ht="15.75" customHeight="1" thickTop="1" thickBot="1">
-      <c r="A62" s="259"/>
-      <c r="B62" s="259"/>
-      <c r="C62" s="255" t="s">
+      <c r="A62" s="262"/>
+      <c r="B62" s="262"/>
+      <c r="C62" s="256" t="s">
         <v>234</v>
       </c>
-      <c r="D62" s="255"/>
-      <c r="E62" s="258">
+      <c r="D62" s="256"/>
+      <c r="E62" s="263">
         <f>E60+E61</f>
         <v>7965620</v>
       </c>
-      <c r="F62" s="258"/>
+      <c r="F62" s="263"/>
     </row>
     <row r="63" spans="1:6" ht="15.75" customHeight="1" thickTop="1" thickBot="1">
-      <c r="A63" s="255" t="s">
+      <c r="A63" s="256" t="s">
         <v>239</v>
       </c>
-      <c r="B63" s="255"/>
-      <c r="C63" s="255"/>
-      <c r="D63" s="255"/>
-      <c r="E63" s="267">
+      <c r="B63" s="256"/>
+      <c r="C63" s="256"/>
+      <c r="D63" s="256"/>
+      <c r="E63" s="257">
         <f>E54+E59+E62</f>
         <v>119220336</v>
       </c>
-      <c r="F63" s="267"/>
+      <c r="F63" s="257"/>
     </row>
     <row r="64" spans="1:6" ht="15.75" customHeight="1" thickTop="1"/>
     <row r="65" spans="7:8" ht="15.75" customHeight="1" thickBot="1"/>
@@ -14184,23 +14162,18 @@
     <row r="67" spans="7:8" ht="15.75" customHeight="1" thickTop="1"/>
   </sheetData>
   <mergeCells count="45">
-    <mergeCell ref="A63:D63"/>
-    <mergeCell ref="E63:F63"/>
-    <mergeCell ref="C60:D60"/>
-    <mergeCell ref="C61:D61"/>
-    <mergeCell ref="E60:F60"/>
-    <mergeCell ref="E61:F61"/>
-    <mergeCell ref="A60:B62"/>
-    <mergeCell ref="C62:D62"/>
-    <mergeCell ref="E62:F62"/>
-    <mergeCell ref="C57:D57"/>
-    <mergeCell ref="C58:D58"/>
-    <mergeCell ref="C59:D59"/>
-    <mergeCell ref="E55:F55"/>
-    <mergeCell ref="E56:F56"/>
-    <mergeCell ref="E57:F57"/>
-    <mergeCell ref="E58:F58"/>
-    <mergeCell ref="E59:F59"/>
+    <mergeCell ref="A1:B1"/>
+    <mergeCell ref="A17:B17"/>
+    <mergeCell ref="D1:E1"/>
+    <mergeCell ref="D17:E17"/>
+    <mergeCell ref="J1:K1"/>
+    <mergeCell ref="E51:F51"/>
+    <mergeCell ref="E52:F52"/>
+    <mergeCell ref="A34:H34"/>
+    <mergeCell ref="A35:H35"/>
+    <mergeCell ref="A47:D47"/>
+    <mergeCell ref="E47:F47"/>
+    <mergeCell ref="A46:F46"/>
     <mergeCell ref="C54:D54"/>
     <mergeCell ref="E54:F54"/>
     <mergeCell ref="A48:B54"/>
@@ -14217,18 +14190,23 @@
     <mergeCell ref="E48:F48"/>
     <mergeCell ref="E49:F49"/>
     <mergeCell ref="E50:F50"/>
-    <mergeCell ref="E51:F51"/>
-    <mergeCell ref="E52:F52"/>
-    <mergeCell ref="A34:H34"/>
-    <mergeCell ref="A35:H35"/>
-    <mergeCell ref="A47:D47"/>
-    <mergeCell ref="E47:F47"/>
-    <mergeCell ref="A46:F46"/>
-    <mergeCell ref="A1:B1"/>
-    <mergeCell ref="A17:B17"/>
-    <mergeCell ref="D1:E1"/>
-    <mergeCell ref="D17:E17"/>
-    <mergeCell ref="J1:K1"/>
+    <mergeCell ref="C57:D57"/>
+    <mergeCell ref="C58:D58"/>
+    <mergeCell ref="C59:D59"/>
+    <mergeCell ref="E55:F55"/>
+    <mergeCell ref="E56:F56"/>
+    <mergeCell ref="E57:F57"/>
+    <mergeCell ref="E58:F58"/>
+    <mergeCell ref="E59:F59"/>
+    <mergeCell ref="A63:D63"/>
+    <mergeCell ref="E63:F63"/>
+    <mergeCell ref="C60:D60"/>
+    <mergeCell ref="C61:D61"/>
+    <mergeCell ref="E60:F60"/>
+    <mergeCell ref="E61:F61"/>
+    <mergeCell ref="A60:B62"/>
+    <mergeCell ref="C62:D62"/>
+    <mergeCell ref="E62:F62"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="N31" r:id="rId1"/>
@@ -14259,28 +14237,28 @@
   <sheetData>
     <row r="1" spans="1:4" ht="15.75" customHeight="1" thickBot="1"/>
     <row r="2" spans="1:4" ht="15.75" customHeight="1" thickTop="1" thickBot="1">
-      <c r="A2" s="255" t="s">
+      <c r="A2" s="256" t="s">
         <v>7</v>
       </c>
-      <c r="B2" s="268"/>
-      <c r="C2" s="268"/>
-      <c r="D2" s="268"/>
+      <c r="B2" s="274"/>
+      <c r="C2" s="274"/>
+      <c r="D2" s="274"/>
     </row>
     <row r="3" spans="1:4" ht="15.75" customHeight="1" thickTop="1">
-      <c r="A3" s="270" t="s">
+      <c r="A3" s="276" t="s">
         <v>14</v>
       </c>
-      <c r="B3" s="251"/>
-      <c r="C3" s="270" t="s">
+      <c r="B3" s="271"/>
+      <c r="C3" s="276" t="s">
         <v>15</v>
       </c>
-      <c r="D3" s="251"/>
+      <c r="D3" s="271"/>
     </row>
     <row r="4" spans="1:4" ht="15.75" customHeight="1">
-      <c r="A4" s="271" t="s">
+      <c r="A4" s="277" t="s">
         <v>16</v>
       </c>
-      <c r="B4" s="274">
+      <c r="B4" s="280">
         <v>1500000</v>
       </c>
       <c r="C4" s="18" t="s">
@@ -14291,16 +14269,16 @@
       </c>
     </row>
     <row r="5" spans="1:4" ht="15.75" customHeight="1">
-      <c r="A5" s="272"/>
-      <c r="B5" s="272"/>
-      <c r="C5" s="270" t="s">
+      <c r="A5" s="278"/>
+      <c r="B5" s="278"/>
+      <c r="C5" s="276" t="s">
         <v>35</v>
       </c>
-      <c r="D5" s="251"/>
+      <c r="D5" s="271"/>
     </row>
     <row r="6" spans="1:4" ht="15.75" customHeight="1">
-      <c r="A6" s="272"/>
-      <c r="B6" s="272"/>
+      <c r="A6" s="278"/>
+      <c r="B6" s="278"/>
       <c r="C6" s="18" t="s">
         <v>36</v>
       </c>
@@ -14309,8 +14287,8 @@
       </c>
     </row>
     <row r="7" spans="1:4" ht="15.75" customHeight="1">
-      <c r="A7" s="272"/>
-      <c r="B7" s="272"/>
+      <c r="A7" s="278"/>
+      <c r="B7" s="278"/>
       <c r="C7" s="18" t="s">
         <v>39</v>
       </c>
@@ -14319,8 +14297,8 @@
       </c>
     </row>
     <row r="8" spans="1:4" ht="15.75" customHeight="1">
-      <c r="A8" s="273"/>
-      <c r="B8" s="273"/>
+      <c r="A8" s="279"/>
+      <c r="B8" s="279"/>
       <c r="C8" s="18" t="s">
         <v>236</v>
       </c>
@@ -14345,15 +14323,15 @@
       </c>
     </row>
     <row r="10" spans="1:4" ht="15.75" customHeight="1" thickTop="1" thickBot="1">
-      <c r="A10" s="255" t="s">
+      <c r="A10" s="256" t="s">
         <v>53</v>
       </c>
-      <c r="B10" s="268"/>
-      <c r="C10" s="269">
+      <c r="B10" s="274"/>
+      <c r="C10" s="275">
         <f>D4+D9</f>
         <v>1500000</v>
       </c>
-      <c r="D10" s="268"/>
+      <c r="D10" s="274"/>
     </row>
     <row r="11" spans="1:4" ht="15.75" customHeight="1" thickTop="1"/>
     <row r="12" spans="1:4" ht="15.75" customHeight="1">
@@ -14389,49 +14367,49 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:6" ht="15">
-      <c r="B2" s="275" t="s">
+      <c r="B2" s="281" t="s">
         <v>238</v>
       </c>
-      <c r="C2" s="275"/>
-      <c r="D2" s="275"/>
-      <c r="E2" s="275"/>
-      <c r="F2" s="275"/>
+      <c r="C2" s="281"/>
+      <c r="D2" s="281"/>
+      <c r="E2" s="281"/>
+      <c r="F2" s="281"/>
     </row>
     <row r="3" spans="2:6">
-      <c r="B3" s="256" t="s">
+      <c r="B3" s="268" t="s">
         <v>240</v>
       </c>
-      <c r="C3" s="256"/>
-      <c r="D3" s="256"/>
-      <c r="E3" s="277">
+      <c r="C3" s="268"/>
+      <c r="D3" s="268"/>
+      <c r="E3" s="283">
         <f>'Salarios, gastos y costos'!E62:F62</f>
         <v>7965620</v>
       </c>
-      <c r="F3" s="277"/>
+      <c r="F3" s="283"/>
     </row>
     <row r="4" spans="2:6">
-      <c r="B4" s="278" t="s">
+      <c r="B4" s="284" t="s">
         <v>241</v>
       </c>
-      <c r="C4" s="256"/>
-      <c r="D4" s="256"/>
-      <c r="E4" s="279">
+      <c r="C4" s="268"/>
+      <c r="D4" s="268"/>
+      <c r="E4" s="285">
         <f>'Salarios, gastos y costos'!B11*7</f>
         <v>64490251</v>
       </c>
-      <c r="F4" s="279"/>
+      <c r="F4" s="285"/>
     </row>
     <row r="5" spans="2:6" ht="15">
-      <c r="B5" s="275" t="s">
+      <c r="B5" s="281" t="s">
         <v>210</v>
       </c>
-      <c r="C5" s="275"/>
-      <c r="D5" s="275"/>
-      <c r="E5" s="276">
+      <c r="C5" s="281"/>
+      <c r="D5" s="281"/>
+      <c r="E5" s="282">
         <f>SUM(E3:F4)</f>
         <v>72455871</v>
       </c>
-      <c r="F5" s="276"/>
+      <c r="F5" s="282"/>
     </row>
   </sheetData>
   <mergeCells count="7">
@@ -14502,30 +14480,30 @@
       <c r="G1" s="123" t="s">
         <v>62</v>
       </c>
-      <c r="H1" s="281" t="s">
+      <c r="H1" s="287" t="s">
         <v>63</v>
       </c>
-      <c r="I1" s="251"/>
-      <c r="J1" s="280" t="s">
+      <c r="I1" s="271"/>
+      <c r="J1" s="286" t="s">
         <v>64</v>
       </c>
-      <c r="K1" s="251"/>
-      <c r="L1" s="280" t="s">
+      <c r="K1" s="271"/>
+      <c r="L1" s="286" t="s">
         <v>65</v>
       </c>
-      <c r="M1" s="251"/>
-      <c r="N1" s="280" t="s">
+      <c r="M1" s="271"/>
+      <c r="N1" s="286" t="s">
         <v>66</v>
       </c>
-      <c r="O1" s="251"/>
-      <c r="P1" s="280" t="s">
+      <c r="O1" s="271"/>
+      <c r="P1" s="286" t="s">
         <v>67</v>
       </c>
-      <c r="Q1" s="251"/>
-      <c r="R1" s="280" t="s">
+      <c r="Q1" s="271"/>
+      <c r="R1" s="286" t="s">
         <v>68</v>
       </c>
-      <c r="S1" s="251"/>
+      <c r="S1" s="271"/>
       <c r="U1" s="140" t="s">
         <v>70</v>
       </c>
@@ -15815,45 +15793,45 @@
     <mergeCell ref="P1:Q1"/>
   </mergeCells>
   <conditionalFormatting sqref="B1:S7 B17:S994 B8:C14 H8:S16 B16:C16">
-    <cfRule type="cellIs" dxfId="18" priority="15" operator="lessThan">
+    <cfRule type="cellIs" dxfId="30" priority="15" operator="lessThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I8">
-    <cfRule type="cellIs" dxfId="17" priority="13" operator="lessThan">
+    <cfRule type="cellIs" dxfId="29" priority="13" operator="lessThan">
       <formula>0</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="16" priority="14" operator="lessThan">
+    <cfRule type="cellIs" dxfId="28" priority="14" operator="lessThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H2:S16">
-    <cfRule type="cellIs" dxfId="15" priority="7" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="27" priority="7" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D2:G14 D16:G16 B15:G15">
-    <cfRule type="cellIs" dxfId="14" priority="5" operator="lessThan">
+    <cfRule type="cellIs" dxfId="26" priority="5" operator="lessThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B8:C8">
-    <cfRule type="cellIs" dxfId="13" priority="4" operator="lessThan">
+    <cfRule type="cellIs" dxfId="25" priority="4" operator="lessThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B11:C11">
-    <cfRule type="cellIs" dxfId="12" priority="3" operator="lessThan">
+    <cfRule type="cellIs" dxfId="24" priority="3" operator="lessThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B14:C14">
-    <cfRule type="cellIs" dxfId="11" priority="2" operator="lessThan">
+    <cfRule type="cellIs" dxfId="23" priority="2" operator="lessThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B16:C16">
-    <cfRule type="cellIs" dxfId="10" priority="1" operator="lessThan">
+    <cfRule type="cellIs" dxfId="22" priority="1" operator="lessThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
@@ -15885,26 +15863,26 @@
   <sheetData>
     <row r="1" spans="1:18" ht="12.75">
       <c r="A1" s="25"/>
-      <c r="B1" s="280" t="s">
+      <c r="B1" s="286" t="s">
         <v>70</v>
       </c>
-      <c r="C1" s="251"/>
-      <c r="D1" s="280" t="s">
+      <c r="C1" s="271"/>
+      <c r="D1" s="286" t="s">
         <v>71</v>
       </c>
-      <c r="E1" s="251"/>
-      <c r="F1" s="280" t="s">
+      <c r="E1" s="271"/>
+      <c r="F1" s="286" t="s">
         <v>72</v>
       </c>
-      <c r="G1" s="251"/>
-      <c r="H1" s="280" t="s">
+      <c r="G1" s="271"/>
+      <c r="H1" s="286" t="s">
         <v>74</v>
       </c>
-      <c r="I1" s="251"/>
-      <c r="J1" s="282" t="s">
+      <c r="I1" s="271"/>
+      <c r="J1" s="288" t="s">
         <v>75</v>
       </c>
-      <c r="K1" s="283"/>
+      <c r="K1" s="289"/>
       <c r="L1" s="27"/>
       <c r="M1" s="27"/>
       <c r="N1" s="27"/>
@@ -16786,7 +16764,7 @@
     <mergeCell ref="J1:K1"/>
   </mergeCells>
   <conditionalFormatting sqref="A1:K16">
-    <cfRule type="cellIs" dxfId="9" priority="1" operator="lessThan">
+    <cfRule type="cellIs" dxfId="21" priority="1" operator="lessThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
@@ -16838,58 +16816,58 @@
   <sheetData>
     <row r="1" spans="1:29" s="149" customFormat="1" ht="15.75" customHeight="1">
       <c r="A1" s="152"/>
-      <c r="B1" s="284" t="s">
+      <c r="B1" s="290" t="s">
         <v>104</v>
       </c>
-      <c r="C1" s="285"/>
-      <c r="D1" s="284" t="s">
+      <c r="C1" s="291"/>
+      <c r="D1" s="290" t="s">
         <v>55</v>
       </c>
-      <c r="E1" s="285"/>
-      <c r="F1" s="284" t="s">
+      <c r="E1" s="291"/>
+      <c r="F1" s="290" t="s">
         <v>58</v>
       </c>
-      <c r="G1" s="285"/>
-      <c r="H1" s="284" t="s">
+      <c r="G1" s="291"/>
+      <c r="H1" s="290" t="s">
         <v>59</v>
       </c>
-      <c r="I1" s="285"/>
-      <c r="J1" s="284" t="s">
+      <c r="I1" s="291"/>
+      <c r="J1" s="290" t="s">
         <v>60</v>
       </c>
-      <c r="K1" s="285"/>
-      <c r="L1" s="284" t="s">
+      <c r="K1" s="291"/>
+      <c r="L1" s="290" t="s">
         <v>61</v>
       </c>
-      <c r="M1" s="285"/>
-      <c r="N1" s="284" t="s">
+      <c r="M1" s="291"/>
+      <c r="N1" s="290" t="s">
         <v>62</v>
       </c>
-      <c r="O1" s="285"/>
-      <c r="P1" s="284" t="s">
+      <c r="O1" s="291"/>
+      <c r="P1" s="290" t="s">
         <v>63</v>
       </c>
-      <c r="Q1" s="285"/>
-      <c r="R1" s="284" t="s">
+      <c r="Q1" s="291"/>
+      <c r="R1" s="290" t="s">
         <v>64</v>
       </c>
-      <c r="S1" s="285"/>
-      <c r="T1" s="284" t="s">
+      <c r="S1" s="291"/>
+      <c r="T1" s="290" t="s">
         <v>65</v>
       </c>
-      <c r="U1" s="285"/>
-      <c r="V1" s="284" t="s">
+      <c r="U1" s="291"/>
+      <c r="V1" s="290" t="s">
         <v>66</v>
       </c>
-      <c r="W1" s="285"/>
-      <c r="X1" s="284" t="s">
+      <c r="W1" s="291"/>
+      <c r="X1" s="290" t="s">
         <v>67</v>
       </c>
-      <c r="Y1" s="285"/>
-      <c r="Z1" s="284" t="s">
+      <c r="Y1" s="291"/>
+      <c r="Z1" s="290" t="s">
         <v>68</v>
       </c>
-      <c r="AA1" s="285"/>
+      <c r="AA1" s="291"/>
     </row>
     <row r="2" spans="1:29" ht="15.75" customHeight="1">
       <c r="A2" s="30" t="s">
@@ -18149,12 +18127,6 @@
     </row>
   </sheetData>
   <mergeCells count="13">
-    <mergeCell ref="X1:Y1"/>
-    <mergeCell ref="Z1:AA1"/>
-    <mergeCell ref="R1:S1"/>
-    <mergeCell ref="P1:Q1"/>
-    <mergeCell ref="V1:W1"/>
-    <mergeCell ref="T1:U1"/>
     <mergeCell ref="N1:O1"/>
     <mergeCell ref="J1:K1"/>
     <mergeCell ref="H1:I1"/>
@@ -18162,6 +18134,12 @@
     <mergeCell ref="B1:C1"/>
     <mergeCell ref="F1:G1"/>
     <mergeCell ref="L1:M1"/>
+    <mergeCell ref="X1:Y1"/>
+    <mergeCell ref="Z1:AA1"/>
+    <mergeCell ref="R1:S1"/>
+    <mergeCell ref="P1:Q1"/>
+    <mergeCell ref="V1:W1"/>
+    <mergeCell ref="T1:U1"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
@@ -18190,30 +18168,30 @@
   <sheetData>
     <row r="1" spans="1:20" ht="15.75" customHeight="1">
       <c r="A1" s="26"/>
-      <c r="B1" s="286" t="s">
+      <c r="B1" s="292" t="s">
         <v>73</v>
       </c>
-      <c r="C1" s="251"/>
-      <c r="D1" s="286" t="s">
+      <c r="C1" s="271"/>
+      <c r="D1" s="292" t="s">
         <v>70</v>
       </c>
-      <c r="E1" s="251"/>
-      <c r="F1" s="286" t="s">
+      <c r="E1" s="271"/>
+      <c r="F1" s="292" t="s">
         <v>71</v>
       </c>
-      <c r="G1" s="251"/>
-      <c r="H1" s="286" t="s">
+      <c r="G1" s="271"/>
+      <c r="H1" s="292" t="s">
         <v>72</v>
       </c>
-      <c r="I1" s="251"/>
-      <c r="J1" s="286" t="s">
+      <c r="I1" s="271"/>
+      <c r="J1" s="292" t="s">
         <v>74</v>
       </c>
-      <c r="K1" s="251"/>
-      <c r="L1" s="286" t="s">
+      <c r="K1" s="271"/>
+      <c r="L1" s="292" t="s">
         <v>75</v>
       </c>
-      <c r="M1" s="251"/>
+      <c r="M1" s="271"/>
       <c r="N1" s="28"/>
       <c r="O1" s="28"/>
       <c r="P1" s="28"/>

</xml_diff>

<commit_message>
se modifa la estructura de las imagenes , tablas para que esten acordes al formato icontec
</commit_message>
<xml_diff>
--- a/Analisis_financiero_Inclusoft_test.xlsx
+++ b/Analisis_financiero_Inclusoft_test.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="21570" windowHeight="8145" tabRatio="920" firstSheet="4" activeTab="9"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="21570" windowHeight="8145" tabRatio="920" firstSheet="4" activeTab="12"/>
   </bookViews>
   <sheets>
     <sheet name="Presupuesto Inicial" sheetId="1" r:id="rId1"/>
@@ -56,7 +56,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="500" uniqueCount="307">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="540" uniqueCount="307">
   <si>
     <t xml:space="preserve">Concepto
 </t>
@@ -1010,7 +1010,7 @@
     <numFmt numFmtId="173" formatCode="_-[$$-240A]\ * #,##0_-;\-[$$-240A]\ * #,##0_-;_-[$$-240A]\ * &quot;-&quot;??_-;_-@_-"/>
     <numFmt numFmtId="174" formatCode="0.0"/>
   </numFmts>
-  <fonts count="35">
+  <fonts count="37">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -1171,17 +1171,6 @@
       <name val="Libre Baskerville"/>
     </font>
     <font>
-      <sz val="10"/>
-      <color rgb="FF000000"/>
-      <name val="Libre Baskerville"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="10"/>
-      <color rgb="FF000000"/>
-      <name val="Libre Baskerville"/>
-    </font>
-    <font>
       <sz val="9"/>
       <name val="Libre Baskerville"/>
     </font>
@@ -1204,6 +1193,30 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="9"/>
+      <color rgb="FF000000"/>
+      <name val="Libre Baskerville"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="9"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <color rgb="FF000000"/>
+      <name val="Libre Baskerville"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="6">
@@ -1635,7 +1648,7 @@
     <xf numFmtId="43" fontId="17" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="26" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="316">
+  <cellXfs count="342">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1980,31 +1993,16 @@
     <xf numFmtId="164" fontId="7" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="28" fillId="3" borderId="13" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="27" fillId="3" borderId="30" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="165" fontId="22" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="164" fontId="22" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="4" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="28" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="28" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="9" fontId="22" fillId="0" borderId="0" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="31" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="165" fontId="29" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="164" fontId="29" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="32" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="165" fontId="30" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="164" fontId="30" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="32" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="165" fontId="30" fillId="0" borderId="28" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="164" fontId="30" fillId="0" borderId="28" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="165" fontId="22" fillId="0" borderId="28" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="164" fontId="22" fillId="0" borderId="28" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="30" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -2022,10 +2020,10 @@
     <xf numFmtId="170" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="33" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="31" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="167" fontId="33" fillId="0" borderId="13" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="167" fontId="31" fillId="0" borderId="13" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
@@ -2039,7 +2037,7 @@
     <xf numFmtId="170" fontId="13" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="34" fillId="4" borderId="12" xfId="3" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="32" fillId="4" borderId="12" xfId="3" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="170" fontId="7" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -2066,16 +2064,45 @@
     <xf numFmtId="43" fontId="12" fillId="0" borderId="13" xfId="5" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="10" fontId="0" fillId="0" borderId="28" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="19" fillId="4" borderId="12" xfId="3" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="170" fontId="19" fillId="4" borderId="12" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="3" borderId="11" xfId="2" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="167" fontId="19" fillId="4" borderId="12" xfId="3" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="20" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="167" fontId="0" fillId="0" borderId="14" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -2084,38 +2111,9 @@
     <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="167" fontId="19" fillId="4" borderId="12" xfId="3" applyNumberFormat="1" applyAlignment="1">
+    <xf numFmtId="170" fontId="19" fillId="4" borderId="12" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="3" borderId="11" xfId="2" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="19" fillId="4" borderId="12" xfId="3"/>
     <xf numFmtId="164" fontId="19" fillId="4" borderId="12" xfId="3" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -2161,26 +2159,17 @@
     <xf numFmtId="0" fontId="11" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="164" fontId="8" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="20" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="26" fillId="0" borderId="27" xfId="6" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="26" fillId="0" borderId="28" xfId="6" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="18" fillId="3" borderId="22" xfId="2" applyBorder="1" applyAlignment="1">
@@ -2190,12 +2179,6 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="18" fillId="3" borderId="23" xfId="2" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="19" fillId="4" borderId="19" xfId="3" applyBorder="1" applyAlignment="1">
@@ -2210,18 +2193,142 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="3" borderId="17" xfId="2" applyBorder="1"/>
-    <xf numFmtId="0" fontId="27" fillId="3" borderId="13" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="27" xfId="6" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="27" fillId="3" borderId="13" xfId="2" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="27" fillId="3" borderId="30" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="28" xfId="6" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="18" fillId="3" borderId="13" xfId="2" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="27" fillId="3" borderId="13" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="27" fillId="3" borderId="30" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="27" fillId="3" borderId="30" xfId="2" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="27" fillId="3" borderId="13" xfId="2" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="18" fillId="3" borderId="17" xfId="2" applyBorder="1"/>
+    <xf numFmtId="0" fontId="31" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="19" fillId="4" borderId="12" xfId="3" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="4" borderId="12" xfId="3" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="13" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="28" fillId="3" borderId="13" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="30" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="30" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="165" fontId="33" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="164" fontId="33" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="165" fontId="35" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="164" fontId="35" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="165" fontId="33" fillId="0" borderId="28" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="164" fontId="33" fillId="0" borderId="28" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="10" fontId="36" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="164" fontId="36" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="165" fontId="36" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="165" fontId="36" fillId="0" borderId="28" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="164" fontId="36" fillId="0" borderId="28" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="10" fontId="36" fillId="0" borderId="28" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="165" fontId="34" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="164" fontId="34" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="9" fontId="34" fillId="0" borderId="0" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="9" fontId="36" fillId="0" borderId="0" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="4" fontId="36" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="165" fontId="36" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="165" fontId="33" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="164" fontId="33" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="165" fontId="35" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="164" fontId="35" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="165" fontId="33" fillId="0" borderId="28" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="164" fontId="33" fillId="0" borderId="28" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="165" fontId="34" fillId="0" borderId="28" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="164" fontId="34" fillId="0" borderId="28" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
   </cellXfs>
   <cellStyles count="7">
     <cellStyle name="Celda de comprobación" xfId="3" builtinId="23"/>
@@ -2232,7 +2339,7 @@
     <cellStyle name="Salida" xfId="2" builtinId="21"/>
     <cellStyle name="Texto de advertencia" xfId="6" builtinId="11"/>
   </cellStyles>
-  <dxfs count="48">
+  <dxfs count="77">
     <dxf>
       <font>
         <color rgb="FFC53929"/>
@@ -2329,6 +2436,592 @@
         <right/>
         <top/>
         <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FFC53929"/>
+      </font>
+      <fill>
+        <patternFill patternType="none"/>
+      </fill>
+      <border>
+        <left/>
+        <right/>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FFC53929"/>
+      </font>
+      <fill>
+        <patternFill patternType="none"/>
+      </fill>
+      <border>
+        <left/>
+        <right/>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FFC53929"/>
+      </font>
+      <fill>
+        <patternFill patternType="none"/>
+      </fill>
+      <border>
+        <left/>
+        <right/>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FFC53929"/>
+      </font>
+      <fill>
+        <patternFill patternType="none"/>
+      </fill>
+      <border>
+        <left/>
+        <right/>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FFC53929"/>
+      </font>
+      <fill>
+        <patternFill patternType="none"/>
+      </fill>
+      <border>
+        <left/>
+        <right/>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FFC53929"/>
+      </font>
+      <fill>
+        <patternFill patternType="none"/>
+      </fill>
+      <border>
+        <left/>
+        <right/>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FFC53929"/>
+      </font>
+      <fill>
+        <patternFill patternType="none"/>
+      </fill>
+      <border>
+        <left/>
+        <right/>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <fgColor theme="1"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FFC53929"/>
+      </font>
+      <fill>
+        <patternFill patternType="none"/>
+      </fill>
+      <border>
+        <left/>
+        <right/>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FFC53929"/>
+      </font>
+      <fill>
+        <patternFill patternType="none"/>
+      </fill>
+      <border>
+        <left/>
+        <right/>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <name val="Arial"/>
+        <scheme val="none"/>
+      </font>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <alignment vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right/>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="10"/>
+        <color rgb="FFFF0000"/>
+        <name val="Arial"/>
+        <scheme val="none"/>
+      </font>
+      <numFmt numFmtId="167" formatCode="[$$-240A]\ #,##0"/>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="167" formatCode="[$$-240A]\ #,##0"/>
+      <alignment vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="10"/>
+        <color rgb="FFFF0000"/>
+        <name val="Arial"/>
+        <scheme val="none"/>
+      </font>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="167" formatCode="[$$-240A]\ #,##0"/>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <name val="Arial"/>
+        <scheme val="none"/>
+      </font>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <alignment vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <name val="Arial"/>
+        <scheme val="none"/>
+      </font>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <alignment vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <name val="Arial"/>
+        <scheme val="none"/>
+      </font>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <alignment vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <name val="Arial"/>
+        <scheme val="none"/>
+      </font>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <alignment vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <alignment vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
       </border>
     </dxf>
     <dxf>
@@ -2534,114 +3227,6 @@
         <scheme val="none"/>
       </font>
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FFC53929"/>
-      </font>
-      <fill>
-        <patternFill patternType="none"/>
-      </fill>
-      <border>
-        <left/>
-        <right/>
-        <top/>
-        <bottom/>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FFC53929"/>
-      </font>
-      <fill>
-        <patternFill patternType="none"/>
-      </fill>
-      <border>
-        <left/>
-        <right/>
-        <top/>
-        <bottom/>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FFC53929"/>
-      </font>
-      <fill>
-        <patternFill patternType="none"/>
-      </fill>
-      <border>
-        <left/>
-        <right/>
-        <top/>
-        <bottom/>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <fgColor theme="1"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FFC53929"/>
-      </font>
-      <fill>
-        <patternFill patternType="none"/>
-      </fill>
-      <border>
-        <left/>
-        <right/>
-        <top/>
-        <bottom/>
-      </border>
     </dxf>
     <dxf>
       <font>
@@ -3097,6 +3682,7 @@
           </a:p>
         </c:rich>
       </c:tx>
+      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -3248,11 +3834,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="303801208"/>
-        <c:axId val="303800424"/>
+        <c:axId val="297345888"/>
+        <c:axId val="297341184"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="303801208"/>
+        <c:axId val="297345888"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3284,6 +3870,7 @@
               </a:p>
             </c:rich>
           </c:tx>
+          <c:layout/>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -3350,7 +3937,7 @@
             <a:endParaRPr lang="es-ES"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="303800424"/>
+        <c:crossAx val="297341184"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -3358,7 +3945,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="303800424"/>
+        <c:axId val="297341184"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3404,6 +3991,7 @@
               </a:p>
             </c:rich>
           </c:tx>
+          <c:layout/>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -3464,7 +4052,7 @@
             <a:endParaRPr lang="es-ES"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="303801208"/>
+        <c:crossAx val="297345888"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -3478,6 +4066,7 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
+      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -3589,6 +4178,7 @@
           </a:p>
         </c:rich>
       </c:tx>
+      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -3740,11 +4330,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="303801600"/>
-        <c:axId val="303801992"/>
+        <c:axId val="297341968"/>
+        <c:axId val="297346280"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="303801600"/>
+        <c:axId val="297341968"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3776,6 +4366,7 @@
               </a:p>
             </c:rich>
           </c:tx>
+          <c:layout/>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -3842,7 +4433,7 @@
             <a:endParaRPr lang="es-ES"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="303801992"/>
+        <c:crossAx val="297346280"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -3850,7 +4441,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="303801992"/>
+        <c:axId val="297346280"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3896,6 +4487,7 @@
               </a:p>
             </c:rich>
           </c:tx>
+          <c:layout/>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -3956,7 +4548,7 @@
             <a:endParaRPr lang="es-ES"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="303801600"/>
+        <c:crossAx val="297341968"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -3970,6 +4562,7 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
+      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -4234,8 +4827,8 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="303803560"/>
-        <c:axId val="303800032"/>
+        <c:axId val="297346672"/>
+        <c:axId val="297342752"/>
         <c:extLst>
           <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
             <c15:filteredBarSeries>
@@ -4323,7 +4916,7 @@
         </c:extLst>
       </c:barChart>
       <c:catAx>
-        <c:axId val="303803560"/>
+        <c:axId val="297346672"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4422,7 +5015,7 @@
             <a:endParaRPr lang="es-ES"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="303800032"/>
+        <c:crossAx val="297342752"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -4430,7 +5023,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="303800032"/>
+        <c:axId val="297342752"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4544,7 +5137,7 @@
             <a:endParaRPr lang="es-ES"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="303803560"/>
+        <c:crossAx val="297346672"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -4993,11 +5586,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="306162792"/>
-        <c:axId val="306166712"/>
+        <c:axId val="297340792"/>
+        <c:axId val="297343536"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="306162792"/>
+        <c:axId val="297340792"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -5112,7 +5705,7 @@
             <a:endParaRPr lang="es-ES"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="306166712"/>
+        <c:crossAx val="297343536"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -5120,7 +5713,7 @@
         <c:noMultiLvlLbl val="1"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="306166712"/>
+        <c:axId val="297343536"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -5221,7 +5814,7 @@
             <a:endParaRPr lang="es-ES"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="306162792"/>
+        <c:crossAx val="297340792"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -7834,29 +8427,47 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="PUBLICIDAD" displayName="PUBLICIDAD" ref="A36:H43" totalsRowCount="1" headerRowDxfId="47" totalsRowDxfId="46" headerRowCellStyle="Celda de comprobación">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="PUBLICIDAD" displayName="PUBLICIDAD" ref="A36:H43" totalsRowCount="1" headerRowDxfId="76" totalsRowDxfId="75" headerRowCellStyle="Celda de comprobación">
   <tableColumns count="8">
-    <tableColumn id="1" name="Promoción" dataDxfId="45"/>
-    <tableColumn id="2" name="Tiempo aproximado de duración" dataDxfId="44" totalsRowDxfId="43"/>
-    <tableColumn id="3" name="Objetivo " dataDxfId="42" totalsRowDxfId="41"/>
-    <tableColumn id="4" name="Cantidad" dataDxfId="40" totalsRowDxfId="39"/>
-    <tableColumn id="5" name="Se requieren" dataDxfId="38" totalsRowDxfId="37"/>
-    <tableColumn id="6" name="Costo Unitario" totalsRowLabel="Total anual" dataDxfId="36" totalsRowDxfId="35" dataCellStyle="Moneda"/>
-    <tableColumn id="7" name="Costo total" totalsRowFunction="sum" dataDxfId="34" totalsRowDxfId="33" dataCellStyle="Moneda">
+    <tableColumn id="1" name="Promoción" dataDxfId="74"/>
+    <tableColumn id="2" name="Tiempo aproximado de duración" dataDxfId="73" totalsRowDxfId="72"/>
+    <tableColumn id="3" name="Objetivo " dataDxfId="71" totalsRowDxfId="70"/>
+    <tableColumn id="4" name="Cantidad" dataDxfId="69" totalsRowDxfId="68"/>
+    <tableColumn id="5" name="Se requieren" dataDxfId="67" totalsRowDxfId="66"/>
+    <tableColumn id="6" name="Costo Unitario" totalsRowLabel="Total anual" dataDxfId="65" totalsRowDxfId="64" dataCellStyle="Moneda"/>
+    <tableColumn id="7" name="Costo total" totalsRowFunction="sum" dataDxfId="63" totalsRowDxfId="62" dataCellStyle="Moneda">
       <calculatedColumnFormula>F37*E37</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="8" name="Proveedor" dataDxfId="32" totalsRowDxfId="31"/>
+    <tableColumn id="8" name="Proveedor" dataDxfId="61" totalsRowDxfId="60"/>
   </tableColumns>
   <tableStyleInfo showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="Tabla3" displayName="Tabla3" ref="A21:G23" totalsRowShown="0" headerRowDxfId="18">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="9" name="PUBLICIDAD10" displayName="PUBLICIDAD10" ref="AX163:BE170" totalsRowCount="1" headerRowDxfId="29" dataDxfId="30" totalsRowDxfId="31" headerRowCellStyle="Celda de comprobación">
+  <tableColumns count="8">
+    <tableColumn id="1" name="Promoción" dataDxfId="47" totalsRowDxfId="46"/>
+    <tableColumn id="2" name="Tiempo aproximado de duración" dataDxfId="45" totalsRowDxfId="44"/>
+    <tableColumn id="3" name="Objetivo " dataDxfId="43" totalsRowDxfId="42"/>
+    <tableColumn id="4" name="Cantidad" dataDxfId="41" totalsRowDxfId="40"/>
+    <tableColumn id="5" name="Se requieren" dataDxfId="39" totalsRowDxfId="38"/>
+    <tableColumn id="6" name="Costo Unitario" totalsRowLabel="Total anual" dataDxfId="37" totalsRowDxfId="36" dataCellStyle="Moneda"/>
+    <tableColumn id="7" name="Costo total" totalsRowFunction="sum" dataDxfId="35" totalsRowDxfId="34" dataCellStyle="Moneda">
+      <calculatedColumnFormula>BC164*BB164</calculatedColumnFormula>
+    </tableColumn>
+    <tableColumn id="8" name="Proveedor" dataDxfId="33" totalsRowDxfId="32"/>
+  </tableColumns>
+  <tableStyleInfo showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="Tabla3" displayName="Tabla3" ref="A21:G23" totalsRowShown="0" headerRowDxfId="59">
   <autoFilter ref="A21:G23"/>
   <tableColumns count="7">
     <tableColumn id="1" name="Columna1"/>
-    <tableColumn id="2" name="Columna2" dataDxfId="17"/>
+    <tableColumn id="2" name="Columna2" dataDxfId="58"/>
     <tableColumn id="3" name="Columna3">
       <calculatedColumnFormula>'Flujo de Caja (Profesor) - 5 añ'!D18</calculatedColumnFormula>
     </tableColumn>
@@ -7877,11 +8488,11 @@
 </table>
 </file>
 
-<file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="5" name="Tabla5" displayName="Tabla5" ref="A31:B34" totalsRowShown="0">
   <autoFilter ref="A31:B34"/>
   <tableColumns count="2">
-    <tableColumn id="1" name="Columna1" dataDxfId="16"/>
+    <tableColumn id="1" name="Columna1" dataDxfId="57"/>
     <tableColumn id="2" name="Columna2">
       <calculatedColumnFormula>B31*2</calculatedColumnFormula>
     </tableColumn>
@@ -7890,36 +8501,36 @@
 </table>
 </file>
 
-<file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/tables/table5.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="6" name="Tabla6" displayName="Tabla6" ref="A36:B41" totalsRowShown="0">
   <autoFilter ref="A36:B41"/>
   <tableColumns count="2">
-    <tableColumn id="1" name="Columna1" dataDxfId="15"/>
-    <tableColumn id="2" name="Columna2" dataDxfId="14"/>
-  </tableColumns>
-  <tableStyleInfo name="TableStyleMedium16" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
-</table>
-</file>
-
-<file path=xl/tables/table5.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="4" name="Tabla4" displayName="Tabla4" ref="A25:C28" totalsRowShown="0">
-  <autoFilter ref="A25:C28"/>
-  <tableColumns count="3">
-    <tableColumn id="1" name="Columna1" dataDxfId="13"/>
-    <tableColumn id="2" name="Columna2" dataDxfId="12"/>
-    <tableColumn id="3" name="Columna3" dataDxfId="11"/>
+    <tableColumn id="1" name="Columna1" dataDxfId="56"/>
+    <tableColumn id="2" name="Columna2" dataDxfId="55"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium16" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table6.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="4" name="Tabla4" displayName="Tabla4" ref="A25:C28" totalsRowShown="0">
+  <autoFilter ref="A25:C28"/>
+  <tableColumns count="3">
+    <tableColumn id="1" name="Columna1" dataDxfId="54"/>
+    <tableColumn id="2" name="Columna2" dataDxfId="53"/>
+    <tableColumn id="3" name="Columna3" dataDxfId="52"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium16" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table7.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Tabla2" displayName="Tabla2" ref="A45:C51" totalsRowShown="0">
   <autoFilter ref="A45:C51"/>
   <tableColumns count="3">
-    <tableColumn id="1" name="Columna1" dataDxfId="10"/>
-    <tableColumn id="2" name="Columna2" dataDxfId="9" dataCellStyle="Porcentaje"/>
-    <tableColumn id="3" name="Columna3" dataDxfId="8" dataCellStyle="Porcentaje">
+    <tableColumn id="1" name="Columna1" dataDxfId="51"/>
+    <tableColumn id="2" name="Columna2" dataDxfId="50" dataCellStyle="Porcentaje"/>
+    <tableColumn id="3" name="Columna3" dataDxfId="49" dataCellStyle="Porcentaje">
       <calculatedColumnFormula xml:space="preserve"> 1 +B46</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -7927,11 +8538,11 @@
 </table>
 </file>
 
-<file path=xl/tables/table7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/tables/table8.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="7" name="Tabla7" displayName="Tabla7" ref="G9:J11" totalsRowShown="0">
   <autoFilter ref="G9:J11"/>
   <tableColumns count="4">
-    <tableColumn id="1" name="CONCEPTO" dataDxfId="7"/>
+    <tableColumn id="1" name="CONCEPTO" dataDxfId="48"/>
     <tableColumn id="2" name="Columna2"/>
     <tableColumn id="3" name="-"/>
     <tableColumn id="4" name="VALOR"/>
@@ -8333,10 +8944,10 @@
         <v>60800</v>
       </c>
       <c r="C11" s="4"/>
-      <c r="L11" s="245" t="s">
+      <c r="L11" s="230" t="s">
         <v>303</v>
       </c>
-      <c r="M11" s="245" t="s">
+      <c r="M11" s="230" t="s">
         <v>1</v>
       </c>
     </row>
@@ -8347,10 +8958,10 @@
       <c r="B12" s="118">
         <v>3000000</v>
       </c>
-      <c r="L12" s="238" t="s">
+      <c r="L12" s="223" t="s">
         <v>167</v>
       </c>
-      <c r="M12" s="240">
+      <c r="M12" s="225">
         <v>3000000</v>
       </c>
     </row>
@@ -8362,10 +8973,10 @@
         <v>500000</v>
       </c>
       <c r="C13" s="4"/>
-      <c r="L13" s="239" t="s">
+      <c r="L13" s="224" t="s">
         <v>56</v>
       </c>
-      <c r="M13" s="240">
+      <c r="M13" s="225">
         <v>500000</v>
       </c>
     </row>
@@ -8378,10 +8989,10 @@
         <v>332010</v>
       </c>
       <c r="C14" s="3"/>
-      <c r="L14" s="241" t="s">
+      <c r="L14" s="226" t="s">
         <v>210</v>
       </c>
-      <c r="M14" s="242">
+      <c r="M14" s="227">
         <f>SUM(M12:M13)</f>
         <v>3500000</v>
       </c>
@@ -8394,10 +9005,10 @@
         <f>B10+B2</f>
         <v>4009510</v>
       </c>
-      <c r="L15" s="243" t="s">
+      <c r="L15" s="228" t="s">
         <v>301</v>
       </c>
-      <c r="M15" s="242">
+      <c r="M15" s="227">
         <f>J17</f>
         <v>58333.333333333336</v>
       </c>
@@ -8418,10 +9029,10 @@
       <c r="J16" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="L16" s="244" t="s">
+      <c r="L16" s="229" t="s">
         <v>302</v>
       </c>
-      <c r="M16" s="232">
+      <c r="M16" s="217">
         <f>M15*12</f>
         <v>700000</v>
       </c>
@@ -8579,7 +9190,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:S31"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+    <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
       <selection activeCell="B21" sqref="B21"/>
     </sheetView>
   </sheetViews>
@@ -8604,26 +9215,26 @@
       <c r="B1" s="200" t="s">
         <v>73</v>
       </c>
-      <c r="C1" s="287" t="s">
+      <c r="C1" s="272" t="s">
         <v>70</v>
       </c>
-      <c r="D1" s="271"/>
-      <c r="E1" s="286" t="s">
+      <c r="D1" s="242"/>
+      <c r="E1" s="271" t="s">
         <v>71</v>
       </c>
-      <c r="F1" s="271"/>
-      <c r="G1" s="286" t="s">
+      <c r="F1" s="242"/>
+      <c r="G1" s="271" t="s">
         <v>72</v>
       </c>
-      <c r="H1" s="271"/>
-      <c r="I1" s="286" t="s">
+      <c r="H1" s="242"/>
+      <c r="I1" s="271" t="s">
         <v>74</v>
       </c>
-      <c r="J1" s="271"/>
-      <c r="K1" s="288" t="s">
+      <c r="J1" s="242"/>
+      <c r="K1" s="273" t="s">
         <v>75</v>
       </c>
-      <c r="L1" s="295"/>
+      <c r="L1" s="278"/>
       <c r="M1" s="27"/>
       <c r="N1" s="27"/>
       <c r="O1" s="27"/>
@@ -8832,10 +9443,10 @@
         <f>D5+F5+H5+J5+L5</f>
         <v>3842803.2126632677</v>
       </c>
-      <c r="O5" s="293" t="s">
+      <c r="O5" s="279" t="s">
         <v>280</v>
       </c>
-      <c r="P5" s="293"/>
+      <c r="P5" s="279"/>
       <c r="Q5" s="52"/>
       <c r="R5" s="52"/>
       <c r="S5" s="52"/>
@@ -8887,10 +9498,10 @@
       </c>
       <c r="M6" s="52"/>
       <c r="N6" s="52"/>
-      <c r="O6" s="293" t="s">
+      <c r="O6" s="279" t="s">
         <v>285</v>
       </c>
-      <c r="P6" s="293"/>
+      <c r="P6" s="279"/>
       <c r="Q6" s="52"/>
       <c r="R6" s="52"/>
       <c r="S6" s="52"/>
@@ -8942,10 +9553,10 @@
       </c>
       <c r="M7" s="52"/>
       <c r="N7" s="52"/>
-      <c r="O7" s="293" t="s">
+      <c r="O7" s="279" t="s">
         <v>286</v>
       </c>
-      <c r="P7" s="293"/>
+      <c r="P7" s="279"/>
       <c r="Q7" s="52"/>
       <c r="R7" s="52"/>
       <c r="S7" s="52"/>
@@ -8997,8 +9608,8 @@
       </c>
       <c r="M8" s="55"/>
       <c r="N8" s="44"/>
-      <c r="O8" s="294"/>
-      <c r="P8" s="294"/>
+      <c r="O8" s="280"/>
+      <c r="P8" s="280"/>
       <c r="Q8" s="44"/>
       <c r="R8" s="44"/>
       <c r="S8" s="44"/>
@@ -9050,10 +9661,10 @@
       </c>
       <c r="M9" s="52"/>
       <c r="N9" s="52"/>
-      <c r="O9" s="293" t="s">
+      <c r="O9" s="279" t="s">
         <v>11</v>
       </c>
-      <c r="P9" s="293"/>
+      <c r="P9" s="279"/>
       <c r="Q9" s="52"/>
       <c r="R9" s="52"/>
       <c r="S9" s="52"/>
@@ -9105,10 +9716,10 @@
       </c>
       <c r="M10" s="52"/>
       <c r="N10" s="52"/>
-      <c r="O10" s="293" t="s">
+      <c r="O10" s="279" t="s">
         <v>248</v>
       </c>
-      <c r="P10" s="293"/>
+      <c r="P10" s="279"/>
       <c r="Q10" s="52"/>
       <c r="R10" s="52"/>
       <c r="S10" s="52"/>
@@ -9678,25 +10289,25 @@
     </row>
   </sheetData>
   <mergeCells count="11">
-    <mergeCell ref="E1:F1"/>
-    <mergeCell ref="C1:D1"/>
-    <mergeCell ref="G1:H1"/>
-    <mergeCell ref="I1:J1"/>
-    <mergeCell ref="K1:L1"/>
     <mergeCell ref="O5:P5"/>
     <mergeCell ref="O6:P6"/>
     <mergeCell ref="O9:P9"/>
     <mergeCell ref="O10:P10"/>
     <mergeCell ref="O7:P7"/>
     <mergeCell ref="O8:P8"/>
+    <mergeCell ref="E1:F1"/>
+    <mergeCell ref="C1:D1"/>
+    <mergeCell ref="G1:H1"/>
+    <mergeCell ref="I1:J1"/>
+    <mergeCell ref="K1:L1"/>
   </mergeCells>
   <conditionalFormatting sqref="A1:B16 C1:C19 D1:D16 E1:E19 F1:F16 G1:G19 H1:H16 I6:I19 J6:J16 K6:K19 L6:L16 I1:L5">
-    <cfRule type="cellIs" dxfId="20" priority="1" operator="lessThan">
+    <cfRule type="cellIs" dxfId="12" priority="1" operator="lessThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B17:L19">
-    <cfRule type="cellIs" dxfId="19" priority="2" operator="lessThan">
+    <cfRule type="cellIs" dxfId="11" priority="2" operator="lessThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
@@ -9709,7 +10320,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M66"/>
   <sheetViews>
-    <sheetView topLeftCell="A16" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+    <sheetView topLeftCell="A7" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <selection activeCell="J10" sqref="J10"/>
     </sheetView>
   </sheetViews>
@@ -10769,30 +11380,30 @@
   <sheetData>
     <row r="1" spans="2:8" ht="13.5" thickBot="1"/>
     <row r="2" spans="2:8" ht="15.75" thickBot="1">
-      <c r="B2" s="306" t="s">
+      <c r="B2" s="286" t="s">
         <v>281</v>
       </c>
-      <c r="C2" s="307"/>
-      <c r="D2" s="307"/>
-      <c r="E2" s="307"/>
-      <c r="F2" s="307"/>
-      <c r="G2" s="307"/>
-      <c r="H2" s="308"/>
+      <c r="C2" s="287"/>
+      <c r="D2" s="287"/>
+      <c r="E2" s="287"/>
+      <c r="F2" s="287"/>
+      <c r="G2" s="287"/>
+      <c r="H2" s="288"/>
     </row>
     <row r="3" spans="2:8" ht="15.75" thickTop="1">
-      <c r="B3" s="301" t="s">
+      <c r="B3" s="283" t="s">
         <v>287</v>
       </c>
-      <c r="C3" s="302"/>
-      <c r="D3" s="302"/>
-      <c r="E3" s="302"/>
-      <c r="F3" s="302"/>
-      <c r="G3" s="302"/>
-      <c r="H3" s="303"/>
+      <c r="C3" s="284"/>
+      <c r="D3" s="284"/>
+      <c r="E3" s="284"/>
+      <c r="F3" s="284"/>
+      <c r="G3" s="284"/>
+      <c r="H3" s="285"/>
     </row>
     <row r="4" spans="2:8">
-      <c r="B4" s="309"/>
-      <c r="C4" s="297"/>
+      <c r="B4" s="289"/>
+      <c r="C4" s="282"/>
       <c r="D4" s="179" t="s">
         <v>70</v>
       </c>
@@ -10810,10 +11421,10 @@
       </c>
     </row>
     <row r="5" spans="2:8">
-      <c r="B5" s="296" t="s">
+      <c r="B5" s="281" t="s">
         <v>118</v>
       </c>
-      <c r="C5" s="297"/>
+      <c r="C5" s="282"/>
       <c r="D5" s="182">
         <f>'Flujo de Caja (Profesor) - 5 añ'!D6+'Flujo de Caja (Profesor) - 5 añ'!D7</f>
         <v>111254717.93098715</v>
@@ -10836,10 +11447,10 @@
       </c>
     </row>
     <row r="6" spans="2:8">
-      <c r="B6" s="296" t="s">
+      <c r="B6" s="281" t="s">
         <v>282</v>
       </c>
-      <c r="C6" s="297"/>
+      <c r="C6" s="282"/>
       <c r="D6" s="182">
         <f>'Flujo de Caja (Profesor) - 5 añ'!D3</f>
         <v>199937934.20591292</v>
@@ -10862,10 +11473,10 @@
       </c>
     </row>
     <row r="7" spans="2:8">
-      <c r="B7" s="296" t="s">
+      <c r="B7" s="281" t="s">
         <v>283</v>
       </c>
-      <c r="C7" s="297"/>
+      <c r="C7" s="282"/>
       <c r="D7" s="182">
         <f>'Flujo de Caja (Profesor) - 5 añ'!D10</f>
         <v>4285000.1176767461</v>
@@ -10888,10 +11499,10 @@
       </c>
     </row>
     <row r="8" spans="2:8">
-      <c r="B8" s="296" t="s">
+      <c r="B8" s="281" t="s">
         <v>291</v>
       </c>
-      <c r="C8" s="300"/>
+      <c r="C8" s="292"/>
       <c r="D8" s="182">
         <f>D5+D7</f>
         <v>115539718.0486639</v>
@@ -10914,10 +11525,10 @@
       </c>
     </row>
     <row r="9" spans="2:8">
-      <c r="B9" s="296" t="s">
+      <c r="B9" s="281" t="s">
         <v>284</v>
       </c>
-      <c r="C9" s="297"/>
+      <c r="C9" s="282"/>
       <c r="D9" s="184">
         <f>D5/(D6-D7)</f>
         <v>0.56863301564807167</v>
@@ -10940,19 +11551,19 @@
       </c>
     </row>
     <row r="10" spans="2:8" ht="15">
-      <c r="B10" s="301" t="s">
+      <c r="B10" s="283" t="s">
         <v>288</v>
       </c>
-      <c r="C10" s="302"/>
-      <c r="D10" s="302"/>
-      <c r="E10" s="302"/>
-      <c r="F10" s="302"/>
-      <c r="G10" s="302"/>
-      <c r="H10" s="303"/>
+      <c r="C10" s="284"/>
+      <c r="D10" s="284"/>
+      <c r="E10" s="284"/>
+      <c r="F10" s="284"/>
+      <c r="G10" s="284"/>
+      <c r="H10" s="285"/>
     </row>
     <row r="11" spans="2:8">
-      <c r="B11" s="304"/>
-      <c r="C11" s="305"/>
+      <c r="B11" s="293"/>
+      <c r="C11" s="294"/>
       <c r="D11" s="181" t="s">
         <v>70</v>
       </c>
@@ -10970,10 +11581,10 @@
       </c>
     </row>
     <row r="12" spans="2:8">
-      <c r="B12" s="296" t="s">
+      <c r="B12" s="281" t="s">
         <v>118</v>
       </c>
-      <c r="C12" s="297"/>
+      <c r="C12" s="282"/>
       <c r="D12" s="182">
         <f>'Flujo de Caja (Profesor) - 5 añ'!D11+'Flujo de Caja (Profesor) - 5 añ'!D12</f>
         <v>79684496.075435549</v>
@@ -10996,10 +11607,10 @@
       </c>
     </row>
     <row r="13" spans="2:8">
-      <c r="B13" s="296" t="s">
+      <c r="B13" s="281" t="s">
         <v>289</v>
       </c>
-      <c r="C13" s="297"/>
+      <c r="C13" s="282"/>
       <c r="D13" s="187">
         <v>5000</v>
       </c>
@@ -11017,10 +11628,10 @@
       </c>
     </row>
     <row r="14" spans="2:8">
-      <c r="B14" s="296" t="s">
+      <c r="B14" s="281" t="s">
         <v>290</v>
       </c>
-      <c r="C14" s="297"/>
+      <c r="C14" s="282"/>
       <c r="D14" s="187">
         <f>('Flujo de Caja (Profesor) - 5 añ'!D6+'Flujo de Caja (Profesor) - 5 añ'!D7)/'Tabla Crecimiento'!B9</f>
         <v>11103.815193643957</v>
@@ -11043,10 +11654,10 @@
       </c>
     </row>
     <row r="15" spans="2:8" ht="15.75" thickBot="1">
-      <c r="B15" s="298" t="s">
+      <c r="B15" s="290" t="s">
         <v>288</v>
       </c>
-      <c r="C15" s="299"/>
+      <c r="C15" s="291"/>
       <c r="D15" s="189">
         <f>D12/D13-D14</f>
         <v>4833.0840214431519</v>
@@ -11082,45 +11693,39 @@
       <c r="N23" s="93"/>
     </row>
     <row r="24" spans="2:14">
-      <c r="B24" s="259"/>
-      <c r="C24" s="264"/>
+      <c r="B24" s="254"/>
+      <c r="C24" s="255"/>
     </row>
     <row r="25" spans="2:14">
-      <c r="B25" s="259"/>
-      <c r="C25" s="264"/>
+      <c r="B25" s="254"/>
+      <c r="C25" s="255"/>
     </row>
     <row r="26" spans="2:14">
-      <c r="B26" s="259"/>
-      <c r="C26" s="264"/>
+      <c r="B26" s="254"/>
+      <c r="C26" s="255"/>
     </row>
     <row r="27" spans="2:14">
-      <c r="B27" s="259"/>
-      <c r="C27" s="259"/>
+      <c r="B27" s="254"/>
+      <c r="C27" s="254"/>
     </row>
     <row r="28" spans="2:14">
-      <c r="B28" s="259"/>
-      <c r="C28" s="264"/>
+      <c r="B28" s="254"/>
+      <c r="C28" s="255"/>
     </row>
     <row r="30" spans="2:14">
-      <c r="B30" s="259"/>
-      <c r="C30" s="264"/>
+      <c r="B30" s="254"/>
+      <c r="C30" s="255"/>
     </row>
     <row r="31" spans="2:14">
-      <c r="B31" s="259"/>
-      <c r="C31" s="264"/>
+      <c r="B31" s="254"/>
+      <c r="C31" s="255"/>
     </row>
     <row r="32" spans="2:14">
-      <c r="B32" s="259"/>
-      <c r="C32" s="264"/>
+      <c r="B32" s="254"/>
+      <c r="C32" s="255"/>
     </row>
   </sheetData>
   <mergeCells count="22">
-    <mergeCell ref="B7:C7"/>
-    <mergeCell ref="B3:H3"/>
-    <mergeCell ref="B2:H2"/>
-    <mergeCell ref="B5:C5"/>
-    <mergeCell ref="B4:C4"/>
-    <mergeCell ref="B6:C6"/>
     <mergeCell ref="B32:C32"/>
     <mergeCell ref="B13:C13"/>
     <mergeCell ref="B14:C14"/>
@@ -11137,6 +11742,12 @@
     <mergeCell ref="B28:C28"/>
     <mergeCell ref="B30:C30"/>
     <mergeCell ref="B31:C31"/>
+    <mergeCell ref="B7:C7"/>
+    <mergeCell ref="B3:H3"/>
+    <mergeCell ref="B2:H2"/>
+    <mergeCell ref="B5:C5"/>
+    <mergeCell ref="B4:C4"/>
+    <mergeCell ref="B6:C6"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -11146,8 +11757,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AA19"/>
   <sheetViews>
-    <sheetView topLeftCell="H1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="X23" sqref="X23"/>
+    <sheetView tabSelected="1" topLeftCell="H1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="U11" sqref="U11:AA19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1"/>
@@ -11162,63 +11773,63 @@
     <col min="9" max="9" width="14.28515625" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="9" customWidth="1"/>
     <col min="11" max="11" width="14.28515625" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="27" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="7" customWidth="1"/>
-    <col min="15" max="15" width="14.7109375" customWidth="1"/>
-    <col min="16" max="16" width="7" customWidth="1"/>
-    <col min="17" max="17" width="14.7109375" customWidth="1"/>
+    <col min="13" max="13" width="15.28515625" customWidth="1"/>
+    <col min="14" max="14" width="6.7109375" hidden="1" customWidth="1"/>
+    <col min="15" max="15" width="14.28515625" hidden="1" customWidth="1"/>
+    <col min="16" max="16" width="6.7109375" hidden="1" customWidth="1"/>
+    <col min="17" max="17" width="14.28515625" hidden="1" customWidth="1"/>
     <col min="18" max="18" width="7" customWidth="1"/>
     <col min="19" max="19" width="14.7109375" customWidth="1"/>
     <col min="20" max="20" width="5.7109375" customWidth="1"/>
-    <col min="21" max="21" width="35.7109375" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="8.28515625" customWidth="1"/>
-    <col min="23" max="23" width="14.7109375" customWidth="1"/>
-    <col min="24" max="24" width="7.28515625" customWidth="1"/>
-    <col min="25" max="25" width="14.7109375" customWidth="1"/>
+    <col min="21" max="21" width="17.7109375" customWidth="1"/>
+    <col min="22" max="22" width="7.28515625" hidden="1" customWidth="1"/>
+    <col min="23" max="23" width="14.7109375" hidden="1" customWidth="1"/>
+    <col min="24" max="24" width="7.28515625" hidden="1" customWidth="1"/>
+    <col min="25" max="25" width="14.7109375" hidden="1" customWidth="1"/>
     <col min="26" max="26" width="7.28515625" customWidth="1"/>
     <col min="27" max="27" width="14.7109375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:27" ht="15.75" customHeight="1">
       <c r="A1" s="152"/>
-      <c r="B1" s="290" t="s">
+      <c r="B1" s="275" t="s">
         <v>70</v>
       </c>
-      <c r="C1" s="291"/>
-      <c r="D1" s="290" t="s">
+      <c r="C1" s="276"/>
+      <c r="D1" s="275" t="s">
         <v>71</v>
       </c>
-      <c r="E1" s="291"/>
-      <c r="F1" s="290" t="s">
+      <c r="E1" s="276"/>
+      <c r="F1" s="275" t="s">
         <v>72</v>
       </c>
-      <c r="G1" s="291"/>
-      <c r="H1" s="290" t="s">
+      <c r="G1" s="276"/>
+      <c r="H1" s="275" t="s">
         <v>74</v>
       </c>
-      <c r="I1" s="291"/>
-      <c r="J1" s="302" t="s">
+      <c r="I1" s="276"/>
+      <c r="J1" s="284" t="s">
         <v>75</v>
       </c>
-      <c r="K1" s="310"/>
+      <c r="K1" s="300"/>
       <c r="M1" s="193"/>
-      <c r="N1" s="311" t="s">
+      <c r="N1" s="296" t="s">
         <v>70</v>
       </c>
-      <c r="O1" s="312"/>
-      <c r="P1" s="311" t="s">
+      <c r="O1" s="299"/>
+      <c r="P1" s="296" t="s">
         <v>71</v>
       </c>
-      <c r="Q1" s="312"/>
+      <c r="Q1" s="299"/>
       <c r="U1" s="194"/>
-      <c r="V1" s="311" t="s">
+      <c r="V1" s="296" t="s">
         <v>70</v>
       </c>
-      <c r="W1" s="311"/>
-      <c r="X1" s="311" t="s">
+      <c r="W1" s="296"/>
+      <c r="X1" s="296" t="s">
         <v>71</v>
       </c>
-      <c r="Y1" s="311"/>
+      <c r="Y1" s="296"/>
     </row>
     <row r="2" spans="1:27" ht="15.75" customHeight="1">
       <c r="A2" s="30" t="s">
@@ -11264,22 +11875,22 @@
         <f>SUM(K4,K8)</f>
         <v>656309430.34961951</v>
       </c>
-      <c r="M2" s="203" t="s">
+      <c r="M2" s="308" t="s">
         <v>137</v>
       </c>
-      <c r="N2" s="311"/>
-      <c r="O2" s="311"/>
-      <c r="P2" s="311"/>
-      <c r="Q2" s="311"/>
+      <c r="N2" s="296"/>
+      <c r="O2" s="296"/>
+      <c r="P2" s="296"/>
+      <c r="Q2" s="296"/>
       <c r="U2" s="195" t="s">
         <v>292</v>
       </c>
-      <c r="V2" s="314"/>
-      <c r="W2" s="314"/>
-      <c r="X2" s="314"/>
-      <c r="Y2" s="314"/>
-    </row>
-    <row r="3" spans="1:27" ht="15.75" customHeight="1">
+      <c r="V2" s="295"/>
+      <c r="W2" s="295"/>
+      <c r="X2" s="295"/>
+      <c r="Y2" s="295"/>
+    </row>
+    <row r="3" spans="1:27" ht="22.5">
       <c r="A3" s="30" t="s">
         <v>137</v>
       </c>
@@ -11296,46 +11907,46 @@
       <c r="I3" s="84"/>
       <c r="J3" s="85"/>
       <c r="K3" s="161"/>
-      <c r="M3" s="221" t="s">
+      <c r="M3" s="309" t="s">
         <v>142</v>
       </c>
-      <c r="N3" s="222">
+      <c r="N3" s="316">
         <f>B4</f>
         <v>0.9861890671276341</v>
       </c>
-      <c r="O3" s="223">
+      <c r="O3" s="317">
         <f>C4</f>
         <v>199937934.20591292</v>
       </c>
-      <c r="P3" s="222">
+      <c r="P3" s="316">
         <f>D4</f>
         <v>0.97953870242057495</v>
       </c>
-      <c r="Q3" s="223">
+      <c r="Q3" s="317">
         <f>E4</f>
         <v>351864755.14782721</v>
       </c>
-      <c r="U3" s="205" t="s">
+      <c r="U3" s="312" t="s">
         <v>251</v>
       </c>
-      <c r="V3" s="254">
+      <c r="V3" s="322">
         <f>W3*1/O7</f>
         <v>3.5987345084564889E-3</v>
       </c>
-      <c r="W3" s="207">
+      <c r="W3" s="323">
         <f>C11</f>
         <v>729600</v>
       </c>
-      <c r="X3" s="254">
+      <c r="X3" s="322">
         <f>Y3/Q7</f>
         <v>2.1529627859572012E-3</v>
       </c>
-      <c r="Y3" s="207">
+      <c r="Y3" s="323">
         <f>E11</f>
         <v>773376</v>
       </c>
     </row>
-    <row r="4" spans="1:27" ht="15.75" customHeight="1">
+    <row r="4" spans="1:27" ht="33.75">
       <c r="A4" s="39" t="s">
         <v>142</v>
       </c>
@@ -11379,46 +11990,46 @@
         <f>'Estado de resultados PyG - 5 añ'!K3</f>
         <v>523090680.34961951</v>
       </c>
-      <c r="M4" s="218" t="s">
+      <c r="M4" s="310" t="s">
         <v>154</v>
       </c>
-      <c r="N4" s="219">
+      <c r="N4" s="318">
         <f t="shared" ref="N4:Q6" si="0">B6</f>
         <v>1.7263666090457389E-2</v>
       </c>
-      <c r="O4" s="220">
+      <c r="O4" s="319">
         <f t="shared" si="0"/>
         <v>3500000</v>
       </c>
-      <c r="P4" s="219">
+      <c r="P4" s="318">
         <f t="shared" si="0"/>
         <v>2.4358687594553636E-2</v>
       </c>
-      <c r="Q4" s="220">
+      <c r="Q4" s="319">
         <f t="shared" si="0"/>
         <v>8750000</v>
       </c>
-      <c r="U4" s="205" t="s">
+      <c r="U4" s="312" t="s">
         <v>252</v>
       </c>
-      <c r="V4" s="206">
+      <c r="V4" s="324">
         <f>W4*1/O7</f>
         <v>0.2323771472279017</v>
       </c>
-      <c r="W4" s="207">
+      <c r="W4" s="323">
         <f t="shared" ref="W4:W6" si="1">C12</f>
         <v>47111662.785648078</v>
       </c>
-      <c r="X4" s="254">
+      <c r="X4" s="322">
         <f>Y4/Q7</f>
         <v>0.22909125677385642</v>
       </c>
-      <c r="Y4" s="207">
+      <c r="Y4" s="323">
         <f t="shared" ref="Y4:Y6" si="2">E12</f>
         <v>82292959.708528847</v>
       </c>
     </row>
-    <row r="5" spans="1:27" ht="15.75" customHeight="1">
+    <row r="5" spans="1:27" ht="24">
       <c r="A5" s="30" t="s">
         <v>150</v>
       </c>
@@ -11432,46 +12043,46 @@
       <c r="I5" s="84"/>
       <c r="J5" s="85"/>
       <c r="K5" s="161"/>
-      <c r="M5" s="218" t="s">
+      <c r="M5" s="310" t="s">
         <v>155</v>
       </c>
-      <c r="N5" s="219">
+      <c r="N5" s="318">
         <f t="shared" si="0"/>
         <v>3.452733218091478E-3</v>
       </c>
-      <c r="O5" s="220">
+      <c r="O5" s="319">
         <f t="shared" si="0"/>
         <v>700000</v>
       </c>
-      <c r="P5" s="219">
+      <c r="P5" s="318">
         <f t="shared" si="0"/>
         <v>3.8973900151285817E-3</v>
       </c>
-      <c r="Q5" s="220">
+      <c r="Q5" s="319">
         <f t="shared" si="0"/>
         <v>1400000</v>
       </c>
-      <c r="U5" s="205" t="s">
+      <c r="U5" s="312" t="s">
         <v>253</v>
       </c>
-      <c r="V5" s="206">
+      <c r="V5" s="324">
         <f>W5*1/O7</f>
         <v>0.54530849567871975</v>
       </c>
-      <c r="W5" s="207">
+      <c r="W5" s="323">
         <f t="shared" si="1"/>
         <v>110554717.91883764</v>
       </c>
-      <c r="X5" s="254">
+      <c r="X5" s="322">
         <f>Y5/Q7</f>
         <v>0.27723804084555675</v>
       </c>
-      <c r="Y5" s="207">
+      <c r="Y5" s="323">
         <f t="shared" si="2"/>
         <v>99587994.959999993</v>
       </c>
     </row>
-    <row r="6" spans="1:27" ht="15.75" customHeight="1" thickBot="1">
+    <row r="6" spans="1:27" ht="24.75" thickBot="1">
       <c r="A6" s="39" t="s">
         <v>154</v>
       </c>
@@ -11515,41 +12126,41 @@
         <f>I6*2.5</f>
         <v>136718750</v>
       </c>
-      <c r="M6" s="224" t="s">
+      <c r="M6" s="311" t="s">
         <v>156</v>
       </c>
-      <c r="N6" s="225">
+      <c r="N6" s="320">
         <f t="shared" si="0"/>
         <v>1.3810932872365912E-2</v>
       </c>
-      <c r="O6" s="226">
+      <c r="O6" s="321">
         <f t="shared" si="0"/>
         <v>2800000</v>
       </c>
-      <c r="P6" s="225">
+      <c r="P6" s="320">
         <f t="shared" si="0"/>
         <v>2.0461297579425053E-2</v>
       </c>
-      <c r="Q6" s="226">
+      <c r="Q6" s="321">
         <f t="shared" si="0"/>
         <v>7350000</v>
       </c>
-      <c r="U6" s="213" t="s">
+      <c r="U6" s="313" t="s">
         <v>254</v>
       </c>
-      <c r="V6" s="214">
+      <c r="V6" s="325">
         <f>W6/O7</f>
         <v>1.9651576725171104E-2</v>
       </c>
-      <c r="W6" s="215">
+      <c r="W6" s="326">
         <f t="shared" si="1"/>
         <v>3984120.0691501889</v>
       </c>
-      <c r="X6" s="255">
+      <c r="X6" s="327">
         <f>Y6/Q7</f>
         <v>1.1756664259410072E-2</v>
       </c>
-      <c r="Y6" s="215">
+      <c r="Y6" s="326">
         <f t="shared" si="2"/>
         <v>4223167.2732992005</v>
       </c>
@@ -11598,41 +12209,41 @@
         <f>I7+$C$7</f>
         <v>3500000</v>
       </c>
-      <c r="M7" s="221" t="s">
+      <c r="M7" s="213" t="s">
         <v>305</v>
       </c>
-      <c r="N7" s="222">
+      <c r="N7" s="316">
         <f>B2</f>
         <v>1</v>
       </c>
-      <c r="O7" s="223">
+      <c r="O7" s="317">
         <f>C2</f>
         <v>202737934.20591292</v>
       </c>
-      <c r="P7" s="222">
+      <c r="P7" s="316">
         <f>D2</f>
         <v>1</v>
       </c>
-      <c r="Q7" s="223">
+      <c r="Q7" s="317">
         <f>E2</f>
         <v>359214755.14782721</v>
       </c>
-      <c r="U7" s="209" t="s">
+      <c r="U7" s="314" t="s">
         <v>306</v>
       </c>
-      <c r="V7" s="210">
+      <c r="V7" s="328">
         <f>SUM(V3:V6)</f>
         <v>0.8009359541402491</v>
       </c>
-      <c r="W7" s="211">
+      <c r="W7" s="329">
         <f>C9</f>
         <v>162380100.77363589</v>
       </c>
-      <c r="X7" s="217">
+      <c r="X7" s="330">
         <f>SUM(X3:X6)</f>
         <v>0.52023892466478039</v>
       </c>
-      <c r="Y7" s="211">
+      <c r="Y7" s="329">
         <f>E9</f>
         <v>186877497.94182804</v>
       </c>
@@ -11682,22 +12293,22 @@
         <f t="shared" si="3"/>
         <v>133218750</v>
       </c>
-      <c r="U8" s="216" t="s">
+      <c r="U8" s="315" t="s">
         <v>159</v>
       </c>
-      <c r="V8" s="214">
+      <c r="V8" s="325">
         <f>W8/O7</f>
         <v>0.19906404585975096</v>
       </c>
-      <c r="W8" s="215">
+      <c r="W8" s="326">
         <f>C15</f>
         <v>40357833.432277024</v>
       </c>
-      <c r="X8" s="214">
+      <c r="X8" s="325">
         <f>Y8/Q7</f>
         <v>0.4797610753352195</v>
       </c>
-      <c r="Y8" s="215">
+      <c r="Y8" s="326">
         <f>E16</f>
         <v>172337257.20599917</v>
       </c>
@@ -11747,19 +12358,19 @@
         <v>245981000.52362499</v>
       </c>
       <c r="U9" s="181"/>
-      <c r="V9" s="184">
+      <c r="V9" s="331">
         <f>V7+V8</f>
         <v>1</v>
       </c>
-      <c r="W9" s="212">
+      <c r="W9" s="332">
         <f>W7+W8</f>
         <v>202737934.20591292</v>
       </c>
-      <c r="X9" s="204">
+      <c r="X9" s="333">
         <f>X7+X8</f>
         <v>0.99999999999999989</v>
       </c>
-      <c r="Y9" s="212">
+      <c r="Y9" s="332">
         <f>Y7+Y8</f>
         <v>359214755.14782721</v>
       </c>
@@ -11824,33 +12435,33 @@
         <v>773376</v>
       </c>
       <c r="M11" s="193"/>
-      <c r="N11" s="311" t="s">
+      <c r="N11" s="296" t="s">
         <v>72</v>
       </c>
-      <c r="O11" s="312"/>
-      <c r="P11" s="311" t="s">
+      <c r="O11" s="299"/>
+      <c r="P11" s="296" t="s">
         <v>74</v>
       </c>
-      <c r="Q11" s="312"/>
-      <c r="R11" s="311" t="s">
+      <c r="Q11" s="299"/>
+      <c r="R11" s="296" t="s">
         <v>75</v>
       </c>
-      <c r="S11" s="312"/>
-      <c r="U11" s="208"/>
-      <c r="V11" s="313" t="s">
+      <c r="S11" s="299"/>
+      <c r="U11" s="205"/>
+      <c r="V11" s="297" t="s">
         <v>72</v>
       </c>
-      <c r="W11" s="313"/>
-      <c r="X11" s="313" t="s">
+      <c r="W11" s="297"/>
+      <c r="X11" s="297" t="s">
         <v>74</v>
       </c>
-      <c r="Y11" s="313"/>
-      <c r="Z11" s="313" t="s">
+      <c r="Y11" s="297"/>
+      <c r="Z11" s="297" t="s">
         <v>75</v>
       </c>
-      <c r="AA11" s="315"/>
-    </row>
-    <row r="12" spans="1:27" ht="15.75" customHeight="1">
+      <c r="AA11" s="298"/>
+    </row>
+    <row r="12" spans="1:27" ht="15">
       <c r="A12" s="39" t="s">
         <v>252</v>
       </c>
@@ -11897,23 +12508,23 @@
       <c r="M12" s="203" t="s">
         <v>137</v>
       </c>
-      <c r="N12" s="311"/>
-      <c r="O12" s="311"/>
-      <c r="P12" s="311"/>
-      <c r="Q12" s="311"/>
-      <c r="R12" s="311"/>
-      <c r="S12" s="311"/>
+      <c r="N12" s="296"/>
+      <c r="O12" s="296"/>
+      <c r="P12" s="296"/>
+      <c r="Q12" s="296"/>
+      <c r="R12" s="296"/>
+      <c r="S12" s="296"/>
       <c r="U12" s="195" t="s">
         <v>292</v>
       </c>
-      <c r="V12" s="314"/>
-      <c r="W12" s="314"/>
-      <c r="X12" s="314"/>
-      <c r="Y12" s="314"/>
-      <c r="Z12" s="314"/>
-      <c r="AA12" s="314"/>
-    </row>
-    <row r="13" spans="1:27" ht="15.75" customHeight="1">
+      <c r="V12" s="295"/>
+      <c r="W12" s="295"/>
+      <c r="X12" s="295"/>
+      <c r="Y12" s="295"/>
+      <c r="Z12" s="295"/>
+      <c r="AA12" s="295"/>
+    </row>
+    <row r="13" spans="1:27" ht="22.5">
       <c r="A13" s="39" t="s">
         <v>253</v>
       </c>
@@ -11957,62 +12568,62 @@
         <f>'Flujo de caja - 5 años'!M3</f>
         <v>100914651.552</v>
       </c>
-      <c r="M13" s="221" t="s">
+      <c r="M13" s="309" t="s">
         <v>142</v>
       </c>
-      <c r="N13" s="222">
+      <c r="N13" s="334">
         <f t="shared" ref="N13:S13" si="5">F4</f>
         <v>0.96261792705375926</v>
       </c>
-      <c r="O13" s="223">
+      <c r="O13" s="335">
         <f t="shared" si="5"/>
         <v>509221881.16382653</v>
       </c>
-      <c r="P13" s="222">
+      <c r="P13" s="334">
         <f t="shared" si="5"/>
         <v>0.90963861551326697</v>
       </c>
-      <c r="Q13" s="223">
+      <c r="Q13" s="335">
         <f t="shared" si="5"/>
         <v>522334556.18837321</v>
       </c>
-      <c r="R13" s="210">
+      <c r="R13" s="328">
         <f t="shared" si="5"/>
         <v>0.79701838212345411</v>
       </c>
-      <c r="S13" s="211">
+      <c r="S13" s="329">
         <f t="shared" si="5"/>
         <v>523090680.34961951</v>
       </c>
-      <c r="U13" s="205" t="s">
+      <c r="U13" s="312" t="s">
         <v>251</v>
       </c>
-      <c r="V13" s="254">
+      <c r="V13" s="239">
         <f>W13/O17</f>
         <v>1.4619670314473764E-3</v>
       </c>
-      <c r="W13" s="207">
+      <c r="W13" s="204">
         <f t="shared" ref="W13:AA16" si="6">G11</f>
         <v>773376</v>
       </c>
-      <c r="X13" s="254">
+      <c r="X13" s="239">
         <f>Y13/$Q$17</f>
         <v>1.3468239188400219E-3</v>
       </c>
-      <c r="Y13" s="207">
+      <c r="Y13" s="204">
         <f t="shared" si="6"/>
         <v>773376</v>
       </c>
-      <c r="Z13" s="254">
+      <c r="Z13" s="239">
         <f>AA13/$S$17</f>
         <v>1.1783710003801385E-3</v>
       </c>
-      <c r="AA13" s="207">
+      <c r="AA13" s="204">
         <f t="shared" si="6"/>
         <v>773376</v>
       </c>
     </row>
-    <row r="14" spans="1:27" ht="15.75" customHeight="1">
+    <row r="14" spans="1:27" ht="33.75">
       <c r="A14" s="39" t="s">
         <v>254</v>
       </c>
@@ -12056,62 +12667,62 @@
         <f>'Flujo de caja - 5 años'!M4+'Flujo de caja - 5 años'!M5+'Flujo de caja - 5 años'!M8</f>
         <v>4270976.7141290028</v>
       </c>
-      <c r="M14" s="218" t="s">
+      <c r="M14" s="310" t="s">
         <v>154</v>
       </c>
-      <c r="N14" s="219">
+      <c r="N14" s="336">
         <f t="shared" ref="N14:S16" si="7">F6</f>
         <v>4.1351850604248591E-2</v>
       </c>
-      <c r="O14" s="220">
+      <c r="O14" s="337">
         <f t="shared" si="7"/>
         <v>21875000</v>
       </c>
-      <c r="P14" s="219">
+      <c r="P14" s="336">
         <f t="shared" si="7"/>
         <v>9.5237546887366159E-2</v>
       </c>
-      <c r="Q14" s="220">
+      <c r="Q14" s="337">
         <f t="shared" si="7"/>
         <v>54687500</v>
       </c>
-      <c r="R14" s="206">
+      <c r="R14" s="324">
         <f t="shared" si="7"/>
         <v>0.20831446826410707</v>
       </c>
-      <c r="S14" s="207">
+      <c r="S14" s="323">
         <f t="shared" si="7"/>
         <v>136718750</v>
       </c>
-      <c r="U14" s="205" t="s">
+      <c r="U14" s="312" t="s">
         <v>252</v>
       </c>
-      <c r="V14" s="254">
+      <c r="V14" s="239">
         <f>W14/O17</f>
         <v>0.25631746904469815</v>
       </c>
-      <c r="W14" s="207">
+      <c r="W14" s="204">
         <f t="shared" si="6"/>
         <v>135591141.71245098</v>
       </c>
-      <c r="X14" s="254">
+      <c r="X14" s="239">
         <f t="shared" ref="X14:X16" si="8">Y14/$Q$17</f>
         <v>0.24354029747231237</v>
       </c>
-      <c r="Y14" s="207">
+      <c r="Y14" s="204">
         <f t="shared" si="6"/>
         <v>139846210.37927929</v>
       </c>
-      <c r="Z14" s="254">
+      <c r="Z14" s="239">
         <f t="shared" ref="Z14:Z16" si="9">AA14/$S$17</f>
         <v>0.21334753057396344</v>
       </c>
-      <c r="AA14" s="207">
+      <c r="AA14" s="204">
         <f t="shared" si="6"/>
         <v>140021996.25749597</v>
       </c>
     </row>
-    <row r="15" spans="1:27" ht="15.75" customHeight="1">
+    <row r="15" spans="1:27" ht="24">
       <c r="A15" s="30" t="s">
         <v>159</v>
       </c>
@@ -12155,62 +12766,62 @@
         <f>K16</f>
         <v>410328429.82599449</v>
       </c>
-      <c r="M15" s="218" t="s">
+      <c r="M15" s="310" t="s">
         <v>155</v>
       </c>
-      <c r="N15" s="219">
+      <c r="N15" s="336">
         <f t="shared" si="7"/>
         <v>3.9697776580078651E-3</v>
       </c>
-      <c r="O15" s="220">
+      <c r="O15" s="337">
         <f t="shared" si="7"/>
         <v>2100000</v>
       </c>
-      <c r="P15" s="219">
+      <c r="P15" s="336">
         <f t="shared" si="7"/>
         <v>4.8761624006331472E-3</v>
       </c>
-      <c r="Q15" s="220">
+      <c r="Q15" s="337">
         <f t="shared" si="7"/>
         <v>2800000</v>
       </c>
-      <c r="R15" s="206">
+      <c r="R15" s="324">
         <f t="shared" si="7"/>
         <v>5.3328503875611413E-3</v>
       </c>
-      <c r="S15" s="207">
+      <c r="S15" s="323">
         <f t="shared" si="7"/>
         <v>3500000</v>
       </c>
-      <c r="U15" s="205" t="s">
+      <c r="U15" s="312" t="s">
         <v>253</v>
       </c>
-      <c r="V15" s="254">
+      <c r="V15" s="239">
         <f>W15/O17</f>
         <v>0.18930313600277565</v>
       </c>
-      <c r="W15" s="207">
+      <c r="W15" s="204">
         <f t="shared" si="6"/>
         <v>100140768.54000001</v>
       </c>
-      <c r="X15" s="254">
+      <c r="X15" s="239">
         <f t="shared" si="8"/>
         <v>0.17535645145432649</v>
       </c>
-      <c r="Y15" s="207">
+      <c r="Y15" s="204">
         <f t="shared" si="6"/>
         <v>100693542.12</v>
       </c>
-      <c r="Z15" s="254">
+      <c r="Z15" s="239">
         <f t="shared" si="9"/>
         <v>0.15376078246848021</v>
       </c>
-      <c r="AA15" s="207">
+      <c r="AA15" s="204">
         <f t="shared" si="6"/>
         <v>100914651.552</v>
       </c>
     </row>
-    <row r="16" spans="1:27" ht="15.75" customHeight="1" thickBot="1">
+    <row r="16" spans="1:27" ht="24.75" thickBot="1">
       <c r="A16" s="39" t="s">
         <v>160</v>
       </c>
@@ -12254,143 +12865,143 @@
         <f>K2-K9</f>
         <v>410328429.82599449</v>
       </c>
-      <c r="M16" s="224" t="s">
+      <c r="M16" s="311" t="s">
         <v>156</v>
       </c>
-      <c r="N16" s="225">
+      <c r="N16" s="338">
         <f t="shared" si="7"/>
         <v>3.7382072946240727E-2</v>
       </c>
-      <c r="O16" s="226">
+      <c r="O16" s="339">
         <f t="shared" si="7"/>
         <v>19775000</v>
       </c>
-      <c r="P16" s="225">
+      <c r="P16" s="338">
         <f t="shared" si="7"/>
         <v>9.0361384486733018E-2</v>
       </c>
-      <c r="Q16" s="226">
+      <c r="Q16" s="339">
         <f t="shared" si="7"/>
         <v>51887500</v>
       </c>
-      <c r="R16" s="227">
+      <c r="R16" s="340">
         <f t="shared" si="7"/>
         <v>0.20298161787654592</v>
       </c>
-      <c r="S16" s="228">
+      <c r="S16" s="341">
         <f t="shared" si="7"/>
         <v>133218750</v>
       </c>
-      <c r="U16" s="213" t="s">
+      <c r="U16" s="313" t="s">
         <v>254</v>
       </c>
-      <c r="V16" s="255">
+      <c r="V16" s="240">
         <f>W16/O17</f>
         <v>8.0210073532189629E-3</v>
       </c>
-      <c r="W16" s="215">
+      <c r="W16" s="211">
         <f t="shared" si="6"/>
         <v>4243087.8736449508</v>
       </c>
-      <c r="X16" s="255">
+      <c r="X16" s="240">
         <f t="shared" si="8"/>
         <v>7.4239720123049826E-3</v>
       </c>
-      <c r="Y16" s="215">
+      <c r="Y16" s="211">
         <f t="shared" si="6"/>
         <v>4263008.4739907021</v>
       </c>
-      <c r="Z16" s="255">
+      <c r="Z16" s="240">
         <f t="shared" si="9"/>
         <v>6.5075656643449886E-3</v>
       </c>
-      <c r="AA16" s="215">
+      <c r="AA16" s="211">
         <f t="shared" si="6"/>
         <v>4270976.7141290028</v>
       </c>
     </row>
     <row r="17" spans="2:27" ht="15.75" customHeight="1">
-      <c r="M17" s="221" t="s">
+      <c r="M17" s="213" t="s">
         <v>123</v>
       </c>
-      <c r="N17" s="222">
+      <c r="N17" s="334">
         <f>B2</f>
         <v>1</v>
       </c>
-      <c r="O17" s="223">
+      <c r="O17" s="335">
         <f>G2</f>
         <v>528996881.16382653</v>
       </c>
-      <c r="P17" s="222">
+      <c r="P17" s="334">
         <f>D2</f>
         <v>1</v>
       </c>
-      <c r="Q17" s="223">
+      <c r="Q17" s="335">
         <f>I2</f>
         <v>574222056.18837321</v>
       </c>
-      <c r="R17" s="210">
+      <c r="R17" s="328">
         <f>F2</f>
         <v>1</v>
       </c>
-      <c r="S17" s="211">
+      <c r="S17" s="329">
         <f>K2</f>
         <v>656309430.34961951</v>
       </c>
-      <c r="U17" s="209" t="s">
+      <c r="U17" s="206" t="s">
         <v>306</v>
       </c>
-      <c r="V17" s="210">
+      <c r="V17" s="207">
         <f>SUM(V13:V16)</f>
         <v>0.45510357943214014</v>
       </c>
-      <c r="W17" s="211">
+      <c r="W17" s="208">
         <f>G9</f>
         <v>240748374.12609595</v>
       </c>
-      <c r="X17" s="210">
+      <c r="X17" s="207">
         <f>SUM(X13:X16)</f>
         <v>0.42766754485778385</v>
       </c>
-      <c r="Y17" s="211">
+      <c r="Y17" s="208">
         <f>I9</f>
         <v>245576136.97327</v>
       </c>
-      <c r="Z17" s="210">
+      <c r="Z17" s="207">
         <f>SUM(Z13:Z16)</f>
         <v>0.37479424970716879</v>
       </c>
-      <c r="AA17" s="211">
+      <c r="AA17" s="208">
         <f>K9</f>
         <v>245981000.52362499</v>
       </c>
     </row>
     <row r="18" spans="2:27" ht="15.75" customHeight="1" thickBot="1">
-      <c r="B18" s="229"/>
-      <c r="U18" s="216" t="s">
+      <c r="B18" s="214"/>
+      <c r="U18" s="212" t="s">
         <v>159</v>
       </c>
-      <c r="V18" s="214">
+      <c r="V18" s="210">
         <f>W18/O17</f>
         <v>0.54489642056785981</v>
       </c>
-      <c r="W18" s="215">
+      <c r="W18" s="211">
         <f>G15</f>
         <v>288248507.03773057</v>
       </c>
-      <c r="X18" s="214">
+      <c r="X18" s="210">
         <f>Y18/Q17</f>
         <v>0.57233245514221609</v>
       </c>
-      <c r="Y18" s="215">
+      <c r="Y18" s="211">
         <f>I16</f>
         <v>328645919.21510321</v>
       </c>
-      <c r="Z18" s="214">
+      <c r="Z18" s="210">
         <f>AA18/S17</f>
         <v>0.62520575029283121</v>
       </c>
-      <c r="AA18" s="215">
+      <c r="AA18" s="211">
         <f>K15</f>
         <v>410328429.82599449</v>
       </c>
@@ -12401,7 +13012,7 @@
         <f t="shared" ref="V19:AA19" si="10">V17+V18</f>
         <v>1</v>
       </c>
-      <c r="W19" s="212">
+      <c r="W19" s="209">
         <f t="shared" si="10"/>
         <v>528996881.16382653</v>
       </c>
@@ -12409,7 +13020,7 @@
         <f t="shared" si="10"/>
         <v>1</v>
       </c>
-      <c r="Y19" s="212">
+      <c r="Y19" s="209">
         <f t="shared" si="10"/>
         <v>574222056.18837321</v>
       </c>
@@ -12417,18 +13028,18 @@
         <f t="shared" si="10"/>
         <v>1</v>
       </c>
-      <c r="AA19" s="212">
+      <c r="AA19" s="209">
         <f t="shared" si="10"/>
         <v>656309430.34961951</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="19">
-    <mergeCell ref="V12:AA12"/>
-    <mergeCell ref="N12:S12"/>
-    <mergeCell ref="Z11:AA11"/>
-    <mergeCell ref="V2:Y2"/>
-    <mergeCell ref="R11:S11"/>
+    <mergeCell ref="B1:C1"/>
+    <mergeCell ref="D1:E1"/>
+    <mergeCell ref="F1:G1"/>
+    <mergeCell ref="H1:I1"/>
+    <mergeCell ref="J1:K1"/>
     <mergeCell ref="V1:W1"/>
     <mergeCell ref="X1:Y1"/>
     <mergeCell ref="N2:Q2"/>
@@ -12438,44 +13049,44 @@
     <mergeCell ref="X11:Y11"/>
     <mergeCell ref="N1:O1"/>
     <mergeCell ref="P1:Q1"/>
-    <mergeCell ref="B1:C1"/>
-    <mergeCell ref="D1:E1"/>
-    <mergeCell ref="F1:G1"/>
-    <mergeCell ref="H1:I1"/>
-    <mergeCell ref="J1:K1"/>
+    <mergeCell ref="V12:AA12"/>
+    <mergeCell ref="N12:S12"/>
+    <mergeCell ref="Z11:AA11"/>
+    <mergeCell ref="V2:Y2"/>
+    <mergeCell ref="R11:S11"/>
   </mergeCells>
   <conditionalFormatting sqref="M1:Q1 A1:K16 M2:M7">
-    <cfRule type="cellIs" dxfId="6" priority="13" operator="lessThan">
+    <cfRule type="cellIs" dxfId="10" priority="13" operator="lessThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="R11:S11">
-    <cfRule type="cellIs" dxfId="5" priority="7" operator="lessThan">
+    <cfRule type="cellIs" dxfId="9" priority="7" operator="lessThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="M11:Q11 M12:M17">
-    <cfRule type="cellIs" dxfId="4" priority="8" operator="lessThan">
+    <cfRule type="cellIs" dxfId="8" priority="8" operator="lessThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="Z11:AA11">
-    <cfRule type="cellIs" dxfId="3" priority="4" operator="lessThan">
+    <cfRule type="cellIs" dxfId="7" priority="4" operator="lessThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="U3:U6 U8">
-    <cfRule type="cellIs" dxfId="2" priority="3" operator="lessThan">
+    <cfRule type="cellIs" dxfId="6" priority="3" operator="lessThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="U13:U16">
-    <cfRule type="cellIs" dxfId="1" priority="2" operator="lessThan">
+    <cfRule type="cellIs" dxfId="5" priority="2" operator="lessThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="U18">
-    <cfRule type="cellIs" dxfId="0" priority="1" operator="lessThan">
+    <cfRule type="cellIs" dxfId="4" priority="1" operator="lessThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
@@ -13261,10 +13872,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:N67"/>
+  <dimension ref="A1:BE170"/>
   <sheetViews>
-    <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="E7" sqref="E7"/>
+    <sheetView topLeftCell="AQ145" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="BE163" sqref="BE163"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1"/>
@@ -13278,21 +13889,28 @@
     <col min="7" max="7" width="15.42578125" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="19.140625" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="17.28515625" customWidth="1"/>
+    <col min="51" max="51" width="16.28515625" customWidth="1"/>
+    <col min="52" max="52" width="27.140625" bestFit="1" customWidth="1"/>
+    <col min="53" max="53" width="13.5703125" bestFit="1" customWidth="1"/>
+    <col min="54" max="54" width="9.85546875" customWidth="1"/>
+    <col min="55" max="55" width="10.7109375" customWidth="1"/>
+    <col min="56" max="56" width="11.85546875" customWidth="1"/>
+    <col min="57" max="57" width="12.85546875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:14" ht="15.75" customHeight="1">
-      <c r="A1" s="270" t="s">
+      <c r="A1" s="241" t="s">
         <v>8</v>
       </c>
-      <c r="B1" s="271"/>
-      <c r="D1" s="270" t="s">
+      <c r="B1" s="242"/>
+      <c r="D1" s="241" t="s">
         <v>9</v>
       </c>
-      <c r="E1" s="271"/>
-      <c r="J1" s="270" t="s">
+      <c r="E1" s="242"/>
+      <c r="J1" s="241" t="s">
         <v>11</v>
       </c>
-      <c r="K1" s="271"/>
+      <c r="K1" s="242"/>
       <c r="M1" s="6" t="s">
         <v>12</v>
       </c>
@@ -13304,10 +13922,10 @@
       <c r="B2" s="8">
         <v>3066667</v>
       </c>
-      <c r="D2" s="233" t="s">
+      <c r="D2" s="218" t="s">
         <v>296</v>
       </c>
-      <c r="E2" s="250">
+      <c r="E2" s="235">
         <v>0</v>
       </c>
       <c r="J2" s="9" t="s">
@@ -13331,10 +13949,10 @@
       <c r="B3" s="8">
         <v>2039963</v>
       </c>
-      <c r="D3" s="233" t="s">
+      <c r="D3" s="218" t="s">
         <v>297</v>
       </c>
-      <c r="E3" s="250">
+      <c r="E3" s="235">
         <v>0</v>
       </c>
       <c r="J3" s="9" t="s">
@@ -13357,10 +13975,10 @@
       <c r="B4" s="8">
         <v>200000</v>
       </c>
-      <c r="D4" s="233" t="s">
+      <c r="D4" s="218" t="s">
         <v>298</v>
       </c>
-      <c r="E4" s="250">
+      <c r="E4" s="235">
         <v>0</v>
       </c>
       <c r="J4" s="12"/>
@@ -13373,10 +13991,10 @@
       <c r="B5" s="8">
         <v>1416857</v>
       </c>
-      <c r="D5" s="233" t="s">
+      <c r="D5" s="218" t="s">
         <v>299</v>
       </c>
-      <c r="E5" s="250">
+      <c r="E5" s="235">
         <v>0</v>
       </c>
       <c r="J5" s="12"/>
@@ -13389,10 +14007,10 @@
       <c r="B6" s="8">
         <v>1244703</v>
       </c>
-      <c r="D6" s="233" t="s">
+      <c r="D6" s="218" t="s">
         <v>300</v>
       </c>
-      <c r="E6" s="250">
+      <c r="E6" s="235">
         <v>0</v>
       </c>
       <c r="J6" s="12"/>
@@ -13405,10 +14023,10 @@
       <c r="B7" s="8">
         <v>1244703</v>
       </c>
-      <c r="D7" s="235" t="s">
+      <c r="D7" s="220" t="s">
         <v>25</v>
       </c>
-      <c r="E7" s="251">
+      <c r="E7" s="236">
         <f>E2+E3+E4+E5+E6</f>
         <v>0</v>
       </c>
@@ -13418,10 +14036,10 @@
     <row r="8" spans="1:14" ht="15.75" customHeight="1">
       <c r="A8" s="7"/>
       <c r="B8" s="8"/>
-      <c r="D8" s="235" t="s">
+      <c r="D8" s="220" t="s">
         <v>293</v>
       </c>
-      <c r="E8" s="251">
+      <c r="E8" s="236">
         <v>0</v>
       </c>
       <c r="J8" s="12"/>
@@ -13430,16 +14048,16 @@
     <row r="9" spans="1:14" ht="15.75" customHeight="1">
       <c r="A9" s="15"/>
       <c r="B9" s="16"/>
-      <c r="D9" s="233"/>
-      <c r="E9" s="234"/>
+      <c r="D9" s="218"/>
+      <c r="E9" s="219"/>
       <c r="J9" s="12"/>
       <c r="K9" s="13"/>
     </row>
     <row r="10" spans="1:14" ht="15.75" customHeight="1">
       <c r="A10" s="15"/>
       <c r="B10" s="16"/>
-      <c r="D10" s="233"/>
-      <c r="E10" s="234"/>
+      <c r="D10" s="218"/>
+      <c r="E10" s="219"/>
       <c r="J10" s="12"/>
       <c r="K10" s="13"/>
     </row>
@@ -13451,10 +14069,10 @@
         <f>SUM(B2:B10)</f>
         <v>9212893</v>
       </c>
-      <c r="J11" s="230" t="s">
+      <c r="J11" s="215" t="s">
         <v>28</v>
       </c>
-      <c r="K11" s="252">
+      <c r="K11" s="237">
         <f>K2+K3</f>
         <v>332010</v>
       </c>
@@ -13474,10 +14092,10 @@
         <f>B11*12</f>
         <v>110554716</v>
       </c>
-      <c r="J12" s="231" t="s">
+      <c r="J12" s="216" t="s">
         <v>294</v>
       </c>
-      <c r="K12" s="253">
+      <c r="K12" s="238">
         <f>K11*12</f>
         <v>3984120</v>
       </c>
@@ -13491,14 +14109,14 @@
       </c>
     </row>
     <row r="17" spans="1:14" ht="15.75" customHeight="1">
-      <c r="A17" s="270" t="s">
+      <c r="A17" s="241" t="s">
         <v>31</v>
       </c>
-      <c r="B17" s="271"/>
-      <c r="D17" s="272" t="s">
+      <c r="B17" s="242"/>
+      <c r="D17" s="243" t="s">
         <v>10</v>
       </c>
-      <c r="E17" s="273"/>
+      <c r="E17" s="244"/>
       <c r="M17" s="11" t="s">
         <v>33</v>
       </c>
@@ -13513,10 +14131,10 @@
       <c r="B18" s="8">
         <v>1600000</v>
       </c>
-      <c r="D18" s="246" t="s">
+      <c r="D18" s="231" t="s">
         <v>17</v>
       </c>
-      <c r="E18" s="247">
+      <c r="E18" s="232">
         <v>60800</v>
       </c>
       <c r="M18" s="11">
@@ -13533,8 +14151,8 @@
       <c r="B19" s="8">
         <v>2039963</v>
       </c>
-      <c r="D19" s="246"/>
-      <c r="E19" s="247"/>
+      <c r="D19" s="231"/>
+      <c r="E19" s="232"/>
       <c r="M19" s="11">
         <v>2007</v>
       </c>
@@ -13549,8 +14167,8 @@
       <c r="B20" s="8">
         <v>200000</v>
       </c>
-      <c r="D20" s="246"/>
-      <c r="E20" s="247"/>
+      <c r="D20" s="231"/>
+      <c r="E20" s="232"/>
       <c r="M20" s="11">
         <v>2008</v>
       </c>
@@ -13565,8 +14183,8 @@
       <c r="B21" s="8">
         <v>1416857</v>
       </c>
-      <c r="D21" s="246"/>
-      <c r="E21" s="247"/>
+      <c r="D21" s="231"/>
+      <c r="E21" s="232"/>
       <c r="M21" s="11">
         <v>2009</v>
       </c>
@@ -13581,8 +14199,8 @@
       <c r="B22" s="8">
         <v>1244703</v>
       </c>
-      <c r="D22" s="246"/>
-      <c r="E22" s="247"/>
+      <c r="D22" s="231"/>
+      <c r="E22" s="232"/>
       <c r="M22" s="11">
         <v>2010</v>
       </c>
@@ -13597,8 +14215,8 @@
       <c r="B23" s="8">
         <v>1244703</v>
       </c>
-      <c r="D23" s="246"/>
-      <c r="E23" s="247"/>
+      <c r="D23" s="231"/>
+      <c r="E23" s="232"/>
       <c r="M23" s="11">
         <v>2011</v>
       </c>
@@ -13609,8 +14227,8 @@
     <row r="24" spans="1:14" ht="15.75" customHeight="1">
       <c r="A24" s="7"/>
       <c r="B24" s="8"/>
-      <c r="D24" s="246"/>
-      <c r="E24" s="247"/>
+      <c r="D24" s="231"/>
+      <c r="E24" s="232"/>
       <c r="M24" s="11">
         <v>2012</v>
       </c>
@@ -13621,8 +14239,8 @@
     <row r="25" spans="1:14" ht="12.75">
       <c r="A25" s="15"/>
       <c r="B25" s="16"/>
-      <c r="D25" s="246"/>
-      <c r="E25" s="247"/>
+      <c r="D25" s="231"/>
+      <c r="E25" s="232"/>
       <c r="M25" s="11">
         <v>2013</v>
       </c>
@@ -13633,8 +14251,8 @@
     <row r="26" spans="1:14" ht="12.75">
       <c r="A26" s="15"/>
       <c r="B26" s="16"/>
-      <c r="D26" s="246"/>
-      <c r="E26" s="247"/>
+      <c r="D26" s="231"/>
+      <c r="E26" s="232"/>
       <c r="M26" s="11">
         <v>2014</v>
       </c>
@@ -13650,10 +14268,10 @@
         <f>SUM(B18:B26)</f>
         <v>7746226</v>
       </c>
-      <c r="D27" s="248" t="s">
+      <c r="D27" s="233" t="s">
         <v>27</v>
       </c>
-      <c r="E27" s="249">
+      <c r="E27" s="234">
         <f>SUM(E18:E26)</f>
         <v>60800</v>
       </c>
@@ -13665,10 +14283,10 @@
       </c>
     </row>
     <row r="28" spans="1:14" ht="12.75">
-      <c r="D28" s="231" t="s">
+      <c r="D28" s="216" t="s">
         <v>304</v>
       </c>
-      <c r="E28" s="232">
+      <c r="E28" s="217">
         <f>E27*12</f>
         <v>729600</v>
       </c>
@@ -13695,26 +14313,26 @@
     </row>
     <row r="33" spans="1:8" ht="15.75" customHeight="1" thickBot="1"/>
     <row r="34" spans="1:8" ht="15.75" customHeight="1" thickTop="1" thickBot="1">
-      <c r="A34" s="256" t="s">
+      <c r="A34" s="246" t="s">
         <v>214</v>
       </c>
-      <c r="B34" s="256"/>
-      <c r="C34" s="256"/>
-      <c r="D34" s="256"/>
-      <c r="E34" s="256"/>
-      <c r="F34" s="256"/>
-      <c r="G34" s="256"/>
-      <c r="H34" s="256"/>
+      <c r="B34" s="246"/>
+      <c r="C34" s="246"/>
+      <c r="D34" s="246"/>
+      <c r="E34" s="246"/>
+      <c r="F34" s="246"/>
+      <c r="G34" s="246"/>
+      <c r="H34" s="246"/>
     </row>
     <row r="35" spans="1:8" ht="15.75" customHeight="1" thickTop="1" thickBot="1">
-      <c r="A35" s="268"/>
-      <c r="B35" s="268"/>
-      <c r="C35" s="268"/>
-      <c r="D35" s="268"/>
-      <c r="E35" s="268"/>
-      <c r="F35" s="268"/>
-      <c r="G35" s="268"/>
-      <c r="H35" s="268"/>
+      <c r="A35" s="247"/>
+      <c r="B35" s="247"/>
+      <c r="C35" s="247"/>
+      <c r="D35" s="247"/>
+      <c r="E35" s="247"/>
+      <c r="F35" s="247"/>
+      <c r="G35" s="247"/>
+      <c r="H35" s="247"/>
     </row>
     <row r="36" spans="1:8" ht="46.5" customHeight="1" thickTop="1" thickBot="1">
       <c r="A36" s="106" t="s">
@@ -13909,10 +14527,10 @@
       <c r="C43" s="100"/>
       <c r="D43" s="100"/>
       <c r="E43" s="100"/>
-      <c r="F43" s="236" t="s">
+      <c r="F43" s="221" t="s">
         <v>293</v>
       </c>
-      <c r="G43" s="237">
+      <c r="G43" s="222">
         <f>SUBTOTAL(109,PUBLICIDAD[Costo total])</f>
         <v>4285000</v>
       </c>
@@ -13920,235 +14538,235 @@
     </row>
     <row r="45" spans="1:8" ht="15.75" customHeight="1" thickBot="1"/>
     <row r="46" spans="1:8" ht="15.75" customHeight="1" thickTop="1" thickBot="1">
-      <c r="A46" s="256" t="s">
+      <c r="A46" s="246" t="s">
         <v>232</v>
       </c>
-      <c r="B46" s="256"/>
-      <c r="C46" s="256"/>
-      <c r="D46" s="256"/>
-      <c r="E46" s="256"/>
-      <c r="F46" s="256"/>
+      <c r="B46" s="246"/>
+      <c r="C46" s="246"/>
+      <c r="D46" s="246"/>
+      <c r="E46" s="246"/>
+      <c r="F46" s="246"/>
     </row>
     <row r="47" spans="1:8" ht="15.75" customHeight="1" thickTop="1">
-      <c r="A47" s="269" t="s">
+      <c r="A47" s="248" t="s">
         <v>217</v>
       </c>
-      <c r="B47" s="269"/>
-      <c r="C47" s="269"/>
-      <c r="D47" s="269"/>
-      <c r="E47" s="269" t="s">
+      <c r="B47" s="248"/>
+      <c r="C47" s="248"/>
+      <c r="D47" s="248"/>
+      <c r="E47" s="248" t="s">
         <v>70</v>
       </c>
-      <c r="F47" s="269"/>
+      <c r="F47" s="248"/>
     </row>
     <row r="48" spans="1:8" ht="15.75" customHeight="1">
-      <c r="A48" s="262" t="s">
+      <c r="A48" s="250" t="s">
         <v>225</v>
       </c>
-      <c r="B48" s="265"/>
-      <c r="C48" s="259" t="s">
+      <c r="B48" s="251"/>
+      <c r="C48" s="254" t="s">
         <v>218</v>
       </c>
-      <c r="D48" s="264"/>
-      <c r="E48" s="267">
-        <v>0</v>
-      </c>
-      <c r="F48" s="267"/>
+      <c r="D48" s="255"/>
+      <c r="E48" s="245">
+        <v>0</v>
+      </c>
+      <c r="F48" s="245"/>
     </row>
     <row r="49" spans="1:6" ht="15.75" customHeight="1">
-      <c r="A49" s="265"/>
-      <c r="B49" s="265"/>
-      <c r="C49" s="259" t="s">
+      <c r="A49" s="251"/>
+      <c r="B49" s="251"/>
+      <c r="C49" s="254" t="s">
         <v>219</v>
       </c>
-      <c r="D49" s="264"/>
-      <c r="E49" s="267">
+      <c r="D49" s="255"/>
+      <c r="E49" s="245">
         <f>B2*12</f>
         <v>36800004</v>
       </c>
-      <c r="F49" s="267"/>
+      <c r="F49" s="245"/>
     </row>
     <row r="50" spans="1:6" ht="15.75" customHeight="1">
-      <c r="A50" s="265"/>
-      <c r="B50" s="265"/>
-      <c r="C50" s="259" t="s">
+      <c r="A50" s="251"/>
+      <c r="B50" s="251"/>
+      <c r="C50" s="254" t="s">
         <v>220</v>
       </c>
-      <c r="D50" s="264"/>
-      <c r="E50" s="267">
+      <c r="D50" s="255"/>
+      <c r="E50" s="245">
         <f>(B19*12+B22*12)</f>
         <v>39415992</v>
       </c>
-      <c r="F50" s="267"/>
+      <c r="F50" s="245"/>
     </row>
     <row r="51" spans="1:6" ht="15.75" customHeight="1">
-      <c r="A51" s="265"/>
-      <c r="B51" s="265"/>
-      <c r="C51" s="259" t="s">
+      <c r="A51" s="251"/>
+      <c r="B51" s="251"/>
+      <c r="C51" s="254" t="s">
         <v>221</v>
       </c>
-      <c r="D51" s="259"/>
-      <c r="E51" s="267">
+      <c r="D51" s="254"/>
+      <c r="E51" s="245">
         <f>B4*12</f>
         <v>2400000</v>
       </c>
-      <c r="F51" s="267"/>
+      <c r="F51" s="245"/>
     </row>
     <row r="52" spans="1:6" ht="15.75" customHeight="1">
-      <c r="A52" s="265"/>
-      <c r="B52" s="265"/>
-      <c r="C52" s="259" t="s">
+      <c r="A52" s="251"/>
+      <c r="B52" s="251"/>
+      <c r="C52" s="254" t="s">
         <v>222</v>
       </c>
-      <c r="D52" s="264"/>
-      <c r="E52" s="267">
+      <c r="D52" s="255"/>
+      <c r="E52" s="245">
         <f>(B21+B23)*12</f>
         <v>31938720</v>
       </c>
-      <c r="F52" s="267"/>
+      <c r="F52" s="245"/>
     </row>
     <row r="53" spans="1:6" ht="15.75" customHeight="1" thickBot="1">
-      <c r="A53" s="265"/>
-      <c r="B53" s="265"/>
-      <c r="C53" s="259" t="s">
+      <c r="A53" s="251"/>
+      <c r="B53" s="251"/>
+      <c r="C53" s="254" t="s">
         <v>223</v>
       </c>
-      <c r="D53" s="264"/>
-      <c r="E53" s="267">
-        <v>0</v>
-      </c>
-      <c r="F53" s="267"/>
+      <c r="D53" s="255"/>
+      <c r="E53" s="245">
+        <v>0</v>
+      </c>
+      <c r="F53" s="245"/>
     </row>
     <row r="54" spans="1:6" ht="15.75" customHeight="1" thickTop="1" thickBot="1">
-      <c r="A54" s="265"/>
-      <c r="B54" s="265"/>
-      <c r="C54" s="256" t="s">
+      <c r="A54" s="251"/>
+      <c r="B54" s="251"/>
+      <c r="C54" s="246" t="s">
         <v>224</v>
       </c>
-      <c r="D54" s="256"/>
-      <c r="E54" s="263">
+      <c r="D54" s="246"/>
+      <c r="E54" s="249">
         <f>SUM(E48:F53)</f>
         <v>110554716</v>
       </c>
-      <c r="F54" s="263"/>
+      <c r="F54" s="249"/>
     </row>
     <row r="55" spans="1:6" ht="15.75" customHeight="1" thickTop="1">
-      <c r="A55" s="262" t="s">
+      <c r="A55" s="250" t="s">
         <v>231</v>
       </c>
-      <c r="B55" s="265"/>
-      <c r="C55" s="258" t="s">
+      <c r="B55" s="251"/>
+      <c r="C55" s="252" t="s">
         <v>226</v>
       </c>
-      <c r="D55" s="266"/>
-      <c r="E55" s="260">
-        <v>0</v>
-      </c>
-      <c r="F55" s="260"/>
+      <c r="D55" s="253"/>
+      <c r="E55" s="256">
+        <v>0</v>
+      </c>
+      <c r="F55" s="256"/>
     </row>
     <row r="56" spans="1:6" ht="15.75" customHeight="1">
-      <c r="A56" s="265"/>
-      <c r="B56" s="265"/>
-      <c r="C56" s="259" t="s">
+      <c r="A56" s="251"/>
+      <c r="B56" s="251"/>
+      <c r="C56" s="254" t="s">
         <v>227</v>
       </c>
-      <c r="D56" s="264"/>
-      <c r="E56" s="261">
+      <c r="D56" s="255"/>
+      <c r="E56" s="257">
         <f>'Presupuesto Inicial'!J20*12</f>
         <v>700000</v>
       </c>
-      <c r="F56" s="261"/>
+      <c r="F56" s="257"/>
     </row>
     <row r="57" spans="1:6" ht="15.75" customHeight="1">
-      <c r="A57" s="265"/>
-      <c r="B57" s="265"/>
-      <c r="C57" s="259" t="s">
+      <c r="A57" s="251"/>
+      <c r="B57" s="251"/>
+      <c r="C57" s="254" t="s">
         <v>228</v>
       </c>
-      <c r="D57" s="264"/>
-      <c r="E57" s="261">
-        <v>0</v>
-      </c>
-      <c r="F57" s="261"/>
+      <c r="D57" s="255"/>
+      <c r="E57" s="257">
+        <v>0</v>
+      </c>
+      <c r="F57" s="257"/>
     </row>
     <row r="58" spans="1:6" ht="15.75" customHeight="1" thickBot="1">
-      <c r="A58" s="265"/>
-      <c r="B58" s="265"/>
-      <c r="C58" s="259" t="s">
+      <c r="A58" s="251"/>
+      <c r="B58" s="251"/>
+      <c r="C58" s="254" t="s">
         <v>229</v>
       </c>
-      <c r="D58" s="264"/>
-      <c r="E58" s="261">
-        <v>0</v>
-      </c>
-      <c r="F58" s="261"/>
+      <c r="D58" s="255"/>
+      <c r="E58" s="257">
+        <v>0</v>
+      </c>
+      <c r="F58" s="257"/>
     </row>
     <row r="59" spans="1:6" ht="15.75" customHeight="1" thickTop="1" thickBot="1">
-      <c r="A59" s="265"/>
-      <c r="B59" s="265"/>
-      <c r="C59" s="256" t="s">
+      <c r="A59" s="251"/>
+      <c r="B59" s="251"/>
+      <c r="C59" s="246" t="s">
         <v>230</v>
       </c>
-      <c r="D59" s="256"/>
-      <c r="E59" s="263">
+      <c r="D59" s="246"/>
+      <c r="E59" s="249">
         <f>SUM(E55:F58)</f>
         <v>700000</v>
       </c>
-      <c r="F59" s="256"/>
+      <c r="F59" s="246"/>
     </row>
     <row r="60" spans="1:6" ht="15.75" customHeight="1" thickTop="1">
-      <c r="A60" s="262" t="s">
+      <c r="A60" s="250" t="s">
         <v>235</v>
       </c>
-      <c r="B60" s="262"/>
-      <c r="C60" s="258" t="s">
+      <c r="B60" s="250"/>
+      <c r="C60" s="252" t="s">
         <v>245</v>
       </c>
-      <c r="D60" s="258"/>
-      <c r="E60" s="260">
+      <c r="D60" s="252"/>
+      <c r="E60" s="256">
         <f>('Presupuesto Inicial'!B12+'Presupuesto Inicial'!B13)+('Presupuesto Inicial'!B11*6)+('Salarios, gastos y costos'!K11*12)</f>
         <v>7848920</v>
       </c>
-      <c r="F60" s="260"/>
+      <c r="F60" s="256"/>
     </row>
     <row r="61" spans="1:6" ht="15.75" customHeight="1" thickBot="1">
-      <c r="A61" s="262"/>
-      <c r="B61" s="262"/>
-      <c r="C61" s="259" t="s">
+      <c r="A61" s="250"/>
+      <c r="B61" s="250"/>
+      <c r="C61" s="254" t="s">
         <v>233</v>
       </c>
-      <c r="D61" s="259"/>
-      <c r="E61" s="261">
+      <c r="D61" s="254"/>
+      <c r="E61" s="257">
         <f>'Presupuesto Inicial'!B2</f>
         <v>116700</v>
       </c>
-      <c r="F61" s="261"/>
+      <c r="F61" s="257"/>
     </row>
     <row r="62" spans="1:6" ht="15.75" customHeight="1" thickTop="1" thickBot="1">
-      <c r="A62" s="262"/>
-      <c r="B62" s="262"/>
-      <c r="C62" s="256" t="s">
+      <c r="A62" s="250"/>
+      <c r="B62" s="250"/>
+      <c r="C62" s="246" t="s">
         <v>234</v>
       </c>
-      <c r="D62" s="256"/>
-      <c r="E62" s="263">
+      <c r="D62" s="246"/>
+      <c r="E62" s="249">
         <f>E60+E61</f>
         <v>7965620</v>
       </c>
-      <c r="F62" s="263"/>
+      <c r="F62" s="249"/>
     </row>
     <row r="63" spans="1:6" ht="15.75" customHeight="1" thickTop="1" thickBot="1">
-      <c r="A63" s="256" t="s">
+      <c r="A63" s="246" t="s">
         <v>239</v>
       </c>
-      <c r="B63" s="256"/>
-      <c r="C63" s="256"/>
-      <c r="D63" s="256"/>
-      <c r="E63" s="257">
+      <c r="B63" s="246"/>
+      <c r="C63" s="246"/>
+      <c r="D63" s="246"/>
+      <c r="E63" s="258">
         <f>E54+E59+E62</f>
         <v>119220336</v>
       </c>
-      <c r="F63" s="257"/>
+      <c r="F63" s="258"/>
     </row>
     <row r="64" spans="1:6" ht="15.75" customHeight="1" thickTop="1"/>
     <row r="65" spans="7:8" ht="15.75" customHeight="1" thickBot="1"/>
@@ -14160,20 +14778,252 @@
       <c r="H66" s="172"/>
     </row>
     <row r="67" spans="7:8" ht="15.75" customHeight="1" thickTop="1"/>
+    <row r="160" ht="15.75" customHeight="1" thickBot="1"/>
+    <row r="161" spans="50:57" ht="15.75" customHeight="1" thickTop="1" thickBot="1">
+      <c r="AX161" s="246" t="s">
+        <v>214</v>
+      </c>
+      <c r="AY161" s="246"/>
+      <c r="AZ161" s="246"/>
+      <c r="BA161" s="246"/>
+      <c r="BB161" s="246"/>
+      <c r="BC161" s="246"/>
+      <c r="BD161" s="246"/>
+      <c r="BE161" s="246"/>
+    </row>
+    <row r="162" spans="50:57" ht="15.75" customHeight="1" thickTop="1" thickBot="1">
+      <c r="AX162" s="247"/>
+      <c r="AY162" s="247"/>
+      <c r="AZ162" s="247"/>
+      <c r="BA162" s="247"/>
+      <c r="BB162" s="247"/>
+      <c r="BC162" s="247"/>
+      <c r="BD162" s="247"/>
+      <c r="BE162" s="247"/>
+    </row>
+    <row r="163" spans="50:57" s="304" customFormat="1" ht="50.25" customHeight="1" thickTop="1" thickBot="1">
+      <c r="AX163" s="302" t="s">
+        <v>182</v>
+      </c>
+      <c r="AY163" s="303" t="s">
+        <v>183</v>
+      </c>
+      <c r="AZ163" s="302" t="s">
+        <v>184</v>
+      </c>
+      <c r="BA163" s="302" t="s">
+        <v>185</v>
+      </c>
+      <c r="BB163" s="303" t="s">
+        <v>186</v>
+      </c>
+      <c r="BC163" s="303" t="s">
+        <v>187</v>
+      </c>
+      <c r="BD163" s="303" t="s">
+        <v>188</v>
+      </c>
+      <c r="BE163" s="302" t="s">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="164" spans="50:57" s="307" customFormat="1" ht="27.75" customHeight="1" thickTop="1">
+      <c r="AX164" s="305" t="s">
+        <v>190</v>
+      </c>
+      <c r="AY164" s="305" t="s">
+        <v>191</v>
+      </c>
+      <c r="AZ164" s="305" t="s">
+        <v>192</v>
+      </c>
+      <c r="BA164" s="305" t="s">
+        <v>193</v>
+      </c>
+      <c r="BB164" s="305">
+        <v>2</v>
+      </c>
+      <c r="BC164" s="306">
+        <v>55000</v>
+      </c>
+      <c r="BD164" s="306">
+        <f>BC164*BB164</f>
+        <v>110000</v>
+      </c>
+      <c r="BE164" s="305" t="s">
+        <v>194</v>
+      </c>
+    </row>
+    <row r="165" spans="50:57" ht="15.75" customHeight="1">
+      <c r="AX165" s="96" t="s">
+        <v>195</v>
+      </c>
+      <c r="AY165" s="96" t="s">
+        <v>191</v>
+      </c>
+      <c r="AZ165" s="96" t="s">
+        <v>196</v>
+      </c>
+      <c r="BA165" s="96" t="s">
+        <v>197</v>
+      </c>
+      <c r="BB165" s="96">
+        <v>1</v>
+      </c>
+      <c r="BC165" s="105">
+        <v>140000</v>
+      </c>
+      <c r="BD165" s="105">
+        <f t="shared" ref="BD165:BD169" si="1">BC165*BB165</f>
+        <v>140000</v>
+      </c>
+      <c r="BE165" s="96" t="s">
+        <v>194</v>
+      </c>
+    </row>
+    <row r="166" spans="50:57" ht="15.75" customHeight="1">
+      <c r="AX166" s="96" t="s">
+        <v>198</v>
+      </c>
+      <c r="AY166" s="96" t="s">
+        <v>191</v>
+      </c>
+      <c r="AZ166" s="96" t="s">
+        <v>196</v>
+      </c>
+      <c r="BA166" s="96" t="s">
+        <v>199</v>
+      </c>
+      <c r="BB166" s="96">
+        <v>1</v>
+      </c>
+      <c r="BC166" s="105">
+        <v>40000</v>
+      </c>
+      <c r="BD166" s="105">
+        <f t="shared" si="1"/>
+        <v>40000</v>
+      </c>
+      <c r="BE166" s="96" t="s">
+        <v>194</v>
+      </c>
+    </row>
+    <row r="167" spans="50:57" ht="15.75" customHeight="1">
+      <c r="AX167" s="96" t="s">
+        <v>200</v>
+      </c>
+      <c r="AY167" s="96" t="s">
+        <v>201</v>
+      </c>
+      <c r="AZ167" s="96" t="s">
+        <v>196</v>
+      </c>
+      <c r="BA167" s="96" t="s">
+        <v>202</v>
+      </c>
+      <c r="BB167" s="96">
+        <v>1</v>
+      </c>
+      <c r="BC167" s="105">
+        <v>40000</v>
+      </c>
+      <c r="BD167" s="105">
+        <f t="shared" si="1"/>
+        <v>40000</v>
+      </c>
+      <c r="BE167" s="96" t="s">
+        <v>194</v>
+      </c>
+    </row>
+    <row r="168" spans="50:57" ht="15.75" customHeight="1">
+      <c r="AX168" s="96" t="s">
+        <v>203</v>
+      </c>
+      <c r="AY168" s="96" t="s">
+        <v>204</v>
+      </c>
+      <c r="AZ168" s="96" t="s">
+        <v>205</v>
+      </c>
+      <c r="BA168" s="96" t="s">
+        <v>206</v>
+      </c>
+      <c r="BB168" s="96">
+        <v>7</v>
+      </c>
+      <c r="BC168" s="105">
+        <v>485000</v>
+      </c>
+      <c r="BD168" s="105">
+        <f>BC168*BB168</f>
+        <v>3395000</v>
+      </c>
+      <c r="BE168" s="96" t="s">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="169" spans="50:57" ht="15.75" customHeight="1">
+      <c r="AX169" s="96" t="s">
+        <v>207</v>
+      </c>
+      <c r="AY169" s="96" t="s">
+        <v>204</v>
+      </c>
+      <c r="AZ169" s="96" t="s">
+        <v>205</v>
+      </c>
+      <c r="BA169" s="96" t="s">
+        <v>208</v>
+      </c>
+      <c r="BB169" s="96">
+        <v>7</v>
+      </c>
+      <c r="BC169" s="105">
+        <v>80000</v>
+      </c>
+      <c r="BD169" s="105">
+        <f t="shared" ref="BD169:BD170" si="2">BC169*BB169</f>
+        <v>560000</v>
+      </c>
+      <c r="BE169" s="96" t="s">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="170" spans="50:57" ht="15.75" customHeight="1">
+      <c r="AY170" s="101"/>
+      <c r="AZ170" s="101"/>
+      <c r="BA170" s="101"/>
+      <c r="BB170" s="101"/>
+      <c r="BC170" s="301" t="s">
+        <v>293</v>
+      </c>
+      <c r="BD170" s="222">
+        <f>SUBTOTAL(109,PUBLICIDAD10[Costo total])</f>
+        <v>4285000</v>
+      </c>
+      <c r="BE170" s="101"/>
+    </row>
   </sheetData>
-  <mergeCells count="45">
-    <mergeCell ref="A1:B1"/>
-    <mergeCell ref="A17:B17"/>
-    <mergeCell ref="D1:E1"/>
-    <mergeCell ref="D17:E17"/>
-    <mergeCell ref="J1:K1"/>
-    <mergeCell ref="E51:F51"/>
-    <mergeCell ref="E52:F52"/>
-    <mergeCell ref="A34:H34"/>
-    <mergeCell ref="A35:H35"/>
-    <mergeCell ref="A47:D47"/>
-    <mergeCell ref="E47:F47"/>
-    <mergeCell ref="A46:F46"/>
+  <mergeCells count="47">
+    <mergeCell ref="AX161:BE161"/>
+    <mergeCell ref="AX162:BE162"/>
+    <mergeCell ref="A63:D63"/>
+    <mergeCell ref="E63:F63"/>
+    <mergeCell ref="C60:D60"/>
+    <mergeCell ref="C61:D61"/>
+    <mergeCell ref="E60:F60"/>
+    <mergeCell ref="E61:F61"/>
+    <mergeCell ref="A60:B62"/>
+    <mergeCell ref="C62:D62"/>
+    <mergeCell ref="E62:F62"/>
+    <mergeCell ref="C57:D57"/>
+    <mergeCell ref="C58:D58"/>
+    <mergeCell ref="C59:D59"/>
+    <mergeCell ref="E55:F55"/>
+    <mergeCell ref="E56:F56"/>
+    <mergeCell ref="E57:F57"/>
+    <mergeCell ref="E58:F58"/>
+    <mergeCell ref="E59:F59"/>
     <mergeCell ref="C54:D54"/>
     <mergeCell ref="E54:F54"/>
     <mergeCell ref="A48:B54"/>
@@ -14190,23 +15040,18 @@
     <mergeCell ref="E48:F48"/>
     <mergeCell ref="E49:F49"/>
     <mergeCell ref="E50:F50"/>
-    <mergeCell ref="C57:D57"/>
-    <mergeCell ref="C58:D58"/>
-    <mergeCell ref="C59:D59"/>
-    <mergeCell ref="E55:F55"/>
-    <mergeCell ref="E56:F56"/>
-    <mergeCell ref="E57:F57"/>
-    <mergeCell ref="E58:F58"/>
-    <mergeCell ref="E59:F59"/>
-    <mergeCell ref="A63:D63"/>
-    <mergeCell ref="E63:F63"/>
-    <mergeCell ref="C60:D60"/>
-    <mergeCell ref="C61:D61"/>
-    <mergeCell ref="E60:F60"/>
-    <mergeCell ref="E61:F61"/>
-    <mergeCell ref="A60:B62"/>
-    <mergeCell ref="C62:D62"/>
-    <mergeCell ref="E62:F62"/>
+    <mergeCell ref="E51:F51"/>
+    <mergeCell ref="E52:F52"/>
+    <mergeCell ref="A34:H34"/>
+    <mergeCell ref="A35:H35"/>
+    <mergeCell ref="A47:D47"/>
+    <mergeCell ref="E47:F47"/>
+    <mergeCell ref="A46:F46"/>
+    <mergeCell ref="A1:B1"/>
+    <mergeCell ref="A17:B17"/>
+    <mergeCell ref="D1:E1"/>
+    <mergeCell ref="D17:E17"/>
+    <mergeCell ref="J1:K1"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="N31" r:id="rId1"/>
@@ -14215,8 +15060,9 @@
   <pageSetup paperSize="9" orientation="portrait" r:id="rId2"/>
   <drawing r:id="rId3"/>
   <legacyDrawing r:id="rId4"/>
-  <tableParts count="1">
+  <tableParts count="2">
     <tablePart r:id="rId5"/>
+    <tablePart r:id="rId6"/>
   </tableParts>
 </worksheet>
 </file>
@@ -14237,28 +15083,28 @@
   <sheetData>
     <row r="1" spans="1:4" ht="15.75" customHeight="1" thickBot="1"/>
     <row r="2" spans="1:4" ht="15.75" customHeight="1" thickTop="1" thickBot="1">
-      <c r="A2" s="256" t="s">
+      <c r="A2" s="246" t="s">
         <v>7</v>
       </c>
-      <c r="B2" s="274"/>
-      <c r="C2" s="274"/>
-      <c r="D2" s="274"/>
+      <c r="B2" s="259"/>
+      <c r="C2" s="259"/>
+      <c r="D2" s="259"/>
     </row>
     <row r="3" spans="1:4" ht="15.75" customHeight="1" thickTop="1">
-      <c r="A3" s="276" t="s">
+      <c r="A3" s="261" t="s">
         <v>14</v>
       </c>
-      <c r="B3" s="271"/>
-      <c r="C3" s="276" t="s">
+      <c r="B3" s="242"/>
+      <c r="C3" s="261" t="s">
         <v>15</v>
       </c>
-      <c r="D3" s="271"/>
+      <c r="D3" s="242"/>
     </row>
     <row r="4" spans="1:4" ht="15.75" customHeight="1">
-      <c r="A4" s="277" t="s">
+      <c r="A4" s="262" t="s">
         <v>16</v>
       </c>
-      <c r="B4" s="280">
+      <c r="B4" s="265">
         <v>1500000</v>
       </c>
       <c r="C4" s="18" t="s">
@@ -14269,16 +15115,16 @@
       </c>
     </row>
     <row r="5" spans="1:4" ht="15.75" customHeight="1">
-      <c r="A5" s="278"/>
-      <c r="B5" s="278"/>
-      <c r="C5" s="276" t="s">
+      <c r="A5" s="263"/>
+      <c r="B5" s="263"/>
+      <c r="C5" s="261" t="s">
         <v>35</v>
       </c>
-      <c r="D5" s="271"/>
+      <c r="D5" s="242"/>
     </row>
     <row r="6" spans="1:4" ht="15.75" customHeight="1">
-      <c r="A6" s="278"/>
-      <c r="B6" s="278"/>
+      <c r="A6" s="263"/>
+      <c r="B6" s="263"/>
       <c r="C6" s="18" t="s">
         <v>36</v>
       </c>
@@ -14287,8 +15133,8 @@
       </c>
     </row>
     <row r="7" spans="1:4" ht="15.75" customHeight="1">
-      <c r="A7" s="278"/>
-      <c r="B7" s="278"/>
+      <c r="A7" s="263"/>
+      <c r="B7" s="263"/>
       <c r="C7" s="18" t="s">
         <v>39</v>
       </c>
@@ -14297,8 +15143,8 @@
       </c>
     </row>
     <row r="8" spans="1:4" ht="15.75" customHeight="1">
-      <c r="A8" s="279"/>
-      <c r="B8" s="279"/>
+      <c r="A8" s="264"/>
+      <c r="B8" s="264"/>
       <c r="C8" s="18" t="s">
         <v>236</v>
       </c>
@@ -14323,15 +15169,15 @@
       </c>
     </row>
     <row r="10" spans="1:4" ht="15.75" customHeight="1" thickTop="1" thickBot="1">
-      <c r="A10" s="256" t="s">
+      <c r="A10" s="246" t="s">
         <v>53</v>
       </c>
-      <c r="B10" s="274"/>
-      <c r="C10" s="275">
+      <c r="B10" s="259"/>
+      <c r="C10" s="260">
         <f>D4+D9</f>
         <v>1500000</v>
       </c>
-      <c r="D10" s="274"/>
+      <c r="D10" s="259"/>
     </row>
     <row r="11" spans="1:4" ht="15.75" customHeight="1" thickTop="1"/>
     <row r="12" spans="1:4" ht="15.75" customHeight="1">
@@ -14367,49 +15213,49 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:6" ht="15">
-      <c r="B2" s="281" t="s">
+      <c r="B2" s="266" t="s">
         <v>238</v>
       </c>
-      <c r="C2" s="281"/>
-      <c r="D2" s="281"/>
-      <c r="E2" s="281"/>
-      <c r="F2" s="281"/>
+      <c r="C2" s="266"/>
+      <c r="D2" s="266"/>
+      <c r="E2" s="266"/>
+      <c r="F2" s="266"/>
     </row>
     <row r="3" spans="2:6">
-      <c r="B3" s="268" t="s">
+      <c r="B3" s="247" t="s">
         <v>240</v>
       </c>
-      <c r="C3" s="268"/>
-      <c r="D3" s="268"/>
-      <c r="E3" s="283">
+      <c r="C3" s="247"/>
+      <c r="D3" s="247"/>
+      <c r="E3" s="268">
         <f>'Salarios, gastos y costos'!E62:F62</f>
         <v>7965620</v>
       </c>
-      <c r="F3" s="283"/>
+      <c r="F3" s="268"/>
     </row>
     <row r="4" spans="2:6">
-      <c r="B4" s="284" t="s">
+      <c r="B4" s="269" t="s">
         <v>241</v>
       </c>
-      <c r="C4" s="268"/>
-      <c r="D4" s="268"/>
-      <c r="E4" s="285">
+      <c r="C4" s="247"/>
+      <c r="D4" s="247"/>
+      <c r="E4" s="270">
         <f>'Salarios, gastos y costos'!B11*7</f>
         <v>64490251</v>
       </c>
-      <c r="F4" s="285"/>
+      <c r="F4" s="270"/>
     </row>
     <row r="5" spans="2:6" ht="15">
-      <c r="B5" s="281" t="s">
+      <c r="B5" s="266" t="s">
         <v>210</v>
       </c>
-      <c r="C5" s="281"/>
-      <c r="D5" s="281"/>
-      <c r="E5" s="282">
+      <c r="C5" s="266"/>
+      <c r="D5" s="266"/>
+      <c r="E5" s="267">
         <f>SUM(E3:F4)</f>
         <v>72455871</v>
       </c>
-      <c r="F5" s="282"/>
+      <c r="F5" s="267"/>
     </row>
   </sheetData>
   <mergeCells count="7">
@@ -14433,16 +15279,16 @@
   </sheetPr>
   <dimension ref="A1:Y24"/>
   <sheetViews>
-    <sheetView zoomScale="175" zoomScaleNormal="175" workbookViewId="0">
-      <pane xSplit="1" topLeftCell="P1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="B1" sqref="B1:G1048576"/>
+    <sheetView topLeftCell="A3" zoomScale="175" zoomScaleNormal="175" workbookViewId="0">
+      <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="F113" sqref="F113"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1"/>
   <cols>
     <col min="1" max="1" width="23.140625" customWidth="1"/>
-    <col min="2" max="2" width="16.42578125" hidden="1" customWidth="1"/>
-    <col min="3" max="7" width="14.5703125" hidden="1" customWidth="1"/>
+    <col min="2" max="2" width="16.42578125" customWidth="1"/>
+    <col min="3" max="7" width="14.5703125" customWidth="1"/>
     <col min="8" max="8" width="7.85546875" customWidth="1"/>
     <col min="9" max="9" width="14.5703125" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="8" customWidth="1"/>
@@ -14458,6 +15304,8 @@
     <col min="21" max="21" width="16.7109375" bestFit="1" customWidth="1"/>
     <col min="22" max="22" width="15.7109375" bestFit="1" customWidth="1"/>
     <col min="24" max="24" width="35.85546875" bestFit="1" customWidth="1"/>
+    <col min="52" max="52" width="14.42578125" customWidth="1"/>
+    <col min="61" max="61" width="14.42578125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:25" ht="12.75">
@@ -14480,30 +15328,30 @@
       <c r="G1" s="123" t="s">
         <v>62</v>
       </c>
-      <c r="H1" s="287" t="s">
+      <c r="H1" s="272" t="s">
         <v>63</v>
       </c>
-      <c r="I1" s="271"/>
-      <c r="J1" s="286" t="s">
+      <c r="I1" s="242"/>
+      <c r="J1" s="271" t="s">
         <v>64</v>
       </c>
-      <c r="K1" s="271"/>
-      <c r="L1" s="286" t="s">
+      <c r="K1" s="242"/>
+      <c r="L1" s="271" t="s">
         <v>65</v>
       </c>
-      <c r="M1" s="271"/>
-      <c r="N1" s="286" t="s">
+      <c r="M1" s="242"/>
+      <c r="N1" s="271" t="s">
         <v>66</v>
       </c>
-      <c r="O1" s="271"/>
-      <c r="P1" s="286" t="s">
+      <c r="O1" s="242"/>
+      <c r="P1" s="271" t="s">
         <v>67</v>
       </c>
-      <c r="Q1" s="271"/>
-      <c r="R1" s="286" t="s">
+      <c r="Q1" s="242"/>
+      <c r="R1" s="271" t="s">
         <v>68</v>
       </c>
-      <c r="S1" s="271"/>
+      <c r="S1" s="242"/>
       <c r="U1" s="140" t="s">
         <v>70</v>
       </c>
@@ -15793,45 +16641,45 @@
     <mergeCell ref="P1:Q1"/>
   </mergeCells>
   <conditionalFormatting sqref="B1:S7 B17:S994 B8:C14 H8:S16 B16:C16">
-    <cfRule type="cellIs" dxfId="30" priority="15" operator="lessThan">
+    <cfRule type="cellIs" dxfId="22" priority="15" operator="lessThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I8">
-    <cfRule type="cellIs" dxfId="29" priority="13" operator="lessThan">
+    <cfRule type="cellIs" dxfId="21" priority="13" operator="lessThan">
       <formula>0</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="28" priority="14" operator="lessThan">
+    <cfRule type="cellIs" dxfId="20" priority="14" operator="lessThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H2:S16">
-    <cfRule type="cellIs" dxfId="27" priority="7" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="19" priority="7" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D2:G14 D16:G16 B15:G15">
-    <cfRule type="cellIs" dxfId="26" priority="5" operator="lessThan">
+    <cfRule type="cellIs" dxfId="18" priority="5" operator="lessThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B8:C8">
-    <cfRule type="cellIs" dxfId="25" priority="4" operator="lessThan">
+    <cfRule type="cellIs" dxfId="17" priority="4" operator="lessThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B11:C11">
-    <cfRule type="cellIs" dxfId="24" priority="3" operator="lessThan">
+    <cfRule type="cellIs" dxfId="16" priority="3" operator="lessThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B14:C14">
-    <cfRule type="cellIs" dxfId="23" priority="2" operator="lessThan">
+    <cfRule type="cellIs" dxfId="15" priority="2" operator="lessThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B16:C16">
-    <cfRule type="cellIs" dxfId="22" priority="1" operator="lessThan">
+    <cfRule type="cellIs" dxfId="14" priority="1" operator="lessThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
@@ -15846,7 +16694,7 @@
   <dimension ref="A1:R25"/>
   <sheetViews>
     <sheetView zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <selection activeCell="K2" sqref="K2"/>
+      <selection activeCell="B2" sqref="B1:E1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1"/>
@@ -15863,26 +16711,26 @@
   <sheetData>
     <row r="1" spans="1:18" ht="12.75">
       <c r="A1" s="25"/>
-      <c r="B1" s="286" t="s">
+      <c r="B1" s="271" t="s">
         <v>70</v>
       </c>
-      <c r="C1" s="271"/>
-      <c r="D1" s="286" t="s">
+      <c r="C1" s="242"/>
+      <c r="D1" s="271" t="s">
         <v>71</v>
       </c>
-      <c r="E1" s="271"/>
-      <c r="F1" s="286" t="s">
+      <c r="E1" s="242"/>
+      <c r="F1" s="271" t="s">
         <v>72</v>
       </c>
-      <c r="G1" s="271"/>
-      <c r="H1" s="286" t="s">
+      <c r="G1" s="242"/>
+      <c r="H1" s="271" t="s">
         <v>74</v>
       </c>
-      <c r="I1" s="271"/>
-      <c r="J1" s="288" t="s">
+      <c r="I1" s="242"/>
+      <c r="J1" s="273" t="s">
         <v>75</v>
       </c>
-      <c r="K1" s="289"/>
+      <c r="K1" s="274"/>
       <c r="L1" s="27"/>
       <c r="M1" s="27"/>
       <c r="N1" s="27"/>
@@ -16764,7 +17612,7 @@
     <mergeCell ref="J1:K1"/>
   </mergeCells>
   <conditionalFormatting sqref="A1:K16">
-    <cfRule type="cellIs" dxfId="21" priority="1" operator="lessThan">
+    <cfRule type="cellIs" dxfId="13" priority="1" operator="lessThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
@@ -16816,58 +17664,58 @@
   <sheetData>
     <row r="1" spans="1:29" s="149" customFormat="1" ht="15.75" customHeight="1">
       <c r="A1" s="152"/>
-      <c r="B1" s="290" t="s">
+      <c r="B1" s="275" t="s">
         <v>104</v>
       </c>
-      <c r="C1" s="291"/>
-      <c r="D1" s="290" t="s">
+      <c r="C1" s="276"/>
+      <c r="D1" s="275" t="s">
         <v>55</v>
       </c>
-      <c r="E1" s="291"/>
-      <c r="F1" s="290" t="s">
+      <c r="E1" s="276"/>
+      <c r="F1" s="275" t="s">
         <v>58</v>
       </c>
-      <c r="G1" s="291"/>
-      <c r="H1" s="290" t="s">
+      <c r="G1" s="276"/>
+      <c r="H1" s="275" t="s">
         <v>59</v>
       </c>
-      <c r="I1" s="291"/>
-      <c r="J1" s="290" t="s">
+      <c r="I1" s="276"/>
+      <c r="J1" s="275" t="s">
         <v>60</v>
       </c>
-      <c r="K1" s="291"/>
-      <c r="L1" s="290" t="s">
+      <c r="K1" s="276"/>
+      <c r="L1" s="275" t="s">
         <v>61</v>
       </c>
-      <c r="M1" s="291"/>
-      <c r="N1" s="290" t="s">
+      <c r="M1" s="276"/>
+      <c r="N1" s="275" t="s">
         <v>62</v>
       </c>
-      <c r="O1" s="291"/>
-      <c r="P1" s="290" t="s">
+      <c r="O1" s="276"/>
+      <c r="P1" s="275" t="s">
         <v>63</v>
       </c>
-      <c r="Q1" s="291"/>
-      <c r="R1" s="290" t="s">
+      <c r="Q1" s="276"/>
+      <c r="R1" s="275" t="s">
         <v>64</v>
       </c>
-      <c r="S1" s="291"/>
-      <c r="T1" s="290" t="s">
+      <c r="S1" s="276"/>
+      <c r="T1" s="275" t="s">
         <v>65</v>
       </c>
-      <c r="U1" s="291"/>
-      <c r="V1" s="290" t="s">
+      <c r="U1" s="276"/>
+      <c r="V1" s="275" t="s">
         <v>66</v>
       </c>
-      <c r="W1" s="291"/>
-      <c r="X1" s="290" t="s">
+      <c r="W1" s="276"/>
+      <c r="X1" s="275" t="s">
         <v>67</v>
       </c>
-      <c r="Y1" s="291"/>
-      <c r="Z1" s="290" t="s">
+      <c r="Y1" s="276"/>
+      <c r="Z1" s="275" t="s">
         <v>68</v>
       </c>
-      <c r="AA1" s="291"/>
+      <c r="AA1" s="276"/>
     </row>
     <row r="2" spans="1:29" ht="15.75" customHeight="1">
       <c r="A2" s="30" t="s">
@@ -18127,6 +18975,12 @@
     </row>
   </sheetData>
   <mergeCells count="13">
+    <mergeCell ref="X1:Y1"/>
+    <mergeCell ref="Z1:AA1"/>
+    <mergeCell ref="R1:S1"/>
+    <mergeCell ref="P1:Q1"/>
+    <mergeCell ref="V1:W1"/>
+    <mergeCell ref="T1:U1"/>
     <mergeCell ref="N1:O1"/>
     <mergeCell ref="J1:K1"/>
     <mergeCell ref="H1:I1"/>
@@ -18134,12 +18988,6 @@
     <mergeCell ref="B1:C1"/>
     <mergeCell ref="F1:G1"/>
     <mergeCell ref="L1:M1"/>
-    <mergeCell ref="X1:Y1"/>
-    <mergeCell ref="Z1:AA1"/>
-    <mergeCell ref="R1:S1"/>
-    <mergeCell ref="P1:Q1"/>
-    <mergeCell ref="V1:W1"/>
-    <mergeCell ref="T1:U1"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
@@ -18168,30 +19016,30 @@
   <sheetData>
     <row r="1" spans="1:20" ht="15.75" customHeight="1">
       <c r="A1" s="26"/>
-      <c r="B1" s="292" t="s">
+      <c r="B1" s="277" t="s">
         <v>73</v>
       </c>
-      <c r="C1" s="271"/>
-      <c r="D1" s="292" t="s">
+      <c r="C1" s="242"/>
+      <c r="D1" s="277" t="s">
         <v>70</v>
       </c>
-      <c r="E1" s="271"/>
-      <c r="F1" s="292" t="s">
+      <c r="E1" s="242"/>
+      <c r="F1" s="277" t="s">
         <v>71</v>
       </c>
-      <c r="G1" s="271"/>
-      <c r="H1" s="292" t="s">
+      <c r="G1" s="242"/>
+      <c r="H1" s="277" t="s">
         <v>72</v>
       </c>
-      <c r="I1" s="271"/>
-      <c r="J1" s="292" t="s">
+      <c r="I1" s="242"/>
+      <c r="J1" s="277" t="s">
         <v>74</v>
       </c>
-      <c r="K1" s="271"/>
-      <c r="L1" s="292" t="s">
+      <c r="K1" s="242"/>
+      <c r="L1" s="277" t="s">
         <v>75</v>
       </c>
-      <c r="M1" s="271"/>
+      <c r="M1" s="242"/>
       <c r="N1" s="28"/>
       <c r="O1" s="28"/>
       <c r="P1" s="28"/>

</xml_diff>

<commit_message>
Comi anteproyecto prnultima version XD y no lo aprobaron hapy hapy XD
</commit_message>
<xml_diff>
--- a/Analisis_financiero_Inclusoft_test.xlsx
+++ b/Analisis_financiero_Inclusoft_test.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="21570" windowHeight="8145" tabRatio="920" firstSheet="4" activeTab="9"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="21570" windowHeight="8145" tabRatio="920" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Presupuesto Inicial" sheetId="1" r:id="rId1"/>
@@ -10254,7 +10254,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:S42"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D25" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+    <sheetView topLeftCell="D25" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
       <selection activeCell="G42" sqref="G42:I42"/>
     </sheetView>
   </sheetViews>
@@ -14474,8 +14474,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:O35"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C8" sqref="C8"/>
+    <sheetView tabSelected="1" topLeftCell="G1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="O2" sqref="O2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1"/>

</xml_diff>

<commit_message>
se arregla la estructura de las tablas de listado de tablas y listado de figuras, se da por terminado la revision del documento
</commit_message>
<xml_diff>
--- a/Analisis_financiero_Inclusoft_test.xlsx
+++ b/Analisis_financiero_Inclusoft_test.xlsx
@@ -5,7 +5,7 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Abeja\Documents\Respositorios\Inclusoft\Documentos\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="H:\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -56,7 +56,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="546" uniqueCount="307">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="543" uniqueCount="310">
   <si>
     <t xml:space="preserve">Concepto
 </t>
@@ -989,6 +989,15 @@
   </si>
   <si>
     <t>PASIVOS</t>
+  </si>
+  <si>
+    <t>egresos</t>
+  </si>
+  <si>
+    <t>utilidad</t>
+  </si>
+  <si>
+    <t>Diferidos</t>
   </si>
 </sst>
 </file>
@@ -1648,7 +1657,7 @@
     <xf numFmtId="165" fontId="17" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="26" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="342">
+  <cellXfs count="343">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -2173,6 +2182,7 @@
     <xf numFmtId="166" fontId="34" fillId="0" borderId="28" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
+    <xf numFmtId="170" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="19" fillId="4" borderId="12" xfId="3" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -3627,7 +3637,7 @@
           <c:idx val="0"/>
           <c:order val="0"/>
           <c:tx>
-            <c:v>Proyeccion de Ventas</c:v>
+            <c:v>Proyeccion de ventas</c:v>
           </c:tx>
           <c:spPr>
             <a:solidFill>
@@ -3641,43 +3651,29 @@
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:strRef>
-              <c:f>'Tabla Crecimiento'!$A$2:$A$13</c:f>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+                  <c15:fullRef>
+                    <c15:sqref>'Tabla Crecimiento'!$A$9:$A$13</c15:sqref>
+                  </c15:fullRef>
+                </c:ext>
+              </c:extLst>
+              <c:f>'Tabla Crecimiento'!$A$9:$A$13</c:f>
               <c:strCache>
-                <c:ptCount val="12"/>
+                <c:ptCount val="5"/>
                 <c:pt idx="0">
-                  <c:v>Mes 1-6</c:v>
+                  <c:v>Año 1</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>Mes 7</c:v>
+                  <c:v>Año 2</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>Mes 8</c:v>
+                  <c:v>Año 3</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>Mes 9</c:v>
+                  <c:v>Año 4</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>Mes 10</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>Mes 11</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>Mes 12</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>Año 1</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>Año 2</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>Año 3</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>Año 4</c:v>
-                </c:pt>
-                <c:pt idx="11">
                   <c:v>Año 5</c:v>
                 </c:pt>
               </c:strCache>
@@ -3685,44 +3681,30 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'Tabla Crecimiento'!$B$2:$B$13</c:f>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+                  <c15:fullRef>
+                    <c15:sqref>'Tabla Crecimiento'!$B$9:$B$13</c15:sqref>
+                  </c15:fullRef>
+                </c:ext>
+              </c:extLst>
+              <c:f>'Tabla Crecimiento'!$B$9:$B$13</c:f>
               <c:numCache>
                 <c:formatCode>#,##0</c:formatCode>
-                <c:ptCount val="12"/>
+                <c:ptCount val="5"/>
                 <c:pt idx="0">
-                  <c:v>0</c:v>
+                  <c:v>10019.503746304383</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>3252.8577359756564</c:v>
+                  <c:v>65175.619953865986</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>4097.8788914930747</c:v>
+                  <c:v>94322.751322401688</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>5150.3451169723749</c:v>
+                  <c:v>96751.601360591376</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>6454.3186472262878</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>8059.4342902610779</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>10019.503746304383</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>10019.503746304383</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>65175.619953865986</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>94322.751322401688</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>96751.601360591376</c:v>
-                </c:pt>
-                <c:pt idx="11">
                   <c:v>96891.657618714249</c:v>
                 </c:pt>
               </c:numCache>
@@ -3730,7 +3712,7 @@
           </c:val>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000000-6B20-4300-A03E-0B4FA17B907F}"/>
+              <c16:uniqueId val="{00000000-2E6E-4C82-ABA7-92ECCBF986C2}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -4078,7 +4060,7 @@
             </a:r>
             <a:r>
               <a:rPr lang="en-US" baseline="0"/>
-              <a:t> de Ingresos * Ventas</a:t>
+              <a:t> de Ingresos por Ventas</a:t>
             </a:r>
             <a:endParaRPr lang="en-US"/>
           </a:p>
@@ -4124,7 +4106,7 @@
           <c:idx val="0"/>
           <c:order val="0"/>
           <c:tx>
-            <c:v>Proyeccion Ventas</c:v>
+            <c:v>Proyeccion Ingresos</c:v>
           </c:tx>
           <c:spPr>
             <a:solidFill>
@@ -4138,43 +4120,22 @@
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:strRef>
-              <c:f>'Tabla Crecimiento'!$A$2:$A$13</c:f>
+              <c:f>'Tabla Crecimiento'!$A$9:$A$13</c:f>
               <c:strCache>
-                <c:ptCount val="12"/>
+                <c:ptCount val="5"/>
                 <c:pt idx="0">
-                  <c:v>Mes 1-6</c:v>
+                  <c:v>Año 1</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>Mes 7</c:v>
+                  <c:v>Año 2</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>Mes 8</c:v>
+                  <c:v>Año 3</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>Mes 9</c:v>
+                  <c:v>Año 4</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>Mes 10</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>Mes 11</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>Mes 12</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>Año 1</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>Año 2</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>Año 3</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>Año 4</c:v>
-                </c:pt>
-                <c:pt idx="11">
                   <c:v>Año 5</c:v>
                 </c:pt>
               </c:strCache>
@@ -4182,44 +4143,23 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'Tabla Crecimiento'!$C$2:$C$13</c:f>
+              <c:f>'Tabla Crecimiento'!$C$9:$C$13</c:f>
               <c:numCache>
                 <c:formatCode>[$$-240A]\ #,##0.00</c:formatCode>
-                <c:ptCount val="12"/>
+                <c:ptCount val="5"/>
                 <c:pt idx="0">
-                  <c:v>0</c:v>
+                  <c:v>199937928.20591292</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>17561259.741141878</c:v>
+                  <c:v>351864755.14782721</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>22123290.178157054</c:v>
+                  <c:v>509221881.16382653</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>27805257.929162167</c:v>
+                  <c:v>522334556.18837321</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>34845042.549037121</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>43510608.340665355</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>54092469.46774932</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>54092469.46774932</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>351864755.14782721</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>509221881.16382653</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>522334556.18837321</c:v>
-                </c:pt>
-                <c:pt idx="11">
                   <c:v>523090680.34961951</c:v>
                 </c:pt>
               </c:numCache>
@@ -4227,7 +4167,7 @@
           </c:val>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000000-B885-4609-BB3F-4D9377408547}"/>
+              <c16:uniqueId val="{00000000-F804-4CA9-BFB3-A37D02C00D15}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -4703,29 +4643,29 @@
                   <c:v>10249282</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>16613549.782486973</c:v>
+                  <c:v>15146882.782486973</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>25988757.65340396</c:v>
+                  <c:v>23055423.65340396</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>39114064.239984326</c:v>
+                  <c:v>34714063.239984326</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>56885628.675682157</c:v>
+                  <c:v>51018960.675682157</c:v>
                 </c:pt>
                 <c:pt idx="22">
-                  <c:v>80376466.533854634</c:v>
+                  <c:v>73043131.533854634</c:v>
                 </c:pt>
                 <c:pt idx="24">
-                  <c:v>110851332.73590252</c:v>
+                  <c:v>102051330.73590252</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000000-4663-45EA-A198-72AC6BB2F9C2}"/>
+              <c16:uniqueId val="{00000000-1A88-465B-AA50-29F7A8001D97}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -4823,7 +4763,7 @@
                 </c:val>
                 <c:extLst>
                   <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-                    <c16:uniqueId val="{00000001-4663-45EA-A198-72AC6BB2F9C2}"/>
+                    <c16:uniqueId val="{00000001-1A88-465B-AA50-29F7A8001D97}"/>
                   </c:ext>
                 </c:extLst>
               </c15:ser>
@@ -5176,21 +5116,17 @@
               </a:defRPr>
             </a:pPr>
             <a:r>
-              <a:rPr lang="es-ES"/>
-              <a:t>Flujo de Caja primer año</a:t>
+              <a:rPr lang="es-CO"/>
+              <a:t>Flujo de</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="es-CO" baseline="0"/>
+              <a:t> Caja (5 años)</a:t>
             </a:r>
             <a:endParaRPr lang="es-CO"/>
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout>
-        <c:manualLayout>
-          <c:xMode val="edge"/>
-          <c:yMode val="edge"/>
-          <c:x val="0.2947152230971129"/>
-          <c:y val="1.8518518518518517E-2"/>
-        </c:manualLayout>
-      </c:layout>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -5222,17 +5158,7 @@
     </c:title>
     <c:autoTitleDeleted val="0"/>
     <c:plotArea>
-      <c:layout>
-        <c:manualLayout>
-          <c:layoutTarget val="inner"/>
-          <c:xMode val="edge"/>
-          <c:yMode val="edge"/>
-          <c:x val="0.35727882808165468"/>
-          <c:y val="0.18300925925925926"/>
-          <c:w val="0.59902368810777562"/>
-          <c:h val="0.7013192621755614"/>
-        </c:manualLayout>
-      </c:layout>
+      <c:layout/>
       <c:barChart>
         <c:barDir val="col"/>
         <c:grouping val="clustered"/>
@@ -5241,11 +5167,59 @@
           <c:idx val="0"/>
           <c:order val="0"/>
           <c:tx>
-            <c:v>flujo de caja</c:v>
+            <c:v>Ingresos por Ventas</c:v>
           </c:tx>
           <c:spPr>
             <a:solidFill>
-              <a:schemeClr val="accent1"/>
+              <a:srgbClr val="92D050"/>
+            </a:solidFill>
+            <a:ln>
+              <a:solidFill>
+                <a:srgbClr val="92D050"/>
+              </a:solidFill>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:val>
+            <c:numRef>
+              <c:f>('Flujo de Caja (Profesor) - 5 añ'!$D$2,'Flujo de Caja (Profesor) - 5 añ'!$F$2,'Flujo de Caja (Profesor) - 5 añ'!$H$2,'Flujo de Caja (Profesor) - 5 añ'!$J$2,'Flujo de Caja (Profesor) - 5 añ'!$L$2)</c:f>
+              <c:numCache>
+                <c:formatCode>"$"#,##0.00</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>199937934.20591292</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>351864755.14782721</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>509221881.16382653</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>522334556.18837321</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>523090680.34961951</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{0000000C-979F-4BDE-8BEA-C7C15B2E34FA}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:v>Utilidad</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:srgbClr val="FFC000"/>
             </a:solidFill>
             <a:ln>
               <a:noFill/>
@@ -5253,62 +5227,79 @@
             <a:effectLst/>
           </c:spPr>
           <c:invertIfNegative val="0"/>
-          <c:cat>
-            <c:strRef>
-              <c:f>'Flujo de Caja (Profesor) - 5 añ'!$D$42:$I$42</c:f>
-              <c:strCache>
-                <c:ptCount val="6"/>
+          <c:val>
+            <c:numRef>
+              <c:f>('Flujo de Caja (Profesor) - 5 añ'!$D$28,'Flujo de Caja (Profesor) - 5 añ'!$F$28,'Flujo de Caja (Profesor) - 5 añ'!$H$28,'Flujo de Caja (Profesor) - 5 añ'!$J$28,'Flujo de Caja (Profesor) - 5 añ'!$L$28)</c:f>
+              <c:numCache>
+                <c:formatCode>"$"#,##0.00</c:formatCode>
+                <c:ptCount val="5"/>
                 <c:pt idx="0">
-                  <c:v>Año 0</c:v>
+                  <c:v>32572833.289787471</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>Año 1</c:v>
+                  <c:v>159745157.08126181</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>Año 2</c:v>
+                  <c:v>263206333.91240484</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>Año 3</c:v>
+                  <c:v>271466173.08918911</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>Año 4</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>Año 5</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:cat>
-          <c:val>
-            <c:numRef>
-              <c:f>('Flujo de Caja (Profesor) - 5 añ'!$B$19,'Flujo de Caja (Profesor) - 5 añ'!$D$19,'Flujo de Caja (Profesor) - 5 añ'!$F$19,'Flujo de Caja (Profesor) - 5 añ'!$H$19,'Flujo de Caja (Profesor) - 5 añ'!$J$19,'Flujo de Caja (Profesor) - 5 añ'!$L$19)</c:f>
-              <c:numCache>
-                <c:formatCode>"$"#,##0.00</c:formatCode>
-                <c:ptCount val="6"/>
-                <c:pt idx="0">
-                  <c:v>-72456000</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>33272833.301936988</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>160445157.08126184</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>263906333.91240484</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>272166173.08918917</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>272507404.49984503</c:v>
+                  <c:v>271807404.49984503</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000005-9677-44C8-9AC0-EE3DB5AE743B}"/>
+              <c16:uniqueId val="{0000000E-979F-4BDE-8BEA-C7C15B2E34FA}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:v>Egresos</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:srgbClr val="FF0000"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:val>
+            <c:numRef>
+              <c:f>('Flujo de Caja (Profesor) - 5 añ'!$D$27,'Flujo de Caja (Profesor) - 5 añ'!$F$27,'Flujo de Caja (Profesor) - 5 añ'!$H$27,'Flujo de Caja (Profesor) - 5 añ'!$J$27,'Flujo de Caja (Profesor) - 5 añ'!$L$27)</c:f>
+              <c:numCache>
+                <c:formatCode>"$"#,##0.00</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0" formatCode="&quot;$&quot;#,##0">
+                  <c:v>-167365100.91612545</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>-192119598.06656539</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>-246015547.25142169</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>-250868383.0991841</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>-251283275.84977445</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{0000000D-979F-4BDE-8BEA-C7C15B2E34FA}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -5320,32 +5311,17 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:gapWidth val="267"/>
-        <c:overlap val="-43"/>
-        <c:axId val="195831008"/>
-        <c:axId val="188039952"/>
+        <c:gapWidth val="300"/>
+        <c:axId val="765547808"/>
+        <c:axId val="765542400"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="195831008"/>
+        <c:axId val="765547808"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="b"/>
-        <c:majorGridlines>
-          <c:spPr>
-            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-              <a:solidFill>
-                <a:schemeClr val="dk1">
-                  <a:lumMod val="15000"/>
-                  <a:lumOff val="85000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:round/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-        </c:majorGridlines>
         <c:title>
           <c:tx>
             <c:rich>
@@ -5366,7 +5342,7 @@
                   </a:defRPr>
                 </a:pPr>
                 <a:r>
-                  <a:rPr lang="es-ES"/>
+                  <a:rPr lang="es-CO"/>
                   <a:t>Periodo anual</a:t>
                 </a:r>
               </a:p>
@@ -5438,15 +5414,15 @@
             <a:endParaRPr lang="es-CO"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="188039952"/>
-        <c:crosses val="autoZero"/>
+        <c:crossAx val="765542400"/>
+        <c:crossesAt val="0"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="188039952"/>
+        <c:axId val="765542400"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -5459,6 +5435,7 @@
                 <a:schemeClr val="dk1">
                   <a:lumMod val="15000"/>
                   <a:lumOff val="85000"/>
+                  <a:alpha val="54000"/>
                 </a:schemeClr>
               </a:solidFill>
               <a:round/>
@@ -5486,10 +5463,9 @@
                   </a:defRPr>
                 </a:pPr>
                 <a:r>
-                  <a:rPr lang="es-ES"/>
-                  <a:t>Valor en Pesos  en caja</a:t>
+                  <a:rPr lang="es-CO"/>
+                  <a:t>Valor en Pesos Colombianos</a:t>
                 </a:r>
-                <a:endParaRPr lang="es-CO"/>
               </a:p>
             </c:rich>
           </c:tx>
@@ -5522,8 +5498,8 @@
             </a:p>
           </c:txPr>
         </c:title>
-        <c:numFmt formatCode="&quot;$&quot;#,##0.00" sourceLinked="1"/>
-        <c:majorTickMark val="none"/>
+        <c:numFmt formatCode="&quot;$&quot;#,##0.00" sourceLinked="0"/>
+        <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
         <c:spPr>
@@ -5553,7 +5529,7 @@
             <a:endParaRPr lang="es-CO"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="195831008"/>
+        <c:crossAx val="765547808"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -5575,8 +5551,39 @@
         <a:effectLst/>
       </c:spPr>
     </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="dk1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="es-CO"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
     <c:plotVisOnly val="1"/>
-    <c:dispBlanksAs val="gap"/>
+    <c:dispBlanksAs val="zero"/>
     <c:showDLblsOverMax val="0"/>
   </c:chart>
   <c:spPr>
@@ -5960,7 +5967,7 @@
           <c:smooth val="0"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000000-B3AB-48B6-8A94-E5BD0B53D7E6}"/>
+              <c16:uniqueId val="{00000000-1EA7-4E0A-AE2E-B9FCDAD680B1}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -8005,7 +8012,7 @@
 </file>
 
 <file path=xl/charts/style4.xml><?xml version="1.0" encoding="utf-8"?>
-<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="208">
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="232">
   <cs:axisTitle>
     <cs:lnRef idx="0"/>
     <cs:fillRef idx="0"/>
@@ -8314,6 +8321,7 @@
           <a:schemeClr val="dk1">
             <a:lumMod val="15000"/>
             <a:lumOff val="85000"/>
+            <a:alpha val="54000"/>
           </a:schemeClr>
         </a:solidFill>
         <a:round/>
@@ -8331,8 +8339,9 @@
       <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
         <a:solidFill>
           <a:schemeClr val="dk1">
-            <a:lumMod val="5000"/>
-            <a:lumOff val="95000"/>
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+            <a:alpha val="51000"/>
           </a:schemeClr>
         </a:solidFill>
         <a:round/>
@@ -9079,13 +9088,13 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>7</xdr:col>
-      <xdr:colOff>838199</xdr:colOff>
+      <xdr:colOff>771524</xdr:colOff>
       <xdr:row>10</xdr:row>
       <xdr:rowOff>185736</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>12</xdr:col>
-      <xdr:colOff>923924</xdr:colOff>
+      <xdr:colOff>857249</xdr:colOff>
       <xdr:row>27</xdr:row>
       <xdr:rowOff>66674</xdr:rowOff>
     </xdr:to>
@@ -9412,23 +9421,23 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>5</xdr:col>
-      <xdr:colOff>337038</xdr:colOff>
-      <xdr:row>26</xdr:row>
-      <xdr:rowOff>71804</xdr:rowOff>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>311393</xdr:colOff>
+      <xdr:row>34</xdr:row>
+      <xdr:rowOff>167053</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>11</xdr:col>
-      <xdr:colOff>827942</xdr:colOff>
-      <xdr:row>40</xdr:row>
-      <xdr:rowOff>45427</xdr:rowOff>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>516547</xdr:colOff>
+      <xdr:row>48</xdr:row>
+      <xdr:rowOff>140676</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="2" name="Gráfico 1">
+        <xdr:cNvPr id="3" name="Gráfico 2">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{256134D2-344F-4846-82F0-F5E1C329C9C5}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0900-000003000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -10252,20 +10261,20 @@
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:S42"/>
+  <dimension ref="A1:S31"/>
   <sheetViews>
-    <sheetView topLeftCell="D25" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="G42" sqref="G42:I42"/>
+    <sheetView topLeftCell="B34" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="K43" sqref="K43"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1"/>
   <cols>
-    <col min="1" max="1" width="23.5703125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="25.7109375" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="12.28515625" customWidth="1"/>
     <col min="3" max="3" width="9.5703125" customWidth="1"/>
     <col min="4" max="4" width="14.7109375" customWidth="1"/>
     <col min="5" max="5" width="7.42578125" customWidth="1"/>
-    <col min="6" max="6" width="14.42578125" customWidth="1"/>
+    <col min="6" max="6" width="15.28515625" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="7" customWidth="1"/>
     <col min="8" max="8" width="15.28515625" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="7.28515625" customWidth="1"/>
@@ -10279,26 +10288,26 @@
       <c r="B1" s="200" t="s">
         <v>73</v>
       </c>
-      <c r="C1" s="313" t="s">
+      <c r="C1" s="314" t="s">
         <v>70</v>
       </c>
-      <c r="D1" s="297"/>
-      <c r="E1" s="312" t="s">
+      <c r="D1" s="298"/>
+      <c r="E1" s="313" t="s">
         <v>71</v>
       </c>
-      <c r="F1" s="297"/>
-      <c r="G1" s="312" t="s">
+      <c r="F1" s="298"/>
+      <c r="G1" s="313" t="s">
         <v>72</v>
       </c>
-      <c r="H1" s="297"/>
-      <c r="I1" s="312" t="s">
+      <c r="H1" s="298"/>
+      <c r="I1" s="313" t="s">
         <v>74</v>
       </c>
-      <c r="J1" s="297"/>
-      <c r="K1" s="314" t="s">
+      <c r="J1" s="298"/>
+      <c r="K1" s="315" t="s">
         <v>75</v>
       </c>
-      <c r="L1" s="321"/>
+      <c r="L1" s="322"/>
       <c r="M1" s="27"/>
       <c r="N1" s="27"/>
       <c r="O1" s="27"/>
@@ -10507,10 +10516,10 @@
         <f>D5+F5+H5+J5+L5</f>
         <v>3842803.2126632677</v>
       </c>
-      <c r="O5" s="319" t="s">
+      <c r="O5" s="320" t="s">
         <v>280</v>
       </c>
-      <c r="P5" s="319"/>
+      <c r="P5" s="320"/>
       <c r="Q5" s="52"/>
       <c r="R5" s="52"/>
       <c r="S5" s="52"/>
@@ -10562,10 +10571,10 @@
       </c>
       <c r="M6" s="52"/>
       <c r="N6" s="52"/>
-      <c r="O6" s="319" t="s">
+      <c r="O6" s="320" t="s">
         <v>285</v>
       </c>
-      <c r="P6" s="319"/>
+      <c r="P6" s="320"/>
       <c r="Q6" s="52"/>
       <c r="R6" s="52"/>
       <c r="S6" s="52"/>
@@ -10617,10 +10626,10 @@
       </c>
       <c r="M7" s="52"/>
       <c r="N7" s="52"/>
-      <c r="O7" s="319" t="s">
+      <c r="O7" s="320" t="s">
         <v>286</v>
       </c>
-      <c r="P7" s="319"/>
+      <c r="P7" s="320"/>
       <c r="Q7" s="52"/>
       <c r="R7" s="52"/>
       <c r="S7" s="52"/>
@@ -10672,8 +10681,8 @@
       </c>
       <c r="M8" s="55"/>
       <c r="N8" s="44"/>
-      <c r="O8" s="320"/>
-      <c r="P8" s="320"/>
+      <c r="O8" s="321"/>
+      <c r="P8" s="321"/>
       <c r="Q8" s="44"/>
       <c r="R8" s="44"/>
       <c r="S8" s="44"/>
@@ -10725,10 +10734,10 @@
       </c>
       <c r="M9" s="52"/>
       <c r="N9" s="52"/>
-      <c r="O9" s="319" t="s">
+      <c r="O9" s="320" t="s">
         <v>11</v>
       </c>
-      <c r="P9" s="319"/>
+      <c r="P9" s="320"/>
       <c r="Q9" s="52"/>
       <c r="R9" s="52"/>
       <c r="S9" s="52"/>
@@ -10780,10 +10789,10 @@
       </c>
       <c r="M10" s="52"/>
       <c r="N10" s="52"/>
-      <c r="O10" s="319" t="s">
+      <c r="O10" s="320" t="s">
         <v>248</v>
       </c>
-      <c r="P10" s="319"/>
+      <c r="P10" s="320"/>
       <c r="Q10" s="52"/>
       <c r="R10" s="52"/>
       <c r="S10" s="52"/>
@@ -11339,6 +11348,64 @@
         <v>0.03</v>
       </c>
     </row>
+    <row r="27" spans="1:19" ht="15.75" customHeight="1">
+      <c r="B27" t="s">
+        <v>307</v>
+      </c>
+      <c r="D27" s="282">
+        <f>(D5+D6+D7+D9+D10+D15)*-1</f>
+        <v>-167365100.91612545</v>
+      </c>
+      <c r="E27" s="192"/>
+      <c r="F27" s="192">
+        <f>(F5+F6+F7+F9+F10+F15)*-1</f>
+        <v>-192119598.06656539</v>
+      </c>
+      <c r="G27" s="192"/>
+      <c r="H27" s="192">
+        <f>(H5+H6+H7+H9+H10+H15)*-1</f>
+        <v>-246015547.25142169</v>
+      </c>
+      <c r="I27" s="192"/>
+      <c r="J27" s="192">
+        <f>(J5+J6+J7+J9+J10+J15)*-1</f>
+        <v>-250868383.0991841</v>
+      </c>
+      <c r="K27" s="192"/>
+      <c r="L27" s="192">
+        <f>(L5+L6+L7+L9+L10+L15)*-1</f>
+        <v>-251283275.84977445</v>
+      </c>
+    </row>
+    <row r="28" spans="1:19" ht="15.75" customHeight="1">
+      <c r="B28" t="s">
+        <v>308</v>
+      </c>
+      <c r="D28" s="192">
+        <f>D2+D27</f>
+        <v>32572833.289787471</v>
+      </c>
+      <c r="E28" s="192"/>
+      <c r="F28" s="192">
+        <f>F2+F27</f>
+        <v>159745157.08126181</v>
+      </c>
+      <c r="G28" s="192"/>
+      <c r="H28" s="192">
+        <f>H2+H27</f>
+        <v>263206333.91240484</v>
+      </c>
+      <c r="I28" s="192"/>
+      <c r="J28" s="192">
+        <f>J2+J27</f>
+        <v>271466173.08918911</v>
+      </c>
+      <c r="K28" s="192"/>
+      <c r="L28" s="192">
+        <f>L2+L27</f>
+        <v>271807404.49984503</v>
+      </c>
+    </row>
     <row r="30" spans="1:19" ht="15.75" customHeight="1">
       <c r="D30" s="43">
         <f>D5+D6+D9+D10+D13+D15</f>
@@ -11349,26 +11416,6 @@
       <c r="D31">
         <f>D30/10022</f>
         <v>16629.924257032122</v>
-      </c>
-    </row>
-    <row r="42" spans="4:9" ht="15.75" customHeight="1">
-      <c r="D42" t="s">
-        <v>73</v>
-      </c>
-      <c r="E42" t="s">
-        <v>70</v>
-      </c>
-      <c r="F42" t="s">
-        <v>71</v>
-      </c>
-      <c r="G42" t="s">
-        <v>72</v>
-      </c>
-      <c r="H42" t="s">
-        <v>74</v>
-      </c>
-      <c r="I42" t="s">
-        <v>75</v>
       </c>
     </row>
   </sheetData>
@@ -11450,8 +11497,8 @@
         <v>800</v>
       </c>
       <c r="H2" s="66">
-        <f>'Flujo de caja - 5 años'!E13</f>
-        <v>91785333.314600259</v>
+        <f>'Flujo de caja - 5 años'!E14</f>
+        <v>91085333.302450746</v>
       </c>
       <c r="J2" s="24">
         <f>'Flujo de Caja (Profesor) - 5 añ'!D19</f>
@@ -11460,8 +11507,8 @@
     </row>
     <row r="3" spans="1:13" ht="15.75" customHeight="1">
       <c r="H3" s="66">
-        <f>'Flujo de caja - 5 años'!G13</f>
-        <v>252230490.39586207</v>
+        <f>'Flujo de caja - 5 años'!G14</f>
+        <v>250830490.38371256</v>
       </c>
       <c r="J3" s="24">
         <f>'Flujo de Caja (Profesor) - 5 añ'!F19</f>
@@ -11471,28 +11518,28 @@
     <row r="4" spans="1:13" ht="15.75" customHeight="1">
       <c r="A4" s="11"/>
       <c r="B4" s="24">
-        <f>'Flujo de caja - 5 años'!E13/((1+$B$2)^1)</f>
-        <v>79813333.317043707</v>
+        <f>'Flujo de caja - 5 años'!E14/((1+$B$2)^1)</f>
+        <v>79204637.654304996</v>
       </c>
       <c r="C4" s="24">
-        <f>'Flujo de caja - 5 años'!G13/((1+$B$2)^2)</f>
-        <v>190722488.01199403</v>
+        <f>'Flujo de caja - 5 años'!G14/((1+$B$2)^2)</f>
+        <v>189663886.86859176</v>
       </c>
       <c r="D4" s="24">
-        <f>'Flujo de caja - 5 años'!I13/((1+$B$2)^3)</f>
-        <v>339370738.75779867</v>
+        <f>'Flujo de caja - 5 años'!I14/((1+$B$2)^3)</f>
+        <v>337989954.66170305</v>
       </c>
       <c r="E4" s="68">
-        <f>'Flujo de caja - 5 años'!K13/((1+$B$2)^4)</f>
-        <v>450721054.54023176</v>
+        <f>'Flujo de caja - 5 años'!K14/((1+$B$2)^4)</f>
+        <v>449120145.44562483</v>
       </c>
       <c r="F4" s="68">
-        <f>'Flujo de caja - 5 años'!M13/((1+$B$2)^5)</f>
-        <v>527420046.36971092</v>
+        <f>'Flujo de caja - 5 años'!M14/((1+$B$2)^5)</f>
+        <v>525679927.79012656</v>
       </c>
       <c r="H4" s="66">
-        <f>'Flujo de caja - 5 años'!I13</f>
-        <v>516140472.30826688</v>
+        <f>'Flujo de caja - 5 años'!I14</f>
+        <v>514040472.29611742</v>
       </c>
       <c r="J4" s="24">
         <f>'Flujo de Caja (Profesor) - 5 añ'!H19</f>
@@ -11505,11 +11552,11 @@
       </c>
       <c r="B5" s="24">
         <f>SUM(B4:F4)-B1</f>
-        <v>1515591660.996779</v>
+        <v>1509202552.4203513</v>
       </c>
       <c r="H5" s="66">
-        <f>'Flujo de caja - 5 años'!K13</f>
-        <v>788313941.39745593</v>
+        <f>'Flujo de caja - 5 años'!K14</f>
+        <v>785513941.3853066</v>
       </c>
       <c r="J5" s="24">
         <f>'Flujo de Caja (Profesor) - 5 añ'!J19</f>
@@ -11522,28 +11569,28 @@
     <row r="6" spans="1:13" ht="15.75" customHeight="1">
       <c r="A6" s="11"/>
       <c r="B6" s="24">
-        <f>'Flujo de caja - 5 años'!E13/(1+$C$2)^1</f>
-        <v>114588.43110436985</v>
+        <f>'Flujo de caja - 5 años'!E14/(1+$C$2)^1</f>
+        <v>113714.52347372127</v>
       </c>
       <c r="C6" s="24">
-        <f>'Flujo de caja - 5 años'!G13/(1+$C$2)^2</f>
-        <v>393.12671020753095</v>
+        <f>'Flujo de caja - 5 años'!G14/(1+$C$2)^2</f>
+        <v>390.94466870175165</v>
       </c>
       <c r="D6" s="24">
-        <f>'Flujo de caja - 5 años'!I13/(1+$C$2)^3</f>
-        <v>1.0043159654141383</v>
+        <f>'Flujo de caja - 5 años'!I14/(1+$C$2)^3</f>
+        <v>1.0002297453776829</v>
       </c>
       <c r="E6" s="68">
-        <f>'Flujo de caja - 5 años'!K13/(1+$B$2)^4</f>
-        <v>450721054.54023176</v>
+        <f>'Flujo de caja - 5 años'!K14/(1+$B$2)^4</f>
+        <v>449120145.44562483</v>
       </c>
       <c r="F6" s="68">
-        <f>'Flujo de caja - 5 años'!M13/(1+$B$2)^5</f>
-        <v>527420046.36971092</v>
+        <f>'Flujo de caja - 5 años'!M14/(1+$B$2)^5</f>
+        <v>525679927.79012656</v>
       </c>
       <c r="H6" s="66">
-        <f>'Flujo de caja - 5 años'!M13</f>
-        <v>1060830101.097301</v>
+        <f>'Flujo de caja - 5 años'!M14</f>
+        <v>1057330101.0851517</v>
       </c>
       <c r="J6" s="24">
         <f>'Flujo de Caja (Profesor) - 5 añ'!L19</f>
@@ -11563,10 +11610,10 @@
       </c>
       <c r="B7" s="24">
         <f>SUM(B6:F6)-B1</f>
-        <v>905800083.47207332</v>
+        <v>902458179.7041235</v>
       </c>
       <c r="H7" s="71">
-        <f>'Flujo de caja - 5 años'!E18</f>
+        <f>'Flujo de caja - 5 años'!E19</f>
         <v>0</v>
       </c>
       <c r="L7" s="11">
@@ -11613,7 +11660,7 @@
       </c>
       <c r="H10" s="43">
         <f t="array" ref="H10">NPV(0.15,H2:H6)+H1</f>
-        <v>1515591660.9967792</v>
+        <v>1509202552.4203513</v>
       </c>
       <c r="J10" s="43">
         <f t="array" ref="J10">NPV(0.15,J2:J6)+J1</f>
@@ -11633,7 +11680,7 @@
       </c>
       <c r="H11" s="73">
         <f>IRR(H1:H6)</f>
-        <v>2.3482376015537989</v>
+        <v>2.3389367063213409</v>
       </c>
       <c r="J11" s="191">
         <f>IRR(J1:J6)</f>
@@ -12465,30 +12512,30 @@
   <sheetData>
     <row r="1" spans="2:8" ht="13.5" thickBot="1"/>
     <row r="2" spans="2:8" ht="15.75" thickBot="1">
-      <c r="B2" s="332" t="s">
+      <c r="B2" s="333" t="s">
         <v>281</v>
       </c>
-      <c r="C2" s="333"/>
-      <c r="D2" s="333"/>
-      <c r="E2" s="333"/>
-      <c r="F2" s="333"/>
-      <c r="G2" s="333"/>
-      <c r="H2" s="334"/>
+      <c r="C2" s="334"/>
+      <c r="D2" s="334"/>
+      <c r="E2" s="334"/>
+      <c r="F2" s="334"/>
+      <c r="G2" s="334"/>
+      <c r="H2" s="335"/>
     </row>
     <row r="3" spans="2:8" ht="15.75" thickTop="1">
-      <c r="B3" s="327" t="s">
+      <c r="B3" s="328" t="s">
         <v>287</v>
       </c>
-      <c r="C3" s="328"/>
-      <c r="D3" s="328"/>
-      <c r="E3" s="328"/>
-      <c r="F3" s="328"/>
-      <c r="G3" s="328"/>
-      <c r="H3" s="329"/>
+      <c r="C3" s="329"/>
+      <c r="D3" s="329"/>
+      <c r="E3" s="329"/>
+      <c r="F3" s="329"/>
+      <c r="G3" s="329"/>
+      <c r="H3" s="330"/>
     </row>
     <row r="4" spans="2:8">
-      <c r="B4" s="335"/>
-      <c r="C4" s="323"/>
+      <c r="B4" s="336"/>
+      <c r="C4" s="324"/>
       <c r="D4" s="179" t="s">
         <v>70</v>
       </c>
@@ -12506,10 +12553,10 @@
       </c>
     </row>
     <row r="5" spans="2:8">
-      <c r="B5" s="322" t="s">
+      <c r="B5" s="323" t="s">
         <v>118</v>
       </c>
-      <c r="C5" s="323"/>
+      <c r="C5" s="324"/>
       <c r="D5" s="182">
         <f>'Flujo de Caja (Profesor) - 5 añ'!D6+'Flujo de Caja (Profesor) - 5 añ'!D7</f>
         <v>111254717.93098715</v>
@@ -12532,10 +12579,10 @@
       </c>
     </row>
     <row r="6" spans="2:8">
-      <c r="B6" s="322" t="s">
+      <c r="B6" s="323" t="s">
         <v>282</v>
       </c>
-      <c r="C6" s="323"/>
+      <c r="C6" s="324"/>
       <c r="D6" s="182">
         <f>'Flujo de Caja (Profesor) - 5 añ'!D3</f>
         <v>199937934.20591292</v>
@@ -12558,10 +12605,10 @@
       </c>
     </row>
     <row r="7" spans="2:8">
-      <c r="B7" s="322" t="s">
+      <c r="B7" s="323" t="s">
         <v>283</v>
       </c>
-      <c r="C7" s="323"/>
+      <c r="C7" s="324"/>
       <c r="D7" s="182">
         <f>'Flujo de Caja (Profesor) - 5 añ'!D10</f>
         <v>4285000.1176767461</v>
@@ -12584,10 +12631,10 @@
       </c>
     </row>
     <row r="8" spans="2:8">
-      <c r="B8" s="322" t="s">
+      <c r="B8" s="323" t="s">
         <v>291</v>
       </c>
-      <c r="C8" s="326"/>
+      <c r="C8" s="327"/>
       <c r="D8" s="182">
         <f>D5+D7</f>
         <v>115539718.0486639</v>
@@ -12610,10 +12657,10 @@
       </c>
     </row>
     <row r="9" spans="2:8">
-      <c r="B9" s="322" t="s">
+      <c r="B9" s="323" t="s">
         <v>284</v>
       </c>
-      <c r="C9" s="323"/>
+      <c r="C9" s="324"/>
       <c r="D9" s="184">
         <f>D5/(D6-D7)</f>
         <v>0.56863301564807167</v>
@@ -12636,19 +12683,19 @@
       </c>
     </row>
     <row r="10" spans="2:8" ht="15">
-      <c r="B10" s="327" t="s">
+      <c r="B10" s="328" t="s">
         <v>288</v>
       </c>
-      <c r="C10" s="328"/>
-      <c r="D10" s="328"/>
-      <c r="E10" s="328"/>
-      <c r="F10" s="328"/>
-      <c r="G10" s="328"/>
-      <c r="H10" s="329"/>
+      <c r="C10" s="329"/>
+      <c r="D10" s="329"/>
+      <c r="E10" s="329"/>
+      <c r="F10" s="329"/>
+      <c r="G10" s="329"/>
+      <c r="H10" s="330"/>
     </row>
     <row r="11" spans="2:8">
-      <c r="B11" s="330"/>
-      <c r="C11" s="331"/>
+      <c r="B11" s="331"/>
+      <c r="C11" s="332"/>
       <c r="D11" s="181" t="s">
         <v>70</v>
       </c>
@@ -12666,10 +12713,10 @@
       </c>
     </row>
     <row r="12" spans="2:8">
-      <c r="B12" s="322" t="s">
+      <c r="B12" s="323" t="s">
         <v>118</v>
       </c>
-      <c r="C12" s="323"/>
+      <c r="C12" s="324"/>
       <c r="D12" s="182">
         <f>'Flujo de Caja (Profesor) - 5 añ'!D11+'Flujo de Caja (Profesor) - 5 añ'!D12</f>
         <v>79684496.075435549</v>
@@ -12692,10 +12739,10 @@
       </c>
     </row>
     <row r="13" spans="2:8">
-      <c r="B13" s="322" t="s">
+      <c r="B13" s="323" t="s">
         <v>289</v>
       </c>
-      <c r="C13" s="323"/>
+      <c r="C13" s="324"/>
       <c r="D13" s="187">
         <v>5000</v>
       </c>
@@ -12713,10 +12760,10 @@
       </c>
     </row>
     <row r="14" spans="2:8">
-      <c r="B14" s="322" t="s">
+      <c r="B14" s="323" t="s">
         <v>290</v>
       </c>
-      <c r="C14" s="323"/>
+      <c r="C14" s="324"/>
       <c r="D14" s="187">
         <f>('Flujo de Caja (Profesor) - 5 añ'!D6+'Flujo de Caja (Profesor) - 5 añ'!D7)/'Tabla Crecimiento'!B9</f>
         <v>11103.815193643957</v>
@@ -12739,10 +12786,10 @@
       </c>
     </row>
     <row r="15" spans="2:8" ht="15.75" thickBot="1">
-      <c r="B15" s="324" t="s">
+      <c r="B15" s="325" t="s">
         <v>288</v>
       </c>
-      <c r="C15" s="325"/>
+      <c r="C15" s="326"/>
       <c r="D15" s="189">
         <f>D12/D13-D14</f>
         <v>4833.0840214431519</v>
@@ -12778,36 +12825,36 @@
       <c r="N23" s="93"/>
     </row>
     <row r="24" spans="2:14">
-      <c r="B24" s="286"/>
-      <c r="C24" s="291"/>
+      <c r="B24" s="287"/>
+      <c r="C24" s="292"/>
     </row>
     <row r="25" spans="2:14">
-      <c r="B25" s="286"/>
-      <c r="C25" s="291"/>
+      <c r="B25" s="287"/>
+      <c r="C25" s="292"/>
     </row>
     <row r="26" spans="2:14">
-      <c r="B26" s="286"/>
-      <c r="C26" s="291"/>
+      <c r="B26" s="287"/>
+      <c r="C26" s="292"/>
     </row>
     <row r="27" spans="2:14">
-      <c r="B27" s="286"/>
-      <c r="C27" s="286"/>
+      <c r="B27" s="287"/>
+      <c r="C27" s="287"/>
     </row>
     <row r="28" spans="2:14">
-      <c r="B28" s="286"/>
-      <c r="C28" s="291"/>
+      <c r="B28" s="287"/>
+      <c r="C28" s="292"/>
     </row>
     <row r="30" spans="2:14">
-      <c r="B30" s="286"/>
-      <c r="C30" s="291"/>
+      <c r="B30" s="287"/>
+      <c r="C30" s="292"/>
     </row>
     <row r="31" spans="2:14">
-      <c r="B31" s="286"/>
-      <c r="C31" s="291"/>
+      <c r="B31" s="287"/>
+      <c r="C31" s="292"/>
     </row>
     <row r="32" spans="2:14">
-      <c r="B32" s="286"/>
-      <c r="C32" s="291"/>
+      <c r="B32" s="287"/>
+      <c r="C32" s="292"/>
     </row>
   </sheetData>
   <mergeCells count="22">
@@ -12842,7 +12889,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AA19"/>
   <sheetViews>
-    <sheetView topLeftCell="H1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView topLeftCell="H10" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="U11" sqref="U11:AA19"/>
     </sheetView>
   </sheetViews>
@@ -12877,44 +12924,44 @@
   <sheetData>
     <row r="1" spans="1:27" ht="15.75" customHeight="1">
       <c r="A1" s="152"/>
-      <c r="B1" s="316" t="s">
+      <c r="B1" s="317" t="s">
         <v>70</v>
       </c>
-      <c r="C1" s="317"/>
-      <c r="D1" s="316" t="s">
+      <c r="C1" s="318"/>
+      <c r="D1" s="317" t="s">
         <v>71</v>
       </c>
-      <c r="E1" s="317"/>
-      <c r="F1" s="316" t="s">
+      <c r="E1" s="318"/>
+      <c r="F1" s="317" t="s">
         <v>72</v>
       </c>
-      <c r="G1" s="317"/>
-      <c r="H1" s="316" t="s">
+      <c r="G1" s="318"/>
+      <c r="H1" s="317" t="s">
         <v>74</v>
       </c>
-      <c r="I1" s="317"/>
-      <c r="J1" s="328" t="s">
+      <c r="I1" s="318"/>
+      <c r="J1" s="329" t="s">
         <v>75</v>
       </c>
-      <c r="K1" s="336"/>
+      <c r="K1" s="337"/>
       <c r="M1" s="193"/>
-      <c r="N1" s="337" t="s">
+      <c r="N1" s="338" t="s">
         <v>70</v>
       </c>
-      <c r="O1" s="338"/>
-      <c r="P1" s="337" t="s">
+      <c r="O1" s="339"/>
+      <c r="P1" s="338" t="s">
         <v>71</v>
       </c>
-      <c r="Q1" s="338"/>
+      <c r="Q1" s="339"/>
       <c r="U1" s="194"/>
-      <c r="V1" s="337" t="s">
+      <c r="V1" s="338" t="s">
         <v>70</v>
       </c>
-      <c r="W1" s="337"/>
-      <c r="X1" s="337" t="s">
+      <c r="W1" s="338"/>
+      <c r="X1" s="338" t="s">
         <v>71</v>
       </c>
-      <c r="Y1" s="337"/>
+      <c r="Y1" s="338"/>
     </row>
     <row r="2" spans="1:27" ht="15.75" customHeight="1">
       <c r="A2" s="30" t="s">
@@ -12963,17 +13010,17 @@
       <c r="M2" s="248" t="s">
         <v>137</v>
       </c>
-      <c r="N2" s="337"/>
-      <c r="O2" s="337"/>
-      <c r="P2" s="337"/>
-      <c r="Q2" s="337"/>
+      <c r="N2" s="338"/>
+      <c r="O2" s="338"/>
+      <c r="P2" s="338"/>
+      <c r="Q2" s="338"/>
       <c r="U2" s="195" t="s">
         <v>292</v>
       </c>
-      <c r="V2" s="340"/>
-      <c r="W2" s="340"/>
-      <c r="X2" s="340"/>
-      <c r="Y2" s="340"/>
+      <c r="V2" s="341"/>
+      <c r="W2" s="341"/>
+      <c r="X2" s="341"/>
+      <c r="Y2" s="341"/>
     </row>
     <row r="3" spans="1:27" ht="22.5">
       <c r="A3" s="30" t="s">
@@ -13520,31 +13567,31 @@
         <v>773376</v>
       </c>
       <c r="M11" s="193"/>
-      <c r="N11" s="337" t="s">
+      <c r="N11" s="338" t="s">
         <v>72</v>
       </c>
-      <c r="O11" s="338"/>
-      <c r="P11" s="337" t="s">
+      <c r="O11" s="339"/>
+      <c r="P11" s="338" t="s">
         <v>74</v>
       </c>
-      <c r="Q11" s="338"/>
-      <c r="R11" s="337" t="s">
+      <c r="Q11" s="339"/>
+      <c r="R11" s="338" t="s">
         <v>75</v>
       </c>
-      <c r="S11" s="338"/>
+      <c r="S11" s="339"/>
       <c r="U11" s="205"/>
-      <c r="V11" s="339" t="s">
+      <c r="V11" s="340" t="s">
         <v>72</v>
       </c>
-      <c r="W11" s="339"/>
-      <c r="X11" s="339" t="s">
+      <c r="W11" s="340"/>
+      <c r="X11" s="340" t="s">
         <v>74</v>
       </c>
-      <c r="Y11" s="339"/>
-      <c r="Z11" s="339" t="s">
+      <c r="Y11" s="340"/>
+      <c r="Z11" s="340" t="s">
         <v>75</v>
       </c>
-      <c r="AA11" s="341"/>
+      <c r="AA11" s="342"/>
     </row>
     <row r="12" spans="1:27" ht="15">
       <c r="A12" s="39" t="s">
@@ -13555,7 +13602,7 @@
         <v>0.2323771472279017</v>
       </c>
       <c r="C12" s="42">
-        <f>'Flujo de caja - 5 años'!E9</f>
+        <f>'Flujo de caja - 5 años'!E10</f>
         <v>47111662.785648078</v>
       </c>
       <c r="D12" s="86">
@@ -13563,7 +13610,7 @@
         <v>0.4403577777681148</v>
       </c>
       <c r="E12" s="42">
-        <f>'Flujo de caja - 5 años'!G9</f>
+        <f>'Flujo de caja - 5 años'!G10</f>
         <v>82292959.708528847</v>
       </c>
       <c r="F12" s="86">
@@ -13571,7 +13618,7 @@
         <v>0.56320688438557376</v>
       </c>
       <c r="G12" s="42">
-        <f>'Flujo de caja - 5 años'!I9</f>
+        <f>'Flujo de caja - 5 años'!I10</f>
         <v>135591141.71245098</v>
       </c>
       <c r="H12" s="86">
@@ -13579,7 +13626,7 @@
         <v>0.56946172418414176</v>
       </c>
       <c r="I12" s="42">
-        <f>'Flujo de caja - 5 años'!K9</f>
+        <f>'Flujo de caja - 5 años'!K10</f>
         <v>139846210.37927929</v>
       </c>
       <c r="J12" s="40">
@@ -13587,27 +13634,27 @@
         <v>0.56923907114544692</v>
       </c>
       <c r="K12" s="162">
-        <f>'Flujo de caja - 5 años'!M9</f>
+        <f>'Flujo de caja - 5 años'!M10</f>
         <v>140021996.25749597</v>
       </c>
       <c r="M12" s="203" t="s">
         <v>137</v>
       </c>
-      <c r="N12" s="337"/>
-      <c r="O12" s="337"/>
-      <c r="P12" s="337"/>
-      <c r="Q12" s="337"/>
-      <c r="R12" s="337"/>
-      <c r="S12" s="337"/>
+      <c r="N12" s="338"/>
+      <c r="O12" s="338"/>
+      <c r="P12" s="338"/>
+      <c r="Q12" s="338"/>
+      <c r="R12" s="338"/>
+      <c r="S12" s="338"/>
       <c r="U12" s="195" t="s">
         <v>292</v>
       </c>
-      <c r="V12" s="340"/>
-      <c r="W12" s="340"/>
-      <c r="X12" s="340"/>
-      <c r="Y12" s="340"/>
-      <c r="Z12" s="340"/>
-      <c r="AA12" s="340"/>
+      <c r="V12" s="341"/>
+      <c r="W12" s="341"/>
+      <c r="X12" s="341"/>
+      <c r="Y12" s="341"/>
+      <c r="Z12" s="341"/>
+      <c r="AA12" s="341"/>
     </row>
     <row r="13" spans="1:27" ht="22.5">
       <c r="A13" s="39" t="s">
@@ -14472,16 +14519,17 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:O35"/>
+  <dimension ref="A1:O47"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="G1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="O2" sqref="O2"/>
+    <sheetView tabSelected="1" topLeftCell="A23" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1"/>
   <cols>
     <col min="2" max="2" width="18.140625" customWidth="1"/>
     <col min="8" max="8" width="17.7109375" customWidth="1"/>
+    <col min="9" max="9" width="15.28515625" bestFit="1" customWidth="1"/>
     <col min="14" max="14" width="23.85546875" bestFit="1" customWidth="1"/>
     <col min="15" max="15" width="19.140625" customWidth="1"/>
   </cols>
@@ -14720,8 +14768,8 @@
         <v>10019.503746304383</v>
       </c>
       <c r="C9" s="111">
-        <f t="shared" si="1"/>
-        <v>54092469.46774932</v>
+        <f>SUM(C2:C8)</f>
+        <v>199937928.20591292</v>
       </c>
       <c r="D9" t="s">
         <v>177</v>
@@ -14921,7 +14969,7 @@
         <v>54236.252613990997</v>
       </c>
     </row>
-    <row r="33" spans="5:6" ht="15.75" customHeight="1">
+    <row r="33" spans="5:9" ht="15.75" customHeight="1">
       <c r="E33">
         <v>23</v>
       </c>
@@ -14930,7 +14978,7 @@
         <v>59859.769065140223</v>
       </c>
     </row>
-    <row r="34" spans="5:6" ht="15.75" customHeight="1">
+    <row r="34" spans="5:9" ht="15.75" customHeight="1">
       <c r="E34">
         <v>24</v>
       </c>
@@ -14939,13 +14987,19 @@
         <v>65175.619953865986</v>
       </c>
     </row>
-    <row r="35" spans="5:6" ht="15.75" customHeight="1">
+    <row r="35" spans="5:9" ht="15.75" customHeight="1">
       <c r="E35">
         <v>25</v>
       </c>
       <c r="F35" s="176">
         <f t="shared" si="3"/>
         <v>70070.502916553378</v>
+      </c>
+    </row>
+    <row r="47" spans="5:9" ht="15.75" customHeight="1">
+      <c r="I47" s="154">
+        <f>SUM(C2:C8)</f>
+        <v>199937928.20591292</v>
       </c>
     </row>
   </sheetData>
@@ -14984,18 +15038,18 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:14" ht="15.75" customHeight="1">
-      <c r="A1" s="296" t="s">
+      <c r="A1" s="297" t="s">
         <v>8</v>
       </c>
-      <c r="B1" s="297"/>
-      <c r="D1" s="296" t="s">
+      <c r="B1" s="298"/>
+      <c r="D1" s="297" t="s">
         <v>9</v>
       </c>
-      <c r="E1" s="297"/>
-      <c r="J1" s="296" t="s">
+      <c r="E1" s="298"/>
+      <c r="J1" s="297" t="s">
         <v>11</v>
       </c>
-      <c r="K1" s="297"/>
+      <c r="K1" s="298"/>
       <c r="M1" s="6" t="s">
         <v>12</v>
       </c>
@@ -15194,14 +15248,14 @@
       </c>
     </row>
     <row r="17" spans="1:14" ht="15.75" customHeight="1">
-      <c r="A17" s="296" t="s">
+      <c r="A17" s="297" t="s">
         <v>31</v>
       </c>
-      <c r="B17" s="297"/>
-      <c r="D17" s="298" t="s">
+      <c r="B17" s="298"/>
+      <c r="D17" s="299" t="s">
         <v>10</v>
       </c>
-      <c r="E17" s="299"/>
+      <c r="E17" s="300"/>
       <c r="M17" s="11" t="s">
         <v>33</v>
       </c>
@@ -15398,26 +15452,26 @@
     </row>
     <row r="33" spans="1:8" ht="15.75" customHeight="1" thickBot="1"/>
     <row r="34" spans="1:8" ht="15.75" customHeight="1" thickTop="1" thickBot="1">
-      <c r="A34" s="282" t="s">
+      <c r="A34" s="283" t="s">
         <v>214</v>
       </c>
-      <c r="B34" s="282"/>
-      <c r="C34" s="282"/>
-      <c r="D34" s="282"/>
-      <c r="E34" s="282"/>
-      <c r="F34" s="282"/>
-      <c r="G34" s="282"/>
-      <c r="H34" s="282"/>
+      <c r="B34" s="283"/>
+      <c r="C34" s="283"/>
+      <c r="D34" s="283"/>
+      <c r="E34" s="283"/>
+      <c r="F34" s="283"/>
+      <c r="G34" s="283"/>
+      <c r="H34" s="283"/>
     </row>
     <row r="35" spans="1:8" ht="15.75" customHeight="1" thickTop="1" thickBot="1">
-      <c r="A35" s="283"/>
-      <c r="B35" s="283"/>
-      <c r="C35" s="283"/>
-      <c r="D35" s="283"/>
-      <c r="E35" s="283"/>
-      <c r="F35" s="283"/>
-      <c r="G35" s="283"/>
-      <c r="H35" s="283"/>
+      <c r="A35" s="284"/>
+      <c r="B35" s="284"/>
+      <c r="C35" s="284"/>
+      <c r="D35" s="284"/>
+      <c r="E35" s="284"/>
+      <c r="F35" s="284"/>
+      <c r="G35" s="284"/>
+      <c r="H35" s="284"/>
     </row>
     <row r="36" spans="1:8" ht="46.5" customHeight="1" thickTop="1" thickBot="1">
       <c r="A36" s="106" t="s">
@@ -15623,235 +15677,235 @@
     </row>
     <row r="45" spans="1:8" ht="15.75" customHeight="1" thickBot="1"/>
     <row r="46" spans="1:8" ht="15.75" customHeight="1" thickTop="1" thickBot="1">
-      <c r="A46" s="282" t="s">
+      <c r="A46" s="283" t="s">
         <v>232</v>
       </c>
-      <c r="B46" s="282"/>
-      <c r="C46" s="282"/>
-      <c r="D46" s="282"/>
-      <c r="E46" s="282"/>
-      <c r="F46" s="282"/>
+      <c r="B46" s="283"/>
+      <c r="C46" s="283"/>
+      <c r="D46" s="283"/>
+      <c r="E46" s="283"/>
+      <c r="F46" s="283"/>
     </row>
     <row r="47" spans="1:8" ht="15.75" customHeight="1" thickTop="1">
-      <c r="A47" s="295" t="s">
+      <c r="A47" s="296" t="s">
         <v>217</v>
       </c>
-      <c r="B47" s="295"/>
-      <c r="C47" s="295"/>
-      <c r="D47" s="295"/>
-      <c r="E47" s="295" t="s">
+      <c r="B47" s="296"/>
+      <c r="C47" s="296"/>
+      <c r="D47" s="296"/>
+      <c r="E47" s="296" t="s">
         <v>70</v>
       </c>
-      <c r="F47" s="295"/>
+      <c r="F47" s="296"/>
     </row>
     <row r="48" spans="1:8" ht="15.75" customHeight="1">
-      <c r="A48" s="289" t="s">
+      <c r="A48" s="290" t="s">
         <v>225</v>
       </c>
-      <c r="B48" s="292"/>
-      <c r="C48" s="286" t="s">
+      <c r="B48" s="293"/>
+      <c r="C48" s="287" t="s">
         <v>218</v>
       </c>
-      <c r="D48" s="291"/>
-      <c r="E48" s="294">
-        <v>0</v>
-      </c>
-      <c r="F48" s="294"/>
+      <c r="D48" s="292"/>
+      <c r="E48" s="295">
+        <v>0</v>
+      </c>
+      <c r="F48" s="295"/>
     </row>
     <row r="49" spans="1:6" ht="15.75" customHeight="1">
-      <c r="A49" s="292"/>
-      <c r="B49" s="292"/>
-      <c r="C49" s="286" t="s">
+      <c r="A49" s="293"/>
+      <c r="B49" s="293"/>
+      <c r="C49" s="287" t="s">
         <v>219</v>
       </c>
-      <c r="D49" s="291"/>
-      <c r="E49" s="294">
+      <c r="D49" s="292"/>
+      <c r="E49" s="295">
         <f>B2*12</f>
         <v>36800004</v>
       </c>
-      <c r="F49" s="294"/>
+      <c r="F49" s="295"/>
     </row>
     <row r="50" spans="1:6" ht="15.75" customHeight="1">
-      <c r="A50" s="292"/>
-      <c r="B50" s="292"/>
-      <c r="C50" s="286" t="s">
+      <c r="A50" s="293"/>
+      <c r="B50" s="293"/>
+      <c r="C50" s="287" t="s">
         <v>220</v>
       </c>
-      <c r="D50" s="291"/>
-      <c r="E50" s="294">
+      <c r="D50" s="292"/>
+      <c r="E50" s="295">
         <f>(B19*12+B22*12)</f>
         <v>39415992</v>
       </c>
-      <c r="F50" s="294"/>
+      <c r="F50" s="295"/>
     </row>
     <row r="51" spans="1:6" ht="15.75" customHeight="1">
-      <c r="A51" s="292"/>
-      <c r="B51" s="292"/>
-      <c r="C51" s="286" t="s">
+      <c r="A51" s="293"/>
+      <c r="B51" s="293"/>
+      <c r="C51" s="287" t="s">
         <v>221</v>
       </c>
-      <c r="D51" s="286"/>
-      <c r="E51" s="294">
+      <c r="D51" s="287"/>
+      <c r="E51" s="295">
         <f>B4*12</f>
         <v>2400000</v>
       </c>
-      <c r="F51" s="294"/>
+      <c r="F51" s="295"/>
     </row>
     <row r="52" spans="1:6" ht="15.75" customHeight="1">
-      <c r="A52" s="292"/>
-      <c r="B52" s="292"/>
-      <c r="C52" s="286" t="s">
+      <c r="A52" s="293"/>
+      <c r="B52" s="293"/>
+      <c r="C52" s="287" t="s">
         <v>222</v>
       </c>
-      <c r="D52" s="291"/>
-      <c r="E52" s="294">
+      <c r="D52" s="292"/>
+      <c r="E52" s="295">
         <f>(B21+B23)*12</f>
         <v>31938720</v>
       </c>
-      <c r="F52" s="294"/>
+      <c r="F52" s="295"/>
     </row>
     <row r="53" spans="1:6" ht="15.75" customHeight="1" thickBot="1">
-      <c r="A53" s="292"/>
-      <c r="B53" s="292"/>
-      <c r="C53" s="286" t="s">
+      <c r="A53" s="293"/>
+      <c r="B53" s="293"/>
+      <c r="C53" s="287" t="s">
         <v>223</v>
       </c>
-      <c r="D53" s="291"/>
-      <c r="E53" s="294">
-        <v>0</v>
-      </c>
-      <c r="F53" s="294"/>
+      <c r="D53" s="292"/>
+      <c r="E53" s="295">
+        <v>0</v>
+      </c>
+      <c r="F53" s="295"/>
     </row>
     <row r="54" spans="1:6" ht="15.75" customHeight="1" thickTop="1" thickBot="1">
-      <c r="A54" s="292"/>
-      <c r="B54" s="292"/>
-      <c r="C54" s="282" t="s">
+      <c r="A54" s="293"/>
+      <c r="B54" s="293"/>
+      <c r="C54" s="283" t="s">
         <v>224</v>
       </c>
-      <c r="D54" s="282"/>
-      <c r="E54" s="290">
+      <c r="D54" s="283"/>
+      <c r="E54" s="291">
         <f>SUM(E48:F53)</f>
         <v>110554716</v>
       </c>
-      <c r="F54" s="290"/>
+      <c r="F54" s="291"/>
     </row>
     <row r="55" spans="1:6" ht="15.75" customHeight="1" thickTop="1">
-      <c r="A55" s="289" t="s">
+      <c r="A55" s="290" t="s">
         <v>231</v>
       </c>
-      <c r="B55" s="292"/>
-      <c r="C55" s="285" t="s">
+      <c r="B55" s="293"/>
+      <c r="C55" s="286" t="s">
         <v>226</v>
       </c>
-      <c r="D55" s="293"/>
-      <c r="E55" s="287">
-        <v>0</v>
-      </c>
-      <c r="F55" s="287"/>
+      <c r="D55" s="294"/>
+      <c r="E55" s="288">
+        <v>0</v>
+      </c>
+      <c r="F55" s="288"/>
     </row>
     <row r="56" spans="1:6" ht="15.75" customHeight="1">
-      <c r="A56" s="292"/>
-      <c r="B56" s="292"/>
-      <c r="C56" s="286" t="s">
+      <c r="A56" s="293"/>
+      <c r="B56" s="293"/>
+      <c r="C56" s="287" t="s">
         <v>227</v>
       </c>
-      <c r="D56" s="291"/>
-      <c r="E56" s="288">
+      <c r="D56" s="292"/>
+      <c r="E56" s="289">
         <f>'Presupuesto Inicial'!J20*12</f>
         <v>700000</v>
       </c>
-      <c r="F56" s="288"/>
+      <c r="F56" s="289"/>
     </row>
     <row r="57" spans="1:6" ht="15.75" customHeight="1">
-      <c r="A57" s="292"/>
-      <c r="B57" s="292"/>
-      <c r="C57" s="286" t="s">
+      <c r="A57" s="293"/>
+      <c r="B57" s="293"/>
+      <c r="C57" s="287" t="s">
         <v>228</v>
       </c>
-      <c r="D57" s="291"/>
-      <c r="E57" s="288">
-        <v>0</v>
-      </c>
-      <c r="F57" s="288"/>
+      <c r="D57" s="292"/>
+      <c r="E57" s="289">
+        <v>0</v>
+      </c>
+      <c r="F57" s="289"/>
     </row>
     <row r="58" spans="1:6" ht="15.75" customHeight="1" thickBot="1">
-      <c r="A58" s="292"/>
-      <c r="B58" s="292"/>
-      <c r="C58" s="286" t="s">
+      <c r="A58" s="293"/>
+      <c r="B58" s="293"/>
+      <c r="C58" s="287" t="s">
         <v>229</v>
       </c>
-      <c r="D58" s="291"/>
-      <c r="E58" s="288">
-        <v>0</v>
-      </c>
-      <c r="F58" s="288"/>
+      <c r="D58" s="292"/>
+      <c r="E58" s="289">
+        <v>0</v>
+      </c>
+      <c r="F58" s="289"/>
     </row>
     <row r="59" spans="1:6" ht="15.75" customHeight="1" thickTop="1" thickBot="1">
-      <c r="A59" s="292"/>
-      <c r="B59" s="292"/>
-      <c r="C59" s="282" t="s">
+      <c r="A59" s="293"/>
+      <c r="B59" s="293"/>
+      <c r="C59" s="283" t="s">
         <v>230</v>
       </c>
-      <c r="D59" s="282"/>
-      <c r="E59" s="290">
+      <c r="D59" s="283"/>
+      <c r="E59" s="291">
         <f>SUM(E55:F58)</f>
         <v>700000</v>
       </c>
-      <c r="F59" s="282"/>
+      <c r="F59" s="283"/>
     </row>
     <row r="60" spans="1:6" ht="15.75" customHeight="1" thickTop="1">
-      <c r="A60" s="289" t="s">
+      <c r="A60" s="290" t="s">
         <v>235</v>
       </c>
-      <c r="B60" s="289"/>
-      <c r="C60" s="285" t="s">
+      <c r="B60" s="290"/>
+      <c r="C60" s="286" t="s">
         <v>245</v>
       </c>
-      <c r="D60" s="285"/>
-      <c r="E60" s="287">
+      <c r="D60" s="286"/>
+      <c r="E60" s="288">
         <f>('Presupuesto Inicial'!B12+'Presupuesto Inicial'!B13)+('Presupuesto Inicial'!B11*6)+('Salarios, gastos y costos'!K11*12)</f>
         <v>7848920</v>
       </c>
-      <c r="F60" s="287"/>
+      <c r="F60" s="288"/>
     </row>
     <row r="61" spans="1:6" ht="15.75" customHeight="1" thickBot="1">
-      <c r="A61" s="289"/>
-      <c r="B61" s="289"/>
-      <c r="C61" s="286" t="s">
+      <c r="A61" s="290"/>
+      <c r="B61" s="290"/>
+      <c r="C61" s="287" t="s">
         <v>233</v>
       </c>
-      <c r="D61" s="286"/>
-      <c r="E61" s="288">
+      <c r="D61" s="287"/>
+      <c r="E61" s="289">
         <f>'Presupuesto Inicial'!B2</f>
         <v>116700</v>
       </c>
-      <c r="F61" s="288"/>
+      <c r="F61" s="289"/>
     </row>
     <row r="62" spans="1:6" ht="15.75" customHeight="1" thickTop="1" thickBot="1">
-      <c r="A62" s="289"/>
-      <c r="B62" s="289"/>
-      <c r="C62" s="282" t="s">
+      <c r="A62" s="290"/>
+      <c r="B62" s="290"/>
+      <c r="C62" s="283" t="s">
         <v>234</v>
       </c>
-      <c r="D62" s="282"/>
-      <c r="E62" s="290">
+      <c r="D62" s="283"/>
+      <c r="E62" s="291">
         <f>E60+E61</f>
         <v>7965620</v>
       </c>
-      <c r="F62" s="290"/>
+      <c r="F62" s="291"/>
     </row>
     <row r="63" spans="1:6" ht="15.75" customHeight="1" thickTop="1" thickBot="1">
-      <c r="A63" s="282" t="s">
+      <c r="A63" s="283" t="s">
         <v>239</v>
       </c>
-      <c r="B63" s="282"/>
-      <c r="C63" s="282"/>
-      <c r="D63" s="282"/>
-      <c r="E63" s="284">
+      <c r="B63" s="283"/>
+      <c r="C63" s="283"/>
+      <c r="D63" s="283"/>
+      <c r="E63" s="285">
         <f>E54+E59+E62</f>
         <v>119220336</v>
       </c>
-      <c r="F63" s="284"/>
+      <c r="F63" s="285"/>
     </row>
     <row r="64" spans="1:6" ht="15.75" customHeight="1" thickTop="1"/>
     <row r="65" spans="7:8" ht="15.75" customHeight="1" thickBot="1"/>
@@ -15865,26 +15919,26 @@
     <row r="67" spans="7:8" ht="15.75" customHeight="1" thickTop="1"/>
     <row r="160" ht="15.75" customHeight="1" thickBot="1"/>
     <row r="161" spans="50:57" ht="15.75" customHeight="1" thickTop="1" thickBot="1">
-      <c r="AX161" s="282" t="s">
+      <c r="AX161" s="283" t="s">
         <v>214</v>
       </c>
-      <c r="AY161" s="282"/>
-      <c r="AZ161" s="282"/>
-      <c r="BA161" s="282"/>
-      <c r="BB161" s="282"/>
-      <c r="BC161" s="282"/>
-      <c r="BD161" s="282"/>
-      <c r="BE161" s="282"/>
+      <c r="AY161" s="283"/>
+      <c r="AZ161" s="283"/>
+      <c r="BA161" s="283"/>
+      <c r="BB161" s="283"/>
+      <c r="BC161" s="283"/>
+      <c r="BD161" s="283"/>
+      <c r="BE161" s="283"/>
     </row>
     <row r="162" spans="50:57" ht="15.75" customHeight="1" thickTop="1" thickBot="1">
-      <c r="AX162" s="283"/>
-      <c r="AY162" s="283"/>
-      <c r="AZ162" s="283"/>
-      <c r="BA162" s="283"/>
-      <c r="BB162" s="283"/>
-      <c r="BC162" s="283"/>
-      <c r="BD162" s="283"/>
-      <c r="BE162" s="283"/>
+      <c r="AX162" s="284"/>
+      <c r="AY162" s="284"/>
+      <c r="AZ162" s="284"/>
+      <c r="BA162" s="284"/>
+      <c r="BB162" s="284"/>
+      <c r="BC162" s="284"/>
+      <c r="BD162" s="284"/>
+      <c r="BE162" s="284"/>
     </row>
     <row r="163" spans="50:57" s="244" customFormat="1" ht="50.25" customHeight="1" thickTop="1" thickBot="1">
       <c r="AX163" s="242" t="s">
@@ -16168,28 +16222,28 @@
   <sheetData>
     <row r="1" spans="1:4" ht="15.75" customHeight="1" thickBot="1"/>
     <row r="2" spans="1:4" ht="15.75" customHeight="1" thickTop="1" thickBot="1">
-      <c r="A2" s="282" t="s">
+      <c r="A2" s="283" t="s">
         <v>7</v>
       </c>
-      <c r="B2" s="300"/>
-      <c r="C2" s="300"/>
-      <c r="D2" s="300"/>
+      <c r="B2" s="301"/>
+      <c r="C2" s="301"/>
+      <c r="D2" s="301"/>
     </row>
     <row r="3" spans="1:4" ht="15.75" customHeight="1" thickTop="1">
-      <c r="A3" s="302" t="s">
+      <c r="A3" s="303" t="s">
         <v>14</v>
       </c>
-      <c r="B3" s="297"/>
-      <c r="C3" s="302" t="s">
+      <c r="B3" s="298"/>
+      <c r="C3" s="303" t="s">
         <v>15</v>
       </c>
-      <c r="D3" s="297"/>
+      <c r="D3" s="298"/>
     </row>
     <row r="4" spans="1:4" ht="15.75" customHeight="1">
-      <c r="A4" s="303" t="s">
+      <c r="A4" s="304" t="s">
         <v>16</v>
       </c>
-      <c r="B4" s="306">
+      <c r="B4" s="307">
         <v>1500000</v>
       </c>
       <c r="C4" s="18" t="s">
@@ -16200,16 +16254,16 @@
       </c>
     </row>
     <row r="5" spans="1:4" ht="15.75" customHeight="1">
-      <c r="A5" s="304"/>
-      <c r="B5" s="304"/>
-      <c r="C5" s="302" t="s">
+      <c r="A5" s="305"/>
+      <c r="B5" s="305"/>
+      <c r="C5" s="303" t="s">
         <v>35</v>
       </c>
-      <c r="D5" s="297"/>
+      <c r="D5" s="298"/>
     </row>
     <row r="6" spans="1:4" ht="15.75" customHeight="1">
-      <c r="A6" s="304"/>
-      <c r="B6" s="304"/>
+      <c r="A6" s="305"/>
+      <c r="B6" s="305"/>
       <c r="C6" s="18" t="s">
         <v>36</v>
       </c>
@@ -16218,8 +16272,8 @@
       </c>
     </row>
     <row r="7" spans="1:4" ht="15.75" customHeight="1">
-      <c r="A7" s="304"/>
-      <c r="B7" s="304"/>
+      <c r="A7" s="305"/>
+      <c r="B7" s="305"/>
       <c r="C7" s="18" t="s">
         <v>39</v>
       </c>
@@ -16228,8 +16282,8 @@
       </c>
     </row>
     <row r="8" spans="1:4" ht="15.75" customHeight="1">
-      <c r="A8" s="305"/>
-      <c r="B8" s="305"/>
+      <c r="A8" s="306"/>
+      <c r="B8" s="306"/>
       <c r="C8" s="18" t="s">
         <v>236</v>
       </c>
@@ -16254,15 +16308,15 @@
       </c>
     </row>
     <row r="10" spans="1:4" ht="15.75" customHeight="1" thickTop="1" thickBot="1">
-      <c r="A10" s="282" t="s">
+      <c r="A10" s="283" t="s">
         <v>53</v>
       </c>
-      <c r="B10" s="300"/>
-      <c r="C10" s="301">
+      <c r="B10" s="301"/>
+      <c r="C10" s="302">
         <f>D4+D9</f>
         <v>1500000</v>
       </c>
-      <c r="D10" s="300"/>
+      <c r="D10" s="301"/>
     </row>
     <row r="11" spans="1:4" ht="15.75" customHeight="1" thickTop="1"/>
     <row r="12" spans="1:4" ht="15.75" customHeight="1">
@@ -16298,49 +16352,49 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:6" ht="15">
-      <c r="B2" s="307" t="s">
+      <c r="B2" s="308" t="s">
         <v>238</v>
       </c>
-      <c r="C2" s="307"/>
-      <c r="D2" s="307"/>
-      <c r="E2" s="307"/>
-      <c r="F2" s="307"/>
+      <c r="C2" s="308"/>
+      <c r="D2" s="308"/>
+      <c r="E2" s="308"/>
+      <c r="F2" s="308"/>
     </row>
     <row r="3" spans="2:6">
-      <c r="B3" s="283" t="s">
+      <c r="B3" s="284" t="s">
         <v>240</v>
       </c>
-      <c r="C3" s="283"/>
-      <c r="D3" s="283"/>
-      <c r="E3" s="309">
+      <c r="C3" s="284"/>
+      <c r="D3" s="284"/>
+      <c r="E3" s="310">
         <f>'Salarios, gastos y costos'!E62:F62</f>
         <v>7965620</v>
       </c>
-      <c r="F3" s="309"/>
+      <c r="F3" s="310"/>
     </row>
     <row r="4" spans="2:6">
-      <c r="B4" s="310" t="s">
+      <c r="B4" s="311" t="s">
         <v>241</v>
       </c>
-      <c r="C4" s="283"/>
-      <c r="D4" s="283"/>
-      <c r="E4" s="311">
+      <c r="C4" s="284"/>
+      <c r="D4" s="284"/>
+      <c r="E4" s="312">
         <f>'Salarios, gastos y costos'!B11*7</f>
         <v>64490251</v>
       </c>
-      <c r="F4" s="311"/>
+      <c r="F4" s="312"/>
     </row>
     <row r="5" spans="2:6" ht="15">
-      <c r="B5" s="307" t="s">
+      <c r="B5" s="308" t="s">
         <v>210</v>
       </c>
-      <c r="C5" s="307"/>
-      <c r="D5" s="307"/>
-      <c r="E5" s="308">
+      <c r="C5" s="308"/>
+      <c r="D5" s="308"/>
+      <c r="E5" s="309">
         <f>SUM(E3:F4)</f>
         <v>72455871</v>
       </c>
-      <c r="F5" s="308"/>
+      <c r="F5" s="309"/>
     </row>
   </sheetData>
   <mergeCells count="7">
@@ -16364,8 +16418,8 @@
   </sheetPr>
   <dimension ref="A1:Y24"/>
   <sheetViews>
-    <sheetView topLeftCell="A3" zoomScale="175" zoomScaleNormal="175" workbookViewId="0">
-      <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
+    <sheetView topLeftCell="A6" zoomScale="175" zoomScaleNormal="175" workbookViewId="0">
+      <pane xSplit="1" topLeftCell="R1" activePane="topRight" state="frozen"/>
       <selection pane="topRight" activeCell="F113" sqref="F113"/>
     </sheetView>
   </sheetViews>
@@ -16413,30 +16467,30 @@
       <c r="G1" s="123" t="s">
         <v>62</v>
       </c>
-      <c r="H1" s="313" t="s">
+      <c r="H1" s="314" t="s">
         <v>63</v>
       </c>
-      <c r="I1" s="297"/>
-      <c r="J1" s="312" t="s">
+      <c r="I1" s="298"/>
+      <c r="J1" s="313" t="s">
         <v>64</v>
       </c>
-      <c r="K1" s="297"/>
-      <c r="L1" s="312" t="s">
+      <c r="K1" s="298"/>
+      <c r="L1" s="313" t="s">
         <v>65</v>
       </c>
-      <c r="M1" s="297"/>
-      <c r="N1" s="312" t="s">
+      <c r="M1" s="298"/>
+      <c r="N1" s="313" t="s">
         <v>66</v>
       </c>
-      <c r="O1" s="297"/>
-      <c r="P1" s="312" t="s">
+      <c r="O1" s="298"/>
+      <c r="P1" s="313" t="s">
         <v>67</v>
       </c>
-      <c r="Q1" s="297"/>
-      <c r="R1" s="312" t="s">
+      <c r="Q1" s="298"/>
+      <c r="R1" s="313" t="s">
         <v>68</v>
       </c>
-      <c r="S1" s="297"/>
+      <c r="S1" s="298"/>
       <c r="U1" s="140" t="s">
         <v>70</v>
       </c>
@@ -17778,8 +17832,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:R25"/>
   <sheetViews>
-    <sheetView zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <selection activeCell="B2" sqref="B1:E1048576"/>
+    <sheetView topLeftCell="B1" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
+      <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1"/>
@@ -17796,26 +17850,26 @@
   <sheetData>
     <row r="1" spans="1:18" ht="12.75">
       <c r="A1" s="25"/>
-      <c r="B1" s="312" t="s">
+      <c r="B1" s="313" t="s">
         <v>70</v>
       </c>
-      <c r="C1" s="297"/>
-      <c r="D1" s="312" t="s">
+      <c r="C1" s="298"/>
+      <c r="D1" s="313" t="s">
         <v>71</v>
       </c>
-      <c r="E1" s="297"/>
-      <c r="F1" s="312" t="s">
+      <c r="E1" s="298"/>
+      <c r="F1" s="313" t="s">
         <v>72</v>
       </c>
-      <c r="G1" s="297"/>
-      <c r="H1" s="312" t="s">
+      <c r="G1" s="298"/>
+      <c r="H1" s="313" t="s">
         <v>74</v>
       </c>
-      <c r="I1" s="297"/>
-      <c r="J1" s="314" t="s">
+      <c r="I1" s="298"/>
+      <c r="J1" s="315" t="s">
         <v>75</v>
       </c>
-      <c r="K1" s="315"/>
+      <c r="K1" s="316"/>
       <c r="L1" s="27"/>
       <c r="M1" s="27"/>
       <c r="N1" s="27"/>
@@ -18710,9 +18764,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AC16"/>
   <sheetViews>
-    <sheetView topLeftCell="A20" zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="C13" sqref="C13"/>
+    <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <pane xSplit="1" topLeftCell="T1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="AA4" sqref="AA4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1"/>
@@ -18749,58 +18803,58 @@
   <sheetData>
     <row r="1" spans="1:29" s="149" customFormat="1" ht="15.75" customHeight="1">
       <c r="A1" s="152"/>
-      <c r="B1" s="316" t="s">
+      <c r="B1" s="317" t="s">
         <v>104</v>
       </c>
-      <c r="C1" s="317"/>
-      <c r="D1" s="316" t="s">
+      <c r="C1" s="318"/>
+      <c r="D1" s="317" t="s">
         <v>55</v>
       </c>
-      <c r="E1" s="317"/>
-      <c r="F1" s="316" t="s">
+      <c r="E1" s="318"/>
+      <c r="F1" s="317" t="s">
         <v>58</v>
       </c>
-      <c r="G1" s="317"/>
-      <c r="H1" s="316" t="s">
+      <c r="G1" s="318"/>
+      <c r="H1" s="317" t="s">
         <v>59</v>
       </c>
-      <c r="I1" s="317"/>
-      <c r="J1" s="316" t="s">
+      <c r="I1" s="318"/>
+      <c r="J1" s="317" t="s">
         <v>60</v>
       </c>
-      <c r="K1" s="317"/>
-      <c r="L1" s="316" t="s">
+      <c r="K1" s="318"/>
+      <c r="L1" s="317" t="s">
         <v>61</v>
       </c>
-      <c r="M1" s="317"/>
-      <c r="N1" s="316" t="s">
+      <c r="M1" s="318"/>
+      <c r="N1" s="317" t="s">
         <v>62</v>
       </c>
-      <c r="O1" s="317"/>
-      <c r="P1" s="316" t="s">
+      <c r="O1" s="318"/>
+      <c r="P1" s="317" t="s">
         <v>63</v>
       </c>
-      <c r="Q1" s="317"/>
-      <c r="R1" s="316" t="s">
+      <c r="Q1" s="318"/>
+      <c r="R1" s="317" t="s">
         <v>64</v>
       </c>
-      <c r="S1" s="317"/>
-      <c r="T1" s="316" t="s">
+      <c r="S1" s="318"/>
+      <c r="T1" s="317" t="s">
         <v>65</v>
       </c>
-      <c r="U1" s="317"/>
-      <c r="V1" s="316" t="s">
+      <c r="U1" s="318"/>
+      <c r="V1" s="317" t="s">
         <v>66</v>
       </c>
-      <c r="W1" s="317"/>
-      <c r="X1" s="316" t="s">
+      <c r="W1" s="318"/>
+      <c r="X1" s="317" t="s">
         <v>67</v>
       </c>
-      <c r="Y1" s="317"/>
-      <c r="Z1" s="316" t="s">
+      <c r="Y1" s="318"/>
+      <c r="Z1" s="317" t="s">
         <v>68</v>
       </c>
-      <c r="AA1" s="317"/>
+      <c r="AA1" s="318"/>
     </row>
     <row r="2" spans="1:29" ht="15.75" customHeight="1">
       <c r="A2" s="30" t="s">
@@ -18868,7 +18922,7 @@
       </c>
       <c r="Q2" s="33">
         <f>SUM(Q3:Q9)</f>
-        <v>11196991.958654905</v>
+        <v>12663658.958654905</v>
       </c>
       <c r="R2" s="32">
         <f t="shared" ref="R2:R9" si="8">S2/$S$2</f>
@@ -18876,7 +18930,7 @@
       </c>
       <c r="S2" s="33">
         <f>SUM(S3:S9)</f>
-        <v>12748082.307240065</v>
+        <v>14214749.307240065</v>
       </c>
       <c r="T2" s="32">
         <f t="shared" ref="T2:T9" si="9">U2/$U$2</f>
@@ -18884,7 +18938,7 @@
       </c>
       <c r="U2" s="33">
         <f>SUM(U3:U9)</f>
-        <v>14679951.342581803</v>
+        <v>16146618.342581803</v>
       </c>
       <c r="V2" s="32">
         <f t="shared" ref="V2:V9" si="10">W2/$W$2</f>
@@ -18892,7 +18946,7 @@
       </c>
       <c r="W2" s="33">
         <f>SUM(W3:W9)</f>
-        <v>17073478.113339286</v>
+        <v>18540145.113339286</v>
       </c>
       <c r="X2" s="32">
         <f t="shared" ref="X2:X9" si="11">Y2/$Y$2</f>
@@ -18900,7 +18954,7 @@
       </c>
       <c r="Y2" s="33">
         <f>SUM(Y3:Y9)</f>
-        <v>20019770.482492886</v>
+        <v>21486437.482492886</v>
       </c>
       <c r="Z2" s="32">
         <f t="shared" ref="Z2:Z9" si="12">AA2/$AA$2</f>
@@ -18908,11 +18962,11 @@
       </c>
       <c r="AA2" s="37">
         <f>SUM(AA3:AA9)</f>
-        <v>23617603.265701436</v>
+        <v>25084270.265701436</v>
       </c>
       <c r="AC2" s="145">
         <f t="shared" ref="AC2:AC6" si="13">AA2+Y2+W2+U2+S2+Q2+O2+M2+K2+I2+G2+E2</f>
-        <v>157865095.4700104</v>
+        <v>166665097.4700104</v>
       </c>
     </row>
     <row r="3" spans="1:29" ht="15.75" customHeight="1">
@@ -18976,55 +19030,55 @@
       </c>
       <c r="P3" s="40">
         <f t="shared" si="7"/>
-        <v>0.69181312522176308</v>
+        <v>0.72750640475069817</v>
       </c>
       <c r="Q3" s="42">
-        <f>'Salarios, gastos y costos'!$B$27</f>
-        <v>7746226</v>
+        <f>'Salarios, gastos y costos'!$B$11</f>
+        <v>9212893</v>
       </c>
       <c r="R3" s="40">
         <f t="shared" si="8"/>
-        <v>0.60763853051063665</v>
+        <v>0.6481220879011601</v>
       </c>
       <c r="S3" s="42">
-        <f>'Salarios, gastos y costos'!$B$27</f>
-        <v>7746226</v>
+        <f>'Salarios, gastos y costos'!$B$11</f>
+        <v>9212893</v>
       </c>
       <c r="T3" s="40">
         <f t="shared" si="9"/>
-        <v>0.52767381983962691</v>
+        <v>0.57057724438211266</v>
       </c>
       <c r="U3" s="42">
-        <f>'Salarios, gastos y costos'!$B$27</f>
-        <v>7746226</v>
+        <f>'Salarios, gastos y costos'!$B$11</f>
+        <v>9212893</v>
       </c>
       <c r="V3" s="40">
         <f t="shared" si="10"/>
-        <v>0.45369935455318705</v>
+        <v>0.49691590565661198</v>
       </c>
       <c r="W3" s="42">
-        <f>'Salarios, gastos y costos'!$B$27</f>
-        <v>7746226</v>
+        <f>'Salarios, gastos y costos'!$B$11</f>
+        <v>9212893</v>
       </c>
       <c r="X3" s="40">
         <f t="shared" si="11"/>
-        <v>0.38692881153527742</v>
+        <v>0.4287771301085464</v>
       </c>
       <c r="Y3" s="42">
-        <f>'Salarios, gastos y costos'!$B$27</f>
-        <v>7746226</v>
+        <f>'Salarios, gastos y costos'!$B$11</f>
+        <v>9212893</v>
       </c>
       <c r="Z3" s="40">
         <f t="shared" si="12"/>
-        <v>0.32798527068364403</v>
+        <v>0.36727769643740038</v>
       </c>
       <c r="AA3" s="45">
-        <f>'Salarios, gastos y costos'!$B$27</f>
-        <v>7746226</v>
+        <f>'Salarios, gastos y costos'!$B$11</f>
+        <v>9212893</v>
       </c>
       <c r="AC3" s="145">
         <f t="shared" si="13"/>
-        <v>101754714</v>
+        <v>110554716</v>
       </c>
     </row>
     <row r="4" spans="1:29" ht="15.75" customHeight="1">
@@ -19088,7 +19142,7 @@
       </c>
       <c r="P4" s="40">
         <f t="shared" si="7"/>
-        <v>2.965171371257146E-2</v>
+        <v>2.6217541161205206E-2</v>
       </c>
       <c r="Q4" s="42">
         <f>'Salarios, gastos y costos'!$K$11</f>
@@ -19096,7 +19150,7 @@
       </c>
       <c r="R4" s="40">
         <f t="shared" si="8"/>
-        <v>2.6043917194623095E-2</v>
+        <v>2.3356725667395047E-2</v>
       </c>
       <c r="S4" s="42">
         <f>'Salarios, gastos y costos'!$K$11</f>
@@ -19104,7 +19158,7 @@
       </c>
       <c r="T4" s="40">
         <f t="shared" si="9"/>
-        <v>2.2616559977072001E-2</v>
+        <v>2.0562200267310739E-2</v>
       </c>
       <c r="U4" s="42">
         <f>'Salarios, gastos y costos'!$K$11</f>
@@ -19112,7 +19166,7 @@
       </c>
       <c r="V4" s="40">
         <f t="shared" si="10"/>
-        <v>1.9445949899370821E-2</v>
+        <v>1.7907626826562703E-2</v>
       </c>
       <c r="W4" s="42">
         <f>'Salarios, gastos y costos'!$K$11</f>
@@ -19120,7 +19174,7 @@
       </c>
       <c r="X4" s="40">
         <f t="shared" si="11"/>
-        <v>1.6584106210924838E-2</v>
+        <v>1.5452072977222082E-2</v>
       </c>
       <c r="Y4" s="42">
         <f>'Salarios, gastos y costos'!$K$11</f>
@@ -19128,7 +19182,7 @@
       </c>
       <c r="Z4" s="40">
         <f t="shared" si="12"/>
-        <v>1.405773465939112E-2</v>
+        <v>1.3235784676342306E-2</v>
       </c>
       <c r="AA4" s="45">
         <f>'Salarios, gastos y costos'!$K$11</f>
@@ -19314,7 +19368,7 @@
       </c>
       <c r="P6" s="40">
         <f t="shared" si="7"/>
-        <v>5.430029799476958E-3</v>
+        <v>4.8011400337377684E-3</v>
       </c>
       <c r="Q6" s="42">
         <f>'Salarios, gastos y costos'!$E$27</f>
@@ -19322,7 +19376,7 @@
       </c>
       <c r="R6" s="40">
         <f t="shared" si="8"/>
-        <v>4.7693447951359423E-3</v>
+        <v>4.2772474340460193E-3</v>
       </c>
       <c r="S6" s="42">
         <f>'Salarios, gastos y costos'!$E$27</f>
@@ -19330,7 +19384,7 @@
       </c>
       <c r="T6" s="40">
         <f t="shared" si="9"/>
-        <v>4.1417031011294165E-3</v>
+        <v>3.7654943412924091E-3</v>
       </c>
       <c r="U6" s="42">
         <f>'Salarios, gastos y costos'!$E$27</f>
@@ -19338,7 +19392,7 @@
       </c>
       <c r="V6" s="40">
         <f t="shared" si="10"/>
-        <v>3.5610787442599498E-3</v>
+        <v>3.2793702329900073E-3</v>
       </c>
       <c r="W6" s="42">
         <f>'Salarios, gastos y costos'!$E$27</f>
@@ -19346,7 +19400,7 @@
       </c>
       <c r="X6" s="40">
         <f t="shared" si="11"/>
-        <v>3.0369978543544774E-3</v>
+        <v>2.8296919882386151E-3</v>
       </c>
       <c r="Y6" s="42">
         <f>'Salarios, gastos y costos'!$E$27</f>
@@ -19354,7 +19408,7 @@
       </c>
       <c r="Z6" s="40">
         <f t="shared" si="12"/>
-        <v>2.5743509752446619E-3</v>
+        <v>2.4238297289889228E-3</v>
       </c>
       <c r="AA6" s="45">
         <f>'Salarios, gastos y costos'!$E$27</f>
@@ -19632,7 +19686,7 @@
       </c>
       <c r="P9" s="40">
         <f t="shared" si="7"/>
-        <v>0.22264515039933852</v>
+        <v>0.19685905683294708</v>
       </c>
       <c r="Q9" s="41">
         <f>'Estado de resultados PyG - 12 m'!I15</f>
@@ -19640,7 +19694,7 @@
       </c>
       <c r="R9" s="40">
         <f t="shared" si="8"/>
-        <v>0.31722781590006799</v>
+        <v>0.28449649162509622</v>
       </c>
       <c r="S9" s="41">
         <f>'Estado de resultados PyG - 12 m'!K15</f>
@@ -19648,7 +19702,7 @@
       </c>
       <c r="T9" s="40">
         <f t="shared" si="9"/>
-        <v>0.40708005109305784</v>
+        <v>0.37010321392326101</v>
       </c>
       <c r="U9" s="41">
         <f>'Estado de resultados PyG - 12 m'!M15</f>
@@ -19656,7 +19710,7 @@
       </c>
       <c r="V9" s="40">
         <f t="shared" si="10"/>
-        <v>0.49020135544616134</v>
+        <v>0.45142268640160915</v>
       </c>
       <c r="W9" s="41">
         <f>'Estado de resultados PyG - 12 m'!O15</f>
@@ -19664,7 +19718,7 @@
       </c>
       <c r="X9" s="40">
         <f t="shared" si="11"/>
-        <v>0.56522798262789276</v>
+        <v>0.52664544746949926</v>
       </c>
       <c r="Y9" s="41">
         <f>'Estado de resultados PyG - 12 m'!Q15</f>
@@ -19672,7 +19726,7 @@
       </c>
       <c r="Z9" s="40">
         <f t="shared" si="12"/>
-        <v>0.63145980978347627</v>
+        <v>0.59453861355071014</v>
       </c>
       <c r="AA9" s="53">
         <f>'Estado de resultados PyG - 12 m'!S15</f>
@@ -20021,36 +20075,42 @@
       <c r="P13" s="150"/>
       <c r="Q13" s="150">
         <f>O13-Q2+Q10</f>
-        <v>16613549.782486973</v>
+        <v>15146882.782486973</v>
       </c>
       <c r="R13" s="150"/>
       <c r="S13" s="150">
         <f>Q13-S2+S10</f>
-        <v>25988757.65340396</v>
+        <v>23055423.65340396</v>
       </c>
       <c r="T13" s="150"/>
       <c r="U13" s="150">
         <f>S13-U2+U10</f>
-        <v>39114064.239984326</v>
+        <v>34714063.239984326</v>
       </c>
       <c r="V13" s="150"/>
       <c r="W13" s="150">
         <f>U13-W2+W10</f>
-        <v>56885628.675682157</v>
+        <v>51018960.675682157</v>
       </c>
       <c r="X13" s="150"/>
       <c r="Y13" s="150">
         <f>W13-Y2+Y10</f>
-        <v>80376466.533854634</v>
+        <v>73043131.533854634</v>
       </c>
       <c r="Z13" s="150"/>
       <c r="AA13" s="150">
         <f>Y13-AA2+AA10</f>
-        <v>110851332.73590252</v>
+        <v>102051330.73590252</v>
       </c>
       <c r="AC13" s="151">
         <f t="shared" si="14"/>
-        <v>538906036.62131453</v>
+        <v>508106029.62131459</v>
+      </c>
+    </row>
+    <row r="15" spans="1:29" ht="15.75" customHeight="1">
+      <c r="AA15" s="192">
+        <f>AA13-C10</f>
+        <v>29595330.735902518</v>
       </c>
     </row>
     <row r="16" spans="1:29" ht="15.75" customHeight="1">
@@ -20081,11 +20141,11 @@
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:T13"/>
+  <dimension ref="A1:T14"/>
   <sheetViews>
     <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="A12" sqref="A12:M13"/>
+      <pane xSplit="1" topLeftCell="D1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="E14" sqref="E14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1"/>
@@ -20101,30 +20161,30 @@
   <sheetData>
     <row r="1" spans="1:20" ht="15.75" customHeight="1">
       <c r="A1" s="26"/>
-      <c r="B1" s="318" t="s">
+      <c r="B1" s="319" t="s">
         <v>73</v>
       </c>
-      <c r="C1" s="297"/>
-      <c r="D1" s="318" t="s">
+      <c r="C1" s="298"/>
+      <c r="D1" s="319" t="s">
         <v>70</v>
       </c>
-      <c r="E1" s="297"/>
-      <c r="F1" s="318" t="s">
+      <c r="E1" s="298"/>
+      <c r="F1" s="319" t="s">
         <v>71</v>
       </c>
-      <c r="G1" s="297"/>
-      <c r="H1" s="318" t="s">
+      <c r="G1" s="298"/>
+      <c r="H1" s="319" t="s">
         <v>72</v>
       </c>
-      <c r="I1" s="297"/>
-      <c r="J1" s="318" t="s">
+      <c r="I1" s="298"/>
+      <c r="J1" s="319" t="s">
         <v>74</v>
       </c>
-      <c r="K1" s="297"/>
-      <c r="L1" s="318" t="s">
+      <c r="K1" s="298"/>
+      <c r="L1" s="319" t="s">
         <v>75</v>
       </c>
-      <c r="M1" s="297"/>
+      <c r="M1" s="298"/>
       <c r="N1" s="28"/>
       <c r="O1" s="28"/>
       <c r="P1" s="28"/>
@@ -20138,52 +20198,52 @@
         <v>76</v>
       </c>
       <c r="B2" s="62">
-        <f t="shared" ref="B2:B9" si="0">C2/$C$2</f>
+        <f t="shared" ref="B2:B10" si="0">C2/$C$2</f>
         <v>1</v>
       </c>
       <c r="C2" s="33">
-        <f>SUM(C3:C9)</f>
+        <f>SUM(C3:C10)</f>
         <v>3677500</v>
       </c>
       <c r="D2" s="32">
-        <f t="shared" ref="D2:D9" si="1">E2/$E$2</f>
+        <f t="shared" ref="D2:D10" si="1">E2/$E$2</f>
         <v>1</v>
       </c>
       <c r="E2" s="33">
-        <f>SUM(E3:E9)</f>
-        <v>166665100.89131266</v>
+        <f>SUM(E3:E10)</f>
+        <v>167365100.90346217</v>
       </c>
       <c r="F2" s="32">
-        <f t="shared" ref="F2:F9" si="2">G2/$G$2</f>
+        <f t="shared" ref="F2:F10" si="2">G2/$G$2</f>
         <v>1</v>
       </c>
       <c r="G2" s="33">
-        <f>SUM(G3:G9)</f>
-        <v>191419598.06656539</v>
+        <f>SUM(G3:G10)</f>
+        <v>192119598.06656539</v>
       </c>
       <c r="H2" s="32">
-        <f t="shared" ref="H2:H9" si="3">I2/$I$2</f>
+        <f t="shared" ref="H2:H10" si="3">I2/$I$2</f>
         <v>1</v>
       </c>
       <c r="I2" s="33">
-        <f>SUM(I3:I9)</f>
-        <v>245311899.25142169</v>
+        <f>SUM(I3:I10)</f>
+        <v>246011899.25142169</v>
       </c>
       <c r="J2" s="32">
-        <f t="shared" ref="J2:J9" si="4">K2/$K$2</f>
+        <f t="shared" ref="J2:J10" si="4">K2/$K$2</f>
         <v>1</v>
       </c>
       <c r="K2" s="33">
-        <f>SUM(K3:K9)</f>
-        <v>250161087.0991841</v>
+        <f>SUM(K3:K10)</f>
+        <v>250861087.0991841</v>
       </c>
       <c r="L2" s="32">
-        <f t="shared" ref="L2:L9" si="5">M2/$M$2</f>
+        <f t="shared" ref="L2:L10" si="5">M2/$M$2</f>
         <v>1</v>
       </c>
       <c r="M2" s="37">
-        <f>SUM(M3:M9)</f>
-        <v>250574520.64977443</v>
+        <f>SUM(M3:M10)</f>
+        <v>251274520.64977443</v>
       </c>
       <c r="N2" s="38"/>
       <c r="O2" s="38"/>
@@ -20206,15 +20266,15 @@
       </c>
       <c r="D3" s="40">
         <f t="shared" si="1"/>
-        <v>0.66333453931026454</v>
-      </c>
-      <c r="E3" s="42">
+        <v>0.66056016052358901</v>
+      </c>
+      <c r="E3" s="80">
         <f>'Estado de resultados PyG - 5 añ'!C6</f>
         <v>110554717.91883764</v>
       </c>
       <c r="F3" s="40">
         <f t="shared" si="2"/>
-        <v>0.52026018216467407</v>
+        <v>0.51836458103298155</v>
       </c>
       <c r="G3" s="42">
         <f>'Estado de resultados PyG - 5 añ'!E6</f>
@@ -20222,7 +20282,7 @@
       </c>
       <c r="H3" s="40">
         <f t="shared" si="3"/>
-        <v>0.40821814533083495</v>
+        <v>0.407056605167123</v>
       </c>
       <c r="I3" s="42">
         <f>'Estado de resultados PyG - 5 añ'!G6</f>
@@ -20230,7 +20290,7 @@
       </c>
       <c r="J3" s="40">
         <f t="shared" si="4"/>
-        <v>0.40251480870834616</v>
+        <v>0.40139163584262211</v>
       </c>
       <c r="K3" s="42">
         <f>'Estado de resultados PyG - 5 añ'!I6</f>
@@ -20238,7 +20298,7 @@
       </c>
       <c r="L3" s="40">
         <f t="shared" si="5"/>
-        <v>0.40273309229651255</v>
+        <v>0.40161115934494013</v>
       </c>
       <c r="M3" s="45">
         <f>'Estado de resultados PyG - 5 añ'!K6</f>
@@ -20265,15 +20325,15 @@
       </c>
       <c r="D4" s="40">
         <f t="shared" si="1"/>
-        <v>2.3904944993543391E-2</v>
-      </c>
-      <c r="E4" s="42">
+        <v>2.380496320704439E-2</v>
+      </c>
+      <c r="E4" s="80">
         <f>'Estado de resultados PyG - 5 añ'!C9</f>
         <v>3984120.0691501889</v>
       </c>
       <c r="F4" s="40">
         <f t="shared" si="2"/>
-        <v>2.2062355766887625E-2</v>
+        <v>2.198197016754096E-2</v>
       </c>
       <c r="G4" s="42">
         <f>'Estado de resultados PyG - 5 añ'!E9</f>
@@ -20281,7 +20341,7 @@
       </c>
       <c r="H4" s="40">
         <f t="shared" si="3"/>
-        <v>1.7296706301622097E-2</v>
+        <v>1.7247490412276998E-2</v>
       </c>
       <c r="I4" s="42">
         <f>'Estado de resultados PyG - 5 añ'!G9</f>
@@ -20289,7 +20349,7 @@
       </c>
       <c r="J4" s="40">
         <f t="shared" si="4"/>
-        <v>1.7041053520448209E-2</v>
+        <v>1.6993502353377019E-2</v>
       </c>
       <c r="K4" s="42">
         <f>'Estado de resultados PyG - 5 añ'!I9</f>
@@ -20297,7 +20357,7 @@
       </c>
       <c r="L4" s="40">
         <f t="shared" si="5"/>
-        <v>1.7044736643828624E-2</v>
+        <v>1.6997253454447438E-2</v>
       </c>
       <c r="M4" s="45">
         <f>'Estado de resultados PyG - 5 añ'!K9</f>
@@ -20385,15 +20445,15 @@
       </c>
       <c r="D6" s="40">
         <f t="shared" si="1"/>
-        <v>4.3776411264155064E-3</v>
-      </c>
-      <c r="E6" s="42">
+        <v>4.359331760692693E-3</v>
+      </c>
+      <c r="E6" s="80">
         <f>'Flujo de caja - 12 meses'!AC6</f>
         <v>729600</v>
       </c>
       <c r="F6" s="40">
         <f t="shared" si="2"/>
-        <v>4.0402132687117108E-3</v>
+        <v>4.0254924941704358E-3</v>
       </c>
       <c r="G6" s="42">
         <f>'Flujo de caja - 12 meses'!AC6+('Estado de resultados PyG - 5 añ'!E21*'Flujo de caja - 12 meses'!AC6)</f>
@@ -20401,7 +20461,7 @@
       </c>
       <c r="H6" s="40">
         <f t="shared" si="3"/>
-        <v>3.152623261896326E-3</v>
+        <v>3.143652816604686E-3</v>
       </c>
       <c r="I6" s="42">
         <f>'Flujo de caja - 12 meses'!AC6+('Estado de resultados PyG - 5 añ'!E21*'Flujo de caja - 12 meses'!AC6)</f>
@@ -20409,7 +20469,7 @@
       </c>
       <c r="J6" s="40">
         <f t="shared" si="4"/>
-        <v>3.0915119892062637E-3</v>
+        <v>3.0828854683796645E-3</v>
       </c>
       <c r="K6" s="42">
         <f>'Flujo de caja - 12 meses'!AC6+('Estado de resultados PyG - 5 añ'!E21*'Flujo de caja - 12 meses'!AC6)</f>
@@ -20417,7 +20477,7 @@
       </c>
       <c r="L6" s="40">
         <f t="shared" si="5"/>
-        <v>3.0864111721915256E-3</v>
+        <v>3.0778130548219365E-3</v>
       </c>
       <c r="M6" s="45">
         <f>'Flujo de caja - 12 meses'!AC6+('Estado de resultados PyG - 5 añ'!E21*'Flujo de caja - 12 meses'!AC6)</f>
@@ -20446,7 +20506,7 @@
         <f>E7/$C$2</f>
         <v>1.1651937777503047</v>
       </c>
-      <c r="E7" s="87">
+      <c r="E7" s="80">
         <f>'Estado de resultados PyG - 5 añ'!C10</f>
         <v>4285000.1176767461</v>
       </c>
@@ -20547,54 +20607,36 @@
     </row>
     <row r="9" spans="1:20" ht="15.75" customHeight="1">
       <c r="A9" s="39" t="s">
-        <v>87</v>
-      </c>
-      <c r="B9" s="63">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
+        <v>309</v>
+      </c>
+      <c r="B9" s="63"/>
       <c r="C9" s="41">
         <v>0</v>
       </c>
-      <c r="D9" s="40">
-        <f t="shared" si="1"/>
-        <v>0.28267263232493417</v>
-      </c>
-      <c r="E9" s="41">
-        <f>'Estado de resultados PyG - 5 añ'!C15</f>
-        <v>47111662.785648078</v>
-      </c>
-      <c r="F9" s="40">
-        <f t="shared" si="2"/>
-        <v>0.42990874779661692</v>
-      </c>
+      <c r="D9" s="40"/>
+      <c r="E9" s="33">
+        <f>'Estado de resultados PyG - 5 añ'!C7</f>
+        <v>700000.01214951661</v>
+      </c>
+      <c r="F9" s="40"/>
       <c r="G9" s="41">
-        <f>'Estado de resultados PyG - 5 añ'!E15</f>
-        <v>82292959.708528847</v>
-      </c>
-      <c r="H9" s="40">
-        <f t="shared" si="3"/>
-        <v>0.55272957457918814</v>
-      </c>
+        <f>'Estado de resultados PyG - 5 añ'!E7</f>
+        <v>700000</v>
+      </c>
+      <c r="H9" s="40"/>
       <c r="I9" s="41">
-        <f>'Estado de resultados PyG - 5 añ'!G15</f>
-        <v>135591141.71245098</v>
-      </c>
-      <c r="J9" s="40">
-        <f t="shared" si="4"/>
-        <v>0.55902463488988974</v>
-      </c>
+        <f>'Estado de resultados PyG - 5 añ'!G7</f>
+        <v>700000</v>
+      </c>
+      <c r="J9" s="40"/>
       <c r="K9" s="41">
-        <f>'Estado de resultados PyG - 5 añ'!I15</f>
-        <v>139846210.37927929</v>
-      </c>
-      <c r="L9" s="40">
-        <f t="shared" si="5"/>
-        <v>0.55880380772314575</v>
-      </c>
+        <f>'Estado de resultados PyG - 5 añ'!I7</f>
+        <v>700000</v>
+      </c>
+      <c r="L9" s="40"/>
       <c r="M9" s="53">
-        <f>'Estado de resultados PyG - 5 añ'!K15</f>
-        <v>140021996.25749597</v>
+        <f>'Estado de resultados PyG - 5 añ'!K7</f>
+        <v>700000</v>
       </c>
       <c r="N9" s="54"/>
       <c r="O9" s="54"/>
@@ -20605,214 +20647,273 @@
       <c r="T9" s="54"/>
     </row>
     <row r="10" spans="1:20" ht="15.75" customHeight="1">
-      <c r="A10" s="30" t="s">
+      <c r="A10" s="39" t="s">
+        <v>87</v>
+      </c>
+      <c r="B10" s="63">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="C10" s="41">
+        <v>0</v>
+      </c>
+      <c r="D10" s="40">
+        <f t="shared" si="1"/>
+        <v>0.28149036167834385</v>
+      </c>
+      <c r="E10" s="33">
+        <f>'Estado de resultados PyG - 5 añ'!C15</f>
+        <v>47111662.785648078</v>
+      </c>
+      <c r="F10" s="40">
+        <f t="shared" si="2"/>
+        <v>0.42834234787445302</v>
+      </c>
+      <c r="G10" s="41">
+        <f>'Estado de resultados PyG - 5 añ'!E15</f>
+        <v>82292959.708528847</v>
+      </c>
+      <c r="H10" s="40">
+        <f t="shared" si="3"/>
+        <v>0.55115684292115563</v>
+      </c>
+      <c r="I10" s="41">
+        <f>'Estado de resultados PyG - 5 añ'!G15</f>
+        <v>135591141.71245098</v>
+      </c>
+      <c r="J10" s="40">
+        <f t="shared" si="4"/>
+        <v>0.55746473873800784</v>
+      </c>
+      <c r="K10" s="41">
+        <f>'Estado de resultados PyG - 5 añ'!I15</f>
+        <v>139846210.37927929</v>
+      </c>
+      <c r="L10" s="40">
+        <f t="shared" si="5"/>
+        <v>0.55724709332013078</v>
+      </c>
+      <c r="M10" s="53">
+        <f>'Estado de resultados PyG - 5 añ'!K15</f>
+        <v>140021996.25749597</v>
+      </c>
+      <c r="N10" s="54"/>
+      <c r="O10" s="54"/>
+      <c r="P10" s="54"/>
+      <c r="Q10" s="54"/>
+      <c r="R10" s="54"/>
+      <c r="S10" s="54"/>
+      <c r="T10" s="54"/>
+    </row>
+    <row r="11" spans="1:20" ht="15.75" customHeight="1">
+      <c r="A11" s="30" t="s">
         <v>89</v>
       </c>
-      <c r="B10" s="62">
-        <f>C10/$C$10</f>
+      <c r="B11" s="62">
+        <f>C11/$C$11</f>
         <v>1</v>
       </c>
-      <c r="C10" s="33">
-        <f>SUM(C11:C12)</f>
+      <c r="C11" s="33">
+        <f>SUM(C12:C13)</f>
         <v>62190000</v>
       </c>
-      <c r="D10" s="32">
-        <f>E10/$E$10</f>
+      <c r="D11" s="32">
+        <f>E11/$E$11</f>
         <v>1</v>
       </c>
-      <c r="E10" s="33">
-        <f>SUM(E11:E12)</f>
+      <c r="E11" s="33">
+        <f>SUM(E12:E13)</f>
         <v>199937934.20591292</v>
       </c>
-      <c r="F10" s="32">
-        <f>G10/$G$10</f>
+      <c r="F11" s="32">
+        <f>G11/$G$11</f>
         <v>1</v>
       </c>
-      <c r="G10" s="33">
-        <f>SUM(G11:G12)</f>
+      <c r="G11" s="33">
+        <f>SUM(G12:G13)</f>
         <v>351864755.14782721</v>
       </c>
-      <c r="H10" s="32">
-        <f>I10/$I$10</f>
+      <c r="H11" s="32">
+        <f>I11/$I$11</f>
         <v>1</v>
       </c>
-      <c r="I10" s="33">
-        <f>SUM(I11:I12)</f>
+      <c r="I11" s="33">
+        <f>SUM(I12:I13)</f>
         <v>509221881.16382653</v>
       </c>
-      <c r="J10" s="32">
-        <f>K10/$K$10</f>
+      <c r="J11" s="32">
+        <f>K11/$K$11</f>
         <v>1</v>
       </c>
-      <c r="K10" s="33">
-        <f>SUM(K11:K12)</f>
+      <c r="K11" s="33">
+        <f>SUM(K12:K13)</f>
         <v>522334556.18837321</v>
       </c>
-      <c r="L10" s="32">
-        <f>M10/$M$10</f>
+      <c r="L11" s="32">
+        <f>M11/$M$11</f>
         <v>1</v>
       </c>
-      <c r="M10" s="37">
-        <f>SUM(M11:M12)</f>
+      <c r="M11" s="37">
+        <f>SUM(M12:M13)</f>
         <v>523090680.34961951</v>
       </c>
-      <c r="N10" s="38"/>
-      <c r="O10" s="38"/>
-      <c r="P10" s="38"/>
-      <c r="Q10" s="38"/>
-      <c r="R10" s="38"/>
-      <c r="S10" s="38"/>
-      <c r="T10" s="38"/>
-    </row>
-    <row r="11" spans="1:20" ht="15.75" customHeight="1">
-      <c r="A11" s="39" t="s">
+      <c r="N11" s="38"/>
+      <c r="O11" s="38"/>
+      <c r="P11" s="38"/>
+      <c r="Q11" s="38"/>
+      <c r="R11" s="38"/>
+      <c r="S11" s="38"/>
+      <c r="T11" s="38"/>
+    </row>
+    <row r="12" spans="1:20" ht="15.75" customHeight="1">
+      <c r="A12" s="39" t="s">
         <v>91</v>
       </c>
-      <c r="B11" s="63">
-        <f>C11/$C$10</f>
-        <v>0</v>
-      </c>
-      <c r="C11" s="41">
-        <v>0</v>
-      </c>
-      <c r="D11" s="40">
-        <f>E11/$E$10</f>
+      <c r="B12" s="63">
+        <f>C12/$C$11</f>
+        <v>0</v>
+      </c>
+      <c r="C12" s="41">
+        <v>0</v>
+      </c>
+      <c r="D12" s="40">
+        <f>E12/$E$11</f>
         <v>1</v>
       </c>
-      <c r="E11" s="41">
+      <c r="E12" s="41">
         <f>'Estado de resultados PyG - 5 añ'!C3</f>
         <v>199937934.20591292</v>
       </c>
-      <c r="F11" s="40">
-        <f>G11/$G$10</f>
+      <c r="F12" s="40">
+        <f>G12/$G$11</f>
         <v>1</v>
       </c>
-      <c r="G11" s="41">
+      <c r="G12" s="41">
         <f>'Estado de resultados PyG - 5 añ'!E3</f>
         <v>351864755.14782721</v>
       </c>
-      <c r="H11" s="40">
-        <f>I11/$I$10</f>
+      <c r="H12" s="40">
+        <f>I12/$I$11</f>
         <v>1</v>
       </c>
-      <c r="I11" s="41">
+      <c r="I12" s="41">
         <f>'Estado de resultados PyG - 5 añ'!G3</f>
         <v>509221881.16382653</v>
       </c>
-      <c r="J11" s="40">
-        <f>K11/$K$10</f>
+      <c r="J12" s="40">
+        <f>K12/$K$11</f>
         <v>1</v>
       </c>
-      <c r="K11" s="41">
+      <c r="K12" s="41">
         <f>'Estado de resultados PyG - 5 añ'!I3</f>
         <v>522334556.18837321</v>
       </c>
-      <c r="L11" s="40">
-        <f>M11/$K$10</f>
+      <c r="L12" s="40">
+        <f>M12/$K$11</f>
         <v>1.0014475859433156</v>
       </c>
-      <c r="M11" s="53">
+      <c r="M12" s="53">
         <f>'Estado de resultados PyG - 5 añ'!K3</f>
         <v>523090680.34961951</v>
       </c>
-      <c r="N11" s="54"/>
-      <c r="O11" s="47"/>
-      <c r="P11" s="47"/>
-      <c r="Q11" s="47"/>
-      <c r="R11" s="47"/>
-      <c r="S11" s="47"/>
-      <c r="T11" s="47"/>
-    </row>
-    <row r="12" spans="1:20" ht="15.75" customHeight="1">
-      <c r="A12" s="39" t="s">
+      <c r="N12" s="54"/>
+      <c r="O12" s="47"/>
+      <c r="P12" s="47"/>
+      <c r="Q12" s="47"/>
+      <c r="R12" s="47"/>
+      <c r="S12" s="47"/>
+      <c r="T12" s="47"/>
+    </row>
+    <row r="13" spans="1:20" ht="15.75" customHeight="1">
+      <c r="A13" s="39" t="s">
         <v>93</v>
       </c>
-      <c r="B12" s="63">
-        <f>C12/$C$10</f>
+      <c r="B13" s="63">
+        <f>C13/$C$11</f>
         <v>1</v>
       </c>
-      <c r="C12" s="41">
+      <c r="C13" s="41">
         <v>62190000</v>
       </c>
-      <c r="D12" s="40">
-        <v>0</v>
-      </c>
-      <c r="E12" s="41">
-        <v>0</v>
-      </c>
-      <c r="F12" s="40">
-        <v>0</v>
-      </c>
-      <c r="G12" s="41">
-        <v>0</v>
-      </c>
-      <c r="H12" s="40">
-        <v>0</v>
-      </c>
-      <c r="I12" s="41">
-        <v>0</v>
-      </c>
-      <c r="J12" s="40">
-        <v>0</v>
-      </c>
-      <c r="K12" s="41">
-        <v>0</v>
-      </c>
-      <c r="L12" s="40">
-        <v>0</v>
-      </c>
-      <c r="M12" s="53">
-        <v>0</v>
-      </c>
-      <c r="N12" s="54"/>
-      <c r="O12" s="54"/>
-      <c r="P12" s="54"/>
-      <c r="Q12" s="54"/>
-      <c r="R12" s="54"/>
-      <c r="S12" s="54"/>
-      <c r="T12" s="54"/>
-    </row>
-    <row r="13" spans="1:20" ht="15.75" customHeight="1">
-      <c r="A13" s="30" t="s">
+      <c r="D13" s="40">
+        <v>0</v>
+      </c>
+      <c r="E13" s="41">
+        <v>0</v>
+      </c>
+      <c r="F13" s="40">
+        <v>0</v>
+      </c>
+      <c r="G13" s="41">
+        <v>0</v>
+      </c>
+      <c r="H13" s="40">
+        <v>0</v>
+      </c>
+      <c r="I13" s="41">
+        <v>0</v>
+      </c>
+      <c r="J13" s="40">
+        <v>0</v>
+      </c>
+      <c r="K13" s="41">
+        <v>0</v>
+      </c>
+      <c r="L13" s="40">
+        <v>0</v>
+      </c>
+      <c r="M13" s="53">
+        <v>0</v>
+      </c>
+      <c r="N13" s="54"/>
+      <c r="O13" s="54"/>
+      <c r="P13" s="54"/>
+      <c r="Q13" s="54"/>
+      <c r="R13" s="54"/>
+      <c r="S13" s="54"/>
+      <c r="T13" s="54"/>
+    </row>
+    <row r="14" spans="1:20" ht="15.75" customHeight="1">
+      <c r="A14" s="30" t="s">
         <v>94</v>
       </c>
-      <c r="B13" s="57"/>
-      <c r="C13" s="58">
-        <f>C10-C2</f>
+      <c r="B14" s="57"/>
+      <c r="C14" s="58">
+        <f>C11-C2</f>
         <v>58512500</v>
       </c>
-      <c r="D13" s="57"/>
-      <c r="E13" s="58">
-        <f>C13-E2+E10</f>
-        <v>91785333.314600259</v>
-      </c>
-      <c r="F13" s="57"/>
-      <c r="G13" s="58">
-        <f>E13-G2+G10</f>
-        <v>252230490.39586207</v>
-      </c>
-      <c r="H13" s="57"/>
-      <c r="I13" s="58">
-        <f>G13-I2+I10</f>
-        <v>516140472.30826688</v>
-      </c>
-      <c r="J13" s="57"/>
-      <c r="K13" s="58">
-        <f>I13-K2+K10</f>
-        <v>788313941.39745593</v>
-      </c>
-      <c r="L13" s="57"/>
-      <c r="M13" s="59">
-        <f>K13-M2+M10</f>
-        <v>1060830101.097301</v>
-      </c>
-      <c r="N13" s="60"/>
-      <c r="O13" s="60"/>
-      <c r="P13" s="60"/>
-      <c r="Q13" s="60"/>
-      <c r="R13" s="60"/>
-      <c r="S13" s="60"/>
-      <c r="T13" s="60"/>
+      <c r="D14" s="57"/>
+      <c r="E14" s="58">
+        <f>C14-E2+E11</f>
+        <v>91085333.302450746</v>
+      </c>
+      <c r="F14" s="57"/>
+      <c r="G14" s="58">
+        <f>E14-G2+G11</f>
+        <v>250830490.38371256</v>
+      </c>
+      <c r="H14" s="57"/>
+      <c r="I14" s="58">
+        <f>G14-I2+I11</f>
+        <v>514040472.29611742</v>
+      </c>
+      <c r="J14" s="57"/>
+      <c r="K14" s="58">
+        <f>I14-K2+K11</f>
+        <v>785513941.3853066</v>
+      </c>
+      <c r="L14" s="57"/>
+      <c r="M14" s="59">
+        <f>K14-M2+M11</f>
+        <v>1057330101.0851517</v>
+      </c>
+      <c r="N14" s="60"/>
+      <c r="O14" s="60"/>
+      <c r="P14" s="60"/>
+      <c r="Q14" s="60"/>
+      <c r="R14" s="60"/>
+      <c r="S14" s="60"/>
+      <c r="T14" s="60"/>
     </row>
   </sheetData>
   <mergeCells count="6">
@@ -20824,5 +20925,6 @@
     <mergeCell ref="J1:K1"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>